<commit_message>
template and stack mods pulling back from 8.1 configs
</commit_message>
<xml_diff>
--- a/templates/panos/set_commands/iron_skillet_panos_full.xlsx
+++ b/templates/panos/set_commands/iron_skillet_panos_full.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="699">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="701">
   <si>
     <t>Variable Name</t>
   </si>
@@ -38,7 +38,7 @@
     <t>PANORAMA_TYPE</t>
   </si>
   <si>
-    <t>cloud</t>
+    <t>static</t>
   </si>
   <si>
     <t>Panorama management IP type - static or cloud (for dhcp)</t>
@@ -47,7 +47,7 @@
     <t>PANORAMA_IP</t>
   </si>
   <si>
-    <t>192.168.55.7</t>
+    <t>192.168.55.8</t>
   </si>
   <si>
     <t>Panorama IP</t>
@@ -80,6 +80,15 @@
     <t>IP address for scheduled config exports</t>
   </si>
   <si>
+    <t>TEMPLATE</t>
+  </si>
+  <si>
+    <t>sample_template</t>
+  </si>
+  <si>
+    <t>Template name for Panorama</t>
+  </si>
+  <si>
     <t>STACK</t>
   </si>
   <si>
@@ -110,10 +119,7 @@
     <t>MGMT_TYPE</t>
   </si>
   <si>
-    <t>dhcp-cloud</t>
-  </si>
-  <si>
-    <t>firewall management IP type (static or dhcp-cloud)</t>
+    <t>firewall management IP type (static or dhcp-client)</t>
   </si>
   <si>
     <t>MGMT_IP</t>
@@ -3068,7 +3074,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3204,73 +3210,73 @@
         <v>33</v>
       </c>
       <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
         <v>34</v>
-      </c>
-      <c r="C12" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" t="s">
         <v>36</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>37</v>
-      </c>
-      <c r="C13" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" t="s">
         <v>39</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>40</v>
-      </c>
-      <c r="C14" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" t="s">
         <v>42</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>43</v>
-      </c>
-      <c r="C15" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" t="s">
         <v>45</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>46</v>
-      </c>
-      <c r="C16" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" t="s">
         <v>48</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>49</v>
-      </c>
-      <c r="C17" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" t="s">
         <v>51</v>
-      </c>
-      <c r="B18" t="s">
-        <v>49</v>
       </c>
       <c r="C18" t="s">
         <v>52</v>
@@ -3281,109 +3287,120 @@
         <v>53</v>
       </c>
       <c r="B19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" t="s">
         <v>54</v>
-      </c>
-      <c r="C19" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" t="s">
         <v>56</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>57</v>
-      </c>
-      <c r="C20" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" t="s">
         <v>59</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>60</v>
-      </c>
-      <c r="C21" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" t="s">
         <v>62</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>63</v>
-      </c>
-      <c r="C22" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" t="s">
         <v>65</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>66</v>
-      </c>
-      <c r="C23" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" t="s">
         <v>68</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>69</v>
-      </c>
-      <c r="C24" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" t="s">
         <v>71</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>72</v>
-      </c>
-      <c r="C25" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" t="s">
         <v>74</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>75</v>
-      </c>
-      <c r="C26" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
+        <v>76</v>
+      </c>
+      <c r="B27" t="s">
         <v>77</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>78</v>
-      </c>
-      <c r="C27" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
+        <v>79</v>
+      </c>
+      <c r="B28" t="s">
         <v>80</v>
-      </c>
-      <c r="B28" t="b">
-        <v>1</v>
       </c>
       <c r="C28" t="s">
         <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29" t="b">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -3401,3358 +3418,3358 @@
   <sheetData>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8">
-        <f>SUBSTITUTE("set deviceconfig system hostname {{ FW_NAME }}", "{{ FW_NAME }}", 'values'!B10)</f>
+        <f>SUBSTITUTE("set deviceconfig system hostname {{ FW_NAME }}", "{{ FW_NAME }}", 'values'!B11)</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9">
-        <f>SUBSTITUTE("set deviceconfig system ip-address {{ MGMT_IP }}", "{{ MGMT_IP }}", 'values'!B12)</f>
+        <f>SUBSTITUTE("set deviceconfig system ip-address {{ MGMT_IP }}", "{{ MGMT_IP }}", 'values'!B13)</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10">
-        <f>SUBSTITUTE("set deviceconfig system netmask {{ MGMT_MASK }}", "{{ MGMT_MASK }}", 'values'!B13)</f>
+        <f>SUBSTITUTE("set deviceconfig system netmask {{ MGMT_MASK }}", "{{ MGMT_MASK }}", 'values'!B14)</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11">
-        <f>SUBSTITUTE("set deviceconfig system default-gateway {{ MGMT_DG }}", "{{ MGMT_DG }}", 'values'!B14)</f>
+        <f>SUBSTITUTE("set deviceconfig system default-gateway {{ MGMT_DG }}", "{{ MGMT_DG }}", 'values'!B15)</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12">
-        <f>SUBSTITUTE("set deviceconfig system dns-setting servers primary {{ DNS_1 }}", "{{ DNS_1 }}", 'values'!B19)</f>
+        <f>SUBSTITUTE("set deviceconfig system dns-setting servers primary {{ DNS_1 }}", "{{ DNS_1 }}", 'values'!B20)</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13">
-        <f>SUBSTITUTE("set deviceconfig system dns-setting servers secondary {{ DNS_2 }}", "{{ DNS_2 }}", 'values'!B20)</f>
+        <f>SUBSTITUTE("set deviceconfig system dns-setting servers secondary {{ DNS_2 }}", "{{ DNS_2 }}", 'values'!B21)</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14">
-        <f>SUBSTITUTE("set deviceconfig system ntp-servers primary-ntp-server ntp-server-address {{ NTP_1 }}", "{{ NTP_1 }}", 'values'!B15)</f>
+        <f>SUBSTITUTE("set deviceconfig system ntp-servers primary-ntp-server ntp-server-address {{ NTP_1 }}", "{{ NTP_1 }}", 'values'!B16)</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15">
-        <f>SUBSTITUTE("set deviceconfig system ntp-servers secondary-ntp-server ntp-server-address {{ NTP_2 }}", "{{ NTP_2 }}", 'values'!B16)</f>
+        <f>SUBSTITUTE("set deviceconfig system ntp-servers secondary-ntp-server ntp-server-address {{ NTP_2 }}", "{{ NTP_2 }}", 'values'!B17)</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18">
-        <f>SUBSTITUTE("set mgt-config users {{ ADMINISTRATOR_USERNAME }} password", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B17)</f>
+        <f>SUBSTITUTE("set mgt-config users {{ ADMINISTRATOR_USERNAME }} password", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B18)</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19">
-        <f>SUBSTITUTE("set mgt-config users {{ ADMINISTRATOR_USERNAME }} permissions role-based superuser yes", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B17)</f>
+        <f>SUBSTITUTE("set mgt-config users {{ ADMINISTRATOR_USERNAME }} permissions role-based superuser yes", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B18)</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73">
-        <f>SUBSTITUTE("set shared log-settings email Sample_Email_Profile server Sample_Email_Profile gateway {{ EMAIL_PROFILE_GATEWAY }}", "{{ EMAIL_PROFILE_GATEWAY }}", 'values'!B24)</f>
+        <f>SUBSTITUTE("set shared log-settings email Sample_Email_Profile server Sample_Email_Profile gateway {{ EMAIL_PROFILE_GATEWAY }}", "{{ EMAIL_PROFILE_GATEWAY }}", 'values'!B25)</f>
         <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74">
-        <f>SUBSTITUTE("set shared log-settings email Sample_Email_Profile server Sample_Email_Profile from {{ EMAIL_PROFILE_FROM }}", "{{ EMAIL_PROFILE_FROM }}", 'values'!B25)</f>
+        <f>SUBSTITUTE("set shared log-settings email Sample_Email_Profile server Sample_Email_Profile from {{ EMAIL_PROFILE_FROM }}", "{{ EMAIL_PROFILE_FROM }}", 'values'!B26)</f>
         <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75">
-        <f>SUBSTITUTE("set shared log-settings email Sample_Email_Profile server Sample_Email_Profile to {{ EMAIL_PROFILE_TO }}", "{{ EMAIL_PROFILE_TO }}", 'values'!B26)</f>
+        <f>SUBSTITUTE("set shared log-settings email Sample_Email_Profile server Sample_Email_Profile to {{ EMAIL_PROFILE_TO }}", "{{ EMAIL_PROFILE_TO }}", 'values'!B27)</f>
         <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79">
-        <f>SUBSTITUTE("set shared log-settings syslog Sample_Syslog_Profile server Sample_Syslog server {{ SYSLOG_SERVER }}", "{{ SYSLOG_SERVER }}", 'values'!B27)</f>
+        <f>SUBSTITUTE("set shared log-settings syslog Sample_Syslog_Profile server Sample_Syslog server {{ SYSLOG_SERVER }}", "{{ SYSLOG_SERVER }}", 'values'!B28)</f>
         <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="85" spans="1:1">
       <c r="A85" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="87" spans="1:1">
       <c r="A87" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="89" spans="1:1">
       <c r="A89" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="90" spans="1:1">
       <c r="A90" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="91" spans="1:1">
       <c r="A91" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="92" spans="1:1">
       <c r="A92" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="94" spans="1:1">
       <c r="A94" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="95" spans="1:1">
       <c r="A95" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="96" spans="1:1">
       <c r="A96" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="97" spans="1:1">
       <c r="A97" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="98" spans="1:1">
       <c r="A98" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="100" spans="1:1">
       <c r="A100" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="102" spans="1:1">
       <c r="A102" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="104" spans="1:1">
       <c r="A104" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="105" spans="1:1">
       <c r="A105" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="106" spans="1:1">
       <c r="A106" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="107" spans="1:1">
       <c r="A107" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="108" spans="1:1">
       <c r="A108" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="109" spans="1:1">
       <c r="A109" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="110" spans="1:1">
       <c r="A110" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="111" spans="1:1">
       <c r="A111" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="112" spans="1:1">
       <c r="A112" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="113" spans="1:1">
       <c r="A113" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="114" spans="1:1">
       <c r="A114" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="115" spans="1:1">
       <c r="A115" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="116" spans="1:1">
       <c r="A116" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="117" spans="1:1">
       <c r="A117" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="118" spans="1:1">
       <c r="A118" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="119" spans="1:1">
       <c r="A119" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="120" spans="1:1">
       <c r="A120" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="121" spans="1:1">
       <c r="A121" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="122" spans="1:1">
       <c r="A122" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="123" spans="1:1">
       <c r="A123" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="124" spans="1:1">
       <c r="A124" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="125" spans="1:1">
       <c r="A125" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="126" spans="1:1">
       <c r="A126" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="127" spans="1:1">
       <c r="A127" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="128" spans="1:1">
       <c r="A128" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="129" spans="1:1">
       <c r="A129" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="130" spans="1:1">
       <c r="A130" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="131" spans="1:1">
       <c r="A131" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="132" spans="1:1">
       <c r="A132" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="133" spans="1:1">
       <c r="A133" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="134" spans="1:1">
       <c r="A134" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="135" spans="1:1">
       <c r="A135" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="136" spans="1:1">
       <c r="A136" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="137" spans="1:1">
       <c r="A137" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="138" spans="1:1">
       <c r="A138" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="139" spans="1:1">
       <c r="A139" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="140" spans="1:1">
       <c r="A140" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="141" spans="1:1">
       <c r="A141" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="142" spans="1:1">
       <c r="A142" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="143" spans="1:1">
       <c r="A143" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="144" spans="1:1">
       <c r="A144" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="145" spans="1:1">
       <c r="A145" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="146" spans="1:1">
       <c r="A146" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="147" spans="1:1">
       <c r="A147" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="148" spans="1:1">
       <c r="A148" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="149" spans="1:1">
       <c r="A149" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="150" spans="1:1">
       <c r="A150" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="151" spans="1:1">
       <c r="A151" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
     <row r="152" spans="1:1">
       <c r="A152" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="153" spans="1:1">
       <c r="A153" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="154" spans="1:1">
       <c r="A154">
-        <f>SUBSTITUTE("set address Sinkhole-IPv4 ip-netmask {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B21)</f>
+        <f>SUBSTITUTE("set address Sinkhole-IPv4 ip-netmask {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
         <v>0</v>
       </c>
     </row>
     <row r="155" spans="1:1">
       <c r="A155">
-        <f>SUBSTITUTE("set address Sinkhole-IPv6 ip-netmask {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B22)</f>
+        <f>SUBSTITUTE("set address Sinkhole-IPv6 ip-netmask {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
         <v>0</v>
       </c>
     </row>
     <row r="156" spans="1:1">
       <c r="A156" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="157" spans="1:1">
       <c r="A157" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="158" spans="1:1">
       <c r="A158" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="159" spans="1:1">
       <c r="A159" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="160" spans="1:1">
       <c r="A160" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="161" spans="1:1">
       <c r="A161" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
     </row>
     <row r="162" spans="1:1">
       <c r="A162" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="163" spans="1:1">
       <c r="A163" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="164" spans="1:1">
       <c r="A164" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="165" spans="1:1">
       <c r="A165" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="166" spans="1:1">
       <c r="A166" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="167" spans="1:1">
       <c r="A167" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
     </row>
     <row r="168" spans="1:1">
       <c r="A168" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="169" spans="1:1">
       <c r="A169" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="170" spans="1:1">
       <c r="A170" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="171" spans="1:1">
       <c r="A171" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="172" spans="1:1">
       <c r="A172" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="173" spans="1:1">
       <c r="A173" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="174" spans="1:1">
       <c r="A174" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="175" spans="1:1">
       <c r="A175" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="176" spans="1:1">
       <c r="A176" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="177" spans="1:1">
       <c r="A177" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="178" spans="1:1">
       <c r="A178" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="179" spans="1:1">
       <c r="A179" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="180" spans="1:1">
       <c r="A180" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="181" spans="1:1">
       <c r="A181" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
     <row r="182" spans="1:1">
       <c r="A182" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="183" spans="1:1">
       <c r="A183" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="184" spans="1:1">
       <c r="A184" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="185" spans="1:1">
       <c r="A185" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="186" spans="1:1">
       <c r="A186" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="187" spans="1:1">
       <c r="A187" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="188" spans="1:1">
       <c r="A188">
-        <f>SUBSTITUTE("set profiles spyware Outbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B21)</f>
+        <f>SUBSTITUTE("set profiles spyware Outbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
         <v>0</v>
       </c>
     </row>
     <row r="189" spans="1:1">
       <c r="A189">
-        <f>SUBSTITUTE("set profiles spyware Outbound-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B22)</f>
+        <f>SUBSTITUTE("set profiles spyware Outbound-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
         <v>0</v>
       </c>
     </row>
     <row r="190" spans="1:1">
       <c r="A190" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
     </row>
     <row r="191" spans="1:1">
       <c r="A191" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="192" spans="1:1">
       <c r="A192" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
     <row r="193" spans="1:1">
       <c r="A193" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="194" spans="1:1">
       <c r="A194" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="195" spans="1:1">
       <c r="A195" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="196" spans="1:1">
       <c r="A196" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="197" spans="1:1">
       <c r="A197" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="198" spans="1:1">
       <c r="A198" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row r="199" spans="1:1">
       <c r="A199" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="200" spans="1:1">
       <c r="A200" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
     </row>
     <row r="201" spans="1:1">
       <c r="A201" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="202" spans="1:1">
       <c r="A202">
-        <f>SUBSTITUTE("set profiles spyware Inbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B21)</f>
+        <f>SUBSTITUTE("set profiles spyware Inbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
         <v>0</v>
       </c>
     </row>
     <row r="203" spans="1:1">
       <c r="A203">
-        <f>SUBSTITUTE("set profiles spyware Inbound-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B22)</f>
+        <f>SUBSTITUTE("set profiles spyware Inbound-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
         <v>0</v>
       </c>
     </row>
     <row r="204" spans="1:1">
       <c r="A204" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="205" spans="1:1">
       <c r="A205" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="206" spans="1:1">
       <c r="A206" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
     <row r="207" spans="1:1">
       <c r="A207" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="208" spans="1:1">
       <c r="A208" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row r="209" spans="1:1">
       <c r="A209" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="210" spans="1:1">
       <c r="A210" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
     <row r="211" spans="1:1">
       <c r="A211" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="212" spans="1:1">
       <c r="A212" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="213" spans="1:1">
       <c r="A213" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="214" spans="1:1">
       <c r="A214" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
     </row>
     <row r="215" spans="1:1">
       <c r="A215" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="216" spans="1:1">
       <c r="A216">
-        <f>SUBSTITUTE("set profiles spyware Internal-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B21)</f>
+        <f>SUBSTITUTE("set profiles spyware Internal-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
         <v>0</v>
       </c>
     </row>
     <row r="217" spans="1:1">
       <c r="A217">
-        <f>SUBSTITUTE("set profiles spyware Internal-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B22)</f>
+        <f>SUBSTITUTE("set profiles spyware Internal-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
         <v>0</v>
       </c>
     </row>
     <row r="218" spans="1:1">
       <c r="A218" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
     </row>
     <row r="219" spans="1:1">
       <c r="A219" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="220" spans="1:1">
       <c r="A220" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="221" spans="1:1">
       <c r="A221" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="222" spans="1:1">
       <c r="A222" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
     </row>
     <row r="223" spans="1:1">
       <c r="A223" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
     <row r="224" spans="1:1">
       <c r="A224" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="225" spans="1:1">
       <c r="A225" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="226" spans="1:1">
       <c r="A226" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="227" spans="1:1">
       <c r="A227" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="228" spans="1:1">
       <c r="A228" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="229" spans="1:1">
       <c r="A229" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
     </row>
     <row r="230" spans="1:1">
       <c r="A230" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
     </row>
     <row r="231" spans="1:1">
       <c r="A231">
-        <f>SUBSTITUTE("set profiles spyware Alert-Only-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B21)</f>
+        <f>SUBSTITUTE("set profiles spyware Alert-Only-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
         <v>0</v>
       </c>
     </row>
     <row r="232" spans="1:1">
       <c r="A232">
-        <f>SUBSTITUTE("set profiles spyware Alert-Only-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B22)</f>
+        <f>SUBSTITUTE("set profiles spyware Alert-Only-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
         <v>0</v>
       </c>
     </row>
     <row r="233" spans="1:1">
       <c r="A233" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="234" spans="1:1">
       <c r="A234" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
     </row>
     <row r="235" spans="1:1">
       <c r="A235" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
     </row>
     <row r="236" spans="1:1">
       <c r="A236" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="237" spans="1:1">
       <c r="A237" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
     </row>
     <row r="238" spans="1:1">
       <c r="A238" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
     </row>
     <row r="239" spans="1:1">
       <c r="A239" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
     </row>
     <row r="240" spans="1:1">
       <c r="A240">
-        <f>SUBSTITUTE("set profiles spyware Exception-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B21)</f>
+        <f>SUBSTITUTE("set profiles spyware Exception-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
         <v>0</v>
       </c>
     </row>
     <row r="241" spans="1:1">
       <c r="A241">
-        <f>SUBSTITUTE("set profiles spyware Exception-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B22)</f>
+        <f>SUBSTITUTE("set profiles spyware Exception-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
         <v>0</v>
       </c>
     </row>
     <row r="242" spans="1:1">
       <c r="A242" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
     </row>
     <row r="243" spans="1:1">
       <c r="A243" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
     </row>
     <row r="244" spans="1:1">
       <c r="A244" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="245" spans="1:1">
       <c r="A245" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="246" spans="1:1">
       <c r="A246" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="247" spans="1:1">
       <c r="A247" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
     </row>
     <row r="248" spans="1:1">
       <c r="A248" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="249" spans="1:1">
       <c r="A249" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="250" spans="1:1">
       <c r="A250" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="251" spans="1:1">
       <c r="A251" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="252" spans="1:1">
       <c r="A252" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="253" spans="1:1">
       <c r="A253" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
     </row>
     <row r="254" spans="1:1">
       <c r="A254" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
     <row r="255" spans="1:1">
       <c r="A255" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
     </row>
     <row r="256" spans="1:1">
       <c r="A256" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
     </row>
     <row r="257" spans="1:1">
       <c r="A257" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
     <row r="258" spans="1:1">
       <c r="A258" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
     </row>
     <row r="259" spans="1:1">
       <c r="A259" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="260" spans="1:1">
       <c r="A260" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="261" spans="1:1">
       <c r="A261" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="262" spans="1:1">
       <c r="A262" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="263" spans="1:1">
       <c r="A263" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="264" spans="1:1">
       <c r="A264" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
     </row>
     <row r="265" spans="1:1">
       <c r="A265" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
     </row>
     <row r="266" spans="1:1">
       <c r="A266" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
     </row>
     <row r="267" spans="1:1">
       <c r="A267" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
     </row>
     <row r="268" spans="1:1">
       <c r="A268" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
     </row>
     <row r="269" spans="1:1">
       <c r="A269" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="270" spans="1:1">
       <c r="A270" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
     </row>
     <row r="271" spans="1:1">
       <c r="A271" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
     </row>
     <row r="272" spans="1:1">
       <c r="A272" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="273" spans="1:1">
       <c r="A273" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
     </row>
     <row r="274" spans="1:1">
       <c r="A274" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
     </row>
     <row r="275" spans="1:1">
       <c r="A275" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
     </row>
     <row r="276" spans="1:1">
       <c r="A276" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
     </row>
     <row r="277" spans="1:1">
       <c r="A277" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
     </row>
     <row r="278" spans="1:1">
       <c r="A278" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
     </row>
     <row r="279" spans="1:1">
       <c r="A279" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
     <row r="280" spans="1:1">
       <c r="A280" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
     <row r="281" spans="1:1">
       <c r="A281" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
     </row>
     <row r="282" spans="1:1">
       <c r="A282" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
     <row r="283" spans="1:1">
       <c r="A283" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
     </row>
     <row r="284" spans="1:1">
       <c r="A284" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
     </row>
     <row r="285" spans="1:1">
       <c r="A285" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
     </row>
     <row r="286" spans="1:1">
       <c r="A286" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
     </row>
     <row r="287" spans="1:1">
       <c r="A287" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
     </row>
     <row r="288" spans="1:1">
       <c r="A288" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
     </row>
     <row r="289" spans="1:1">
       <c r="A289" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
     </row>
     <row r="290" spans="1:1">
       <c r="A290" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
     </row>
     <row r="291" spans="1:1">
       <c r="A291" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
     </row>
     <row r="292" spans="1:1">
       <c r="A292" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row r="293" spans="1:1">
       <c r="A293" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
     </row>
     <row r="294" spans="1:1">
       <c r="A294" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
     </row>
     <row r="295" spans="1:1">
       <c r="A295" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
     </row>
     <row r="296" spans="1:1">
       <c r="A296" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
     </row>
     <row r="297" spans="1:1">
       <c r="A297" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
     </row>
     <row r="298" spans="1:1">
       <c r="A298" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
     </row>
     <row r="299" spans="1:1">
       <c r="A299" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
     </row>
     <row r="300" spans="1:1">
       <c r="A300" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
     </row>
     <row r="301" spans="1:1">
       <c r="A301" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
     </row>
     <row r="302" spans="1:1">
       <c r="A302" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
     </row>
     <row r="303" spans="1:1">
       <c r="A303" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
     </row>
     <row r="304" spans="1:1">
       <c r="A304" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
     </row>
     <row r="305" spans="1:1">
       <c r="A305" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="306" spans="1:1">
       <c r="A306" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
     </row>
     <row r="307" spans="1:1">
       <c r="A307" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
     </row>
     <row r="308" spans="1:1">
       <c r="A308" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
     </row>
     <row r="309" spans="1:1">
       <c r="A309" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
     </row>
     <row r="310" spans="1:1">
       <c r="A310" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="311" spans="1:1">
       <c r="A311" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="312" spans="1:1">
       <c r="A312" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
     </row>
     <row r="313" spans="1:1">
       <c r="A313" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
     </row>
     <row r="314" spans="1:1">
       <c r="A314" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
     </row>
     <row r="315" spans="1:1">
       <c r="A315" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
     </row>
     <row r="316" spans="1:1">
       <c r="A316" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
     </row>
     <row r="317" spans="1:1">
       <c r="A317" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
     </row>
     <row r="318" spans="1:1">
       <c r="A318" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
     </row>
     <row r="319" spans="1:1">
       <c r="A319" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
     <row r="320" spans="1:1">
       <c r="A320" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
     </row>
     <row r="321" spans="1:1">
       <c r="A321" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
     </row>
     <row r="322" spans="1:1">
       <c r="A322" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
     </row>
     <row r="323" spans="1:1">
       <c r="A323" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
     </row>
     <row r="324" spans="1:1">
       <c r="A324" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="325" spans="1:1">
       <c r="A325" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
     </row>
     <row r="326" spans="1:1">
       <c r="A326" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
     </row>
     <row r="327" spans="1:1">
       <c r="A327" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
     </row>
     <row r="328" spans="1:1">
       <c r="A328" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
     </row>
     <row r="329" spans="1:1">
       <c r="A329" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
     </row>
     <row r="330" spans="1:1">
       <c r="A330" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
     </row>
     <row r="331" spans="1:1">
       <c r="A331" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
     </row>
     <row r="332" spans="1:1">
       <c r="A332" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
     </row>
     <row r="333" spans="1:1">
       <c r="A333" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
     </row>
     <row r="334" spans="1:1">
       <c r="A334" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
     </row>
     <row r="335" spans="1:1">
       <c r="A335" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="336" spans="1:1">
       <c r="A336" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
     </row>
     <row r="337" spans="1:1">
       <c r="A337" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
     </row>
     <row r="338" spans="1:1">
       <c r="A338" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
     </row>
     <row r="339" spans="1:1">
       <c r="A339" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
     </row>
     <row r="340" spans="1:1">
       <c r="A340" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
     </row>
     <row r="341" spans="1:1">
       <c r="A341" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
     </row>
     <row r="342" spans="1:1">
       <c r="A342" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
     </row>
     <row r="343" spans="1:1">
       <c r="A343" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
     </row>
     <row r="344" spans="1:1">
       <c r="A344" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
     </row>
     <row r="345" spans="1:1">
       <c r="A345" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
     </row>
     <row r="346" spans="1:1">
       <c r="A346" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
     </row>
     <row r="347" spans="1:1">
       <c r="A347" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
     </row>
     <row r="348" spans="1:1">
       <c r="A348" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
     </row>
     <row r="349" spans="1:1">
       <c r="A349" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
     </row>
     <row r="350" spans="1:1">
       <c r="A350" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
     </row>
     <row r="351" spans="1:1">
       <c r="A351" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
     </row>
     <row r="352" spans="1:1">
       <c r="A352" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
     </row>
     <row r="353" spans="1:1">
       <c r="A353" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
     </row>
     <row r="354" spans="1:1">
       <c r="A354" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
     </row>
     <row r="355" spans="1:1">
       <c r="A355" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
     </row>
     <row r="356" spans="1:1">
       <c r="A356" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
     </row>
     <row r="357" spans="1:1">
       <c r="A357" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
     </row>
     <row r="358" spans="1:1">
       <c r="A358" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
     </row>
     <row r="359" spans="1:1">
       <c r="A359" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
     </row>
     <row r="360" spans="1:1">
       <c r="A360" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
     </row>
     <row r="361" spans="1:1">
       <c r="A361" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
     </row>
     <row r="362" spans="1:1">
       <c r="A362" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
     </row>
     <row r="363" spans="1:1">
       <c r="A363" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
     </row>
     <row r="364" spans="1:1">
       <c r="A364" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
     </row>
     <row r="365" spans="1:1">
       <c r="A365" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
     </row>
     <row r="366" spans="1:1">
       <c r="A366" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
     </row>
     <row r="367" spans="1:1">
       <c r="A367" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
     </row>
     <row r="368" spans="1:1">
       <c r="A368" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
     </row>
     <row r="369" spans="1:1">
       <c r="A369" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
     </row>
     <row r="370" spans="1:1">
       <c r="A370" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
     </row>
     <row r="371" spans="1:1">
       <c r="A371" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
     </row>
     <row r="372" spans="1:1">
       <c r="A372" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
     </row>
     <row r="373" spans="1:1">
       <c r="A373" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
     </row>
     <row r="374" spans="1:1">
       <c r="A374" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
     </row>
     <row r="375" spans="1:1">
       <c r="A375" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
     </row>
     <row r="376" spans="1:1">
       <c r="A376" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
     </row>
     <row r="377" spans="1:1">
       <c r="A377" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
     </row>
     <row r="378" spans="1:1">
       <c r="A378" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
     </row>
     <row r="379" spans="1:1">
       <c r="A379" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
     </row>
     <row r="380" spans="1:1">
       <c r="A380" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
     </row>
     <row r="381" spans="1:1">
       <c r="A381" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
     </row>
     <row r="382" spans="1:1">
       <c r="A382" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
     </row>
     <row r="383" spans="1:1">
       <c r="A383" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
     </row>
     <row r="384" spans="1:1">
       <c r="A384" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
     </row>
     <row r="385" spans="1:1">
       <c r="A385" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
     </row>
     <row r="386" spans="1:1">
       <c r="A386" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
     </row>
     <row r="387" spans="1:1">
       <c r="A387" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
     </row>
     <row r="388" spans="1:1">
       <c r="A388" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
     </row>
     <row r="389" spans="1:1">
       <c r="A389" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
     </row>
     <row r="390" spans="1:1">
       <c r="A390" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
     </row>
     <row r="391" spans="1:1">
       <c r="A391" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
     </row>
     <row r="392" spans="1:1">
       <c r="A392" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
     </row>
     <row r="393" spans="1:1">
       <c r="A393" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
     </row>
     <row r="394" spans="1:1">
       <c r="A394" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="395" spans="1:1">
       <c r="A395" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
     </row>
     <row r="396" spans="1:1">
       <c r="A396" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
     </row>
     <row r="397" spans="1:1">
       <c r="A397" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
     </row>
     <row r="398" spans="1:1">
       <c r="A398" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
     </row>
     <row r="399" spans="1:1">
       <c r="A399" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
     </row>
     <row r="400" spans="1:1">
       <c r="A400" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
     </row>
     <row r="401" spans="1:1">
       <c r="A401" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="402" spans="1:1">
       <c r="A402" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
     </row>
     <row r="403" spans="1:1">
       <c r="A403" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
     </row>
     <row r="404" spans="1:1">
       <c r="A404" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
     </row>
     <row r="405" spans="1:1">
       <c r="A405" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
     </row>
     <row r="406" spans="1:1">
       <c r="A406" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
     </row>
     <row r="407" spans="1:1">
       <c r="A407" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
     </row>
     <row r="408" spans="1:1">
       <c r="A408" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
     </row>
     <row r="409" spans="1:1">
       <c r="A409" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
     </row>
     <row r="410" spans="1:1">
       <c r="A410" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
     </row>
     <row r="411" spans="1:1">
       <c r="A411" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
     </row>
     <row r="412" spans="1:1">
       <c r="A412" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="413" spans="1:1">
       <c r="A413" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
     </row>
     <row r="414" spans="1:1">
       <c r="A414" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
     </row>
     <row r="415" spans="1:1">
       <c r="A415" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
     </row>
     <row r="416" spans="1:1">
       <c r="A416" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
     </row>
     <row r="417" spans="1:1">
       <c r="A417" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
     </row>
     <row r="418" spans="1:1">
       <c r="A418" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
     </row>
     <row r="419" spans="1:1">
       <c r="A419" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="420" spans="1:1">
       <c r="A420" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
     </row>
     <row r="421" spans="1:1">
       <c r="A421" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
     </row>
     <row r="422" spans="1:1">
       <c r="A422" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
     </row>
     <row r="423" spans="1:1">
       <c r="A423" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
     </row>
     <row r="424" spans="1:1">
       <c r="A424" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
     </row>
     <row r="425" spans="1:1">
       <c r="A425" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
     </row>
     <row r="426" spans="1:1">
       <c r="A426" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
     </row>
     <row r="427" spans="1:1">
       <c r="A427" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
     </row>
     <row r="428" spans="1:1">
       <c r="A428" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
     </row>
     <row r="429" spans="1:1">
       <c r="A429" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
     </row>
     <row r="430" spans="1:1">
       <c r="A430" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
     </row>
     <row r="431" spans="1:1">
       <c r="A431" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
     </row>
     <row r="432" spans="1:1">
       <c r="A432" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
     </row>
     <row r="433" spans="1:1">
       <c r="A433" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
     </row>
     <row r="434" spans="1:1">
       <c r="A434" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
     </row>
     <row r="435" spans="1:1">
       <c r="A435" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
     </row>
     <row r="436" spans="1:1">
       <c r="A436" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
     </row>
     <row r="437" spans="1:1">
       <c r="A437" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
     </row>
     <row r="438" spans="1:1">
       <c r="A438" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
     </row>
     <row r="439" spans="1:1">
       <c r="A439" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
     </row>
     <row r="440" spans="1:1">
       <c r="A440" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
     </row>
     <row r="441" spans="1:1">
       <c r="A441" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
     </row>
     <row r="442" spans="1:1">
       <c r="A442" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="443" spans="1:1">
       <c r="A443" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
     </row>
     <row r="444" spans="1:1">
       <c r="A444" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
     </row>
     <row r="445" spans="1:1">
       <c r="A445" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
     </row>
     <row r="446" spans="1:1">
       <c r="A446" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
     </row>
     <row r="447" spans="1:1">
       <c r="A447" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
     </row>
     <row r="448" spans="1:1">
       <c r="A448" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
     </row>
     <row r="449" spans="1:1">
       <c r="A449" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
     </row>
     <row r="450" spans="1:1">
       <c r="A450" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
     </row>
     <row r="451" spans="1:1">
       <c r="A451" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
     </row>
     <row r="452" spans="1:1">
       <c r="A452" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
     </row>
     <row r="453" spans="1:1">
       <c r="A453" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
     </row>
     <row r="454" spans="1:1">
       <c r="A454" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
     </row>
     <row r="455" spans="1:1">
       <c r="A455" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
     </row>
     <row r="456" spans="1:1">
       <c r="A456" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
     </row>
     <row r="457" spans="1:1">
       <c r="A457" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
     </row>
     <row r="458" spans="1:1">
       <c r="A458" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
     </row>
     <row r="459" spans="1:1">
       <c r="A459" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
     </row>
     <row r="460" spans="1:1">
       <c r="A460" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
     </row>
     <row r="461" spans="1:1">
       <c r="A461" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
     </row>
     <row r="462" spans="1:1">
       <c r="A462" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
     </row>
     <row r="463" spans="1:1">
       <c r="A463" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
     </row>
     <row r="464" spans="1:1">
       <c r="A464" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
     </row>
     <row r="465" spans="1:1">
       <c r="A465" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
     </row>
     <row r="466" spans="1:1">
       <c r="A466" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
     </row>
     <row r="467" spans="1:1">
       <c r="A467" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
     </row>
     <row r="468" spans="1:1">
       <c r="A468" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
     </row>
     <row r="469" spans="1:1">
       <c r="A469" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
     </row>
     <row r="470" spans="1:1">
       <c r="A470" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
     </row>
     <row r="471" spans="1:1">
       <c r="A471" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
     </row>
     <row r="472" spans="1:1">
       <c r="A472" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
     </row>
     <row r="473" spans="1:1">
       <c r="A473" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
     </row>
     <row r="474" spans="1:1">
       <c r="A474" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
     </row>
     <row r="475" spans="1:1">
       <c r="A475" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
     </row>
     <row r="476" spans="1:1">
       <c r="A476" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
     </row>
     <row r="477" spans="1:1">
       <c r="A477" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
     </row>
     <row r="478" spans="1:1">
       <c r="A478" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
     </row>
     <row r="479" spans="1:1">
       <c r="A479" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
     </row>
     <row r="480" spans="1:1">
       <c r="A480" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
     </row>
     <row r="481" spans="1:1">
       <c r="A481" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
     </row>
     <row r="482" spans="1:1">
       <c r="A482" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
     </row>
     <row r="483" spans="1:1">
       <c r="A483" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
     </row>
     <row r="484" spans="1:1">
       <c r="A484" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
     </row>
     <row r="485" spans="1:1">
       <c r="A485" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
     </row>
     <row r="486" spans="1:1">
       <c r="A486" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
     </row>
     <row r="487" spans="1:1">
       <c r="A487" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
     </row>
     <row r="488" spans="1:1">
       <c r="A488" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
     </row>
     <row r="489" spans="1:1">
       <c r="A489" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
     </row>
     <row r="490" spans="1:1">
       <c r="A490" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
     </row>
     <row r="491" spans="1:1">
       <c r="A491" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
     </row>
     <row r="492" spans="1:1">
       <c r="A492" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
     </row>
     <row r="493" spans="1:1">
       <c r="A493" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
     </row>
     <row r="494" spans="1:1">
       <c r="A494" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
     </row>
     <row r="495" spans="1:1">
       <c r="A495" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
     </row>
     <row r="496" spans="1:1">
       <c r="A496" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
     </row>
     <row r="497" spans="1:1">
       <c r="A497" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
     </row>
     <row r="498" spans="1:1">
       <c r="A498" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
     </row>
     <row r="499" spans="1:1">
       <c r="A499" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
     </row>
     <row r="500" spans="1:1">
       <c r="A500" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
     </row>
     <row r="501" spans="1:1">
       <c r="A501" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="502" spans="1:1">
       <c r="A502" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="503" spans="1:1">
       <c r="A503" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
     </row>
     <row r="504" spans="1:1">
       <c r="A504" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="505" spans="1:1">
       <c r="A505" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
     </row>
     <row r="506" spans="1:1">
       <c r="A506" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="507" spans="1:1">
       <c r="A507" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
     </row>
     <row r="508" spans="1:1">
       <c r="A508" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
     </row>
     <row r="509" spans="1:1">
       <c r="A509" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
     </row>
     <row r="510" spans="1:1">
       <c r="A510" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
     </row>
     <row r="511" spans="1:1">
       <c r="A511" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
     </row>
     <row r="512" spans="1:1">
       <c r="A512" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
     </row>
     <row r="513" spans="1:1">
       <c r="A513" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
     </row>
     <row r="514" spans="1:1">
       <c r="A514" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
     </row>
     <row r="515" spans="1:1">
       <c r="A515" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
     </row>
     <row r="516" spans="1:1">
       <c r="A516" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
     </row>
     <row r="517" spans="1:1">
       <c r="A517" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
     </row>
     <row r="518" spans="1:1">
       <c r="A518" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
     </row>
     <row r="519" spans="1:1">
       <c r="A519" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
     </row>
     <row r="520" spans="1:1">
       <c r="A520" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="521" spans="1:1">
       <c r="A521" t="s">
-        <v>557</v>
+        <v>559</v>
       </c>
     </row>
     <row r="522" spans="1:1">
       <c r="A522" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
     </row>
     <row r="523" spans="1:1">
       <c r="A523" t="s">
-        <v>559</v>
+        <v>561</v>
       </c>
     </row>
     <row r="524" spans="1:1">
       <c r="A524" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
     </row>
     <row r="525" spans="1:1">
       <c r="A525" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
     </row>
     <row r="526" spans="1:1">
       <c r="A526" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
     </row>
     <row r="527" spans="1:1">
       <c r="A527" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
     </row>
     <row r="528" spans="1:1">
       <c r="A528" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
     </row>
     <row r="529" spans="1:1">
       <c r="A529" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
     </row>
     <row r="530" spans="1:1">
       <c r="A530" t="s">
-        <v>566</v>
+        <v>568</v>
       </c>
     </row>
     <row r="531" spans="1:1">
       <c r="A531" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
     </row>
     <row r="532" spans="1:1">
       <c r="A532" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
     </row>
     <row r="533" spans="1:1">
       <c r="A533" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
     </row>
     <row r="534" spans="1:1">
       <c r="A534" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
     </row>
     <row r="535" spans="1:1">
       <c r="A535" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
     </row>
     <row r="536" spans="1:1">
       <c r="A536" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
     </row>
     <row r="537" spans="1:1">
       <c r="A537" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
     </row>
     <row r="538" spans="1:1">
       <c r="A538" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
     </row>
     <row r="539" spans="1:1">
       <c r="A539" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="540" spans="1:1">
       <c r="A540" t="s">
-        <v>575</v>
+        <v>577</v>
       </c>
     </row>
     <row r="541" spans="1:1">
       <c r="A541" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
     </row>
     <row r="542" spans="1:1">
       <c r="A542" t="s">
-        <v>577</v>
+        <v>579</v>
       </c>
     </row>
     <row r="543" spans="1:1">
       <c r="A543" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
     </row>
     <row r="544" spans="1:1">
       <c r="A544" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
     </row>
     <row r="545" spans="1:1">
       <c r="A545" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
     </row>
     <row r="546" spans="1:1">
       <c r="A546" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
     </row>
     <row r="547" spans="1:1">
       <c r="A547" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
     </row>
     <row r="548" spans="1:1">
       <c r="A548" t="s">
-        <v>583</v>
+        <v>585</v>
       </c>
     </row>
     <row r="549" spans="1:1">
       <c r="A549" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
     </row>
     <row r="550" spans="1:1">
       <c r="A550" t="s">
-        <v>585</v>
+        <v>587</v>
       </c>
     </row>
     <row r="551" spans="1:1">
       <c r="A551" t="s">
-        <v>586</v>
+        <v>588</v>
       </c>
     </row>
     <row r="552" spans="1:1">
       <c r="A552" t="s">
-        <v>587</v>
+        <v>589</v>
       </c>
     </row>
     <row r="553" spans="1:1">
       <c r="A553" t="s">
-        <v>588</v>
+        <v>590</v>
       </c>
     </row>
     <row r="554" spans="1:1">
       <c r="A554" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
     </row>
     <row r="555" spans="1:1">
       <c r="A555" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
     </row>
     <row r="556" spans="1:1">
       <c r="A556" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
     </row>
     <row r="557" spans="1:1">
       <c r="A557" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
     </row>
     <row r="558" spans="1:1">
       <c r="A558" t="s">
-        <v>593</v>
+        <v>595</v>
       </c>
     </row>
     <row r="559" spans="1:1">
       <c r="A559" t="s">
-        <v>594</v>
+        <v>596</v>
       </c>
     </row>
     <row r="560" spans="1:1">
       <c r="A560" t="s">
-        <v>595</v>
+        <v>597</v>
       </c>
     </row>
     <row r="561" spans="1:1">
       <c r="A561" t="s">
-        <v>596</v>
+        <v>598</v>
       </c>
     </row>
     <row r="562" spans="1:1">
       <c r="A562" t="s">
-        <v>597</v>
+        <v>599</v>
       </c>
     </row>
     <row r="563" spans="1:1">
       <c r="A563" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
     </row>
     <row r="564" spans="1:1">
       <c r="A564" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="565" spans="1:1">
       <c r="A565" t="s">
-        <v>599</v>
+        <v>601</v>
       </c>
     </row>
     <row r="566" spans="1:1">
       <c r="A566" t="s">
-        <v>600</v>
+        <v>602</v>
       </c>
     </row>
     <row r="567" spans="1:1">
       <c r="A567" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
     </row>
     <row r="568" spans="1:1">
       <c r="A568" t="s">
-        <v>602</v>
+        <v>604</v>
       </c>
     </row>
     <row r="569" spans="1:1">
       <c r="A569" t="s">
-        <v>603</v>
+        <v>605</v>
       </c>
     </row>
     <row r="570" spans="1:1">
       <c r="A570" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
     </row>
     <row r="571" spans="1:1">
       <c r="A571" t="s">
-        <v>605</v>
+        <v>607</v>
       </c>
     </row>
     <row r="572" spans="1:1">
       <c r="A572" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
     </row>
     <row r="573" spans="1:1">
       <c r="A573" t="s">
-        <v>607</v>
+        <v>609</v>
       </c>
     </row>
     <row r="574" spans="1:1">
       <c r="A574" t="s">
-        <v>608</v>
+        <v>610</v>
       </c>
     </row>
     <row r="575" spans="1:1">
       <c r="A575" t="s">
-        <v>609</v>
+        <v>611</v>
       </c>
     </row>
     <row r="576" spans="1:1">
       <c r="A576" t="s">
-        <v>610</v>
+        <v>612</v>
       </c>
     </row>
     <row r="577" spans="1:1">
       <c r="A577" t="s">
-        <v>611</v>
+        <v>613</v>
       </c>
     </row>
     <row r="578" spans="1:1">
       <c r="A578" t="s">
-        <v>612</v>
+        <v>614</v>
       </c>
     </row>
     <row r="579" spans="1:1">
       <c r="A579" t="s">
-        <v>613</v>
+        <v>615</v>
       </c>
     </row>
     <row r="580" spans="1:1">
       <c r="A580" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="581" spans="1:1">
       <c r="A581" t="s">
-        <v>614</v>
+        <v>616</v>
       </c>
     </row>
     <row r="582" spans="1:1">
       <c r="A582" t="s">
-        <v>615</v>
+        <v>617</v>
       </c>
     </row>
     <row r="583" spans="1:1">
       <c r="A583" t="s">
-        <v>616</v>
+        <v>618</v>
       </c>
     </row>
     <row r="584" spans="1:1">
       <c r="A584" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
     </row>
     <row r="585" spans="1:1">
       <c r="A585" t="s">
-        <v>618</v>
+        <v>620</v>
       </c>
     </row>
     <row r="586" spans="1:1">
       <c r="A586" t="s">
-        <v>619</v>
+        <v>621</v>
       </c>
     </row>
     <row r="587" spans="1:1">
       <c r="A587" t="s">
-        <v>620</v>
+        <v>622</v>
       </c>
     </row>
     <row r="588" spans="1:1">
       <c r="A588" t="s">
-        <v>621</v>
+        <v>623</v>
       </c>
     </row>
     <row r="589" spans="1:1">
       <c r="A589" t="s">
-        <v>622</v>
+        <v>624</v>
       </c>
     </row>
     <row r="590" spans="1:1">
       <c r="A590" t="s">
-        <v>623</v>
+        <v>625</v>
       </c>
     </row>
     <row r="591" spans="1:1">
       <c r="A591" t="s">
-        <v>624</v>
+        <v>626</v>
       </c>
     </row>
     <row r="592" spans="1:1">
       <c r="A592" t="s">
-        <v>625</v>
+        <v>627</v>
       </c>
     </row>
     <row r="593" spans="1:1">
       <c r="A593" t="s">
-        <v>626</v>
+        <v>628</v>
       </c>
     </row>
     <row r="594" spans="1:1">
       <c r="A594" t="s">
-        <v>627</v>
+        <v>629</v>
       </c>
     </row>
     <row r="595" spans="1:1">
       <c r="A595" t="s">
-        <v>628</v>
+        <v>630</v>
       </c>
     </row>
     <row r="596" spans="1:1">
       <c r="A596" t="s">
-        <v>629</v>
+        <v>631</v>
       </c>
     </row>
     <row r="597" spans="1:1">
       <c r="A597" t="s">
-        <v>630</v>
+        <v>632</v>
       </c>
     </row>
     <row r="598" spans="1:1">
       <c r="A598" t="s">
-        <v>631</v>
+        <v>633</v>
       </c>
     </row>
     <row r="599" spans="1:1">
       <c r="A599" t="s">
-        <v>632</v>
+        <v>634</v>
       </c>
     </row>
     <row r="600" spans="1:1">
       <c r="A600" t="s">
-        <v>633</v>
+        <v>635</v>
       </c>
     </row>
     <row r="601" spans="1:1">
       <c r="A601" t="s">
-        <v>634</v>
+        <v>636</v>
       </c>
     </row>
     <row r="602" spans="1:1">
       <c r="A602" t="s">
-        <v>635</v>
+        <v>637</v>
       </c>
     </row>
     <row r="603" spans="1:1">
       <c r="A603" t="s">
-        <v>636</v>
+        <v>638</v>
       </c>
     </row>
     <row r="604" spans="1:1">
       <c r="A604" t="s">
-        <v>637</v>
+        <v>639</v>
       </c>
     </row>
     <row r="605" spans="1:1">
       <c r="A605" t="s">
-        <v>638</v>
+        <v>640</v>
       </c>
     </row>
     <row r="606" spans="1:1">
       <c r="A606" t="s">
-        <v>639</v>
+        <v>641</v>
       </c>
     </row>
     <row r="607" spans="1:1">
       <c r="A607" t="s">
-        <v>640</v>
+        <v>642</v>
       </c>
     </row>
     <row r="608" spans="1:1">
       <c r="A608" t="s">
-        <v>641</v>
+        <v>643</v>
       </c>
     </row>
     <row r="609" spans="1:1">
       <c r="A609" t="s">
-        <v>642</v>
+        <v>644</v>
       </c>
     </row>
     <row r="610" spans="1:1">
       <c r="A610" t="s">
-        <v>643</v>
+        <v>645</v>
       </c>
     </row>
     <row r="611" spans="1:1">
       <c r="A611" t="s">
-        <v>644</v>
+        <v>646</v>
       </c>
     </row>
     <row r="612" spans="1:1">
       <c r="A612" t="s">
-        <v>645</v>
+        <v>647</v>
       </c>
     </row>
     <row r="613" spans="1:1">
       <c r="A613" t="s">
-        <v>646</v>
+        <v>648</v>
       </c>
     </row>
     <row r="614" spans="1:1">
       <c r="A614" t="s">
-        <v>647</v>
+        <v>649</v>
       </c>
     </row>
     <row r="615" spans="1:1">
       <c r="A615" t="s">
-        <v>648</v>
+        <v>650</v>
       </c>
     </row>
     <row r="616" spans="1:1">
       <c r="A616" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
     </row>
     <row r="617" spans="1:1">
       <c r="A617" t="s">
-        <v>650</v>
+        <v>652</v>
       </c>
     </row>
     <row r="618" spans="1:1">
       <c r="A618" t="s">
-        <v>651</v>
+        <v>653</v>
       </c>
     </row>
     <row r="619" spans="1:1">
       <c r="A619" t="s">
-        <v>652</v>
+        <v>654</v>
       </c>
     </row>
     <row r="620" spans="1:1">
       <c r="A620" t="s">
-        <v>653</v>
+        <v>655</v>
       </c>
     </row>
     <row r="621" spans="1:1">
       <c r="A621" t="s">
-        <v>654</v>
+        <v>656</v>
       </c>
     </row>
     <row r="622" spans="1:1">
       <c r="A622" t="s">
-        <v>655</v>
+        <v>657</v>
       </c>
     </row>
     <row r="623" spans="1:1">
       <c r="A623" t="s">
-        <v>656</v>
+        <v>658</v>
       </c>
     </row>
     <row r="624" spans="1:1">
       <c r="A624" t="s">
-        <v>657</v>
+        <v>659</v>
       </c>
     </row>
     <row r="625" spans="1:1">
       <c r="A625" t="s">
-        <v>658</v>
+        <v>660</v>
       </c>
     </row>
     <row r="626" spans="1:1">
       <c r="A626" t="s">
-        <v>659</v>
+        <v>661</v>
       </c>
     </row>
     <row r="627" spans="1:1">
       <c r="A627" t="s">
-        <v>660</v>
+        <v>662</v>
       </c>
     </row>
     <row r="628" spans="1:1">
       <c r="A628" t="s">
-        <v>661</v>
+        <v>663</v>
       </c>
     </row>
     <row r="629" spans="1:1">
       <c r="A629" t="s">
-        <v>662</v>
+        <v>664</v>
       </c>
     </row>
     <row r="630" spans="1:1">
       <c r="A630" t="s">
-        <v>663</v>
+        <v>665</v>
       </c>
     </row>
     <row r="631" spans="1:1">
       <c r="A631" t="s">
-        <v>664</v>
+        <v>666</v>
       </c>
     </row>
     <row r="632" spans="1:1">
       <c r="A632" t="s">
-        <v>665</v>
+        <v>667</v>
       </c>
     </row>
     <row r="633" spans="1:1">
       <c r="A633" t="s">
-        <v>666</v>
+        <v>668</v>
       </c>
     </row>
     <row r="634" spans="1:1">
       <c r="A634" t="s">
-        <v>667</v>
+        <v>669</v>
       </c>
     </row>
     <row r="635" spans="1:1">
       <c r="A635" t="s">
-        <v>668</v>
+        <v>670</v>
       </c>
     </row>
     <row r="636" spans="1:1">
       <c r="A636" t="s">
-        <v>669</v>
+        <v>671</v>
       </c>
     </row>
     <row r="637" spans="1:1">
       <c r="A637" t="s">
-        <v>670</v>
+        <v>672</v>
       </c>
     </row>
     <row r="638" spans="1:1">
       <c r="A638" t="s">
-        <v>671</v>
+        <v>673</v>
       </c>
     </row>
     <row r="639" spans="1:1">
       <c r="A639" t="s">
-        <v>672</v>
+        <v>674</v>
       </c>
     </row>
     <row r="640" spans="1:1">
       <c r="A640" t="s">
-        <v>673</v>
+        <v>675</v>
       </c>
     </row>
     <row r="641" spans="1:1">
       <c r="A641" t="s">
-        <v>674</v>
+        <v>676</v>
       </c>
     </row>
     <row r="642" spans="1:1">
       <c r="A642" t="s">
-        <v>675</v>
+        <v>677</v>
       </c>
     </row>
     <row r="643" spans="1:1">
       <c r="A643" t="s">
-        <v>676</v>
+        <v>678</v>
       </c>
     </row>
     <row r="644" spans="1:1">
       <c r="A644" t="s">
-        <v>677</v>
+        <v>679</v>
       </c>
     </row>
     <row r="645" spans="1:1">
       <c r="A645" t="s">
-        <v>678</v>
+        <v>680</v>
       </c>
     </row>
     <row r="646" spans="1:1">
       <c r="A646" t="s">
-        <v>679</v>
+        <v>681</v>
       </c>
     </row>
     <row r="647" spans="1:1">
       <c r="A647" t="s">
-        <v>680</v>
+        <v>682</v>
       </c>
     </row>
     <row r="648" spans="1:1">
       <c r="A648" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
     </row>
     <row r="649" spans="1:1">
       <c r="A649" t="s">
-        <v>682</v>
+        <v>684</v>
       </c>
     </row>
     <row r="650" spans="1:1">
       <c r="A650" t="s">
-        <v>683</v>
+        <v>685</v>
       </c>
     </row>
     <row r="651" spans="1:1">
       <c r="A651" t="s">
-        <v>684</v>
+        <v>686</v>
       </c>
     </row>
     <row r="652" spans="1:1">
       <c r="A652" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="653" spans="1:1">
       <c r="A653" t="s">
-        <v>685</v>
+        <v>687</v>
       </c>
     </row>
     <row r="654" spans="1:1">
       <c r="A654" t="s">
-        <v>686</v>
+        <v>688</v>
       </c>
     </row>
     <row r="655" spans="1:1">
       <c r="A655" t="s">
-        <v>687</v>
+        <v>689</v>
       </c>
     </row>
     <row r="656" spans="1:1">
       <c r="A656" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
     </row>
     <row r="657" spans="1:1">
       <c r="A657" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
     </row>
     <row r="658" spans="1:1">
       <c r="A658" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
     </row>
     <row r="659" spans="1:1">
       <c r="A659" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
     </row>
     <row r="660" spans="1:1">
       <c r="A660" t="s">
-        <v>692</v>
+        <v>694</v>
       </c>
     </row>
     <row r="661" spans="1:1">
       <c r="A661" t="s">
-        <v>693</v>
+        <v>695</v>
       </c>
     </row>
     <row r="662" spans="1:1">
       <c r="A662" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
     </row>
     <row r="663" spans="1:1">
       <c r="A663" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="664" spans="1:1">
       <c r="A664" t="s">
-        <v>695</v>
+        <v>697</v>
       </c>
     </row>
     <row r="665" spans="1:1">
       <c r="A665" t="s">
-        <v>696</v>
+        <v>698</v>
       </c>
     </row>
     <row r="666" spans="1:1">
       <c r="A666" t="s">
-        <v>697</v>
+        <v>699</v>
       </c>
     </row>
     <row r="667" spans="1:1">
       <c r="A667" t="s">
-        <v>698</v>
+        <v>700</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
panorama snippet and set updates for 90
</commit_message>
<xml_diff>
--- a/templates/panos/set_commands/iron_skillet_panos_full.xlsx
+++ b/templates/panos/set_commands/iron_skillet_panos_full.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="722">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="723">
   <si>
     <t>Variable Name</t>
   </si>
@@ -269,6 +269,12 @@
     <t>syslog server ip address</t>
   </si>
   <si>
+    <t>API_KEY_LIFETIME</t>
+  </si>
+  <si>
+    <t>lifetime for the api key in minutes</t>
+  </si>
+  <si>
     <t>INCLUDE_PAN_EDL</t>
   </si>
   <si>
@@ -378,9 +384,6 @@
   </si>
   <si>
     <t>set deviceconfig setting management enable-log-high-dp-load yes</t>
-  </si>
-  <si>
-    <t>set deviceconfig setting management api key lifetime 525600</t>
   </si>
   <si>
     <t>set deviceconfig setting management max-rows-in-csv-export 1048576</t>
@@ -2521,7 +2524,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2843,11 +2846,22 @@
       <c r="A29" t="s">
         <v>84</v>
       </c>
-      <c r="B29" t="b">
-        <v>1</v>
+      <c r="B29">
+        <v>525600</v>
       </c>
       <c r="C29" t="s">
         <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>86</v>
+      </c>
+      <c r="B30" t="b">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -2865,27 +2879,27 @@
   <sheetData>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:1">
@@ -2938,7 +2952,7 @@
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:1">
@@ -2955,272 +2969,273 @@
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="50" spans="1:1">
-      <c r="A50" t="s">
-        <v>121</v>
+      <c r="A50">
+        <f>SUBSTITUTE("set deviceconfig setting management api key lifetime {{ API_KEY_LIFETIME }}", "{{ API_KEY_LIFETIME }}", 'values'!B29)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="77" spans="1:1">
@@ -3243,17 +3258,17 @@
     </row>
     <row r="80" spans="1:1">
       <c r="A80" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="83" spans="1:1">
@@ -3264,347 +3279,347 @@
     </row>
     <row r="84" spans="1:1">
       <c r="A84" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="87" spans="1:1">
       <c r="A87" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="89" spans="1:1">
       <c r="A89" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="90" spans="1:1">
       <c r="A90" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="91" spans="1:1">
       <c r="A91" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="92" spans="1:1">
       <c r="A92" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="94" spans="1:1">
       <c r="A94" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="95" spans="1:1">
       <c r="A95" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="96" spans="1:1">
       <c r="A96" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="97" spans="1:1">
       <c r="A97" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="98" spans="1:1">
       <c r="A98" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="100" spans="1:1">
       <c r="A100" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="104" spans="1:1">
       <c r="A104" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="105" spans="1:1">
       <c r="A105" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="106" spans="1:1">
       <c r="A106" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="107" spans="1:1">
       <c r="A107" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="108" spans="1:1">
       <c r="A108" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="109" spans="1:1">
       <c r="A109" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="110" spans="1:1">
       <c r="A110" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="111" spans="1:1">
       <c r="A111" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="112" spans="1:1">
       <c r="A112" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="113" spans="1:1">
       <c r="A113" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="114" spans="1:1">
       <c r="A114" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="115" spans="1:1">
       <c r="A115" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="116" spans="1:1">
       <c r="A116" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="117" spans="1:1">
       <c r="A117" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="118" spans="1:1">
       <c r="A118" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="119" spans="1:1">
       <c r="A119" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="120" spans="1:1">
       <c r="A120" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="121" spans="1:1">
       <c r="A121" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="122" spans="1:1">
       <c r="A122" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="123" spans="1:1">
       <c r="A123" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="124" spans="1:1">
       <c r="A124" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="125" spans="1:1">
       <c r="A125" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="126" spans="1:1">
       <c r="A126" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="127" spans="1:1">
       <c r="A127" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="128" spans="1:1">
       <c r="A128" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="129" spans="1:1">
       <c r="A129" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="130" spans="1:1">
       <c r="A130" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="131" spans="1:1">
       <c r="A131" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="132" spans="1:1">
       <c r="A132" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="133" spans="1:1">
       <c r="A133" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="134" spans="1:1">
       <c r="A134" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="135" spans="1:1">
       <c r="A135" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="136" spans="1:1">
       <c r="A136" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="137" spans="1:1">
       <c r="A137" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="138" spans="1:1">
       <c r="A138" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="139" spans="1:1">
       <c r="A139" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="140" spans="1:1">
       <c r="A140" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="141" spans="1:1">
       <c r="A141" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="143" spans="1:1">
       <c r="A143" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="144" spans="1:1">
       <c r="A144" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="145" spans="1:1">
       <c r="A145" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="146" spans="1:1">
       <c r="A146" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="147" spans="1:1">
       <c r="A147" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="149" spans="1:1">
       <c r="A149" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="150" spans="1:1">
       <c r="A150" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="151" spans="1:1">
       <c r="A151" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="152" spans="1:1">
       <c r="A152" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="153" spans="1:1">
       <c r="A153" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="154" spans="1:1">
       <c r="A154" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="155" spans="1:1">
       <c r="A155" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="157" spans="1:1">
       <c r="A157" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="158" spans="1:1">
@@ -3621,152 +3636,152 @@
     </row>
     <row r="161" spans="1:1">
       <c r="A161" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="162" spans="1:1">
       <c r="A162" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="163" spans="1:1">
       <c r="A163" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="164" spans="1:1">
       <c r="A164" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="165" spans="1:1">
       <c r="A165" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="166" spans="1:1">
       <c r="A166" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="167" spans="1:1">
       <c r="A167" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="168" spans="1:1">
       <c r="A168" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="169" spans="1:1">
       <c r="A169" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="170" spans="1:1">
       <c r="A170" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="171" spans="1:1">
       <c r="A171" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="172" spans="1:1">
       <c r="A172" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="173" spans="1:1">
       <c r="A173" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="174" spans="1:1">
       <c r="A174" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="175" spans="1:1">
       <c r="A175" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="176" spans="1:1">
       <c r="A176" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="177" spans="1:1">
       <c r="A177" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="178" spans="1:1">
       <c r="A178" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="179" spans="1:1">
       <c r="A179" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="180" spans="1:1">
       <c r="A180" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="181" spans="1:1">
       <c r="A181" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="182" spans="1:1">
       <c r="A182" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="183" spans="1:1">
       <c r="A183" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="184" spans="1:1">
       <c r="A184" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="185" spans="1:1">
       <c r="A185" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="186" spans="1:1">
       <c r="A186" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="187" spans="1:1">
       <c r="A187" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="188" spans="1:1">
       <c r="A188" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="189" spans="1:1">
       <c r="A189" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="191" spans="1:1">
       <c r="A191" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="192" spans="1:1">
@@ -3783,72 +3798,72 @@
     </row>
     <row r="194" spans="1:1">
       <c r="A194" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="195" spans="1:1">
       <c r="A195" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="196" spans="1:1">
       <c r="A196" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="197" spans="1:1">
       <c r="A197" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="198" spans="1:1">
       <c r="A198" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="199" spans="1:1">
       <c r="A199" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="200" spans="1:1">
       <c r="A200" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="201" spans="1:1">
       <c r="A201" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="202" spans="1:1">
       <c r="A202" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="203" spans="1:1">
       <c r="A203" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="204" spans="1:1">
       <c r="A204" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="205" spans="1:1">
       <c r="A205" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="206" spans="1:1">
       <c r="A206" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="207" spans="1:1">
       <c r="A207" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="208" spans="1:1">
@@ -3865,72 +3880,72 @@
     </row>
     <row r="210" spans="1:1">
       <c r="A210" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="211" spans="1:1">
       <c r="A211" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="212" spans="1:1">
       <c r="A212" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="213" spans="1:1">
       <c r="A213" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="214" spans="1:1">
       <c r="A214" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="215" spans="1:1">
       <c r="A215" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="216" spans="1:1">
       <c r="A216" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="217" spans="1:1">
       <c r="A217" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="218" spans="1:1">
       <c r="A218" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="219" spans="1:1">
       <c r="A219" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="220" spans="1:1">
       <c r="A220" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="221" spans="1:1">
       <c r="A221" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="222" spans="1:1">
       <c r="A222" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="223" spans="1:1">
       <c r="A223" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="224" spans="1:1">
@@ -3947,77 +3962,77 @@
     </row>
     <row r="226" spans="1:1">
       <c r="A226" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="227" spans="1:1">
       <c r="A227" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="228" spans="1:1">
       <c r="A228" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="229" spans="1:1">
       <c r="A229" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="230" spans="1:1">
       <c r="A230" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="231" spans="1:1">
       <c r="A231" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="232" spans="1:1">
       <c r="A232" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="233" spans="1:1">
       <c r="A233" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="234" spans="1:1">
       <c r="A234" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="235" spans="1:1">
       <c r="A235" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="236" spans="1:1">
       <c r="A236" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="237" spans="1:1">
       <c r="A237" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="238" spans="1:1">
       <c r="A238" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="239" spans="1:1">
       <c r="A239" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="240" spans="1:1">
       <c r="A240" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="241" spans="1:1">
@@ -4034,47 +4049,47 @@
     </row>
     <row r="243" spans="1:1">
       <c r="A243" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="244" spans="1:1">
       <c r="A244" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="245" spans="1:1">
       <c r="A245" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="246" spans="1:1">
       <c r="A246" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="247" spans="1:1">
       <c r="A247" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="248" spans="1:1">
       <c r="A248" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="249" spans="1:1">
       <c r="A249" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="250" spans="1:1">
       <c r="A250" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="251" spans="1:1">
       <c r="A251" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="252" spans="1:1">
@@ -4091,2117 +4106,2117 @@
     </row>
     <row r="254" spans="1:1">
       <c r="A254" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="255" spans="1:1">
       <c r="A255" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="256" spans="1:1">
       <c r="A256" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="257" spans="1:1">
       <c r="A257" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="259" spans="1:1">
       <c r="A259" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="260" spans="1:1">
       <c r="A260" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="261" spans="1:1">
       <c r="A261" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="262" spans="1:1">
       <c r="A262" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="263" spans="1:1">
       <c r="A263" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="264" spans="1:1">
       <c r="A264" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="265" spans="1:1">
       <c r="A265" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="266" spans="1:1">
       <c r="A266" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="267" spans="1:1">
       <c r="A267" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="268" spans="1:1">
       <c r="A268" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="269" spans="1:1">
       <c r="A269" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="270" spans="1:1">
       <c r="A270" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="271" spans="1:1">
       <c r="A271" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="272" spans="1:1">
       <c r="A272" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="273" spans="1:1">
       <c r="A273" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="274" spans="1:1">
       <c r="A274" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="275" spans="1:1">
       <c r="A275" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="276" spans="1:1">
       <c r="A276" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="277" spans="1:1">
       <c r="A277" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="278" spans="1:1">
       <c r="A278" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="279" spans="1:1">
       <c r="A279" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="280" spans="1:1">
       <c r="A280" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="281" spans="1:1">
       <c r="A281" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="282" spans="1:1">
       <c r="A282" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="284" spans="1:1">
       <c r="A284" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="285" spans="1:1">
       <c r="A285" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="286" spans="1:1">
       <c r="A286" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="287" spans="1:1">
       <c r="A287" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="288" spans="1:1">
       <c r="A288" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="289" spans="1:1">
       <c r="A289" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="290" spans="1:1">
       <c r="A290" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="291" spans="1:1">
       <c r="A291" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="292" spans="1:1">
       <c r="A292" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="293" spans="1:1">
       <c r="A293" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="294" spans="1:1">
       <c r="A294" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="295" spans="1:1">
       <c r="A295" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="296" spans="1:1">
       <c r="A296" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="297" spans="1:1">
       <c r="A297" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="298" spans="1:1">
       <c r="A298" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="299" spans="1:1">
       <c r="A299" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="300" spans="1:1">
       <c r="A300" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="301" spans="1:1">
       <c r="A301" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="302" spans="1:1">
       <c r="A302" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="303" spans="1:1">
       <c r="A303" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="304" spans="1:1">
       <c r="A304" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="305" spans="1:1">
       <c r="A305" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="306" spans="1:1">
       <c r="A306" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="307" spans="1:1">
       <c r="A307" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="308" spans="1:1">
       <c r="A308" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="309" spans="1:1">
       <c r="A309" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="310" spans="1:1">
       <c r="A310" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="311" spans="1:1">
       <c r="A311" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="312" spans="1:1">
       <c r="A312" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="313" spans="1:1">
       <c r="A313" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="314" spans="1:1">
       <c r="A314" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="315" spans="1:1">
       <c r="A315" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="316" spans="1:1">
       <c r="A316" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="317" spans="1:1">
       <c r="A317" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="318" spans="1:1">
       <c r="A318" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="319" spans="1:1">
       <c r="A319" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="320" spans="1:1">
       <c r="A320" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row r="321" spans="1:1">
       <c r="A321" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="322" spans="1:1">
       <c r="A322" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
     <row r="323" spans="1:1">
       <c r="A323" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="324" spans="1:1">
       <c r="A324" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="325" spans="1:1">
       <c r="A325" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="326" spans="1:1">
       <c r="A326" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="327" spans="1:1">
       <c r="A327" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="328" spans="1:1">
       <c r="A328" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="329" spans="1:1">
       <c r="A329" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="330" spans="1:1">
       <c r="A330" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="331" spans="1:1">
       <c r="A331" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="332" spans="1:1">
       <c r="A332" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="333" spans="1:1">
       <c r="A333" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
     </row>
     <row r="334" spans="1:1">
       <c r="A334" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="335" spans="1:1">
       <c r="A335" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
     </row>
     <row r="336" spans="1:1">
       <c r="A336" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="337" spans="1:1">
       <c r="A337" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="338" spans="1:1">
       <c r="A338" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
     </row>
     <row r="339" spans="1:1">
       <c r="A339" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="340" spans="1:1">
       <c r="A340" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="341" spans="1:1">
       <c r="A341" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
     </row>
     <row r="342" spans="1:1">
       <c r="A342" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
     <row r="343" spans="1:1">
       <c r="A343" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
     </row>
     <row r="344" spans="1:1">
       <c r="A344" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
     <row r="345" spans="1:1">
       <c r="A345" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="346" spans="1:1">
       <c r="A346" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
     </row>
     <row r="347" spans="1:1">
       <c r="A347" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
     <row r="348" spans="1:1">
       <c r="A348" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="349" spans="1:1">
       <c r="A349" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="350" spans="1:1">
       <c r="A350" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="351" spans="1:1">
       <c r="A351" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="352" spans="1:1">
       <c r="A352" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="353" spans="1:1">
       <c r="A353" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
     </row>
     <row r="354" spans="1:1">
       <c r="A354" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
     </row>
     <row r="355" spans="1:1">
       <c r="A355" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
     <row r="357" spans="1:1">
       <c r="A357" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
     </row>
     <row r="358" spans="1:1">
       <c r="A358" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
     </row>
     <row r="359" spans="1:1">
       <c r="A359" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="360" spans="1:1">
       <c r="A360" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
     </row>
     <row r="361" spans="1:1">
       <c r="A361" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
     </row>
     <row r="362" spans="1:1">
       <c r="A362" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
     </row>
     <row r="363" spans="1:1">
       <c r="A363" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="364" spans="1:1">
       <c r="A364" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
     </row>
     <row r="365" spans="1:1">
       <c r="A365" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
     </row>
     <row r="366" spans="1:1">
       <c r="A366" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
     </row>
     <row r="367" spans="1:1">
       <c r="A367" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="368" spans="1:1">
       <c r="A368" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="369" spans="1:1">
       <c r="A369" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
     </row>
     <row r="370" spans="1:1">
       <c r="A370" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="371" spans="1:1">
       <c r="A371" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
     </row>
     <row r="372" spans="1:1">
       <c r="A372" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
     </row>
     <row r="373" spans="1:1">
       <c r="A373" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="374" spans="1:1">
       <c r="A374" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
     </row>
     <row r="375" spans="1:1">
       <c r="A375" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
     </row>
     <row r="376" spans="1:1">
       <c r="A376" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="377" spans="1:1">
       <c r="A377" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="378" spans="1:1">
       <c r="A378" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
     </row>
     <row r="379" spans="1:1">
       <c r="A379" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="380" spans="1:1">
       <c r="A380" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="381" spans="1:1">
       <c r="A381" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="382" spans="1:1">
       <c r="A382" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
     </row>
     <row r="383" spans="1:1">
       <c r="A383" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="384" spans="1:1">
       <c r="A384" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="385" spans="1:1">
       <c r="A385" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
     </row>
     <row r="386" spans="1:1">
       <c r="A386" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
     </row>
     <row r="387" spans="1:1">
       <c r="A387" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="388" spans="1:1">
       <c r="A388" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
     </row>
     <row r="389" spans="1:1">
       <c r="A389" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="390" spans="1:1">
       <c r="A390" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
     <row r="391" spans="1:1">
       <c r="A391" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
     </row>
     <row r="392" spans="1:1">
       <c r="A392" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="393" spans="1:1">
       <c r="A393" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
     </row>
     <row r="394" spans="1:1">
       <c r="A394" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row r="395" spans="1:1">
       <c r="A395" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
     </row>
     <row r="396" spans="1:1">
       <c r="A396" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="397" spans="1:1">
       <c r="A397" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
     </row>
     <row r="398" spans="1:1">
       <c r="A398" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row r="399" spans="1:1">
       <c r="A399" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
     </row>
     <row r="400" spans="1:1">
       <c r="A400" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
     </row>
     <row r="401" spans="1:1">
       <c r="A401" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
     </row>
     <row r="402" spans="1:1">
       <c r="A402" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
     </row>
     <row r="403" spans="1:1">
       <c r="A403" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
     </row>
     <row r="404" spans="1:1">
       <c r="A404" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
     </row>
     <row r="405" spans="1:1">
       <c r="A405" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
     </row>
     <row r="406" spans="1:1">
       <c r="A406" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
     </row>
     <row r="407" spans="1:1">
       <c r="A407" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="408" spans="1:1">
       <c r="A408" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
     </row>
     <row r="409" spans="1:1">
       <c r="A409" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
     </row>
     <row r="410" spans="1:1">
       <c r="A410" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
     </row>
     <row r="411" spans="1:1">
       <c r="A411" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
     </row>
     <row r="412" spans="1:1">
       <c r="A412" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
     </row>
     <row r="413" spans="1:1">
       <c r="A413" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
     </row>
     <row r="414" spans="1:1">
       <c r="A414" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="416" spans="1:1">
       <c r="A416" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="417" spans="1:1">
       <c r="A417" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="418" spans="1:1">
       <c r="A418" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
     </row>
     <row r="419" spans="1:1">
       <c r="A419" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
     </row>
     <row r="420" spans="1:1">
       <c r="A420" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
     </row>
     <row r="421" spans="1:1">
       <c r="A421" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
     </row>
     <row r="422" spans="1:1">
       <c r="A422" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
     </row>
     <row r="423" spans="1:1">
       <c r="A423" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
     </row>
     <row r="424" spans="1:1">
       <c r="A424" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
     </row>
     <row r="425" spans="1:1">
       <c r="A425" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
     </row>
     <row r="426" spans="1:1">
       <c r="A426" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
     </row>
     <row r="427" spans="1:1">
       <c r="A427" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
     </row>
     <row r="428" spans="1:1">
       <c r="A428" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
     </row>
     <row r="429" spans="1:1">
       <c r="A429" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
     </row>
     <row r="430" spans="1:1">
       <c r="A430" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
     </row>
     <row r="431" spans="1:1">
       <c r="A431" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="432" spans="1:1">
       <c r="A432" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
     </row>
     <row r="434" spans="1:1">
       <c r="A434" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
     </row>
     <row r="435" spans="1:1">
       <c r="A435" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
     </row>
     <row r="436" spans="1:1">
       <c r="A436" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
     </row>
     <row r="437" spans="1:1">
       <c r="A437" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
     </row>
     <row r="438" spans="1:1">
       <c r="A438" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
     </row>
     <row r="439" spans="1:1">
       <c r="A439" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
     </row>
     <row r="440" spans="1:1">
       <c r="A440" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
     </row>
     <row r="441" spans="1:1">
       <c r="A441" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row r="442" spans="1:1">
       <c r="A442" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
     </row>
     <row r="443" spans="1:1">
       <c r="A443" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
     </row>
     <row r="444" spans="1:1">
       <c r="A444" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
     </row>
     <row r="445" spans="1:1">
       <c r="A445" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
     </row>
     <row r="446" spans="1:1">
       <c r="A446" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
     </row>
     <row r="447" spans="1:1">
       <c r="A447" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="448" spans="1:1">
       <c r="A448" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
     </row>
     <row r="449" spans="1:1">
       <c r="A449" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
     </row>
     <row r="450" spans="1:1">
       <c r="A450" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
     </row>
     <row r="451" spans="1:1">
       <c r="A451" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
     </row>
     <row r="452" spans="1:1">
       <c r="A452" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
     </row>
     <row r="453" spans="1:1">
       <c r="A453" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
     </row>
     <row r="454" spans="1:1">
       <c r="A454" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
     </row>
     <row r="455" spans="1:1">
       <c r="A455" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="456" spans="1:1">
       <c r="A456" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
     </row>
     <row r="457" spans="1:1">
       <c r="A457" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
     </row>
     <row r="458" spans="1:1">
       <c r="A458" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
     </row>
     <row r="459" spans="1:1">
       <c r="A459" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
     </row>
     <row r="460" spans="1:1">
       <c r="A460" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
     </row>
     <row r="461" spans="1:1">
       <c r="A461" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="462" spans="1:1">
       <c r="A462" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
     </row>
     <row r="464" spans="1:1">
       <c r="A464" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
     </row>
     <row r="465" spans="1:1">
       <c r="A465" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
     </row>
     <row r="466" spans="1:1">
       <c r="A466" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
     </row>
     <row r="467" spans="1:1">
       <c r="A467" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
     </row>
     <row r="468" spans="1:1">
       <c r="A468" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
     </row>
     <row r="469" spans="1:1">
       <c r="A469" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
     </row>
     <row r="470" spans="1:1">
       <c r="A470" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
     </row>
     <row r="471" spans="1:1">
       <c r="A471" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
     </row>
     <row r="472" spans="1:1">
       <c r="A472" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
     </row>
     <row r="473" spans="1:1">
       <c r="A473" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
     </row>
     <row r="474" spans="1:1">
       <c r="A474" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
     </row>
     <row r="475" spans="1:1">
       <c r="A475" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
     </row>
     <row r="476" spans="1:1">
       <c r="A476" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
     </row>
     <row r="477" spans="1:1">
       <c r="A477" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="478" spans="1:1">
       <c r="A478" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
     </row>
     <row r="479" spans="1:1">
       <c r="A479" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
     </row>
     <row r="480" spans="1:1">
       <c r="A480" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
     </row>
     <row r="481" spans="1:1">
       <c r="A481" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="482" spans="1:1">
       <c r="A482" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
     </row>
     <row r="483" spans="1:1">
       <c r="A483" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
     </row>
     <row r="484" spans="1:1">
       <c r="A484" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
     </row>
     <row r="485" spans="1:1">
       <c r="A485" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
     </row>
     <row r="486" spans="1:1">
       <c r="A486" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
     </row>
     <row r="487" spans="1:1">
       <c r="A487" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
     </row>
     <row r="488" spans="1:1">
       <c r="A488" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
     </row>
     <row r="489" spans="1:1">
       <c r="A489" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
     </row>
     <row r="490" spans="1:1">
       <c r="A490" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
     </row>
     <row r="491" spans="1:1">
       <c r="A491" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
     </row>
     <row r="492" spans="1:1">
       <c r="A492" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
     </row>
     <row r="493" spans="1:1">
       <c r="A493" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
     </row>
     <row r="494" spans="1:1">
       <c r="A494" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
     </row>
     <row r="495" spans="1:1">
       <c r="A495" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
     </row>
     <row r="496" spans="1:1">
       <c r="A496" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
     </row>
     <row r="497" spans="1:1">
       <c r="A497" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
     </row>
     <row r="498" spans="1:1">
       <c r="A498" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
     </row>
     <row r="499" spans="1:1">
       <c r="A499" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
     </row>
     <row r="500" spans="1:1">
       <c r="A500" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
     </row>
     <row r="501" spans="1:1">
       <c r="A501" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
     </row>
     <row r="502" spans="1:1">
       <c r="A502" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="503" spans="1:1">
       <c r="A503" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
     </row>
     <row r="504" spans="1:1">
       <c r="A504" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
     </row>
     <row r="505" spans="1:1">
       <c r="A505" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
     </row>
     <row r="506" spans="1:1">
       <c r="A506" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
     </row>
     <row r="507" spans="1:1">
       <c r="A507" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
     </row>
     <row r="508" spans="1:1">
       <c r="A508" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
     </row>
     <row r="509" spans="1:1">
       <c r="A509" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
     </row>
     <row r="510" spans="1:1">
       <c r="A510" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
     </row>
     <row r="511" spans="1:1">
       <c r="A511" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
     </row>
     <row r="512" spans="1:1">
       <c r="A512" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
     </row>
     <row r="513" spans="1:1">
       <c r="A513" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
     </row>
     <row r="514" spans="1:1">
       <c r="A514" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
     </row>
     <row r="515" spans="1:1">
       <c r="A515" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
     </row>
     <row r="516" spans="1:1">
       <c r="A516" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
     </row>
     <row r="517" spans="1:1">
       <c r="A517" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
     </row>
     <row r="518" spans="1:1">
       <c r="A518" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
     </row>
     <row r="519" spans="1:1">
       <c r="A519" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
     </row>
     <row r="520" spans="1:1">
       <c r="A520" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
     </row>
     <row r="521" spans="1:1">
       <c r="A521" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
     </row>
     <row r="522" spans="1:1">
       <c r="A522" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
     </row>
     <row r="523" spans="1:1">
       <c r="A523" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
     </row>
     <row r="524" spans="1:1">
       <c r="A524" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
     </row>
     <row r="525" spans="1:1">
       <c r="A525" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
     </row>
     <row r="526" spans="1:1">
       <c r="A526" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
     </row>
     <row r="527" spans="1:1">
       <c r="A527" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
     </row>
     <row r="528" spans="1:1">
       <c r="A528" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
     </row>
     <row r="529" spans="1:1">
       <c r="A529" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
     </row>
     <row r="530" spans="1:1">
       <c r="A530" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
     </row>
     <row r="531" spans="1:1">
       <c r="A531" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
     </row>
     <row r="532" spans="1:1">
       <c r="A532" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
     </row>
     <row r="533" spans="1:1">
       <c r="A533" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
     </row>
     <row r="534" spans="1:1">
       <c r="A534" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
     </row>
     <row r="535" spans="1:1">
       <c r="A535" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
     </row>
     <row r="536" spans="1:1">
       <c r="A536" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
     </row>
     <row r="537" spans="1:1">
       <c r="A537" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
     </row>
     <row r="538" spans="1:1">
       <c r="A538" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
     </row>
     <row r="539" spans="1:1">
       <c r="A539" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
     </row>
     <row r="540" spans="1:1">
       <c r="A540" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
     </row>
     <row r="542" spans="1:1">
       <c r="A542" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
     </row>
     <row r="543" spans="1:1">
       <c r="A543" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
     </row>
     <row r="544" spans="1:1">
       <c r="A544" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
     </row>
     <row r="545" spans="1:1">
       <c r="A545" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
     </row>
     <row r="546" spans="1:1">
       <c r="A546" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
     </row>
     <row r="547" spans="1:1">
       <c r="A547" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
     </row>
     <row r="548" spans="1:1">
       <c r="A548" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
     </row>
     <row r="549" spans="1:1">
       <c r="A549" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
     </row>
     <row r="550" spans="1:1">
       <c r="A550" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
     </row>
     <row r="551" spans="1:1">
       <c r="A551" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
     </row>
     <row r="552" spans="1:1">
       <c r="A552" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
     </row>
     <row r="553" spans="1:1">
       <c r="A553" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
     </row>
     <row r="554" spans="1:1">
       <c r="A554" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
     </row>
     <row r="555" spans="1:1">
       <c r="A555" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
     </row>
     <row r="556" spans="1:1">
       <c r="A556" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
     </row>
     <row r="557" spans="1:1">
       <c r="A557" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
     </row>
     <row r="558" spans="1:1">
       <c r="A558" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
     </row>
     <row r="559" spans="1:1">
       <c r="A559" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
     </row>
     <row r="561" spans="1:1">
       <c r="A561" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
     </row>
     <row r="562" spans="1:1">
       <c r="A562" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
     </row>
     <row r="563" spans="1:1">
       <c r="A563" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
     </row>
     <row r="564" spans="1:1">
       <c r="A564" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
     </row>
     <row r="565" spans="1:1">
       <c r="A565" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
     </row>
     <row r="566" spans="1:1">
       <c r="A566" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
     </row>
     <row r="567" spans="1:1">
       <c r="A567" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
     </row>
     <row r="568" spans="1:1">
       <c r="A568" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
     </row>
     <row r="569" spans="1:1">
       <c r="A569" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
     </row>
     <row r="570" spans="1:1">
       <c r="A570" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
     </row>
     <row r="571" spans="1:1">
       <c r="A571" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
     </row>
     <row r="572" spans="1:1">
       <c r="A572" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
     </row>
     <row r="573" spans="1:1">
       <c r="A573" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
     </row>
     <row r="574" spans="1:1">
       <c r="A574" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
     </row>
     <row r="575" spans="1:1">
       <c r="A575" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
     </row>
     <row r="576" spans="1:1">
       <c r="A576" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
     </row>
     <row r="577" spans="1:1">
       <c r="A577" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
     </row>
     <row r="578" spans="1:1">
       <c r="A578" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
     </row>
     <row r="579" spans="1:1">
       <c r="A579" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
     </row>
     <row r="580" spans="1:1">
       <c r="A580" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
     </row>
     <row r="581" spans="1:1">
       <c r="A581" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
     </row>
     <row r="582" spans="1:1">
       <c r="A582" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
     </row>
     <row r="583" spans="1:1">
       <c r="A583" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
     </row>
     <row r="584" spans="1:1">
       <c r="A584" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
     </row>
     <row r="586" spans="1:1">
       <c r="A586" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
     </row>
     <row r="587" spans="1:1">
       <c r="A587" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
     </row>
     <row r="588" spans="1:1">
       <c r="A588" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
     </row>
     <row r="589" spans="1:1">
       <c r="A589" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
     </row>
     <row r="590" spans="1:1">
       <c r="A590" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
     </row>
     <row r="591" spans="1:1">
       <c r="A591" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
     </row>
     <row r="592" spans="1:1">
       <c r="A592" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
     </row>
     <row r="593" spans="1:1">
       <c r="A593" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
     </row>
     <row r="594" spans="1:1">
       <c r="A594" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
     </row>
     <row r="595" spans="1:1">
       <c r="A595" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
     </row>
     <row r="596" spans="1:1">
       <c r="A596" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
     </row>
     <row r="597" spans="1:1">
       <c r="A597" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
     </row>
     <row r="598" spans="1:1">
       <c r="A598" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
     </row>
     <row r="599" spans="1:1">
       <c r="A599" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
     </row>
     <row r="600" spans="1:1">
       <c r="A600" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
     </row>
     <row r="602" spans="1:1">
       <c r="A602" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
     </row>
     <row r="603" spans="1:1">
       <c r="A603" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
     </row>
     <row r="604" spans="1:1">
       <c r="A604" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
     </row>
     <row r="605" spans="1:1">
       <c r="A605" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
     </row>
     <row r="606" spans="1:1">
       <c r="A606" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
     </row>
     <row r="607" spans="1:1">
       <c r="A607" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
     </row>
     <row r="608" spans="1:1">
       <c r="A608" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
     </row>
     <row r="609" spans="1:1">
       <c r="A609" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
     </row>
     <row r="610" spans="1:1">
       <c r="A610" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
     </row>
     <row r="611" spans="1:1">
       <c r="A611" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
     </row>
     <row r="612" spans="1:1">
       <c r="A612" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
     </row>
     <row r="613" spans="1:1">
       <c r="A613" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row r="614" spans="1:1">
       <c r="A614" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
     </row>
     <row r="615" spans="1:1">
       <c r="A615" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
     </row>
     <row r="616" spans="1:1">
       <c r="A616" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
     </row>
     <row r="617" spans="1:1">
       <c r="A617" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
     </row>
     <row r="618" spans="1:1">
       <c r="A618" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
     </row>
     <row r="619" spans="1:1">
       <c r="A619" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
     </row>
     <row r="620" spans="1:1">
       <c r="A620" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
     </row>
     <row r="621" spans="1:1">
       <c r="A621" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
     </row>
     <row r="622" spans="1:1">
       <c r="A622" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
     </row>
     <row r="623" spans="1:1">
       <c r="A623" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
     </row>
     <row r="624" spans="1:1">
       <c r="A624" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
     </row>
     <row r="625" spans="1:1">
       <c r="A625" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
     </row>
     <row r="626" spans="1:1">
       <c r="A626" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
     </row>
     <row r="627" spans="1:1">
       <c r="A627" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
     </row>
     <row r="628" spans="1:1">
       <c r="A628" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
     </row>
     <row r="629" spans="1:1">
       <c r="A629" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
     </row>
     <row r="630" spans="1:1">
       <c r="A630" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
     </row>
     <row r="631" spans="1:1">
       <c r="A631" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
     </row>
     <row r="632" spans="1:1">
       <c r="A632" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
     </row>
     <row r="633" spans="1:1">
       <c r="A633" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
     </row>
     <row r="634" spans="1:1">
       <c r="A634" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
     </row>
     <row r="635" spans="1:1">
       <c r="A635" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
     </row>
     <row r="636" spans="1:1">
       <c r="A636" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
     </row>
     <row r="637" spans="1:1">
       <c r="A637" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
     </row>
     <row r="638" spans="1:1">
       <c r="A638" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="639" spans="1:1">
       <c r="A639" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
     </row>
     <row r="640" spans="1:1">
       <c r="A640" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
     </row>
     <row r="641" spans="1:1">
       <c r="A641" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
     </row>
     <row r="642" spans="1:1">
       <c r="A642" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
     </row>
     <row r="643" spans="1:1">
       <c r="A643" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
     </row>
     <row r="644" spans="1:1">
       <c r="A644" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
     </row>
     <row r="645" spans="1:1">
       <c r="A645" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
     </row>
     <row r="646" spans="1:1">
       <c r="A646" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
     </row>
     <row r="647" spans="1:1">
       <c r="A647" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
     </row>
     <row r="648" spans="1:1">
       <c r="A648" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
     </row>
     <row r="649" spans="1:1">
       <c r="A649" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
     </row>
     <row r="650" spans="1:1">
       <c r="A650" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
     </row>
     <row r="651" spans="1:1">
       <c r="A651" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
     </row>
     <row r="652" spans="1:1">
       <c r="A652" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
     </row>
     <row r="653" spans="1:1">
       <c r="A653" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
     </row>
     <row r="654" spans="1:1">
       <c r="A654" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
     </row>
     <row r="655" spans="1:1">
       <c r="A655" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
     </row>
     <row r="656" spans="1:1">
       <c r="A656" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
     </row>
     <row r="657" spans="1:1">
       <c r="A657" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
     </row>
     <row r="658" spans="1:1">
       <c r="A658" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
     </row>
     <row r="659" spans="1:1">
       <c r="A659" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
     </row>
     <row r="660" spans="1:1">
       <c r="A660" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
     </row>
     <row r="661" spans="1:1">
       <c r="A661" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
     </row>
     <row r="662" spans="1:1">
       <c r="A662" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
     </row>
     <row r="663" spans="1:1">
       <c r="A663" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
     </row>
     <row r="664" spans="1:1">
       <c r="A664" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
     </row>
     <row r="665" spans="1:1">
       <c r="A665" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
     </row>
     <row r="666" spans="1:1">
       <c r="A666" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
     </row>
     <row r="667" spans="1:1">
       <c r="A667" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
     </row>
     <row r="668" spans="1:1">
       <c r="A668" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
     </row>
     <row r="669" spans="1:1">
       <c r="A669" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
     </row>
     <row r="670" spans="1:1">
       <c r="A670" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
     </row>
     <row r="671" spans="1:1">
       <c r="A671" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
     </row>
     <row r="672" spans="1:1">
       <c r="A672" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
     </row>
     <row r="674" spans="1:1">
       <c r="A674" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
     </row>
     <row r="675" spans="1:1">
       <c r="A675" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
     </row>
     <row r="676" spans="1:1">
       <c r="A676" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
     </row>
     <row r="677" spans="1:1">
       <c r="A677" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
     </row>
     <row r="678" spans="1:1">
       <c r="A678" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
     </row>
     <row r="679" spans="1:1">
       <c r="A679" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
     </row>
     <row r="680" spans="1:1">
       <c r="A680" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
     </row>
     <row r="681" spans="1:1">
       <c r="A681" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
     </row>
     <row r="682" spans="1:1">
       <c r="A682" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
     </row>
     <row r="683" spans="1:1">
       <c r="A683" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
     </row>
     <row r="685" spans="1:1">
       <c r="A685" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
     </row>
     <row r="686" spans="1:1">
       <c r="A686" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
     </row>
     <row r="687" spans="1:1">
       <c r="A687" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
     </row>
     <row r="688" spans="1:1">
       <c r="A688" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove brute force exceptions and add to placeholder branch
</commit_message>
<xml_diff>
--- a/templates/panos/set_commands/iron_skillet_panos_full.xlsx
+++ b/templates/panos/set_commands/iron_skillet_panos_full.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1118" uniqueCount="1115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="707">
   <si>
     <t>Variable Name</t>
   </si>
@@ -1304,414 +1304,6 @@
     <t>set profiles vulnerability Outbound-VP rules Default-Low-Info packet-capture disable</t>
   </si>
   <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40001 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40001 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40001 time-attribute threshold 10</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40001 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40003 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40003 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40003 time-attribute threshold 100</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40003 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40004 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40004 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40004 time-attribute threshold 30</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40004 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40005 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40005 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40005 time-attribute threshold 20</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40005 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40006 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40006 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40006 time-attribute threshold 20</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40006 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40007 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40007 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40007 time-attribute threshold 10</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40007 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40008 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40008 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40008 time-attribute threshold 25</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40008 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40009 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40009 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40009 time-attribute threshold 10</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40009 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40010 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40010 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40010 time-attribute threshold 20</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40010 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40011 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40011 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40011 time-attribute threshold 10</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40011 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40012 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40012 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40012 time-attribute threshold 7</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40012 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40013 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40013 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40013 time-attribute threshold 10</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40013 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40014 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40014 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40014 time-attribute threshold 20</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40014 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40015 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40015 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40015 time-attribute threshold 20</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40015 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40016 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40016 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40016 time-attribute threshold 20</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40016 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40017 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40017 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40017 time-attribute threshold 10</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40017 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40018 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40018 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40018 time-attribute threshold 40</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40018 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40019 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40019 time-attribute interval 30</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40019 time-attribute threshold 12</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40019 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40020 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40020 time-attribute interval 30</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40020 time-attribute threshold 10</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40020 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40021 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40021 time-attribute interval 100</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40021 time-attribute threshold 8</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40021 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40022 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40022 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40022 time-attribute threshold 30</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40022 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40023 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40023 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40023 time-attribute threshold 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40023 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40028 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40028 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40028 time-attribute threshold 20</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40028 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40030 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40030 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40030 time-attribute threshold 20</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40030 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40031 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40031 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40031 time-attribute threshold 100</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40031 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40032 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40032 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40032 time-attribute threshold 100</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40032 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40033 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40033 time-attribute interval 30</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40033 time-attribute threshold 250</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40033 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40034 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40034 time-attribute interval 10</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40034 time-attribute threshold 20</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40034 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40036 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40036 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40036 time-attribute threshold 7</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40036 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40037 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40037 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40037 time-attribute threshold 10</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40037 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40040 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40040 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40040 time-attribute threshold 20</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40040 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40044 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40044 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40044 time-attribute threshold 10</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40044 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40059 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40059 time-attribute interval 30</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40059 time-attribute threshold 100</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40059 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40078 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40078 time-attribute interval 10</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40078 time-attribute threshold 100</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Outbound-VP threat-exception 40078 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
     <t>set profiles vulnerability Inbound-VP rules Block-Critical-High-Medium action reset-both</t>
   </si>
   <si>
@@ -1760,414 +1352,6 @@
     <t>set profiles vulnerability Inbound-VP rules Default-Low-Info packet-capture disable</t>
   </si>
   <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40001 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40001 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40001 time-attribute threshold 10</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40001 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40003 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40003 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40003 time-attribute threshold 100</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40003 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40004 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40004 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40004 time-attribute threshold 30</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40004 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40005 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40005 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40005 time-attribute threshold 20</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40005 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40006 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40006 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40006 time-attribute threshold 20</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40006 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40007 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40007 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40007 time-attribute threshold 10</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40007 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40008 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40008 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40008 time-attribute threshold 25</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40008 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40009 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40009 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40009 time-attribute threshold 10</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40009 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40010 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40010 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40010 time-attribute threshold 20</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40010 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40011 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40011 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40011 time-attribute threshold 10</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40011 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40012 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40012 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40012 time-attribute threshold 7</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40012 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40013 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40013 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40013 time-attribute threshold 10</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40013 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40014 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40014 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40014 time-attribute threshold 20</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40014 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40015 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40015 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40015 time-attribute threshold 20</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40015 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40016 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40016 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40016 time-attribute threshold 20</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40016 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40017 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40017 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40017 time-attribute threshold 10</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40017 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40018 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40018 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40018 time-attribute threshold 40</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40018 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40019 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40019 time-attribute interval 30</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40019 time-attribute threshold 12</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40019 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40020 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40020 time-attribute interval 30</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40020 time-attribute threshold 10</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40020 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40021 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40021 time-attribute interval 100</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40021 time-attribute threshold 8</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40021 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40022 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40022 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40022 time-attribute threshold 30</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40022 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40023 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40023 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40023 time-attribute threshold 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40023 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40028 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40028 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40028 time-attribute threshold 20</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40028 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40030 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40030 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40030 time-attribute threshold 20</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40030 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40031 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40031 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40031 time-attribute threshold 100</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40031 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40032 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40032 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40032 time-attribute threshold 100</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40032 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40033 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40033 time-attribute interval 30</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40033 time-attribute threshold 250</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40033 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40034 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40034 time-attribute interval 10</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40034 time-attribute threshold 20</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40034 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40036 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40036 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40036 time-attribute threshold 7</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40036 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40037 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40037 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40037 time-attribute threshold 10</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40037 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40040 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40040 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40040 time-attribute threshold 20</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40040 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40044 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40044 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40044 time-attribute threshold 10</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40044 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40059 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40059 time-attribute interval 30</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40059 time-attribute threshold 100</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40059 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40078 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40078 time-attribute interval 10</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40078 time-attribute threshold 100</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Inbound-VP threat-exception 40078 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
     <t>set profiles vulnerability Internal-VP rules Block-Critical-High action reset-both</t>
   </si>
   <si>
@@ -2214,414 +1398,6 @@
   </si>
   <si>
     <t>set profiles vulnerability Internal-VP rules Default-Medium-Low-Info packet-capture disable</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40001 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40001 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40001 time-attribute threshold 10</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40001 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40003 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40003 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40003 time-attribute threshold 100</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40003 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40004 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40004 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40004 time-attribute threshold 30</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40004 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40005 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40005 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40005 time-attribute threshold 20</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40005 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40006 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40006 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40006 time-attribute threshold 20</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40006 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40007 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40007 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40007 time-attribute threshold 10</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40007 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40008 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40008 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40008 time-attribute threshold 25</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40008 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40009 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40009 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40009 time-attribute threshold 10</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40009 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40010 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40010 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40010 time-attribute threshold 20</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40010 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40011 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40011 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40011 time-attribute threshold 10</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40011 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40012 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40012 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40012 time-attribute threshold 7</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40012 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40013 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40013 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40013 time-attribute threshold 10</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40013 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40014 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40014 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40014 time-attribute threshold 20</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40014 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40015 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40015 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40015 time-attribute threshold 20</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40015 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40016 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40016 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40016 time-attribute threshold 20</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40016 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40017 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40017 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40017 time-attribute threshold 10</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40017 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40018 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40018 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40018 time-attribute threshold 40</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40018 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40019 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40019 time-attribute interval 30</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40019 time-attribute threshold 12</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40019 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40020 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40020 time-attribute interval 30</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40020 time-attribute threshold 10</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40020 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40021 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40021 time-attribute interval 100</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40021 time-attribute threshold 8</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40021 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40022 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40022 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40022 time-attribute threshold 30</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40022 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40023 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40023 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40023 time-attribute threshold 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40023 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40028 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40028 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40028 time-attribute threshold 20</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40028 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40030 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40030 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40030 time-attribute threshold 20</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40030 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40031 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40031 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40031 time-attribute threshold 100</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40031 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40032 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40032 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40032 time-attribute threshold 100</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40032 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40033 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40033 time-attribute interval 30</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40033 time-attribute threshold 250</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40033 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40034 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40034 time-attribute interval 10</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40034 time-attribute threshold 20</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40034 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40036 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40036 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40036 time-attribute threshold 7</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40036 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40037 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40037 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40037 time-attribute threshold 10</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40037 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40040 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40040 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40040 time-attribute threshold 20</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40040 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40044 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40044 time-attribute interval 60</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40044 time-attribute threshold 10</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40044 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40059 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40059 time-attribute interval 30</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40059 time-attribute threshold 100</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40059 time-attribute track-by source-and-destination</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40078 action alert</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40078 time-attribute interval 10</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40078 time-attribute threshold 100</t>
-  </si>
-  <si>
-    <t>set profiles vulnerability Internal-VP threat-exception 40078 time-attribute track-by source-and-destination</t>
   </si>
   <si>
     <t>set profiles vulnerability Alert-Only-VP rules Alert-All action alert</t>
@@ -4047,7 +2823,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:A1082"/>
+  <dimension ref="A2:A674"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -6135,3229 +4911,1189 @@
         <v>469</v>
       </c>
     </row>
-    <row r="429" spans="1:1">
-      <c r="A429" t="s">
-        <v>470</v>
-      </c>
-    </row>
     <row r="430" spans="1:1">
       <c r="A430" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="431" spans="1:1">
       <c r="A431" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="432" spans="1:1">
       <c r="A432" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="433" spans="1:1">
       <c r="A433" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="434" spans="1:1">
       <c r="A434" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="435" spans="1:1">
       <c r="A435" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="436" spans="1:1">
       <c r="A436" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="437" spans="1:1">
       <c r="A437" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="438" spans="1:1">
       <c r="A438" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="439" spans="1:1">
       <c r="A439" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="440" spans="1:1">
       <c r="A440" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="441" spans="1:1">
       <c r="A441" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="442" spans="1:1">
       <c r="A442" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="443" spans="1:1">
       <c r="A443" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="444" spans="1:1">
       <c r="A444" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="445" spans="1:1">
       <c r="A445" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="446" spans="1:1">
       <c r="A446" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="447" spans="1:1">
-      <c r="A447" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="448" spans="1:1">
       <c r="A448" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="449" spans="1:1">
       <c r="A449" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="450" spans="1:1">
       <c r="A450" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="451" spans="1:1">
       <c r="A451" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="452" spans="1:1">
       <c r="A452" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="453" spans="1:1">
       <c r="A453" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="454" spans="1:1">
       <c r="A454" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="455" spans="1:1">
       <c r="A455" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="456" spans="1:1">
       <c r="A456" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="457" spans="1:1">
       <c r="A457" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="458" spans="1:1">
       <c r="A458" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="459" spans="1:1">
       <c r="A459" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="460" spans="1:1">
       <c r="A460" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="461" spans="1:1">
       <c r="A461" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="462" spans="1:1">
       <c r="A462" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="463" spans="1:1">
       <c r="A463" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="464" spans="1:1">
       <c r="A464" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="465" spans="1:1">
       <c r="A465" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="466" spans="1:1">
       <c r="A466" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="467" spans="1:1">
       <c r="A467" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="468" spans="1:1">
       <c r="A468" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="469" spans="1:1">
       <c r="A469" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="470" spans="1:1">
       <c r="A470" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="471" spans="1:1">
       <c r="A471" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="472" spans="1:1">
       <c r="A472" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="473" spans="1:1">
       <c r="A473" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="474" spans="1:1">
       <c r="A474" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="475" spans="1:1">
       <c r="A475" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="476" spans="1:1">
       <c r="A476" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="477" spans="1:1">
-      <c r="A477" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
     </row>
     <row r="478" spans="1:1">
       <c r="A478" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
     </row>
     <row r="479" spans="1:1">
       <c r="A479" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="480" spans="1:1">
       <c r="A480" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
     </row>
     <row r="481" spans="1:1">
       <c r="A481" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
     </row>
     <row r="482" spans="1:1">
       <c r="A482" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
     </row>
     <row r="483" spans="1:1">
       <c r="A483" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
     </row>
     <row r="484" spans="1:1">
       <c r="A484" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
     </row>
     <row r="485" spans="1:1">
       <c r="A485" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
     </row>
     <row r="486" spans="1:1">
       <c r="A486" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
     </row>
     <row r="487" spans="1:1">
       <c r="A487" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
     </row>
     <row r="488" spans="1:1">
       <c r="A488" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
     <row r="489" spans="1:1">
       <c r="A489" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="490" spans="1:1">
       <c r="A490" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
     </row>
     <row r="491" spans="1:1">
       <c r="A491" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
     </row>
     <row r="492" spans="1:1">
       <c r="A492" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
     </row>
     <row r="493" spans="1:1">
       <c r="A493" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
     </row>
     <row r="494" spans="1:1">
       <c r="A494" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
     </row>
     <row r="495" spans="1:1">
       <c r="A495" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
     </row>
     <row r="496" spans="1:1">
       <c r="A496" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
     </row>
     <row r="497" spans="1:1">
       <c r="A497" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="498" spans="1:1">
       <c r="A498" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
     </row>
     <row r="499" spans="1:1">
       <c r="A499" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
     </row>
     <row r="500" spans="1:1">
       <c r="A500" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
     </row>
     <row r="501" spans="1:1">
       <c r="A501" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
     </row>
     <row r="502" spans="1:1">
       <c r="A502" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
     </row>
     <row r="503" spans="1:1">
       <c r="A503" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
     </row>
     <row r="504" spans="1:1">
       <c r="A504" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
     </row>
     <row r="505" spans="1:1">
       <c r="A505" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
     </row>
     <row r="506" spans="1:1">
       <c r="A506" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
     </row>
     <row r="507" spans="1:1">
       <c r="A507" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
     </row>
     <row r="508" spans="1:1">
       <c r="A508" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
     </row>
     <row r="509" spans="1:1">
       <c r="A509" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
     </row>
     <row r="510" spans="1:1">
       <c r="A510" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
     </row>
     <row r="511" spans="1:1">
       <c r="A511" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
     </row>
     <row r="512" spans="1:1">
       <c r="A512" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
     </row>
     <row r="513" spans="1:1">
       <c r="A513" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
     </row>
     <row r="514" spans="1:1">
       <c r="A514" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
     </row>
     <row r="515" spans="1:1">
       <c r="A515" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
     </row>
     <row r="516" spans="1:1">
       <c r="A516" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
     </row>
     <row r="517" spans="1:1">
       <c r="A517" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
     </row>
     <row r="518" spans="1:1">
       <c r="A518" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
     </row>
     <row r="519" spans="1:1">
       <c r="A519" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
     </row>
     <row r="520" spans="1:1">
       <c r="A520" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
     </row>
     <row r="521" spans="1:1">
       <c r="A521" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
     </row>
     <row r="522" spans="1:1">
       <c r="A522" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
     </row>
     <row r="523" spans="1:1">
       <c r="A523" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
     </row>
     <row r="524" spans="1:1">
       <c r="A524" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
     </row>
     <row r="525" spans="1:1">
       <c r="A525" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
     </row>
     <row r="526" spans="1:1">
       <c r="A526" t="s">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="527" spans="1:1">
-      <c r="A527" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
     </row>
     <row r="528" spans="1:1">
       <c r="A528" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
     </row>
     <row r="529" spans="1:1">
       <c r="A529" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
     </row>
     <row r="530" spans="1:1">
       <c r="A530" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
     </row>
     <row r="531" spans="1:1">
       <c r="A531" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
     </row>
     <row r="532" spans="1:1">
       <c r="A532" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
     </row>
     <row r="533" spans="1:1">
       <c r="A533" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
     </row>
     <row r="534" spans="1:1">
       <c r="A534" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
     </row>
     <row r="535" spans="1:1">
       <c r="A535" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
     </row>
     <row r="536" spans="1:1">
       <c r="A536" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
     </row>
     <row r="537" spans="1:1">
       <c r="A537" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
     </row>
     <row r="538" spans="1:1">
       <c r="A538" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
     </row>
     <row r="539" spans="1:1">
       <c r="A539" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
     </row>
     <row r="540" spans="1:1">
       <c r="A540" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
     </row>
     <row r="541" spans="1:1">
       <c r="A541" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
     </row>
     <row r="542" spans="1:1">
       <c r="A542" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
     </row>
     <row r="543" spans="1:1">
       <c r="A543" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
     </row>
     <row r="544" spans="1:1">
       <c r="A544" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
     </row>
     <row r="545" spans="1:1">
       <c r="A545" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="546" spans="1:1">
-      <c r="A546" t="s">
-        <v>587</v>
+        <v>582</v>
       </c>
     </row>
     <row r="547" spans="1:1">
       <c r="A547" t="s">
-        <v>588</v>
+        <v>583</v>
       </c>
     </row>
     <row r="548" spans="1:1">
       <c r="A548" t="s">
-        <v>589</v>
+        <v>584</v>
       </c>
     </row>
     <row r="549" spans="1:1">
       <c r="A549" t="s">
-        <v>590</v>
+        <v>585</v>
       </c>
     </row>
     <row r="550" spans="1:1">
       <c r="A550" t="s">
-        <v>591</v>
+        <v>586</v>
       </c>
     </row>
     <row r="551" spans="1:1">
       <c r="A551" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
     </row>
     <row r="552" spans="1:1">
       <c r="A552" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
     </row>
     <row r="553" spans="1:1">
       <c r="A553" t="s">
-        <v>594</v>
+        <v>589</v>
       </c>
     </row>
     <row r="554" spans="1:1">
       <c r="A554" t="s">
-        <v>595</v>
+        <v>590</v>
       </c>
     </row>
     <row r="555" spans="1:1">
       <c r="A555" t="s">
-        <v>596</v>
+        <v>591</v>
       </c>
     </row>
     <row r="556" spans="1:1">
       <c r="A556" t="s">
-        <v>597</v>
+        <v>592</v>
       </c>
     </row>
     <row r="557" spans="1:1">
       <c r="A557" t="s">
-        <v>598</v>
+        <v>593</v>
       </c>
     </row>
     <row r="558" spans="1:1">
       <c r="A558" t="s">
-        <v>599</v>
+        <v>594</v>
       </c>
     </row>
     <row r="559" spans="1:1">
       <c r="A559" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
     </row>
     <row r="560" spans="1:1">
       <c r="A560" t="s">
-        <v>601</v>
+        <v>596</v>
       </c>
     </row>
     <row r="561" spans="1:1">
       <c r="A561" t="s">
-        <v>602</v>
+        <v>597</v>
       </c>
     </row>
     <row r="562" spans="1:1">
       <c r="A562" t="s">
-        <v>603</v>
+        <v>598</v>
       </c>
     </row>
     <row r="563" spans="1:1">
       <c r="A563" t="s">
-        <v>604</v>
+        <v>599</v>
       </c>
     </row>
     <row r="564" spans="1:1">
       <c r="A564" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
     </row>
     <row r="565" spans="1:1">
       <c r="A565" t="s">
-        <v>606</v>
+        <v>601</v>
       </c>
     </row>
     <row r="566" spans="1:1">
       <c r="A566" t="s">
-        <v>607</v>
+        <v>602</v>
       </c>
     </row>
     <row r="567" spans="1:1">
       <c r="A567" t="s">
-        <v>608</v>
+        <v>603</v>
       </c>
     </row>
     <row r="568" spans="1:1">
       <c r="A568" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
     </row>
     <row r="569" spans="1:1">
       <c r="A569" t="s">
-        <v>610</v>
+        <v>605</v>
       </c>
     </row>
     <row r="570" spans="1:1">
       <c r="A570" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="571" spans="1:1">
-      <c r="A571" t="s">
-        <v>612</v>
+        <v>606</v>
       </c>
     </row>
     <row r="572" spans="1:1">
       <c r="A572" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
     </row>
     <row r="573" spans="1:1">
       <c r="A573" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
     </row>
     <row r="574" spans="1:1">
       <c r="A574" t="s">
-        <v>615</v>
+        <v>609</v>
       </c>
     </row>
     <row r="575" spans="1:1">
       <c r="A575" t="s">
-        <v>616</v>
+        <v>610</v>
       </c>
     </row>
     <row r="576" spans="1:1">
       <c r="A576" t="s">
-        <v>617</v>
+        <v>611</v>
       </c>
     </row>
     <row r="577" spans="1:1">
       <c r="A577" t="s">
-        <v>618</v>
+        <v>612</v>
       </c>
     </row>
     <row r="578" spans="1:1">
       <c r="A578" t="s">
-        <v>619</v>
+        <v>613</v>
       </c>
     </row>
     <row r="579" spans="1:1">
       <c r="A579" t="s">
-        <v>620</v>
+        <v>614</v>
       </c>
     </row>
     <row r="580" spans="1:1">
       <c r="A580" t="s">
-        <v>621</v>
+        <v>615</v>
       </c>
     </row>
     <row r="581" spans="1:1">
       <c r="A581" t="s">
-        <v>622</v>
+        <v>616</v>
       </c>
     </row>
     <row r="582" spans="1:1">
       <c r="A582" t="s">
-        <v>623</v>
+        <v>617</v>
       </c>
     </row>
     <row r="583" spans="1:1">
       <c r="A583" t="s">
-        <v>624</v>
+        <v>618</v>
       </c>
     </row>
     <row r="584" spans="1:1">
       <c r="A584" t="s">
-        <v>625</v>
+        <v>619</v>
       </c>
     </row>
     <row r="585" spans="1:1">
       <c r="A585" t="s">
-        <v>626</v>
+        <v>620</v>
       </c>
     </row>
     <row r="586" spans="1:1">
       <c r="A586" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="587" spans="1:1">
-      <c r="A587" t="s">
-        <v>628</v>
+        <v>621</v>
       </c>
     </row>
     <row r="588" spans="1:1">
       <c r="A588" t="s">
-        <v>629</v>
+        <v>622</v>
       </c>
     </row>
     <row r="589" spans="1:1">
       <c r="A589" t="s">
-        <v>630</v>
+        <v>623</v>
       </c>
     </row>
     <row r="590" spans="1:1">
       <c r="A590" t="s">
-        <v>631</v>
+        <v>624</v>
       </c>
     </row>
     <row r="591" spans="1:1">
       <c r="A591" t="s">
-        <v>632</v>
+        <v>625</v>
       </c>
     </row>
     <row r="592" spans="1:1">
       <c r="A592" t="s">
-        <v>633</v>
+        <v>626</v>
       </c>
     </row>
     <row r="593" spans="1:1">
       <c r="A593" t="s">
-        <v>634</v>
+        <v>627</v>
       </c>
     </row>
     <row r="594" spans="1:1">
       <c r="A594" t="s">
-        <v>635</v>
+        <v>628</v>
       </c>
     </row>
     <row r="595" spans="1:1">
       <c r="A595" t="s">
-        <v>636</v>
+        <v>629</v>
       </c>
     </row>
     <row r="596" spans="1:1">
       <c r="A596" t="s">
-        <v>637</v>
+        <v>630</v>
       </c>
     </row>
     <row r="597" spans="1:1">
       <c r="A597" t="s">
-        <v>638</v>
+        <v>631</v>
       </c>
     </row>
     <row r="598" spans="1:1">
       <c r="A598" t="s">
-        <v>639</v>
+        <v>632</v>
       </c>
     </row>
     <row r="599" spans="1:1">
       <c r="A599" t="s">
-        <v>640</v>
+        <v>633</v>
       </c>
     </row>
     <row r="600" spans="1:1">
       <c r="A600" t="s">
-        <v>641</v>
+        <v>634</v>
       </c>
     </row>
     <row r="601" spans="1:1">
       <c r="A601" t="s">
-        <v>642</v>
+        <v>635</v>
       </c>
     </row>
     <row r="602" spans="1:1">
       <c r="A602" t="s">
-        <v>643</v>
+        <v>636</v>
       </c>
     </row>
     <row r="603" spans="1:1">
       <c r="A603" t="s">
-        <v>644</v>
+        <v>637</v>
       </c>
     </row>
     <row r="604" spans="1:1">
       <c r="A604" t="s">
-        <v>645</v>
+        <v>638</v>
       </c>
     </row>
     <row r="605" spans="1:1">
       <c r="A605" t="s">
-        <v>646</v>
+        <v>639</v>
       </c>
     </row>
     <row r="606" spans="1:1">
       <c r="A606" t="s">
-        <v>647</v>
+        <v>640</v>
       </c>
     </row>
     <row r="607" spans="1:1">
       <c r="A607" t="s">
-        <v>648</v>
+        <v>641</v>
       </c>
     </row>
     <row r="608" spans="1:1">
       <c r="A608" t="s">
-        <v>649</v>
+        <v>642</v>
       </c>
     </row>
     <row r="609" spans="1:1">
       <c r="A609" t="s">
-        <v>650</v>
+        <v>643</v>
       </c>
     </row>
     <row r="610" spans="1:1">
       <c r="A610" t="s">
-        <v>651</v>
+        <v>644</v>
       </c>
     </row>
     <row r="611" spans="1:1">
       <c r="A611" t="s">
-        <v>652</v>
+        <v>645</v>
       </c>
     </row>
     <row r="612" spans="1:1">
       <c r="A612" t="s">
-        <v>653</v>
+        <v>646</v>
       </c>
     </row>
     <row r="613" spans="1:1">
       <c r="A613" t="s">
-        <v>654</v>
+        <v>647</v>
       </c>
     </row>
     <row r="614" spans="1:1">
       <c r="A614" t="s">
-        <v>655</v>
+        <v>648</v>
       </c>
     </row>
     <row r="615" spans="1:1">
       <c r="A615" t="s">
-        <v>656</v>
+        <v>649</v>
       </c>
     </row>
     <row r="616" spans="1:1">
       <c r="A616" t="s">
-        <v>657</v>
+        <v>650</v>
       </c>
     </row>
     <row r="617" spans="1:1">
       <c r="A617" t="s">
-        <v>658</v>
+        <v>651</v>
       </c>
     </row>
     <row r="618" spans="1:1">
       <c r="A618" t="s">
-        <v>659</v>
+        <v>652</v>
       </c>
     </row>
     <row r="619" spans="1:1">
       <c r="A619" t="s">
-        <v>660</v>
+        <v>653</v>
       </c>
     </row>
     <row r="620" spans="1:1">
       <c r="A620" t="s">
-        <v>661</v>
+        <v>654</v>
       </c>
     </row>
     <row r="621" spans="1:1">
       <c r="A621" t="s">
-        <v>662</v>
+        <v>655</v>
       </c>
     </row>
     <row r="622" spans="1:1">
       <c r="A622" t="s">
-        <v>663</v>
+        <v>656</v>
       </c>
     </row>
     <row r="623" spans="1:1">
       <c r="A623" t="s">
-        <v>664</v>
+        <v>657</v>
       </c>
     </row>
     <row r="624" spans="1:1">
       <c r="A624" t="s">
-        <v>665</v>
+        <v>658</v>
       </c>
     </row>
     <row r="625" spans="1:1">
       <c r="A625" t="s">
-        <v>666</v>
+        <v>659</v>
       </c>
     </row>
     <row r="626" spans="1:1">
       <c r="A626" t="s">
-        <v>667</v>
+        <v>660</v>
       </c>
     </row>
     <row r="627" spans="1:1">
       <c r="A627" t="s">
-        <v>668</v>
+        <v>661</v>
       </c>
     </row>
     <row r="628" spans="1:1">
       <c r="A628" t="s">
-        <v>669</v>
+        <v>662</v>
       </c>
     </row>
     <row r="629" spans="1:1">
       <c r="A629" t="s">
-        <v>670</v>
+        <v>663</v>
       </c>
     </row>
     <row r="630" spans="1:1">
       <c r="A630" t="s">
-        <v>671</v>
+        <v>664</v>
       </c>
     </row>
     <row r="631" spans="1:1">
       <c r="A631" t="s">
-        <v>672</v>
+        <v>665</v>
       </c>
     </row>
     <row r="632" spans="1:1">
       <c r="A632" t="s">
-        <v>673</v>
+        <v>666</v>
       </c>
     </row>
     <row r="633" spans="1:1">
       <c r="A633" t="s">
-        <v>674</v>
+        <v>667</v>
       </c>
     </row>
     <row r="634" spans="1:1">
       <c r="A634" t="s">
-        <v>675</v>
+        <v>668</v>
       </c>
     </row>
     <row r="635" spans="1:1">
       <c r="A635" t="s">
-        <v>676</v>
+        <v>669</v>
       </c>
     </row>
     <row r="636" spans="1:1">
       <c r="A636" t="s">
-        <v>677</v>
+        <v>670</v>
       </c>
     </row>
     <row r="637" spans="1:1">
       <c r="A637" t="s">
-        <v>678</v>
+        <v>671</v>
       </c>
     </row>
     <row r="638" spans="1:1">
       <c r="A638" t="s">
-        <v>679</v>
+        <v>672</v>
       </c>
     </row>
     <row r="639" spans="1:1">
       <c r="A639" t="s">
-        <v>680</v>
+        <v>673</v>
       </c>
     </row>
     <row r="640" spans="1:1">
       <c r="A640" t="s">
-        <v>681</v>
+        <v>674</v>
       </c>
     </row>
     <row r="641" spans="1:1">
       <c r="A641" t="s">
-        <v>682</v>
+        <v>675</v>
       </c>
     </row>
     <row r="642" spans="1:1">
       <c r="A642" t="s">
-        <v>683</v>
+        <v>676</v>
       </c>
     </row>
     <row r="643" spans="1:1">
       <c r="A643" t="s">
-        <v>684</v>
+        <v>677</v>
       </c>
     </row>
     <row r="644" spans="1:1">
       <c r="A644" t="s">
-        <v>685</v>
+        <v>678</v>
       </c>
     </row>
     <row r="645" spans="1:1">
       <c r="A645" t="s">
-        <v>686</v>
+        <v>679</v>
       </c>
     </row>
     <row r="646" spans="1:1">
       <c r="A646" t="s">
-        <v>687</v>
+        <v>680</v>
       </c>
     </row>
     <row r="647" spans="1:1">
       <c r="A647" t="s">
-        <v>688</v>
+        <v>681</v>
       </c>
     </row>
     <row r="648" spans="1:1">
       <c r="A648" t="s">
-        <v>689</v>
+        <v>682</v>
       </c>
     </row>
     <row r="649" spans="1:1">
       <c r="A649" t="s">
-        <v>690</v>
+        <v>683</v>
       </c>
     </row>
     <row r="650" spans="1:1">
       <c r="A650" t="s">
-        <v>691</v>
+        <v>684</v>
       </c>
     </row>
     <row r="651" spans="1:1">
       <c r="A651" t="s">
-        <v>692</v>
+        <v>685</v>
       </c>
     </row>
     <row r="652" spans="1:1">
       <c r="A652" t="s">
-        <v>693</v>
+        <v>686</v>
       </c>
     </row>
     <row r="653" spans="1:1">
       <c r="A653" t="s">
-        <v>694</v>
+        <v>687</v>
       </c>
     </row>
     <row r="654" spans="1:1">
       <c r="A654" t="s">
-        <v>695</v>
+        <v>688</v>
       </c>
     </row>
     <row r="655" spans="1:1">
       <c r="A655" t="s">
-        <v>696</v>
+        <v>689</v>
       </c>
     </row>
     <row r="656" spans="1:1">
       <c r="A656" t="s">
-        <v>697</v>
+        <v>690</v>
       </c>
     </row>
     <row r="657" spans="1:1">
       <c r="A657" t="s">
-        <v>698</v>
+        <v>691</v>
       </c>
     </row>
     <row r="658" spans="1:1">
       <c r="A658" t="s">
-        <v>699</v>
-      </c>
-    </row>
-    <row r="659" spans="1:1">
-      <c r="A659" t="s">
-        <v>700</v>
+        <v>692</v>
       </c>
     </row>
     <row r="660" spans="1:1">
       <c r="A660" t="s">
-        <v>701</v>
+        <v>693</v>
       </c>
     </row>
     <row r="661" spans="1:1">
       <c r="A661" t="s">
-        <v>702</v>
+        <v>694</v>
       </c>
     </row>
     <row r="662" spans="1:1">
       <c r="A662" t="s">
-        <v>703</v>
+        <v>695</v>
       </c>
     </row>
     <row r="663" spans="1:1">
       <c r="A663" t="s">
-        <v>704</v>
+        <v>696</v>
       </c>
     </row>
     <row r="664" spans="1:1">
       <c r="A664" t="s">
-        <v>705</v>
+        <v>697</v>
       </c>
     </row>
     <row r="665" spans="1:1">
       <c r="A665" t="s">
-        <v>706</v>
+        <v>698</v>
       </c>
     </row>
     <row r="666" spans="1:1">
       <c r="A666" t="s">
-        <v>707</v>
+        <v>699</v>
       </c>
     </row>
     <row r="667" spans="1:1">
       <c r="A667" t="s">
-        <v>708</v>
+        <v>700</v>
       </c>
     </row>
     <row r="668" spans="1:1">
       <c r="A668" t="s">
-        <v>709</v>
+        <v>701</v>
       </c>
     </row>
     <row r="669" spans="1:1">
       <c r="A669" t="s">
-        <v>710</v>
-      </c>
-    </row>
-    <row r="670" spans="1:1">
-      <c r="A670" t="s">
-        <v>711</v>
+        <v>702</v>
       </c>
     </row>
     <row r="671" spans="1:1">
       <c r="A671" t="s">
-        <v>712</v>
+        <v>703</v>
       </c>
     </row>
     <row r="672" spans="1:1">
       <c r="A672" t="s">
-        <v>713</v>
+        <v>704</v>
       </c>
     </row>
     <row r="673" spans="1:1">
       <c r="A673" t="s">
-        <v>714</v>
+        <v>705</v>
       </c>
     </row>
     <row r="674" spans="1:1">
       <c r="A674" t="s">
-        <v>715</v>
-      </c>
-    </row>
-    <row r="675" spans="1:1">
-      <c r="A675" t="s">
-        <v>716</v>
-      </c>
-    </row>
-    <row r="676" spans="1:1">
-      <c r="A676" t="s">
-        <v>717</v>
-      </c>
-    </row>
-    <row r="677" spans="1:1">
-      <c r="A677" t="s">
-        <v>718</v>
-      </c>
-    </row>
-    <row r="678" spans="1:1">
-      <c r="A678" t="s">
-        <v>719</v>
-      </c>
-    </row>
-    <row r="679" spans="1:1">
-      <c r="A679" t="s">
-        <v>720</v>
-      </c>
-    </row>
-    <row r="680" spans="1:1">
-      <c r="A680" t="s">
-        <v>721</v>
-      </c>
-    </row>
-    <row r="681" spans="1:1">
-      <c r="A681" t="s">
-        <v>722</v>
-      </c>
-    </row>
-    <row r="682" spans="1:1">
-      <c r="A682" t="s">
-        <v>723</v>
-      </c>
-    </row>
-    <row r="683" spans="1:1">
-      <c r="A683" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="684" spans="1:1">
-      <c r="A684" t="s">
-        <v>725</v>
-      </c>
-    </row>
-    <row r="685" spans="1:1">
-      <c r="A685" t="s">
-        <v>726</v>
-      </c>
-    </row>
-    <row r="686" spans="1:1">
-      <c r="A686" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="687" spans="1:1">
-      <c r="A687" t="s">
-        <v>728</v>
-      </c>
-    </row>
-    <row r="688" spans="1:1">
-      <c r="A688" t="s">
-        <v>729</v>
-      </c>
-    </row>
-    <row r="689" spans="1:1">
-      <c r="A689" t="s">
-        <v>730</v>
-      </c>
-    </row>
-    <row r="690" spans="1:1">
-      <c r="A690" t="s">
-        <v>731</v>
-      </c>
-    </row>
-    <row r="691" spans="1:1">
-      <c r="A691" t="s">
-        <v>732</v>
-      </c>
-    </row>
-    <row r="692" spans="1:1">
-      <c r="A692" t="s">
-        <v>733</v>
-      </c>
-    </row>
-    <row r="693" spans="1:1">
-      <c r="A693" t="s">
-        <v>734</v>
-      </c>
-    </row>
-    <row r="694" spans="1:1">
-      <c r="A694" t="s">
-        <v>735</v>
-      </c>
-    </row>
-    <row r="695" spans="1:1">
-      <c r="A695" t="s">
-        <v>736</v>
-      </c>
-    </row>
-    <row r="696" spans="1:1">
-      <c r="A696" t="s">
-        <v>737</v>
-      </c>
-    </row>
-    <row r="697" spans="1:1">
-      <c r="A697" t="s">
-        <v>738</v>
-      </c>
-    </row>
-    <row r="698" spans="1:1">
-      <c r="A698" t="s">
-        <v>739</v>
-      </c>
-    </row>
-    <row r="699" spans="1:1">
-      <c r="A699" t="s">
-        <v>740</v>
-      </c>
-    </row>
-    <row r="700" spans="1:1">
-      <c r="A700" t="s">
-        <v>741</v>
-      </c>
-    </row>
-    <row r="701" spans="1:1">
-      <c r="A701" t="s">
-        <v>742</v>
-      </c>
-    </row>
-    <row r="702" spans="1:1">
-      <c r="A702" t="s">
-        <v>743</v>
-      </c>
-    </row>
-    <row r="703" spans="1:1">
-      <c r="A703" t="s">
-        <v>744</v>
-      </c>
-    </row>
-    <row r="704" spans="1:1">
-      <c r="A704" t="s">
-        <v>745</v>
-      </c>
-    </row>
-    <row r="705" spans="1:1">
-      <c r="A705" t="s">
-        <v>746</v>
-      </c>
-    </row>
-    <row r="706" spans="1:1">
-      <c r="A706" t="s">
-        <v>747</v>
-      </c>
-    </row>
-    <row r="707" spans="1:1">
-      <c r="A707" t="s">
-        <v>748</v>
-      </c>
-    </row>
-    <row r="708" spans="1:1">
-      <c r="A708" t="s">
-        <v>749</v>
-      </c>
-    </row>
-    <row r="709" spans="1:1">
-      <c r="A709" t="s">
-        <v>750</v>
-      </c>
-    </row>
-    <row r="710" spans="1:1">
-      <c r="A710" t="s">
-        <v>751</v>
-      </c>
-    </row>
-    <row r="711" spans="1:1">
-      <c r="A711" t="s">
-        <v>752</v>
-      </c>
-    </row>
-    <row r="712" spans="1:1">
-      <c r="A712" t="s">
-        <v>753</v>
-      </c>
-    </row>
-    <row r="713" spans="1:1">
-      <c r="A713" t="s">
-        <v>754</v>
-      </c>
-    </row>
-    <row r="714" spans="1:1">
-      <c r="A714" t="s">
-        <v>755</v>
-      </c>
-    </row>
-    <row r="715" spans="1:1">
-      <c r="A715" t="s">
-        <v>756</v>
-      </c>
-    </row>
-    <row r="716" spans="1:1">
-      <c r="A716" t="s">
-        <v>757</v>
-      </c>
-    </row>
-    <row r="717" spans="1:1">
-      <c r="A717" t="s">
-        <v>758</v>
-      </c>
-    </row>
-    <row r="718" spans="1:1">
-      <c r="A718" t="s">
-        <v>759</v>
-      </c>
-    </row>
-    <row r="719" spans="1:1">
-      <c r="A719" t="s">
-        <v>760</v>
-      </c>
-    </row>
-    <row r="720" spans="1:1">
-      <c r="A720" t="s">
-        <v>761</v>
-      </c>
-    </row>
-    <row r="721" spans="1:1">
-      <c r="A721" t="s">
-        <v>762</v>
-      </c>
-    </row>
-    <row r="722" spans="1:1">
-      <c r="A722" t="s">
-        <v>763</v>
-      </c>
-    </row>
-    <row r="723" spans="1:1">
-      <c r="A723" t="s">
-        <v>764</v>
-      </c>
-    </row>
-    <row r="724" spans="1:1">
-      <c r="A724" t="s">
-        <v>765</v>
-      </c>
-    </row>
-    <row r="725" spans="1:1">
-      <c r="A725" t="s">
-        <v>766</v>
-      </c>
-    </row>
-    <row r="726" spans="1:1">
-      <c r="A726" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="727" spans="1:1">
-      <c r="A727" t="s">
-        <v>768</v>
-      </c>
-    </row>
-    <row r="728" spans="1:1">
-      <c r="A728" t="s">
-        <v>769</v>
-      </c>
-    </row>
-    <row r="729" spans="1:1">
-      <c r="A729" t="s">
-        <v>770</v>
-      </c>
-    </row>
-    <row r="730" spans="1:1">
-      <c r="A730" t="s">
-        <v>771</v>
-      </c>
-    </row>
-    <row r="731" spans="1:1">
-      <c r="A731" t="s">
-        <v>772</v>
-      </c>
-    </row>
-    <row r="732" spans="1:1">
-      <c r="A732" t="s">
-        <v>773</v>
-      </c>
-    </row>
-    <row r="733" spans="1:1">
-      <c r="A733" t="s">
-        <v>774</v>
-      </c>
-    </row>
-    <row r="734" spans="1:1">
-      <c r="A734" t="s">
-        <v>775</v>
-      </c>
-    </row>
-    <row r="735" spans="1:1">
-      <c r="A735" t="s">
-        <v>776</v>
-      </c>
-    </row>
-    <row r="736" spans="1:1">
-      <c r="A736" t="s">
-        <v>777</v>
-      </c>
-    </row>
-    <row r="737" spans="1:1">
-      <c r="A737" t="s">
-        <v>778</v>
-      </c>
-    </row>
-    <row r="738" spans="1:1">
-      <c r="A738" t="s">
-        <v>779</v>
-      </c>
-    </row>
-    <row r="739" spans="1:1">
-      <c r="A739" t="s">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="740" spans="1:1">
-      <c r="A740" t="s">
-        <v>781</v>
-      </c>
-    </row>
-    <row r="741" spans="1:1">
-      <c r="A741" t="s">
-        <v>782</v>
-      </c>
-    </row>
-    <row r="742" spans="1:1">
-      <c r="A742" t="s">
-        <v>783</v>
-      </c>
-    </row>
-    <row r="743" spans="1:1">
-      <c r="A743" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="744" spans="1:1">
-      <c r="A744" t="s">
-        <v>785</v>
-      </c>
-    </row>
-    <row r="745" spans="1:1">
-      <c r="A745" t="s">
-        <v>786</v>
-      </c>
-    </row>
-    <row r="746" spans="1:1">
-      <c r="A746" t="s">
-        <v>787</v>
-      </c>
-    </row>
-    <row r="747" spans="1:1">
-      <c r="A747" t="s">
-        <v>788</v>
-      </c>
-    </row>
-    <row r="748" spans="1:1">
-      <c r="A748" t="s">
-        <v>789</v>
-      </c>
-    </row>
-    <row r="749" spans="1:1">
-      <c r="A749" t="s">
-        <v>790</v>
-      </c>
-    </row>
-    <row r="750" spans="1:1">
-      <c r="A750" t="s">
-        <v>791</v>
-      </c>
-    </row>
-    <row r="751" spans="1:1">
-      <c r="A751" t="s">
-        <v>792</v>
-      </c>
-    </row>
-    <row r="752" spans="1:1">
-      <c r="A752" t="s">
-        <v>793</v>
-      </c>
-    </row>
-    <row r="753" spans="1:1">
-      <c r="A753" t="s">
-        <v>794</v>
-      </c>
-    </row>
-    <row r="754" spans="1:1">
-      <c r="A754" t="s">
-        <v>795</v>
-      </c>
-    </row>
-    <row r="755" spans="1:1">
-      <c r="A755" t="s">
-        <v>796</v>
-      </c>
-    </row>
-    <row r="756" spans="1:1">
-      <c r="A756" t="s">
-        <v>797</v>
-      </c>
-    </row>
-    <row r="757" spans="1:1">
-      <c r="A757" t="s">
-        <v>798</v>
-      </c>
-    </row>
-    <row r="758" spans="1:1">
-      <c r="A758" t="s">
-        <v>799</v>
-      </c>
-    </row>
-    <row r="759" spans="1:1">
-      <c r="A759" t="s">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="760" spans="1:1">
-      <c r="A760" t="s">
-        <v>801</v>
-      </c>
-    </row>
-    <row r="761" spans="1:1">
-      <c r="A761" t="s">
-        <v>802</v>
-      </c>
-    </row>
-    <row r="762" spans="1:1">
-      <c r="A762" t="s">
-        <v>803</v>
-      </c>
-    </row>
-    <row r="763" spans="1:1">
-      <c r="A763" t="s">
-        <v>804</v>
-      </c>
-    </row>
-    <row r="764" spans="1:1">
-      <c r="A764" t="s">
-        <v>805</v>
-      </c>
-    </row>
-    <row r="765" spans="1:1">
-      <c r="A765" t="s">
-        <v>806</v>
-      </c>
-    </row>
-    <row r="766" spans="1:1">
-      <c r="A766" t="s">
-        <v>807</v>
-      </c>
-    </row>
-    <row r="767" spans="1:1">
-      <c r="A767" t="s">
-        <v>808</v>
-      </c>
-    </row>
-    <row r="768" spans="1:1">
-      <c r="A768" t="s">
-        <v>809</v>
-      </c>
-    </row>
-    <row r="769" spans="1:1">
-      <c r="A769" t="s">
-        <v>810</v>
-      </c>
-    </row>
-    <row r="770" spans="1:1">
-      <c r="A770" t="s">
-        <v>811</v>
-      </c>
-    </row>
-    <row r="771" spans="1:1">
-      <c r="A771" t="s">
-        <v>812</v>
-      </c>
-    </row>
-    <row r="772" spans="1:1">
-      <c r="A772" t="s">
-        <v>813</v>
-      </c>
-    </row>
-    <row r="773" spans="1:1">
-      <c r="A773" t="s">
-        <v>814</v>
-      </c>
-    </row>
-    <row r="774" spans="1:1">
-      <c r="A774" t="s">
-        <v>815</v>
-      </c>
-    </row>
-    <row r="775" spans="1:1">
-      <c r="A775" t="s">
-        <v>816</v>
-      </c>
-    </row>
-    <row r="776" spans="1:1">
-      <c r="A776" t="s">
-        <v>817</v>
-      </c>
-    </row>
-    <row r="777" spans="1:1">
-      <c r="A777" t="s">
-        <v>818</v>
-      </c>
-    </row>
-    <row r="778" spans="1:1">
-      <c r="A778" t="s">
-        <v>819</v>
-      </c>
-    </row>
-    <row r="779" spans="1:1">
-      <c r="A779" t="s">
-        <v>820</v>
-      </c>
-    </row>
-    <row r="780" spans="1:1">
-      <c r="A780" t="s">
-        <v>821</v>
-      </c>
-    </row>
-    <row r="781" spans="1:1">
-      <c r="A781" t="s">
-        <v>822</v>
-      </c>
-    </row>
-    <row r="782" spans="1:1">
-      <c r="A782" t="s">
-        <v>823</v>
-      </c>
-    </row>
-    <row r="783" spans="1:1">
-      <c r="A783" t="s">
-        <v>824</v>
-      </c>
-    </row>
-    <row r="784" spans="1:1">
-      <c r="A784" t="s">
-        <v>825</v>
-      </c>
-    </row>
-    <row r="785" spans="1:1">
-      <c r="A785" t="s">
-        <v>826</v>
-      </c>
-    </row>
-    <row r="786" spans="1:1">
-      <c r="A786" t="s">
-        <v>827</v>
-      </c>
-    </row>
-    <row r="787" spans="1:1">
-      <c r="A787" t="s">
-        <v>828</v>
-      </c>
-    </row>
-    <row r="788" spans="1:1">
-      <c r="A788" t="s">
-        <v>829</v>
-      </c>
-    </row>
-    <row r="789" spans="1:1">
-      <c r="A789" t="s">
-        <v>830</v>
-      </c>
-    </row>
-    <row r="790" spans="1:1">
-      <c r="A790" t="s">
-        <v>831</v>
-      </c>
-    </row>
-    <row r="791" spans="1:1">
-      <c r="A791" t="s">
-        <v>832</v>
-      </c>
-    </row>
-    <row r="792" spans="1:1">
-      <c r="A792" t="s">
-        <v>833</v>
-      </c>
-    </row>
-    <row r="793" spans="1:1">
-      <c r="A793" t="s">
-        <v>834</v>
-      </c>
-    </row>
-    <row r="794" spans="1:1">
-      <c r="A794" t="s">
-        <v>835</v>
-      </c>
-    </row>
-    <row r="795" spans="1:1">
-      <c r="A795" t="s">
-        <v>836</v>
-      </c>
-    </row>
-    <row r="796" spans="1:1">
-      <c r="A796" t="s">
-        <v>837</v>
-      </c>
-    </row>
-    <row r="797" spans="1:1">
-      <c r="A797" t="s">
-        <v>838</v>
-      </c>
-    </row>
-    <row r="798" spans="1:1">
-      <c r="A798" t="s">
-        <v>839</v>
-      </c>
-    </row>
-    <row r="799" spans="1:1">
-      <c r="A799" t="s">
-        <v>840</v>
-      </c>
-    </row>
-    <row r="800" spans="1:1">
-      <c r="A800" t="s">
-        <v>841</v>
-      </c>
-    </row>
-    <row r="801" spans="1:1">
-      <c r="A801" t="s">
-        <v>842</v>
-      </c>
-    </row>
-    <row r="802" spans="1:1">
-      <c r="A802" t="s">
-        <v>843</v>
-      </c>
-    </row>
-    <row r="803" spans="1:1">
-      <c r="A803" t="s">
-        <v>844</v>
-      </c>
-    </row>
-    <row r="804" spans="1:1">
-      <c r="A804" t="s">
-        <v>845</v>
-      </c>
-    </row>
-    <row r="805" spans="1:1">
-      <c r="A805" t="s">
-        <v>846</v>
-      </c>
-    </row>
-    <row r="806" spans="1:1">
-      <c r="A806" t="s">
-        <v>847</v>
-      </c>
-    </row>
-    <row r="807" spans="1:1">
-      <c r="A807" t="s">
-        <v>848</v>
-      </c>
-    </row>
-    <row r="808" spans="1:1">
-      <c r="A808" t="s">
-        <v>849</v>
-      </c>
-    </row>
-    <row r="809" spans="1:1">
-      <c r="A809" t="s">
-        <v>850</v>
-      </c>
-    </row>
-    <row r="810" spans="1:1">
-      <c r="A810" t="s">
-        <v>851</v>
-      </c>
-    </row>
-    <row r="811" spans="1:1">
-      <c r="A811" t="s">
-        <v>852</v>
-      </c>
-    </row>
-    <row r="812" spans="1:1">
-      <c r="A812" t="s">
-        <v>853</v>
-      </c>
-    </row>
-    <row r="813" spans="1:1">
-      <c r="A813" t="s">
-        <v>854</v>
-      </c>
-    </row>
-    <row r="814" spans="1:1">
-      <c r="A814" t="s">
-        <v>855</v>
-      </c>
-    </row>
-    <row r="815" spans="1:1">
-      <c r="A815" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="816" spans="1:1">
-      <c r="A816" t="s">
-        <v>857</v>
-      </c>
-    </row>
-    <row r="817" spans="1:1">
-      <c r="A817" t="s">
-        <v>858</v>
-      </c>
-    </row>
-    <row r="818" spans="1:1">
-      <c r="A818" t="s">
-        <v>859</v>
-      </c>
-    </row>
-    <row r="819" spans="1:1">
-      <c r="A819" t="s">
-        <v>860</v>
-      </c>
-    </row>
-    <row r="820" spans="1:1">
-      <c r="A820" t="s">
-        <v>861</v>
-      </c>
-    </row>
-    <row r="821" spans="1:1">
-      <c r="A821" t="s">
-        <v>862</v>
-      </c>
-    </row>
-    <row r="822" spans="1:1">
-      <c r="A822" t="s">
-        <v>863</v>
-      </c>
-    </row>
-    <row r="823" spans="1:1">
-      <c r="A823" t="s">
-        <v>864</v>
-      </c>
-    </row>
-    <row r="824" spans="1:1">
-      <c r="A824" t="s">
-        <v>865</v>
-      </c>
-    </row>
-    <row r="825" spans="1:1">
-      <c r="A825" t="s">
-        <v>866</v>
-      </c>
-    </row>
-    <row r="826" spans="1:1">
-      <c r="A826" t="s">
-        <v>867</v>
-      </c>
-    </row>
-    <row r="827" spans="1:1">
-      <c r="A827" t="s">
-        <v>868</v>
-      </c>
-    </row>
-    <row r="828" spans="1:1">
-      <c r="A828" t="s">
-        <v>869</v>
-      </c>
-    </row>
-    <row r="829" spans="1:1">
-      <c r="A829" t="s">
-        <v>870</v>
-      </c>
-    </row>
-    <row r="830" spans="1:1">
-      <c r="A830" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="831" spans="1:1">
-      <c r="A831" t="s">
-        <v>872</v>
-      </c>
-    </row>
-    <row r="832" spans="1:1">
-      <c r="A832" t="s">
-        <v>873</v>
-      </c>
-    </row>
-    <row r="833" spans="1:1">
-      <c r="A833" t="s">
-        <v>874</v>
-      </c>
-    </row>
-    <row r="834" spans="1:1">
-      <c r="A834" t="s">
-        <v>875</v>
-      </c>
-    </row>
-    <row r="835" spans="1:1">
-      <c r="A835" t="s">
-        <v>876</v>
-      </c>
-    </row>
-    <row r="836" spans="1:1">
-      <c r="A836" t="s">
-        <v>877</v>
-      </c>
-    </row>
-    <row r="838" spans="1:1">
-      <c r="A838" t="s">
-        <v>878</v>
-      </c>
-    </row>
-    <row r="839" spans="1:1">
-      <c r="A839" t="s">
-        <v>879</v>
-      </c>
-    </row>
-    <row r="840" spans="1:1">
-      <c r="A840" t="s">
-        <v>880</v>
-      </c>
-    </row>
-    <row r="841" spans="1:1">
-      <c r="A841" t="s">
-        <v>881</v>
-      </c>
-    </row>
-    <row r="842" spans="1:1">
-      <c r="A842" t="s">
-        <v>882</v>
-      </c>
-    </row>
-    <row r="843" spans="1:1">
-      <c r="A843" t="s">
-        <v>883</v>
-      </c>
-    </row>
-    <row r="844" spans="1:1">
-      <c r="A844" t="s">
-        <v>884</v>
-      </c>
-    </row>
-    <row r="845" spans="1:1">
-      <c r="A845" t="s">
-        <v>885</v>
-      </c>
-    </row>
-    <row r="846" spans="1:1">
-      <c r="A846" t="s">
-        <v>886</v>
-      </c>
-    </row>
-    <row r="847" spans="1:1">
-      <c r="A847" t="s">
-        <v>887</v>
-      </c>
-    </row>
-    <row r="848" spans="1:1">
-      <c r="A848" t="s">
-        <v>888</v>
-      </c>
-    </row>
-    <row r="849" spans="1:1">
-      <c r="A849" t="s">
-        <v>889</v>
-      </c>
-    </row>
-    <row r="850" spans="1:1">
-      <c r="A850" t="s">
-        <v>890</v>
-      </c>
-    </row>
-    <row r="851" spans="1:1">
-      <c r="A851" t="s">
-        <v>891</v>
-      </c>
-    </row>
-    <row r="852" spans="1:1">
-      <c r="A852" t="s">
-        <v>892</v>
-      </c>
-    </row>
-    <row r="853" spans="1:1">
-      <c r="A853" t="s">
-        <v>893</v>
-      </c>
-    </row>
-    <row r="854" spans="1:1">
-      <c r="A854" t="s">
-        <v>894</v>
-      </c>
-    </row>
-    <row r="856" spans="1:1">
-      <c r="A856" t="s">
-        <v>895</v>
-      </c>
-    </row>
-    <row r="857" spans="1:1">
-      <c r="A857" t="s">
-        <v>896</v>
-      </c>
-    </row>
-    <row r="858" spans="1:1">
-      <c r="A858" t="s">
-        <v>897</v>
-      </c>
-    </row>
-    <row r="859" spans="1:1">
-      <c r="A859" t="s">
-        <v>898</v>
-      </c>
-    </row>
-    <row r="860" spans="1:1">
-      <c r="A860" t="s">
-        <v>899</v>
-      </c>
-    </row>
-    <row r="861" spans="1:1">
-      <c r="A861" t="s">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="862" spans="1:1">
-      <c r="A862" t="s">
-        <v>901</v>
-      </c>
-    </row>
-    <row r="863" spans="1:1">
-      <c r="A863" t="s">
-        <v>902</v>
-      </c>
-    </row>
-    <row r="864" spans="1:1">
-      <c r="A864" t="s">
-        <v>903</v>
-      </c>
-    </row>
-    <row r="865" spans="1:1">
-      <c r="A865" t="s">
-        <v>904</v>
-      </c>
-    </row>
-    <row r="866" spans="1:1">
-      <c r="A866" t="s">
-        <v>905</v>
-      </c>
-    </row>
-    <row r="867" spans="1:1">
-      <c r="A867" t="s">
-        <v>906</v>
-      </c>
-    </row>
-    <row r="868" spans="1:1">
-      <c r="A868" t="s">
-        <v>907</v>
-      </c>
-    </row>
-    <row r="869" spans="1:1">
-      <c r="A869" t="s">
-        <v>908</v>
-      </c>
-    </row>
-    <row r="870" spans="1:1">
-      <c r="A870" t="s">
-        <v>909</v>
-      </c>
-    </row>
-    <row r="871" spans="1:1">
-      <c r="A871" t="s">
-        <v>910</v>
-      </c>
-    </row>
-    <row r="872" spans="1:1">
-      <c r="A872" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="873" spans="1:1">
-      <c r="A873" t="s">
-        <v>912</v>
-      </c>
-    </row>
-    <row r="874" spans="1:1">
-      <c r="A874" t="s">
-        <v>913</v>
-      </c>
-    </row>
-    <row r="875" spans="1:1">
-      <c r="A875" t="s">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="876" spans="1:1">
-      <c r="A876" t="s">
-        <v>915</v>
-      </c>
-    </row>
-    <row r="877" spans="1:1">
-      <c r="A877" t="s">
-        <v>916</v>
-      </c>
-    </row>
-    <row r="878" spans="1:1">
-      <c r="A878" t="s">
-        <v>917</v>
-      </c>
-    </row>
-    <row r="879" spans="1:1">
-      <c r="A879" t="s">
-        <v>918</v>
-      </c>
-    </row>
-    <row r="880" spans="1:1">
-      <c r="A880" t="s">
-        <v>919</v>
-      </c>
-    </row>
-    <row r="881" spans="1:1">
-      <c r="A881" t="s">
-        <v>920</v>
-      </c>
-    </row>
-    <row r="882" spans="1:1">
-      <c r="A882" t="s">
-        <v>921</v>
-      </c>
-    </row>
-    <row r="883" spans="1:1">
-      <c r="A883" t="s">
-        <v>922</v>
-      </c>
-    </row>
-    <row r="884" spans="1:1">
-      <c r="A884" t="s">
-        <v>923</v>
-      </c>
-    </row>
-    <row r="886" spans="1:1">
-      <c r="A886" t="s">
-        <v>924</v>
-      </c>
-    </row>
-    <row r="887" spans="1:1">
-      <c r="A887" t="s">
-        <v>925</v>
-      </c>
-    </row>
-    <row r="888" spans="1:1">
-      <c r="A888" t="s">
-        <v>926</v>
-      </c>
-    </row>
-    <row r="889" spans="1:1">
-      <c r="A889" t="s">
-        <v>927</v>
-      </c>
-    </row>
-    <row r="890" spans="1:1">
-      <c r="A890" t="s">
-        <v>928</v>
-      </c>
-    </row>
-    <row r="891" spans="1:1">
-      <c r="A891" t="s">
-        <v>929</v>
-      </c>
-    </row>
-    <row r="892" spans="1:1">
-      <c r="A892" t="s">
-        <v>930</v>
-      </c>
-    </row>
-    <row r="893" spans="1:1">
-      <c r="A893" t="s">
-        <v>931</v>
-      </c>
-    </row>
-    <row r="894" spans="1:1">
-      <c r="A894" t="s">
-        <v>932</v>
-      </c>
-    </row>
-    <row r="895" spans="1:1">
-      <c r="A895" t="s">
-        <v>933</v>
-      </c>
-    </row>
-    <row r="896" spans="1:1">
-      <c r="A896" t="s">
-        <v>934</v>
-      </c>
-    </row>
-    <row r="897" spans="1:1">
-      <c r="A897" t="s">
-        <v>935</v>
-      </c>
-    </row>
-    <row r="898" spans="1:1">
-      <c r="A898" t="s">
-        <v>936</v>
-      </c>
-    </row>
-    <row r="899" spans="1:1">
-      <c r="A899" t="s">
-        <v>937</v>
-      </c>
-    </row>
-    <row r="900" spans="1:1">
-      <c r="A900" t="s">
-        <v>938</v>
-      </c>
-    </row>
-    <row r="901" spans="1:1">
-      <c r="A901" t="s">
-        <v>939</v>
-      </c>
-    </row>
-    <row r="902" spans="1:1">
-      <c r="A902" t="s">
-        <v>940</v>
-      </c>
-    </row>
-    <row r="903" spans="1:1">
-      <c r="A903" t="s">
-        <v>941</v>
-      </c>
-    </row>
-    <row r="904" spans="1:1">
-      <c r="A904" t="s">
-        <v>942</v>
-      </c>
-    </row>
-    <row r="905" spans="1:1">
-      <c r="A905" t="s">
-        <v>943</v>
-      </c>
-    </row>
-    <row r="906" spans="1:1">
-      <c r="A906" t="s">
-        <v>944</v>
-      </c>
-    </row>
-    <row r="907" spans="1:1">
-      <c r="A907" t="s">
-        <v>945</v>
-      </c>
-    </row>
-    <row r="908" spans="1:1">
-      <c r="A908" t="s">
-        <v>946</v>
-      </c>
-    </row>
-    <row r="909" spans="1:1">
-      <c r="A909" t="s">
-        <v>947</v>
-      </c>
-    </row>
-    <row r="910" spans="1:1">
-      <c r="A910" t="s">
-        <v>948</v>
-      </c>
-    </row>
-    <row r="911" spans="1:1">
-      <c r="A911" t="s">
-        <v>949</v>
-      </c>
-    </row>
-    <row r="912" spans="1:1">
-      <c r="A912" t="s">
-        <v>950</v>
-      </c>
-    </row>
-    <row r="913" spans="1:1">
-      <c r="A913" t="s">
-        <v>951</v>
-      </c>
-    </row>
-    <row r="914" spans="1:1">
-      <c r="A914" t="s">
-        <v>952</v>
-      </c>
-    </row>
-    <row r="915" spans="1:1">
-      <c r="A915" t="s">
-        <v>953</v>
-      </c>
-    </row>
-    <row r="916" spans="1:1">
-      <c r="A916" t="s">
-        <v>954</v>
-      </c>
-    </row>
-    <row r="917" spans="1:1">
-      <c r="A917" t="s">
-        <v>955</v>
-      </c>
-    </row>
-    <row r="918" spans="1:1">
-      <c r="A918" t="s">
-        <v>956</v>
-      </c>
-    </row>
-    <row r="919" spans="1:1">
-      <c r="A919" t="s">
-        <v>957</v>
-      </c>
-    </row>
-    <row r="920" spans="1:1">
-      <c r="A920" t="s">
-        <v>958</v>
-      </c>
-    </row>
-    <row r="921" spans="1:1">
-      <c r="A921" t="s">
-        <v>959</v>
-      </c>
-    </row>
-    <row r="922" spans="1:1">
-      <c r="A922" t="s">
-        <v>960</v>
-      </c>
-    </row>
-    <row r="923" spans="1:1">
-      <c r="A923" t="s">
-        <v>961</v>
-      </c>
-    </row>
-    <row r="924" spans="1:1">
-      <c r="A924" t="s">
-        <v>962</v>
-      </c>
-    </row>
-    <row r="925" spans="1:1">
-      <c r="A925" t="s">
-        <v>963</v>
-      </c>
-    </row>
-    <row r="926" spans="1:1">
-      <c r="A926" t="s">
-        <v>964</v>
-      </c>
-    </row>
-    <row r="927" spans="1:1">
-      <c r="A927" t="s">
-        <v>965</v>
-      </c>
-    </row>
-    <row r="928" spans="1:1">
-      <c r="A928" t="s">
-        <v>966</v>
-      </c>
-    </row>
-    <row r="929" spans="1:1">
-      <c r="A929" t="s">
-        <v>967</v>
-      </c>
-    </row>
-    <row r="930" spans="1:1">
-      <c r="A930" t="s">
-        <v>968</v>
-      </c>
-    </row>
-    <row r="931" spans="1:1">
-      <c r="A931" t="s">
-        <v>969</v>
-      </c>
-    </row>
-    <row r="932" spans="1:1">
-      <c r="A932" t="s">
-        <v>970</v>
-      </c>
-    </row>
-    <row r="933" spans="1:1">
-      <c r="A933" t="s">
-        <v>971</v>
-      </c>
-    </row>
-    <row r="934" spans="1:1">
-      <c r="A934" t="s">
-        <v>972</v>
-      </c>
-    </row>
-    <row r="936" spans="1:1">
-      <c r="A936" t="s">
-        <v>973</v>
-      </c>
-    </row>
-    <row r="937" spans="1:1">
-      <c r="A937" t="s">
-        <v>974</v>
-      </c>
-    </row>
-    <row r="938" spans="1:1">
-      <c r="A938" t="s">
-        <v>975</v>
-      </c>
-    </row>
-    <row r="939" spans="1:1">
-      <c r="A939" t="s">
-        <v>976</v>
-      </c>
-    </row>
-    <row r="940" spans="1:1">
-      <c r="A940" t="s">
-        <v>977</v>
-      </c>
-    </row>
-    <row r="941" spans="1:1">
-      <c r="A941" t="s">
-        <v>978</v>
-      </c>
-    </row>
-    <row r="942" spans="1:1">
-      <c r="A942" t="s">
-        <v>979</v>
-      </c>
-    </row>
-    <row r="943" spans="1:1">
-      <c r="A943" t="s">
-        <v>980</v>
-      </c>
-    </row>
-    <row r="944" spans="1:1">
-      <c r="A944" t="s">
-        <v>981</v>
-      </c>
-    </row>
-    <row r="945" spans="1:1">
-      <c r="A945" t="s">
-        <v>982</v>
-      </c>
-    </row>
-    <row r="946" spans="1:1">
-      <c r="A946" t="s">
-        <v>983</v>
-      </c>
-    </row>
-    <row r="947" spans="1:1">
-      <c r="A947" t="s">
-        <v>984</v>
-      </c>
-    </row>
-    <row r="948" spans="1:1">
-      <c r="A948" t="s">
-        <v>985</v>
-      </c>
-    </row>
-    <row r="949" spans="1:1">
-      <c r="A949" t="s">
-        <v>986</v>
-      </c>
-    </row>
-    <row r="950" spans="1:1">
-      <c r="A950" t="s">
-        <v>987</v>
-      </c>
-    </row>
-    <row r="951" spans="1:1">
-      <c r="A951" t="s">
-        <v>988</v>
-      </c>
-    </row>
-    <row r="952" spans="1:1">
-      <c r="A952" t="s">
-        <v>989</v>
-      </c>
-    </row>
-    <row r="953" spans="1:1">
-      <c r="A953" t="s">
-        <v>990</v>
-      </c>
-    </row>
-    <row r="955" spans="1:1">
-      <c r="A955" t="s">
-        <v>991</v>
-      </c>
-    </row>
-    <row r="956" spans="1:1">
-      <c r="A956" t="s">
-        <v>992</v>
-      </c>
-    </row>
-    <row r="957" spans="1:1">
-      <c r="A957" t="s">
-        <v>993</v>
-      </c>
-    </row>
-    <row r="958" spans="1:1">
-      <c r="A958" t="s">
-        <v>994</v>
-      </c>
-    </row>
-    <row r="959" spans="1:1">
-      <c r="A959" t="s">
-        <v>995</v>
-      </c>
-    </row>
-    <row r="960" spans="1:1">
-      <c r="A960" t="s">
-        <v>996</v>
-      </c>
-    </row>
-    <row r="961" spans="1:1">
-      <c r="A961" t="s">
-        <v>997</v>
-      </c>
-    </row>
-    <row r="962" spans="1:1">
-      <c r="A962" t="s">
-        <v>998</v>
-      </c>
-    </row>
-    <row r="963" spans="1:1">
-      <c r="A963" t="s">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="964" spans="1:1">
-      <c r="A964" t="s">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="965" spans="1:1">
-      <c r="A965" t="s">
-        <v>1001</v>
-      </c>
-    </row>
-    <row r="966" spans="1:1">
-      <c r="A966" t="s">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="967" spans="1:1">
-      <c r="A967" t="s">
-        <v>1003</v>
-      </c>
-    </row>
-    <row r="968" spans="1:1">
-      <c r="A968" t="s">
-        <v>1004</v>
-      </c>
-    </row>
-    <row r="969" spans="1:1">
-      <c r="A969" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="970" spans="1:1">
-      <c r="A970" t="s">
-        <v>1006</v>
-      </c>
-    </row>
-    <row r="971" spans="1:1">
-      <c r="A971" t="s">
-        <v>1007</v>
-      </c>
-    </row>
-    <row r="972" spans="1:1">
-      <c r="A972" t="s">
-        <v>1008</v>
-      </c>
-    </row>
-    <row r="973" spans="1:1">
-      <c r="A973" t="s">
-        <v>1009</v>
-      </c>
-    </row>
-    <row r="974" spans="1:1">
-      <c r="A974" t="s">
-        <v>1010</v>
-      </c>
-    </row>
-    <row r="975" spans="1:1">
-      <c r="A975" t="s">
-        <v>1011</v>
-      </c>
-    </row>
-    <row r="976" spans="1:1">
-      <c r="A976" t="s">
-        <v>1012</v>
-      </c>
-    </row>
-    <row r="977" spans="1:1">
-      <c r="A977" t="s">
-        <v>1013</v>
-      </c>
-    </row>
-    <row r="978" spans="1:1">
-      <c r="A978" t="s">
-        <v>1014</v>
-      </c>
-    </row>
-    <row r="980" spans="1:1">
-      <c r="A980" t="s">
-        <v>1015</v>
-      </c>
-    </row>
-    <row r="981" spans="1:1">
-      <c r="A981" t="s">
-        <v>1016</v>
-      </c>
-    </row>
-    <row r="982" spans="1:1">
-      <c r="A982" t="s">
-        <v>1017</v>
-      </c>
-    </row>
-    <row r="983" spans="1:1">
-      <c r="A983" t="s">
-        <v>1018</v>
-      </c>
-    </row>
-    <row r="984" spans="1:1">
-      <c r="A984" t="s">
-        <v>1019</v>
-      </c>
-    </row>
-    <row r="985" spans="1:1">
-      <c r="A985" t="s">
-        <v>1020</v>
-      </c>
-    </row>
-    <row r="986" spans="1:1">
-      <c r="A986" t="s">
-        <v>1021</v>
-      </c>
-    </row>
-    <row r="987" spans="1:1">
-      <c r="A987" t="s">
-        <v>1022</v>
-      </c>
-    </row>
-    <row r="988" spans="1:1">
-      <c r="A988" t="s">
-        <v>1023</v>
-      </c>
-    </row>
-    <row r="989" spans="1:1">
-      <c r="A989" t="s">
-        <v>1024</v>
-      </c>
-    </row>
-    <row r="990" spans="1:1">
-      <c r="A990" t="s">
-        <v>1025</v>
-      </c>
-    </row>
-    <row r="991" spans="1:1">
-      <c r="A991" t="s">
-        <v>1026</v>
-      </c>
-    </row>
-    <row r="992" spans="1:1">
-      <c r="A992" t="s">
-        <v>1027</v>
-      </c>
-    </row>
-    <row r="993" spans="1:1">
-      <c r="A993" t="s">
-        <v>1028</v>
-      </c>
-    </row>
-    <row r="994" spans="1:1">
-      <c r="A994" t="s">
-        <v>1029</v>
-      </c>
-    </row>
-    <row r="996" spans="1:1">
-      <c r="A996" t="s">
-        <v>1030</v>
-      </c>
-    </row>
-    <row r="997" spans="1:1">
-      <c r="A997" t="s">
-        <v>1031</v>
-      </c>
-    </row>
-    <row r="998" spans="1:1">
-      <c r="A998" t="s">
-        <v>1032</v>
-      </c>
-    </row>
-    <row r="999" spans="1:1">
-      <c r="A999" t="s">
-        <v>1033</v>
-      </c>
-    </row>
-    <row r="1000" spans="1:1">
-      <c r="A1000" t="s">
-        <v>1034</v>
-      </c>
-    </row>
-    <row r="1001" spans="1:1">
-      <c r="A1001" t="s">
-        <v>1035</v>
-      </c>
-    </row>
-    <row r="1002" spans="1:1">
-      <c r="A1002" t="s">
-        <v>1036</v>
-      </c>
-    </row>
-    <row r="1003" spans="1:1">
-      <c r="A1003" t="s">
-        <v>1037</v>
-      </c>
-    </row>
-    <row r="1004" spans="1:1">
-      <c r="A1004" t="s">
-        <v>1038</v>
-      </c>
-    </row>
-    <row r="1005" spans="1:1">
-      <c r="A1005" t="s">
-        <v>1039</v>
-      </c>
-    </row>
-    <row r="1006" spans="1:1">
-      <c r="A1006" t="s">
-        <v>1040</v>
-      </c>
-    </row>
-    <row r="1007" spans="1:1">
-      <c r="A1007" t="s">
-        <v>1041</v>
-      </c>
-    </row>
-    <row r="1008" spans="1:1">
-      <c r="A1008" t="s">
-        <v>1042</v>
-      </c>
-    </row>
-    <row r="1009" spans="1:1">
-      <c r="A1009" t="s">
-        <v>1043</v>
-      </c>
-    </row>
-    <row r="1010" spans="1:1">
-      <c r="A1010" t="s">
-        <v>1044</v>
-      </c>
-    </row>
-    <row r="1011" spans="1:1">
-      <c r="A1011" t="s">
-        <v>1045</v>
-      </c>
-    </row>
-    <row r="1012" spans="1:1">
-      <c r="A1012" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="1013" spans="1:1">
-      <c r="A1013" t="s">
-        <v>1047</v>
-      </c>
-    </row>
-    <row r="1014" spans="1:1">
-      <c r="A1014" t="s">
-        <v>1048</v>
-      </c>
-    </row>
-    <row r="1015" spans="1:1">
-      <c r="A1015" t="s">
-        <v>1049</v>
-      </c>
-    </row>
-    <row r="1016" spans="1:1">
-      <c r="A1016" t="s">
-        <v>1050</v>
-      </c>
-    </row>
-    <row r="1017" spans="1:1">
-      <c r="A1017" t="s">
-        <v>1051</v>
-      </c>
-    </row>
-    <row r="1018" spans="1:1">
-      <c r="A1018" t="s">
-        <v>1052</v>
-      </c>
-    </row>
-    <row r="1019" spans="1:1">
-      <c r="A1019" t="s">
-        <v>1053</v>
-      </c>
-    </row>
-    <row r="1020" spans="1:1">
-      <c r="A1020" t="s">
-        <v>1054</v>
-      </c>
-    </row>
-    <row r="1021" spans="1:1">
-      <c r="A1021" t="s">
-        <v>1055</v>
-      </c>
-    </row>
-    <row r="1022" spans="1:1">
-      <c r="A1022" t="s">
-        <v>1056</v>
-      </c>
-    </row>
-    <row r="1023" spans="1:1">
-      <c r="A1023" t="s">
-        <v>1057</v>
-      </c>
-    </row>
-    <row r="1024" spans="1:1">
-      <c r="A1024" t="s">
-        <v>1058</v>
-      </c>
-    </row>
-    <row r="1025" spans="1:1">
-      <c r="A1025" t="s">
-        <v>1059</v>
-      </c>
-    </row>
-    <row r="1026" spans="1:1">
-      <c r="A1026" t="s">
-        <v>1060</v>
-      </c>
-    </row>
-    <row r="1027" spans="1:1">
-      <c r="A1027" t="s">
-        <v>1061</v>
-      </c>
-    </row>
-    <row r="1028" spans="1:1">
-      <c r="A1028" t="s">
-        <v>1062</v>
-      </c>
-    </row>
-    <row r="1029" spans="1:1">
-      <c r="A1029" t="s">
-        <v>1063</v>
-      </c>
-    </row>
-    <row r="1030" spans="1:1">
-      <c r="A1030" t="s">
-        <v>1064</v>
-      </c>
-    </row>
-    <row r="1031" spans="1:1">
-      <c r="A1031" t="s">
-        <v>1065</v>
-      </c>
-    </row>
-    <row r="1032" spans="1:1">
-      <c r="A1032" t="s">
-        <v>1066</v>
-      </c>
-    </row>
-    <row r="1033" spans="1:1">
-      <c r="A1033" t="s">
-        <v>1067</v>
-      </c>
-    </row>
-    <row r="1034" spans="1:1">
-      <c r="A1034" t="s">
-        <v>1068</v>
-      </c>
-    </row>
-    <row r="1035" spans="1:1">
-      <c r="A1035" t="s">
-        <v>1069</v>
-      </c>
-    </row>
-    <row r="1036" spans="1:1">
-      <c r="A1036" t="s">
-        <v>1070</v>
-      </c>
-    </row>
-    <row r="1037" spans="1:1">
-      <c r="A1037" t="s">
-        <v>1071</v>
-      </c>
-    </row>
-    <row r="1038" spans="1:1">
-      <c r="A1038" t="s">
-        <v>1072</v>
-      </c>
-    </row>
-    <row r="1039" spans="1:1">
-      <c r="A1039" t="s">
-        <v>1073</v>
-      </c>
-    </row>
-    <row r="1040" spans="1:1">
-      <c r="A1040" t="s">
-        <v>1074</v>
-      </c>
-    </row>
-    <row r="1041" spans="1:1">
-      <c r="A1041" t="s">
-        <v>1075</v>
-      </c>
-    </row>
-    <row r="1042" spans="1:1">
-      <c r="A1042" t="s">
-        <v>1076</v>
-      </c>
-    </row>
-    <row r="1043" spans="1:1">
-      <c r="A1043" t="s">
-        <v>1077</v>
-      </c>
-    </row>
-    <row r="1044" spans="1:1">
-      <c r="A1044" t="s">
-        <v>1078</v>
-      </c>
-    </row>
-    <row r="1045" spans="1:1">
-      <c r="A1045" t="s">
-        <v>1079</v>
-      </c>
-    </row>
-    <row r="1046" spans="1:1">
-      <c r="A1046" t="s">
-        <v>1080</v>
-      </c>
-    </row>
-    <row r="1047" spans="1:1">
-      <c r="A1047" t="s">
-        <v>1081</v>
-      </c>
-    </row>
-    <row r="1048" spans="1:1">
-      <c r="A1048" t="s">
-        <v>1082</v>
-      </c>
-    </row>
-    <row r="1049" spans="1:1">
-      <c r="A1049" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="1050" spans="1:1">
-      <c r="A1050" t="s">
-        <v>1084</v>
-      </c>
-    </row>
-    <row r="1051" spans="1:1">
-      <c r="A1051" t="s">
-        <v>1085</v>
-      </c>
-    </row>
-    <row r="1052" spans="1:1">
-      <c r="A1052" t="s">
-        <v>1086</v>
-      </c>
-    </row>
-    <row r="1053" spans="1:1">
-      <c r="A1053" t="s">
-        <v>1087</v>
-      </c>
-    </row>
-    <row r="1054" spans="1:1">
-      <c r="A1054" t="s">
-        <v>1088</v>
-      </c>
-    </row>
-    <row r="1055" spans="1:1">
-      <c r="A1055" t="s">
-        <v>1089</v>
-      </c>
-    </row>
-    <row r="1056" spans="1:1">
-      <c r="A1056" t="s">
-        <v>1090</v>
-      </c>
-    </row>
-    <row r="1057" spans="1:1">
-      <c r="A1057" t="s">
-        <v>1091</v>
-      </c>
-    </row>
-    <row r="1058" spans="1:1">
-      <c r="A1058" t="s">
-        <v>1092</v>
-      </c>
-    </row>
-    <row r="1059" spans="1:1">
-      <c r="A1059" t="s">
-        <v>1093</v>
-      </c>
-    </row>
-    <row r="1060" spans="1:1">
-      <c r="A1060" t="s">
-        <v>1094</v>
-      </c>
-    </row>
-    <row r="1061" spans="1:1">
-      <c r="A1061" t="s">
-        <v>1095</v>
-      </c>
-    </row>
-    <row r="1062" spans="1:1">
-      <c r="A1062" t="s">
-        <v>1096</v>
-      </c>
-    </row>
-    <row r="1063" spans="1:1">
-      <c r="A1063" t="s">
-        <v>1097</v>
-      </c>
-    </row>
-    <row r="1064" spans="1:1">
-      <c r="A1064" t="s">
-        <v>1098</v>
-      </c>
-    </row>
-    <row r="1065" spans="1:1">
-      <c r="A1065" t="s">
-        <v>1099</v>
-      </c>
-    </row>
-    <row r="1066" spans="1:1">
-      <c r="A1066" t="s">
-        <v>1100</v>
-      </c>
-    </row>
-    <row r="1068" spans="1:1">
-      <c r="A1068" t="s">
-        <v>1101</v>
-      </c>
-    </row>
-    <row r="1069" spans="1:1">
-      <c r="A1069" t="s">
-        <v>1102</v>
-      </c>
-    </row>
-    <row r="1070" spans="1:1">
-      <c r="A1070" t="s">
-        <v>1103</v>
-      </c>
-    </row>
-    <row r="1071" spans="1:1">
-      <c r="A1071" t="s">
-        <v>1104</v>
-      </c>
-    </row>
-    <row r="1072" spans="1:1">
-      <c r="A1072" t="s">
-        <v>1105</v>
-      </c>
-    </row>
-    <row r="1073" spans="1:1">
-      <c r="A1073" t="s">
-        <v>1106</v>
-      </c>
-    </row>
-    <row r="1074" spans="1:1">
-      <c r="A1074" t="s">
-        <v>1107</v>
-      </c>
-    </row>
-    <row r="1075" spans="1:1">
-      <c r="A1075" t="s">
-        <v>1108</v>
-      </c>
-    </row>
-    <row r="1076" spans="1:1">
-      <c r="A1076" t="s">
-        <v>1109</v>
-      </c>
-    </row>
-    <row r="1077" spans="1:1">
-      <c r="A1077" t="s">
-        <v>1110</v>
-      </c>
-    </row>
-    <row r="1079" spans="1:1">
-      <c r="A1079" t="s">
-        <v>1111</v>
-      </c>
-    </row>
-    <row r="1080" spans="1:1">
-      <c r="A1080" t="s">
-        <v>1112</v>
-      </c>
-    </row>
-    <row r="1081" spans="1:1">
-      <c r="A1081" t="s">
-        <v>1113</v>
-      </c>
-    </row>
-    <row r="1082" spans="1:1">
-      <c r="A1082" t="s">
-        <v>1114</v>
+        <v>706</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add config export bundle variables added
</commit_message>
<xml_diff>
--- a/templates/panos/set_commands/iron_skillet_panos_full.xlsx
+++ b/templates/panos/set_commands/iron_skillet_panos_full.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="707">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="712">
   <si>
     <t>Variable Name</t>
   </si>
@@ -78,6 +78,21 @@
   </si>
   <si>
     <t>IP address for scheduled config exports</t>
+  </si>
+  <si>
+    <t>CONFIG_EXPORT_USER</t>
+  </si>
+  <si>
+    <t>testuser</t>
+  </si>
+  <si>
+    <t>username for config export</t>
+  </si>
+  <si>
+    <t>CONFIG_EXPORT_PASSWORD</t>
+  </si>
+  <si>
+    <t>password for config export</t>
   </si>
   <si>
     <t>TEMPLATE</t>
@@ -2476,7 +2491,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2579,40 +2594,40 @@
         <v>24</v>
       </c>
       <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
         <v>25</v>
-      </c>
-      <c r="C9" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
         <v>27</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>28</v>
-      </c>
-      <c r="C10" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
         <v>30</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>31</v>
-      </c>
-      <c r="C11" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
         <v>33</v>
-      </c>
-      <c r="B12" t="s">
-        <v>7</v>
       </c>
       <c r="C12" t="s">
         <v>34</v>
@@ -2634,62 +2649,62 @@
         <v>38</v>
       </c>
       <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" t="s">
         <v>39</v>
-      </c>
-      <c r="C14" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" t="s">
         <v>41</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>42</v>
-      </c>
-      <c r="C15" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" t="s">
         <v>44</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>45</v>
-      </c>
-      <c r="C16" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" t="s">
         <v>47</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>48</v>
-      </c>
-      <c r="C17" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" t="s">
         <v>50</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>51</v>
-      </c>
-      <c r="C18" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" t="s">
         <v>53</v>
-      </c>
-      <c r="B19" t="s">
-        <v>51</v>
       </c>
       <c r="C19" t="s">
         <v>54</v>
@@ -2711,95 +2726,95 @@
         <v>58</v>
       </c>
       <c r="B21" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" t="s">
         <v>59</v>
-      </c>
-      <c r="C21" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" t="s">
         <v>61</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>62</v>
-      </c>
-      <c r="C22" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" t="s">
         <v>64</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>65</v>
-      </c>
-      <c r="C23" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" t="s">
         <v>67</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>68</v>
-      </c>
-      <c r="C24" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" t="s">
         <v>70</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>71</v>
-      </c>
-      <c r="C25" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
+        <v>72</v>
+      </c>
+      <c r="B26" t="s">
         <v>73</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>74</v>
-      </c>
-      <c r="C26" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
+        <v>75</v>
+      </c>
+      <c r="B27" t="s">
         <v>76</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>77</v>
-      </c>
-      <c r="C27" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" t="s">
         <v>79</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>80</v>
-      </c>
-      <c r="C28" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
+        <v>81</v>
+      </c>
+      <c r="B29" t="s">
         <v>82</v>
-      </c>
-      <c r="B29">
-        <v>525600</v>
       </c>
       <c r="C29" t="s">
         <v>83</v>
@@ -2814,6 +2829,28 @@
       </c>
       <c r="C30" t="s">
         <v>86</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>87</v>
+      </c>
+      <c r="B31">
+        <v>525600</v>
+      </c>
+      <c r="C31" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>89</v>
+      </c>
+      <c r="B32" t="s">
+        <v>90</v>
+      </c>
+      <c r="C32" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -2831,3269 +2868,3269 @@
   <sheetData>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8">
-        <f>SUBSTITUTE("set deviceconfig system hostname {{ FW_NAME }}", "{{ FW_NAME }}", 'values'!B11)</f>
+        <f>SUBSTITUTE("set deviceconfig system hostname {{ FW_NAME }}", "{{ FW_NAME }}", 'values'!B13)</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9">
-        <f>SUBSTITUTE("set deviceconfig system ip-address {{ MGMT_IP }}", "{{ MGMT_IP }}", 'values'!B13)</f>
+        <f>SUBSTITUTE("set deviceconfig system ip-address {{ MGMT_IP }}", "{{ MGMT_IP }}", 'values'!B15)</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10">
-        <f>SUBSTITUTE("set deviceconfig system netmask {{ MGMT_MASK }}", "{{ MGMT_MASK }}", 'values'!B14)</f>
+        <f>SUBSTITUTE("set deviceconfig system netmask {{ MGMT_MASK }}", "{{ MGMT_MASK }}", 'values'!B16)</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11">
-        <f>SUBSTITUTE("set deviceconfig system default-gateway {{ MGMT_DG }}", "{{ MGMT_DG }}", 'values'!B15)</f>
+        <f>SUBSTITUTE("set deviceconfig system default-gateway {{ MGMT_DG }}", "{{ MGMT_DG }}", 'values'!B17)</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12">
-        <f>SUBSTITUTE("set deviceconfig system dns-setting servers primary {{ DNS_1 }}", "{{ DNS_1 }}", 'values'!B20)</f>
+        <f>SUBSTITUTE("set deviceconfig system dns-setting servers primary {{ DNS_1 }}", "{{ DNS_1 }}", 'values'!B22)</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13">
-        <f>SUBSTITUTE("set deviceconfig system dns-setting servers secondary {{ DNS_2 }}", "{{ DNS_2 }}", 'values'!B21)</f>
+        <f>SUBSTITUTE("set deviceconfig system dns-setting servers secondary {{ DNS_2 }}", "{{ DNS_2 }}", 'values'!B23)</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14">
-        <f>SUBSTITUTE("set deviceconfig system ntp-servers primary-ntp-server ntp-server-address {{ NTP_1 }}", "{{ NTP_1 }}", 'values'!B16)</f>
+        <f>SUBSTITUTE("set deviceconfig system ntp-servers primary-ntp-server ntp-server-address {{ NTP_1 }}", "{{ NTP_1 }}", 'values'!B18)</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15">
-        <f>SUBSTITUTE("set deviceconfig system ntp-servers secondary-ntp-server ntp-server-address {{ NTP_2 }}", "{{ NTP_2 }}", 'values'!B17)</f>
+        <f>SUBSTITUTE("set deviceconfig system ntp-servers secondary-ntp-server ntp-server-address {{ NTP_2 }}", "{{ NTP_2 }}", 'values'!B19)</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18">
-        <f>SUBSTITUTE("set mgt-config users {{ ADMINISTRATOR_USERNAME }} password", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B18)</f>
+        <f>SUBSTITUTE("set mgt-config users {{ ADMINISTRATOR_USERNAME }} password", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B20)</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19">
-        <f>SUBSTITUTE("set mgt-config users {{ ADMINISTRATOR_USERNAME }} permissions role-based superuser yes", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B18)</f>
+        <f>SUBSTITUTE("set mgt-config users {{ ADMINISTRATOR_USERNAME }} permissions role-based superuser yes", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B20)</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68">
-        <f>SUBSTITUTE("set deviceconfig setting management api key lifetime {{ API_KEY_LIFETIME }}", "{{ API_KEY_LIFETIME }}", 'values'!B29)</f>
+        <f>SUBSTITUTE("set deviceconfig setting management api key lifetime {{ API_KEY_LIFETIME }}", "{{ API_KEY_LIFETIME }}", 'values'!B31)</f>
         <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
     </row>
     <row r="85" spans="1:1">
       <c r="A85" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
     </row>
     <row r="87" spans="1:1">
       <c r="A87" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
     </row>
     <row r="89" spans="1:1">
       <c r="A89" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
     </row>
     <row r="90" spans="1:1">
       <c r="A90" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
     </row>
     <row r="91" spans="1:1">
       <c r="A91" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
     </row>
     <row r="92" spans="1:1">
       <c r="A92" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
     </row>
     <row r="94" spans="1:1">
       <c r="A94" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
     </row>
     <row r="97" spans="1:1">
       <c r="A97" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
     </row>
     <row r="98" spans="1:1">
       <c r="A98" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99">
-        <f>SUBSTITUTE("set shared log-settings email Sample_Email_Profile server Sample_Email_Profile gateway {{ EMAIL_PROFILE_GATEWAY }}", "{{ EMAIL_PROFILE_GATEWAY }}", 'values'!B25)</f>
+        <f>SUBSTITUTE("set shared log-settings email Sample_Email_Profile server Sample_Email_Profile gateway {{ EMAIL_PROFILE_GATEWAY }}", "{{ EMAIL_PROFILE_GATEWAY }}", 'values'!B27)</f>
         <v>0</v>
       </c>
     </row>
     <row r="100" spans="1:1">
       <c r="A100">
-        <f>SUBSTITUTE("set shared log-settings email Sample_Email_Profile server Sample_Email_Profile from {{ EMAIL_PROFILE_FROM }}", "{{ EMAIL_PROFILE_FROM }}", 'values'!B26)</f>
+        <f>SUBSTITUTE("set shared log-settings email Sample_Email_Profile server Sample_Email_Profile from {{ EMAIL_PROFILE_FROM }}", "{{ EMAIL_PROFILE_FROM }}", 'values'!B28)</f>
         <v>0</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101">
-        <f>SUBSTITUTE("set shared log-settings email Sample_Email_Profile server Sample_Email_Profile to {{ EMAIL_PROFILE_TO }}", "{{ EMAIL_PROFILE_TO }}", 'values'!B27)</f>
+        <f>SUBSTITUTE("set shared log-settings email Sample_Email_Profile server Sample_Email_Profile to {{ EMAIL_PROFILE_TO }}", "{{ EMAIL_PROFILE_TO }}", 'values'!B29)</f>
         <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:1">
       <c r="A102" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
     </row>
     <row r="104" spans="1:1">
       <c r="A104" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
     </row>
     <row r="105" spans="1:1">
       <c r="A105">
-        <f>SUBSTITUTE("set shared log-settings syslog Sample_Syslog_Profile server Sample_Syslog server {{ SYSLOG_SERVER }}", "{{ SYSLOG_SERVER }}", 'values'!B28)</f>
+        <f>SUBSTITUTE("set shared log-settings syslog Sample_Syslog_Profile server Sample_Syslog server {{ SYSLOG_SERVER }}", "{{ SYSLOG_SERVER }}", 'values'!B30)</f>
         <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:1">
       <c r="A106" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
     </row>
     <row r="108" spans="1:1">
       <c r="A108" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
     </row>
     <row r="109" spans="1:1">
       <c r="A109" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
     </row>
     <row r="110" spans="1:1">
       <c r="A110" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
     </row>
     <row r="111" spans="1:1">
       <c r="A111" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
     </row>
     <row r="112" spans="1:1">
       <c r="A112" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
     </row>
     <row r="113" spans="1:1">
       <c r="A113" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
     </row>
     <row r="114" spans="1:1">
       <c r="A114" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
     </row>
     <row r="115" spans="1:1">
       <c r="A115" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
     </row>
     <row r="116" spans="1:1">
       <c r="A116" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
     </row>
     <row r="117" spans="1:1">
       <c r="A117" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
     </row>
     <row r="118" spans="1:1">
       <c r="A118" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
     </row>
     <row r="119" spans="1:1">
       <c r="A119" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
     </row>
     <row r="120" spans="1:1">
       <c r="A120" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
     </row>
     <row r="121" spans="1:1">
       <c r="A121" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
     </row>
     <row r="122" spans="1:1">
       <c r="A122" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
     </row>
     <row r="123" spans="1:1">
       <c r="A123" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
     </row>
     <row r="125" spans="1:1">
       <c r="A125" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
     </row>
     <row r="126" spans="1:1">
       <c r="A126" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
     </row>
     <row r="127" spans="1:1">
       <c r="A127" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
     </row>
     <row r="128" spans="1:1">
       <c r="A128" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
     </row>
     <row r="129" spans="1:1">
       <c r="A129" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
     </row>
     <row r="130" spans="1:1">
       <c r="A130" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
     </row>
     <row r="131" spans="1:1">
       <c r="A131" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
     </row>
     <row r="132" spans="1:1">
       <c r="A132" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
     </row>
     <row r="133" spans="1:1">
       <c r="A133" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
     </row>
     <row r="134" spans="1:1">
       <c r="A134" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
     </row>
     <row r="135" spans="1:1">
       <c r="A135" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
     </row>
     <row r="136" spans="1:1">
       <c r="A136" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
     </row>
     <row r="137" spans="1:1">
       <c r="A137" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
     </row>
     <row r="138" spans="1:1">
       <c r="A138" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="139" spans="1:1">
       <c r="A139" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
     </row>
     <row r="140" spans="1:1">
       <c r="A140" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
     </row>
     <row r="141" spans="1:1">
       <c r="A141" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
     </row>
     <row r="142" spans="1:1">
       <c r="A142" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
     </row>
     <row r="143" spans="1:1">
       <c r="A143" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
     </row>
     <row r="144" spans="1:1">
       <c r="A144" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
     </row>
     <row r="145" spans="1:1">
       <c r="A145" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
     </row>
     <row r="146" spans="1:1">
       <c r="A146" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
     </row>
     <row r="147" spans="1:1">
       <c r="A147" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
     </row>
     <row r="148" spans="1:1">
       <c r="A148" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
     </row>
     <row r="149" spans="1:1">
       <c r="A149" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
     </row>
     <row r="150" spans="1:1">
       <c r="A150" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
     </row>
     <row r="151" spans="1:1">
       <c r="A151" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
     </row>
     <row r="152" spans="1:1">
       <c r="A152" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
     </row>
     <row r="153" spans="1:1">
       <c r="A153" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
     </row>
     <row r="154" spans="1:1">
       <c r="A154" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
     </row>
     <row r="155" spans="1:1">
       <c r="A155" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
     </row>
     <row r="156" spans="1:1">
       <c r="A156" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
     </row>
     <row r="157" spans="1:1">
       <c r="A157" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
     </row>
     <row r="158" spans="1:1">
       <c r="A158" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
     </row>
     <row r="159" spans="1:1">
       <c r="A159" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
     </row>
     <row r="160" spans="1:1">
       <c r="A160" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
     </row>
     <row r="161" spans="1:1">
       <c r="A161" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
     </row>
     <row r="162" spans="1:1">
       <c r="A162" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
     </row>
     <row r="163" spans="1:1">
       <c r="A163" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
     </row>
     <row r="165" spans="1:1">
       <c r="A165" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
     </row>
     <row r="166" spans="1:1">
       <c r="A166" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
     </row>
     <row r="167" spans="1:1">
       <c r="A167" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
     </row>
     <row r="168" spans="1:1">
       <c r="A168" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
     </row>
     <row r="169" spans="1:1">
       <c r="A169" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
     </row>
     <row r="171" spans="1:1">
       <c r="A171" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
     </row>
     <row r="172" spans="1:1">
       <c r="A172">
-        <f>SUBSTITUTE("set address Sinkhole-IPv4 ip-netmask {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
+        <f>SUBSTITUTE("set address Sinkhole-IPv4 ip-netmask {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B24)</f>
         <v>0</v>
       </c>
     </row>
     <row r="173" spans="1:1">
       <c r="A173">
-        <f>SUBSTITUTE("set address Sinkhole-IPv6 ip-netmask {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
+        <f>SUBSTITUTE("set address Sinkhole-IPv6 ip-netmask {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B25)</f>
         <v>0</v>
       </c>
     </row>
     <row r="175" spans="1:1">
       <c r="A175" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
     </row>
     <row r="176" spans="1:1">
       <c r="A176" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
     </row>
     <row r="177" spans="1:1">
       <c r="A177" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
     </row>
     <row r="178" spans="1:1">
       <c r="A178" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
     </row>
     <row r="179" spans="1:1">
       <c r="A179" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
     </row>
     <row r="180" spans="1:1">
       <c r="A180" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
     </row>
     <row r="181" spans="1:1">
       <c r="A181" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
     </row>
     <row r="182" spans="1:1">
       <c r="A182" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
     </row>
     <row r="183" spans="1:1">
       <c r="A183" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
     </row>
     <row r="184" spans="1:1">
       <c r="A184" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
     </row>
     <row r="185" spans="1:1">
       <c r="A185" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
     </row>
     <row r="186" spans="1:1">
       <c r="A186" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
     </row>
     <row r="187" spans="1:1">
       <c r="A187" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
     </row>
     <row r="188" spans="1:1">
       <c r="A188" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
     </row>
     <row r="189" spans="1:1">
       <c r="A189" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
     </row>
     <row r="190" spans="1:1">
       <c r="A190" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
     </row>
     <row r="191" spans="1:1">
       <c r="A191" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
     </row>
     <row r="192" spans="1:1">
       <c r="A192" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
     </row>
     <row r="193" spans="1:1">
       <c r="A193" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
     </row>
     <row r="194" spans="1:1">
       <c r="A194" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
     </row>
     <row r="195" spans="1:1">
       <c r="A195" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
     </row>
     <row r="196" spans="1:1">
       <c r="A196" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
     </row>
     <row r="197" spans="1:1">
       <c r="A197" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
     </row>
     <row r="198" spans="1:1">
       <c r="A198" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
     </row>
     <row r="199" spans="1:1">
       <c r="A199" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
     </row>
     <row r="200" spans="1:1">
       <c r="A200" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
     </row>
     <row r="201" spans="1:1">
       <c r="A201" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
     </row>
     <row r="202" spans="1:1">
       <c r="A202" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
     </row>
     <row r="203" spans="1:1">
       <c r="A203" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
     </row>
     <row r="205" spans="1:1">
       <c r="A205" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
     </row>
     <row r="206" spans="1:1">
       <c r="A206">
-        <f>SUBSTITUTE("set profiles spyware Outbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
+        <f>SUBSTITUTE("set profiles spyware Outbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B24)</f>
         <v>0</v>
       </c>
     </row>
     <row r="207" spans="1:1">
       <c r="A207">
-        <f>SUBSTITUTE("set profiles spyware Outbound-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
+        <f>SUBSTITUTE("set profiles spyware Outbound-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B25)</f>
         <v>0</v>
       </c>
     </row>
     <row r="208" spans="1:1">
       <c r="A208" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
     </row>
     <row r="209" spans="1:1">
       <c r="A209" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
     </row>
     <row r="210" spans="1:1">
       <c r="A210" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
     </row>
     <row r="211" spans="1:1">
       <c r="A211" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
     </row>
     <row r="212" spans="1:1">
       <c r="A212" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
     </row>
     <row r="213" spans="1:1">
       <c r="A213" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
     </row>
     <row r="214" spans="1:1">
       <c r="A214" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
     </row>
     <row r="215" spans="1:1">
       <c r="A215" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
     </row>
     <row r="216" spans="1:1">
       <c r="A216" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
     </row>
     <row r="217" spans="1:1">
       <c r="A217" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
     </row>
     <row r="218" spans="1:1">
       <c r="A218" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
     </row>
     <row r="219" spans="1:1">
       <c r="A219" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
     </row>
     <row r="220" spans="1:1">
       <c r="A220" t="s">
-        <v>273</v>
+        <v>278</v>
       </c>
     </row>
     <row r="221" spans="1:1">
       <c r="A221" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
     </row>
     <row r="222" spans="1:1">
       <c r="A222">
-        <f>SUBSTITUTE("set profiles spyware Inbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
+        <f>SUBSTITUTE("set profiles spyware Inbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B24)</f>
         <v>0</v>
       </c>
     </row>
     <row r="223" spans="1:1">
       <c r="A223">
-        <f>SUBSTITUTE("set profiles spyware Inbound-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
+        <f>SUBSTITUTE("set profiles spyware Inbound-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B25)</f>
         <v>0</v>
       </c>
     </row>
     <row r="224" spans="1:1">
       <c r="A224" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
     </row>
     <row r="225" spans="1:1">
       <c r="A225" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
     </row>
     <row r="226" spans="1:1">
       <c r="A226" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
     </row>
     <row r="227" spans="1:1">
       <c r="A227" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
     </row>
     <row r="228" spans="1:1">
       <c r="A228" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
     </row>
     <row r="229" spans="1:1">
       <c r="A229" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="230" spans="1:1">
       <c r="A230" t="s">
-        <v>281</v>
+        <v>286</v>
       </c>
     </row>
     <row r="231" spans="1:1">
       <c r="A231" t="s">
-        <v>282</v>
+        <v>287</v>
       </c>
     </row>
     <row r="232" spans="1:1">
       <c r="A232" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
     </row>
     <row r="233" spans="1:1">
       <c r="A233" t="s">
-        <v>284</v>
+        <v>289</v>
       </c>
     </row>
     <row r="234" spans="1:1">
       <c r="A234" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
     </row>
     <row r="235" spans="1:1">
       <c r="A235" t="s">
-        <v>286</v>
+        <v>291</v>
       </c>
     </row>
     <row r="236" spans="1:1">
       <c r="A236" t="s">
-        <v>287</v>
+        <v>292</v>
       </c>
     </row>
     <row r="237" spans="1:1">
       <c r="A237" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
     </row>
     <row r="238" spans="1:1">
       <c r="A238">
-        <f>SUBSTITUTE("set profiles spyware Internal-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
+        <f>SUBSTITUTE("set profiles spyware Internal-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B24)</f>
         <v>0</v>
       </c>
     </row>
     <row r="239" spans="1:1">
       <c r="A239">
-        <f>SUBSTITUTE("set profiles spyware Internal-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
+        <f>SUBSTITUTE("set profiles spyware Internal-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B25)</f>
         <v>0</v>
       </c>
     </row>
     <row r="240" spans="1:1">
       <c r="A240" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
     </row>
     <row r="241" spans="1:1">
       <c r="A241" t="s">
-        <v>290</v>
+        <v>295</v>
       </c>
     </row>
     <row r="242" spans="1:1">
       <c r="A242" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
     </row>
     <row r="243" spans="1:1">
       <c r="A243" t="s">
-        <v>292</v>
+        <v>297</v>
       </c>
     </row>
     <row r="244" spans="1:1">
       <c r="A244" t="s">
-        <v>293</v>
+        <v>298</v>
       </c>
     </row>
     <row r="245" spans="1:1">
       <c r="A245" t="s">
-        <v>294</v>
+        <v>299</v>
       </c>
     </row>
     <row r="246" spans="1:1">
       <c r="A246" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
     </row>
     <row r="247" spans="1:1">
       <c r="A247" t="s">
-        <v>296</v>
+        <v>301</v>
       </c>
     </row>
     <row r="248" spans="1:1">
       <c r="A248" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
     </row>
     <row r="249" spans="1:1">
       <c r="A249" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
     </row>
     <row r="250" spans="1:1">
       <c r="A250" t="s">
-        <v>299</v>
+        <v>304</v>
       </c>
     </row>
     <row r="251" spans="1:1">
       <c r="A251" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
     </row>
     <row r="252" spans="1:1">
       <c r="A252" t="s">
-        <v>301</v>
+        <v>306</v>
       </c>
     </row>
     <row r="253" spans="1:1">
       <c r="A253" t="s">
-        <v>302</v>
+        <v>307</v>
       </c>
     </row>
     <row r="254" spans="1:1">
       <c r="A254" t="s">
-        <v>303</v>
+        <v>308</v>
       </c>
     </row>
     <row r="255" spans="1:1">
       <c r="A255">
-        <f>SUBSTITUTE("set profiles spyware Alert-Only-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
+        <f>SUBSTITUTE("set profiles spyware Alert-Only-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B24)</f>
         <v>0</v>
       </c>
     </row>
     <row r="256" spans="1:1">
       <c r="A256">
-        <f>SUBSTITUTE("set profiles spyware Alert-Only-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
+        <f>SUBSTITUTE("set profiles spyware Alert-Only-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B25)</f>
         <v>0</v>
       </c>
     </row>
     <row r="257" spans="1:1">
       <c r="A257" t="s">
-        <v>304</v>
+        <v>309</v>
       </c>
     </row>
     <row r="258" spans="1:1">
       <c r="A258" t="s">
-        <v>303</v>
+        <v>308</v>
       </c>
     </row>
     <row r="259" spans="1:1">
       <c r="A259" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
     </row>
     <row r="260" spans="1:1">
       <c r="A260" t="s">
-        <v>306</v>
+        <v>311</v>
       </c>
     </row>
     <row r="261" spans="1:1">
       <c r="A261" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
     </row>
     <row r="262" spans="1:1">
       <c r="A262" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
     </row>
     <row r="263" spans="1:1">
       <c r="A263" t="s">
-        <v>309</v>
+        <v>314</v>
       </c>
     </row>
     <row r="264" spans="1:1">
       <c r="A264" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
     </row>
     <row r="265" spans="1:1">
       <c r="A265" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
     </row>
     <row r="266" spans="1:1">
       <c r="A266">
-        <f>SUBSTITUTE("set profiles spyware Exception-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
+        <f>SUBSTITUTE("set profiles spyware Exception-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B24)</f>
         <v>0</v>
       </c>
     </row>
     <row r="267" spans="1:1">
       <c r="A267">
-        <f>SUBSTITUTE("set profiles spyware Exception-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
+        <f>SUBSTITUTE("set profiles spyware Exception-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B25)</f>
         <v>0</v>
       </c>
     </row>
     <row r="268" spans="1:1">
       <c r="A268" t="s">
-        <v>312</v>
+        <v>317</v>
       </c>
     </row>
     <row r="269" spans="1:1">
       <c r="A269" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
     </row>
     <row r="270" spans="1:1">
       <c r="A270" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
     </row>
     <row r="271" spans="1:1">
       <c r="A271" t="s">
-        <v>315</v>
+        <v>320</v>
       </c>
     </row>
     <row r="273" spans="1:1">
       <c r="A273" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
     </row>
     <row r="274" spans="1:1">
       <c r="A274" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
     </row>
     <row r="275" spans="1:1">
       <c r="A275" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
     </row>
     <row r="276" spans="1:1">
       <c r="A276" t="s">
-        <v>319</v>
+        <v>324</v>
       </c>
     </row>
     <row r="277" spans="1:1">
       <c r="A277" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
     </row>
     <row r="278" spans="1:1">
       <c r="A278" t="s">
-        <v>321</v>
+        <v>326</v>
       </c>
     </row>
     <row r="279" spans="1:1">
       <c r="A279" t="s">
-        <v>322</v>
+        <v>327</v>
       </c>
     </row>
     <row r="280" spans="1:1">
       <c r="A280" t="s">
-        <v>323</v>
+        <v>328</v>
       </c>
     </row>
     <row r="281" spans="1:1">
       <c r="A281" t="s">
-        <v>324</v>
+        <v>329</v>
       </c>
     </row>
     <row r="282" spans="1:1">
       <c r="A282" t="s">
-        <v>325</v>
+        <v>330</v>
       </c>
     </row>
     <row r="283" spans="1:1">
       <c r="A283" t="s">
-        <v>326</v>
+        <v>331</v>
       </c>
     </row>
     <row r="284" spans="1:1">
       <c r="A284" t="s">
-        <v>327</v>
+        <v>332</v>
       </c>
     </row>
     <row r="285" spans="1:1">
       <c r="A285" t="s">
-        <v>328</v>
+        <v>333</v>
       </c>
     </row>
     <row r="286" spans="1:1">
       <c r="A286" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
     </row>
     <row r="287" spans="1:1">
       <c r="A287" t="s">
-        <v>330</v>
+        <v>335</v>
       </c>
     </row>
     <row r="288" spans="1:1">
       <c r="A288" t="s">
-        <v>331</v>
+        <v>336</v>
       </c>
     </row>
     <row r="289" spans="1:1">
       <c r="A289" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
     </row>
     <row r="290" spans="1:1">
       <c r="A290" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
     </row>
     <row r="291" spans="1:1">
       <c r="A291" t="s">
-        <v>334</v>
+        <v>339</v>
       </c>
     </row>
     <row r="292" spans="1:1">
       <c r="A292" t="s">
-        <v>335</v>
+        <v>340</v>
       </c>
     </row>
     <row r="293" spans="1:1">
       <c r="A293" t="s">
-        <v>336</v>
+        <v>341</v>
       </c>
     </row>
     <row r="294" spans="1:1">
       <c r="A294" t="s">
-        <v>337</v>
+        <v>342</v>
       </c>
     </row>
     <row r="295" spans="1:1">
       <c r="A295" t="s">
-        <v>338</v>
+        <v>343</v>
       </c>
     </row>
     <row r="296" spans="1:1">
       <c r="A296" t="s">
-        <v>339</v>
+        <v>344</v>
       </c>
     </row>
     <row r="298" spans="1:1">
       <c r="A298" t="s">
-        <v>340</v>
+        <v>345</v>
       </c>
     </row>
     <row r="299" spans="1:1">
       <c r="A299" t="s">
-        <v>341</v>
+        <v>346</v>
       </c>
     </row>
     <row r="300" spans="1:1">
       <c r="A300" t="s">
-        <v>342</v>
+        <v>347</v>
       </c>
     </row>
     <row r="301" spans="1:1">
       <c r="A301" t="s">
-        <v>343</v>
+        <v>348</v>
       </c>
     </row>
     <row r="302" spans="1:1">
       <c r="A302" t="s">
-        <v>344</v>
+        <v>349</v>
       </c>
     </row>
     <row r="303" spans="1:1">
       <c r="A303" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
     </row>
     <row r="304" spans="1:1">
       <c r="A304" t="s">
-        <v>346</v>
+        <v>351</v>
       </c>
     </row>
     <row r="305" spans="1:1">
       <c r="A305" t="s">
-        <v>347</v>
+        <v>352</v>
       </c>
     </row>
     <row r="306" spans="1:1">
       <c r="A306" t="s">
-        <v>348</v>
+        <v>353</v>
       </c>
     </row>
     <row r="307" spans="1:1">
       <c r="A307" t="s">
-        <v>349</v>
+        <v>354</v>
       </c>
     </row>
     <row r="308" spans="1:1">
       <c r="A308" t="s">
-        <v>350</v>
+        <v>355</v>
       </c>
     </row>
     <row r="309" spans="1:1">
       <c r="A309" t="s">
-        <v>351</v>
+        <v>356</v>
       </c>
     </row>
     <row r="310" spans="1:1">
       <c r="A310" t="s">
-        <v>352</v>
+        <v>357</v>
       </c>
     </row>
     <row r="311" spans="1:1">
       <c r="A311" t="s">
-        <v>353</v>
+        <v>358</v>
       </c>
     </row>
     <row r="312" spans="1:1">
       <c r="A312" t="s">
-        <v>354</v>
+        <v>359</v>
       </c>
     </row>
     <row r="313" spans="1:1">
       <c r="A313" t="s">
-        <v>355</v>
+        <v>360</v>
       </c>
     </row>
     <row r="314" spans="1:1">
       <c r="A314" t="s">
-        <v>356</v>
+        <v>361</v>
       </c>
     </row>
     <row r="315" spans="1:1">
       <c r="A315" t="s">
-        <v>357</v>
+        <v>362</v>
       </c>
     </row>
     <row r="316" spans="1:1">
       <c r="A316" t="s">
-        <v>358</v>
+        <v>363</v>
       </c>
     </row>
     <row r="317" spans="1:1">
       <c r="A317" t="s">
-        <v>359</v>
+        <v>364</v>
       </c>
     </row>
     <row r="318" spans="1:1">
       <c r="A318" t="s">
-        <v>360</v>
+        <v>365</v>
       </c>
     </row>
     <row r="319" spans="1:1">
       <c r="A319" t="s">
-        <v>361</v>
+        <v>366</v>
       </c>
     </row>
     <row r="320" spans="1:1">
       <c r="A320" t="s">
-        <v>362</v>
+        <v>367</v>
       </c>
     </row>
     <row r="321" spans="1:1">
       <c r="A321" t="s">
-        <v>363</v>
+        <v>368</v>
       </c>
     </row>
     <row r="322" spans="1:1">
       <c r="A322" t="s">
-        <v>364</v>
+        <v>369</v>
       </c>
     </row>
     <row r="323" spans="1:1">
       <c r="A323" t="s">
-        <v>365</v>
+        <v>370</v>
       </c>
     </row>
     <row r="324" spans="1:1">
       <c r="A324" t="s">
-        <v>366</v>
+        <v>371</v>
       </c>
     </row>
     <row r="325" spans="1:1">
       <c r="A325" t="s">
-        <v>367</v>
+        <v>372</v>
       </c>
     </row>
     <row r="326" spans="1:1">
       <c r="A326" t="s">
-        <v>368</v>
+        <v>373</v>
       </c>
     </row>
     <row r="327" spans="1:1">
       <c r="A327" t="s">
-        <v>369</v>
+        <v>374</v>
       </c>
     </row>
     <row r="328" spans="1:1">
       <c r="A328" t="s">
-        <v>370</v>
+        <v>375</v>
       </c>
     </row>
     <row r="329" spans="1:1">
       <c r="A329" t="s">
-        <v>371</v>
+        <v>376</v>
       </c>
     </row>
     <row r="330" spans="1:1">
       <c r="A330" t="s">
-        <v>372</v>
+        <v>377</v>
       </c>
     </row>
     <row r="331" spans="1:1">
       <c r="A331" t="s">
-        <v>373</v>
+        <v>378</v>
       </c>
     </row>
     <row r="332" spans="1:1">
       <c r="A332" t="s">
-        <v>374</v>
+        <v>379</v>
       </c>
     </row>
     <row r="333" spans="1:1">
       <c r="A333" t="s">
-        <v>375</v>
+        <v>380</v>
       </c>
     </row>
     <row r="334" spans="1:1">
       <c r="A334" t="s">
-        <v>376</v>
+        <v>381</v>
       </c>
     </row>
     <row r="335" spans="1:1">
       <c r="A335" t="s">
-        <v>377</v>
+        <v>382</v>
       </c>
     </row>
     <row r="336" spans="1:1">
       <c r="A336" t="s">
-        <v>378</v>
+        <v>383</v>
       </c>
     </row>
     <row r="337" spans="1:1">
       <c r="A337" t="s">
-        <v>379</v>
+        <v>384</v>
       </c>
     </row>
     <row r="338" spans="1:1">
       <c r="A338" t="s">
-        <v>380</v>
+        <v>385</v>
       </c>
     </row>
     <row r="339" spans="1:1">
       <c r="A339" t="s">
-        <v>381</v>
+        <v>386</v>
       </c>
     </row>
     <row r="340" spans="1:1">
       <c r="A340" t="s">
-        <v>382</v>
+        <v>387</v>
       </c>
     </row>
     <row r="341" spans="1:1">
       <c r="A341" t="s">
-        <v>383</v>
+        <v>388</v>
       </c>
     </row>
     <row r="342" spans="1:1">
       <c r="A342" t="s">
-        <v>384</v>
+        <v>389</v>
       </c>
     </row>
     <row r="343" spans="1:1">
       <c r="A343" t="s">
-        <v>385</v>
+        <v>390</v>
       </c>
     </row>
     <row r="344" spans="1:1">
       <c r="A344" t="s">
-        <v>386</v>
+        <v>391</v>
       </c>
     </row>
     <row r="345" spans="1:1">
       <c r="A345" t="s">
-        <v>387</v>
+        <v>392</v>
       </c>
     </row>
     <row r="346" spans="1:1">
       <c r="A346" t="s">
-        <v>388</v>
+        <v>393</v>
       </c>
     </row>
     <row r="347" spans="1:1">
       <c r="A347" t="s">
-        <v>389</v>
+        <v>394</v>
       </c>
     </row>
     <row r="348" spans="1:1">
       <c r="A348" t="s">
-        <v>390</v>
+        <v>395</v>
       </c>
     </row>
     <row r="349" spans="1:1">
       <c r="A349" t="s">
-        <v>391</v>
+        <v>396</v>
       </c>
     </row>
     <row r="350" spans="1:1">
       <c r="A350" t="s">
-        <v>392</v>
+        <v>397</v>
       </c>
     </row>
     <row r="351" spans="1:1">
       <c r="A351" t="s">
-        <v>393</v>
+        <v>398</v>
       </c>
     </row>
     <row r="352" spans="1:1">
       <c r="A352" t="s">
-        <v>394</v>
+        <v>399</v>
       </c>
     </row>
     <row r="353" spans="1:1">
       <c r="A353" t="s">
-        <v>395</v>
+        <v>400</v>
       </c>
     </row>
     <row r="354" spans="1:1">
       <c r="A354" t="s">
-        <v>396</v>
+        <v>401</v>
       </c>
     </row>
     <row r="355" spans="1:1">
       <c r="A355" t="s">
-        <v>397</v>
+        <v>402</v>
       </c>
     </row>
     <row r="356" spans="1:1">
       <c r="A356" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
     </row>
     <row r="357" spans="1:1">
       <c r="A357" t="s">
-        <v>399</v>
+        <v>404</v>
       </c>
     </row>
     <row r="358" spans="1:1">
       <c r="A358" t="s">
-        <v>400</v>
+        <v>405</v>
       </c>
     </row>
     <row r="359" spans="1:1">
       <c r="A359" t="s">
-        <v>401</v>
+        <v>406</v>
       </c>
     </row>
     <row r="360" spans="1:1">
       <c r="A360" t="s">
-        <v>402</v>
+        <v>407</v>
       </c>
     </row>
     <row r="361" spans="1:1">
       <c r="A361" t="s">
-        <v>403</v>
+        <v>408</v>
       </c>
     </row>
     <row r="362" spans="1:1">
       <c r="A362" t="s">
-        <v>404</v>
+        <v>409</v>
       </c>
     </row>
     <row r="363" spans="1:1">
       <c r="A363" t="s">
-        <v>405</v>
+        <v>410</v>
       </c>
     </row>
     <row r="364" spans="1:1">
       <c r="A364" t="s">
-        <v>406</v>
+        <v>411</v>
       </c>
     </row>
     <row r="365" spans="1:1">
       <c r="A365" t="s">
-        <v>407</v>
+        <v>412</v>
       </c>
     </row>
     <row r="366" spans="1:1">
       <c r="A366" t="s">
-        <v>408</v>
+        <v>413</v>
       </c>
     </row>
     <row r="367" spans="1:1">
       <c r="A367" t="s">
-        <v>409</v>
+        <v>414</v>
       </c>
     </row>
     <row r="368" spans="1:1">
       <c r="A368" t="s">
-        <v>410</v>
+        <v>415</v>
       </c>
     </row>
     <row r="369" spans="1:1">
       <c r="A369" t="s">
-        <v>411</v>
+        <v>416</v>
       </c>
     </row>
     <row r="371" spans="1:1">
       <c r="A371" t="s">
-        <v>412</v>
+        <v>417</v>
       </c>
     </row>
     <row r="372" spans="1:1">
       <c r="A372" t="s">
-        <v>413</v>
+        <v>418</v>
       </c>
     </row>
     <row r="373" spans="1:1">
       <c r="A373" t="s">
-        <v>414</v>
+        <v>419</v>
       </c>
     </row>
     <row r="374" spans="1:1">
       <c r="A374" t="s">
-        <v>415</v>
+        <v>420</v>
       </c>
     </row>
     <row r="375" spans="1:1">
       <c r="A375" t="s">
-        <v>416</v>
+        <v>421</v>
       </c>
     </row>
     <row r="376" spans="1:1">
       <c r="A376" t="s">
-        <v>417</v>
+        <v>422</v>
       </c>
     </row>
     <row r="377" spans="1:1">
       <c r="A377" t="s">
-        <v>418</v>
+        <v>423</v>
       </c>
     </row>
     <row r="378" spans="1:1">
       <c r="A378" t="s">
-        <v>419</v>
+        <v>424</v>
       </c>
     </row>
     <row r="379" spans="1:1">
       <c r="A379" t="s">
-        <v>420</v>
+        <v>425</v>
       </c>
     </row>
     <row r="380" spans="1:1">
       <c r="A380" t="s">
-        <v>421</v>
+        <v>426</v>
       </c>
     </row>
     <row r="381" spans="1:1">
       <c r="A381" t="s">
-        <v>422</v>
+        <v>427</v>
       </c>
     </row>
     <row r="382" spans="1:1">
       <c r="A382" t="s">
-        <v>423</v>
+        <v>428</v>
       </c>
     </row>
     <row r="383" spans="1:1">
       <c r="A383" t="s">
-        <v>424</v>
+        <v>429</v>
       </c>
     </row>
     <row r="384" spans="1:1">
       <c r="A384" t="s">
-        <v>425</v>
+        <v>430</v>
       </c>
     </row>
     <row r="385" spans="1:1">
       <c r="A385" t="s">
-        <v>426</v>
+        <v>431</v>
       </c>
     </row>
     <row r="386" spans="1:1">
       <c r="A386" t="s">
-        <v>427</v>
+        <v>432</v>
       </c>
     </row>
     <row r="387" spans="1:1">
       <c r="A387" t="s">
-        <v>428</v>
+        <v>433</v>
       </c>
     </row>
     <row r="388" spans="1:1">
       <c r="A388" t="s">
-        <v>429</v>
+        <v>434</v>
       </c>
     </row>
     <row r="389" spans="1:1">
       <c r="A389" t="s">
-        <v>430</v>
+        <v>435</v>
       </c>
     </row>
     <row r="390" spans="1:1">
       <c r="A390" t="s">
-        <v>431</v>
+        <v>436</v>
       </c>
     </row>
     <row r="391" spans="1:1">
       <c r="A391" t="s">
-        <v>432</v>
+        <v>437</v>
       </c>
     </row>
     <row r="392" spans="1:1">
       <c r="A392" t="s">
-        <v>433</v>
+        <v>438</v>
       </c>
     </row>
     <row r="393" spans="1:1">
       <c r="A393" t="s">
-        <v>434</v>
+        <v>439</v>
       </c>
     </row>
     <row r="394" spans="1:1">
       <c r="A394" t="s">
-        <v>435</v>
+        <v>440</v>
       </c>
     </row>
     <row r="395" spans="1:1">
       <c r="A395" t="s">
-        <v>436</v>
+        <v>441</v>
       </c>
     </row>
     <row r="396" spans="1:1">
       <c r="A396" t="s">
-        <v>437</v>
+        <v>442</v>
       </c>
     </row>
     <row r="397" spans="1:1">
       <c r="A397" t="s">
-        <v>438</v>
+        <v>443</v>
       </c>
     </row>
     <row r="398" spans="1:1">
       <c r="A398" t="s">
-        <v>439</v>
+        <v>444</v>
       </c>
     </row>
     <row r="399" spans="1:1">
       <c r="A399" t="s">
-        <v>440</v>
+        <v>445</v>
       </c>
     </row>
     <row r="400" spans="1:1">
       <c r="A400" t="s">
-        <v>441</v>
+        <v>446</v>
       </c>
     </row>
     <row r="401" spans="1:1">
       <c r="A401" t="s">
-        <v>442</v>
+        <v>447</v>
       </c>
     </row>
     <row r="402" spans="1:1">
       <c r="A402" t="s">
-        <v>443</v>
+        <v>448</v>
       </c>
     </row>
     <row r="403" spans="1:1">
       <c r="A403" t="s">
-        <v>444</v>
+        <v>449</v>
       </c>
     </row>
     <row r="404" spans="1:1">
       <c r="A404" t="s">
-        <v>445</v>
+        <v>450</v>
       </c>
     </row>
     <row r="405" spans="1:1">
       <c r="A405" t="s">
-        <v>446</v>
+        <v>451</v>
       </c>
     </row>
     <row r="406" spans="1:1">
       <c r="A406" t="s">
-        <v>447</v>
+        <v>452</v>
       </c>
     </row>
     <row r="407" spans="1:1">
       <c r="A407" t="s">
-        <v>448</v>
+        <v>453</v>
       </c>
     </row>
     <row r="408" spans="1:1">
       <c r="A408" t="s">
-        <v>449</v>
+        <v>454</v>
       </c>
     </row>
     <row r="409" spans="1:1">
       <c r="A409" t="s">
-        <v>450</v>
+        <v>455</v>
       </c>
     </row>
     <row r="410" spans="1:1">
       <c r="A410" t="s">
-        <v>451</v>
+        <v>456</v>
       </c>
     </row>
     <row r="411" spans="1:1">
       <c r="A411" t="s">
-        <v>452</v>
+        <v>457</v>
       </c>
     </row>
     <row r="412" spans="1:1">
       <c r="A412" t="s">
-        <v>453</v>
+        <v>458</v>
       </c>
     </row>
     <row r="413" spans="1:1">
       <c r="A413" t="s">
-        <v>454</v>
+        <v>459</v>
       </c>
     </row>
     <row r="414" spans="1:1">
       <c r="A414" t="s">
-        <v>455</v>
+        <v>460</v>
       </c>
     </row>
     <row r="415" spans="1:1">
       <c r="A415" t="s">
-        <v>456</v>
+        <v>461</v>
       </c>
     </row>
     <row r="416" spans="1:1">
       <c r="A416" t="s">
-        <v>457</v>
+        <v>462</v>
       </c>
     </row>
     <row r="417" spans="1:1">
       <c r="A417" t="s">
-        <v>458</v>
+        <v>463</v>
       </c>
     </row>
     <row r="418" spans="1:1">
       <c r="A418" t="s">
-        <v>459</v>
+        <v>464</v>
       </c>
     </row>
     <row r="419" spans="1:1">
       <c r="A419" t="s">
-        <v>460</v>
+        <v>465</v>
       </c>
     </row>
     <row r="420" spans="1:1">
       <c r="A420" t="s">
-        <v>461</v>
+        <v>466</v>
       </c>
     </row>
     <row r="421" spans="1:1">
       <c r="A421" t="s">
-        <v>462</v>
+        <v>467</v>
       </c>
     </row>
     <row r="422" spans="1:1">
       <c r="A422" t="s">
-        <v>463</v>
+        <v>468</v>
       </c>
     </row>
     <row r="423" spans="1:1">
       <c r="A423" t="s">
-        <v>464</v>
+        <v>469</v>
       </c>
     </row>
     <row r="424" spans="1:1">
       <c r="A424" t="s">
-        <v>465</v>
+        <v>470</v>
       </c>
     </row>
     <row r="425" spans="1:1">
       <c r="A425" t="s">
-        <v>466</v>
+        <v>471</v>
       </c>
     </row>
     <row r="426" spans="1:1">
       <c r="A426" t="s">
-        <v>467</v>
+        <v>472</v>
       </c>
     </row>
     <row r="427" spans="1:1">
       <c r="A427" t="s">
-        <v>468</v>
+        <v>473</v>
       </c>
     </row>
     <row r="428" spans="1:1">
       <c r="A428" t="s">
-        <v>469</v>
+        <v>474</v>
       </c>
     </row>
     <row r="430" spans="1:1">
       <c r="A430" t="s">
-        <v>470</v>
+        <v>475</v>
       </c>
     </row>
     <row r="431" spans="1:1">
       <c r="A431" t="s">
-        <v>471</v>
+        <v>476</v>
       </c>
     </row>
     <row r="432" spans="1:1">
       <c r="A432" t="s">
-        <v>472</v>
+        <v>477</v>
       </c>
     </row>
     <row r="433" spans="1:1">
       <c r="A433" t="s">
-        <v>473</v>
+        <v>478</v>
       </c>
     </row>
     <row r="434" spans="1:1">
       <c r="A434" t="s">
-        <v>474</v>
+        <v>479</v>
       </c>
     </row>
     <row r="435" spans="1:1">
       <c r="A435" t="s">
-        <v>475</v>
+        <v>480</v>
       </c>
     </row>
     <row r="436" spans="1:1">
       <c r="A436" t="s">
-        <v>476</v>
+        <v>481</v>
       </c>
     </row>
     <row r="437" spans="1:1">
       <c r="A437" t="s">
-        <v>477</v>
+        <v>482</v>
       </c>
     </row>
     <row r="438" spans="1:1">
       <c r="A438" t="s">
-        <v>478</v>
+        <v>483</v>
       </c>
     </row>
     <row r="439" spans="1:1">
       <c r="A439" t="s">
-        <v>479</v>
+        <v>484</v>
       </c>
     </row>
     <row r="440" spans="1:1">
       <c r="A440" t="s">
-        <v>480</v>
+        <v>485</v>
       </c>
     </row>
     <row r="441" spans="1:1">
       <c r="A441" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
     </row>
     <row r="442" spans="1:1">
       <c r="A442" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
     </row>
     <row r="443" spans="1:1">
       <c r="A443" t="s">
-        <v>483</v>
+        <v>488</v>
       </c>
     </row>
     <row r="444" spans="1:1">
       <c r="A444" t="s">
-        <v>484</v>
+        <v>489</v>
       </c>
     </row>
     <row r="445" spans="1:1">
       <c r="A445" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
     </row>
     <row r="446" spans="1:1">
       <c r="A446" t="s">
-        <v>486</v>
+        <v>491</v>
       </c>
     </row>
     <row r="448" spans="1:1">
       <c r="A448" t="s">
-        <v>487</v>
+        <v>492</v>
       </c>
     </row>
     <row r="449" spans="1:1">
       <c r="A449" t="s">
-        <v>488</v>
+        <v>493</v>
       </c>
     </row>
     <row r="450" spans="1:1">
       <c r="A450" t="s">
-        <v>489</v>
+        <v>494</v>
       </c>
     </row>
     <row r="451" spans="1:1">
       <c r="A451" t="s">
-        <v>490</v>
+        <v>495</v>
       </c>
     </row>
     <row r="452" spans="1:1">
       <c r="A452" t="s">
-        <v>491</v>
+        <v>496</v>
       </c>
     </row>
     <row r="453" spans="1:1">
       <c r="A453" t="s">
-        <v>492</v>
+        <v>497</v>
       </c>
     </row>
     <row r="454" spans="1:1">
       <c r="A454" t="s">
-        <v>493</v>
+        <v>498</v>
       </c>
     </row>
     <row r="455" spans="1:1">
       <c r="A455" t="s">
-        <v>494</v>
+        <v>499</v>
       </c>
     </row>
     <row r="456" spans="1:1">
       <c r="A456" t="s">
-        <v>495</v>
+        <v>500</v>
       </c>
     </row>
     <row r="457" spans="1:1">
       <c r="A457" t="s">
-        <v>496</v>
+        <v>501</v>
       </c>
     </row>
     <row r="458" spans="1:1">
       <c r="A458" t="s">
-        <v>497</v>
+        <v>502</v>
       </c>
     </row>
     <row r="459" spans="1:1">
       <c r="A459" t="s">
-        <v>498</v>
+        <v>503</v>
       </c>
     </row>
     <row r="460" spans="1:1">
       <c r="A460" t="s">
-        <v>499</v>
+        <v>504</v>
       </c>
     </row>
     <row r="461" spans="1:1">
       <c r="A461" t="s">
-        <v>500</v>
+        <v>505</v>
       </c>
     </row>
     <row r="462" spans="1:1">
       <c r="A462" t="s">
-        <v>501</v>
+        <v>506</v>
       </c>
     </row>
     <row r="463" spans="1:1">
       <c r="A463" t="s">
-        <v>502</v>
+        <v>507</v>
       </c>
     </row>
     <row r="464" spans="1:1">
       <c r="A464" t="s">
-        <v>503</v>
+        <v>508</v>
       </c>
     </row>
     <row r="465" spans="1:1">
       <c r="A465" t="s">
-        <v>504</v>
+        <v>509</v>
       </c>
     </row>
     <row r="466" spans="1:1">
       <c r="A466" t="s">
-        <v>505</v>
+        <v>510</v>
       </c>
     </row>
     <row r="467" spans="1:1">
       <c r="A467" t="s">
-        <v>506</v>
+        <v>511</v>
       </c>
     </row>
     <row r="468" spans="1:1">
       <c r="A468" t="s">
-        <v>507</v>
+        <v>512</v>
       </c>
     </row>
     <row r="469" spans="1:1">
       <c r="A469" t="s">
-        <v>508</v>
+        <v>513</v>
       </c>
     </row>
     <row r="470" spans="1:1">
       <c r="A470" t="s">
-        <v>509</v>
+        <v>514</v>
       </c>
     </row>
     <row r="471" spans="1:1">
       <c r="A471" t="s">
-        <v>510</v>
+        <v>515</v>
       </c>
     </row>
     <row r="472" spans="1:1">
       <c r="A472" t="s">
-        <v>511</v>
+        <v>516</v>
       </c>
     </row>
     <row r="473" spans="1:1">
       <c r="A473" t="s">
-        <v>512</v>
+        <v>517</v>
       </c>
     </row>
     <row r="474" spans="1:1">
       <c r="A474" t="s">
-        <v>513</v>
+        <v>518</v>
       </c>
     </row>
     <row r="475" spans="1:1">
       <c r="A475" t="s">
-        <v>514</v>
+        <v>519</v>
       </c>
     </row>
     <row r="476" spans="1:1">
       <c r="A476" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
     </row>
     <row r="478" spans="1:1">
       <c r="A478" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
     </row>
     <row r="479" spans="1:1">
       <c r="A479" t="s">
-        <v>517</v>
+        <v>522</v>
       </c>
     </row>
     <row r="480" spans="1:1">
       <c r="A480" t="s">
-        <v>518</v>
+        <v>523</v>
       </c>
     </row>
     <row r="481" spans="1:1">
       <c r="A481" t="s">
-        <v>519</v>
+        <v>524</v>
       </c>
     </row>
     <row r="482" spans="1:1">
       <c r="A482" t="s">
-        <v>520</v>
+        <v>525</v>
       </c>
     </row>
     <row r="483" spans="1:1">
       <c r="A483" t="s">
-        <v>521</v>
+        <v>526</v>
       </c>
     </row>
     <row r="484" spans="1:1">
       <c r="A484" t="s">
-        <v>522</v>
+        <v>527</v>
       </c>
     </row>
     <row r="485" spans="1:1">
       <c r="A485" t="s">
-        <v>523</v>
+        <v>528</v>
       </c>
     </row>
     <row r="486" spans="1:1">
       <c r="A486" t="s">
-        <v>524</v>
+        <v>529</v>
       </c>
     </row>
     <row r="487" spans="1:1">
       <c r="A487" t="s">
-        <v>525</v>
+        <v>530</v>
       </c>
     </row>
     <row r="488" spans="1:1">
       <c r="A488" t="s">
-        <v>526</v>
+        <v>531</v>
       </c>
     </row>
     <row r="489" spans="1:1">
       <c r="A489" t="s">
-        <v>527</v>
+        <v>532</v>
       </c>
     </row>
     <row r="490" spans="1:1">
       <c r="A490" t="s">
-        <v>528</v>
+        <v>533</v>
       </c>
     </row>
     <row r="491" spans="1:1">
       <c r="A491" t="s">
-        <v>529</v>
+        <v>534</v>
       </c>
     </row>
     <row r="492" spans="1:1">
       <c r="A492" t="s">
-        <v>530</v>
+        <v>535</v>
       </c>
     </row>
     <row r="493" spans="1:1">
       <c r="A493" t="s">
-        <v>531</v>
+        <v>536</v>
       </c>
     </row>
     <row r="494" spans="1:1">
       <c r="A494" t="s">
-        <v>532</v>
+        <v>537</v>
       </c>
     </row>
     <row r="495" spans="1:1">
       <c r="A495" t="s">
-        <v>533</v>
+        <v>538</v>
       </c>
     </row>
     <row r="496" spans="1:1">
       <c r="A496" t="s">
-        <v>534</v>
+        <v>539</v>
       </c>
     </row>
     <row r="497" spans="1:1">
       <c r="A497" t="s">
-        <v>535</v>
+        <v>540</v>
       </c>
     </row>
     <row r="498" spans="1:1">
       <c r="A498" t="s">
-        <v>536</v>
+        <v>541</v>
       </c>
     </row>
     <row r="499" spans="1:1">
       <c r="A499" t="s">
-        <v>537</v>
+        <v>542</v>
       </c>
     </row>
     <row r="500" spans="1:1">
       <c r="A500" t="s">
-        <v>538</v>
+        <v>543</v>
       </c>
     </row>
     <row r="501" spans="1:1">
       <c r="A501" t="s">
-        <v>539</v>
+        <v>544</v>
       </c>
     </row>
     <row r="502" spans="1:1">
       <c r="A502" t="s">
-        <v>540</v>
+        <v>545</v>
       </c>
     </row>
     <row r="503" spans="1:1">
       <c r="A503" t="s">
-        <v>541</v>
+        <v>546</v>
       </c>
     </row>
     <row r="504" spans="1:1">
       <c r="A504" t="s">
-        <v>542</v>
+        <v>547</v>
       </c>
     </row>
     <row r="505" spans="1:1">
       <c r="A505" t="s">
-        <v>543</v>
+        <v>548</v>
       </c>
     </row>
     <row r="506" spans="1:1">
       <c r="A506" t="s">
-        <v>544</v>
+        <v>549</v>
       </c>
     </row>
     <row r="507" spans="1:1">
       <c r="A507" t="s">
-        <v>545</v>
+        <v>550</v>
       </c>
     </row>
     <row r="508" spans="1:1">
       <c r="A508" t="s">
-        <v>546</v>
+        <v>551</v>
       </c>
     </row>
     <row r="509" spans="1:1">
       <c r="A509" t="s">
-        <v>547</v>
+        <v>552</v>
       </c>
     </row>
     <row r="510" spans="1:1">
       <c r="A510" t="s">
-        <v>548</v>
+        <v>553</v>
       </c>
     </row>
     <row r="511" spans="1:1">
       <c r="A511" t="s">
-        <v>549</v>
+        <v>554</v>
       </c>
     </row>
     <row r="512" spans="1:1">
       <c r="A512" t="s">
-        <v>550</v>
+        <v>555</v>
       </c>
     </row>
     <row r="513" spans="1:1">
       <c r="A513" t="s">
-        <v>551</v>
+        <v>556</v>
       </c>
     </row>
     <row r="514" spans="1:1">
       <c r="A514" t="s">
-        <v>552</v>
+        <v>557</v>
       </c>
     </row>
     <row r="515" spans="1:1">
       <c r="A515" t="s">
-        <v>553</v>
+        <v>558</v>
       </c>
     </row>
     <row r="516" spans="1:1">
       <c r="A516" t="s">
-        <v>554</v>
+        <v>559</v>
       </c>
     </row>
     <row r="517" spans="1:1">
       <c r="A517" t="s">
-        <v>555</v>
+        <v>560</v>
       </c>
     </row>
     <row r="518" spans="1:1">
       <c r="A518" t="s">
-        <v>556</v>
+        <v>561</v>
       </c>
     </row>
     <row r="519" spans="1:1">
       <c r="A519" t="s">
-        <v>557</v>
+        <v>562</v>
       </c>
     </row>
     <row r="520" spans="1:1">
       <c r="A520" t="s">
-        <v>558</v>
+        <v>563</v>
       </c>
     </row>
     <row r="521" spans="1:1">
       <c r="A521" t="s">
-        <v>559</v>
+        <v>564</v>
       </c>
     </row>
     <row r="522" spans="1:1">
       <c r="A522" t="s">
-        <v>560</v>
+        <v>565</v>
       </c>
     </row>
     <row r="523" spans="1:1">
       <c r="A523" t="s">
-        <v>561</v>
+        <v>566</v>
       </c>
     </row>
     <row r="524" spans="1:1">
       <c r="A524" t="s">
-        <v>562</v>
+        <v>567</v>
       </c>
     </row>
     <row r="525" spans="1:1">
       <c r="A525" t="s">
-        <v>563</v>
+        <v>568</v>
       </c>
     </row>
     <row r="526" spans="1:1">
       <c r="A526" t="s">
-        <v>564</v>
+        <v>569</v>
       </c>
     </row>
     <row r="528" spans="1:1">
       <c r="A528" t="s">
-        <v>565</v>
+        <v>570</v>
       </c>
     </row>
     <row r="529" spans="1:1">
       <c r="A529" t="s">
-        <v>566</v>
+        <v>571</v>
       </c>
     </row>
     <row r="530" spans="1:1">
       <c r="A530" t="s">
-        <v>567</v>
+        <v>572</v>
       </c>
     </row>
     <row r="531" spans="1:1">
       <c r="A531" t="s">
-        <v>568</v>
+        <v>573</v>
       </c>
     </row>
     <row r="532" spans="1:1">
       <c r="A532" t="s">
-        <v>569</v>
+        <v>574</v>
       </c>
     </row>
     <row r="533" spans="1:1">
       <c r="A533" t="s">
-        <v>570</v>
+        <v>575</v>
       </c>
     </row>
     <row r="534" spans="1:1">
       <c r="A534" t="s">
-        <v>571</v>
+        <v>576</v>
       </c>
     </row>
     <row r="535" spans="1:1">
       <c r="A535" t="s">
-        <v>572</v>
+        <v>577</v>
       </c>
     </row>
     <row r="536" spans="1:1">
       <c r="A536" t="s">
-        <v>573</v>
+        <v>578</v>
       </c>
     </row>
     <row r="537" spans="1:1">
       <c r="A537" t="s">
-        <v>574</v>
+        <v>579</v>
       </c>
     </row>
     <row r="538" spans="1:1">
       <c r="A538" t="s">
-        <v>575</v>
+        <v>580</v>
       </c>
     </row>
     <row r="539" spans="1:1">
       <c r="A539" t="s">
-        <v>576</v>
+        <v>581</v>
       </c>
     </row>
     <row r="540" spans="1:1">
       <c r="A540" t="s">
-        <v>577</v>
+        <v>582</v>
       </c>
     </row>
     <row r="541" spans="1:1">
       <c r="A541" t="s">
-        <v>578</v>
+        <v>583</v>
       </c>
     </row>
     <row r="542" spans="1:1">
       <c r="A542" t="s">
-        <v>579</v>
+        <v>584</v>
       </c>
     </row>
     <row r="543" spans="1:1">
       <c r="A543" t="s">
-        <v>580</v>
+        <v>585</v>
       </c>
     </row>
     <row r="544" spans="1:1">
       <c r="A544" t="s">
-        <v>581</v>
+        <v>586</v>
       </c>
     </row>
     <row r="545" spans="1:1">
       <c r="A545" t="s">
-        <v>582</v>
+        <v>587</v>
       </c>
     </row>
     <row r="547" spans="1:1">
       <c r="A547" t="s">
-        <v>583</v>
+        <v>588</v>
       </c>
     </row>
     <row r="548" spans="1:1">
       <c r="A548" t="s">
-        <v>584</v>
+        <v>589</v>
       </c>
     </row>
     <row r="549" spans="1:1">
       <c r="A549" t="s">
-        <v>585</v>
+        <v>590</v>
       </c>
     </row>
     <row r="550" spans="1:1">
       <c r="A550" t="s">
-        <v>586</v>
+        <v>591</v>
       </c>
     </row>
     <row r="551" spans="1:1">
       <c r="A551" t="s">
-        <v>587</v>
+        <v>592</v>
       </c>
     </row>
     <row r="552" spans="1:1">
       <c r="A552" t="s">
-        <v>588</v>
+        <v>593</v>
       </c>
     </row>
     <row r="553" spans="1:1">
       <c r="A553" t="s">
-        <v>589</v>
+        <v>594</v>
       </c>
     </row>
     <row r="554" spans="1:1">
       <c r="A554" t="s">
-        <v>590</v>
+        <v>595</v>
       </c>
     </row>
     <row r="555" spans="1:1">
       <c r="A555" t="s">
-        <v>591</v>
+        <v>596</v>
       </c>
     </row>
     <row r="556" spans="1:1">
       <c r="A556" t="s">
-        <v>592</v>
+        <v>597</v>
       </c>
     </row>
     <row r="557" spans="1:1">
       <c r="A557" t="s">
-        <v>593</v>
+        <v>598</v>
       </c>
     </row>
     <row r="558" spans="1:1">
       <c r="A558" t="s">
-        <v>594</v>
+        <v>599</v>
       </c>
     </row>
     <row r="559" spans="1:1">
       <c r="A559" t="s">
-        <v>595</v>
+        <v>600</v>
       </c>
     </row>
     <row r="560" spans="1:1">
       <c r="A560" t="s">
-        <v>596</v>
+        <v>601</v>
       </c>
     </row>
     <row r="561" spans="1:1">
       <c r="A561" t="s">
-        <v>597</v>
+        <v>602</v>
       </c>
     </row>
     <row r="562" spans="1:1">
       <c r="A562" t="s">
-        <v>598</v>
+        <v>603</v>
       </c>
     </row>
     <row r="563" spans="1:1">
       <c r="A563" t="s">
-        <v>599</v>
+        <v>604</v>
       </c>
     </row>
     <row r="564" spans="1:1">
       <c r="A564" t="s">
-        <v>600</v>
+        <v>605</v>
       </c>
     </row>
     <row r="565" spans="1:1">
       <c r="A565" t="s">
-        <v>601</v>
+        <v>606</v>
       </c>
     </row>
     <row r="566" spans="1:1">
       <c r="A566" t="s">
-        <v>602</v>
+        <v>607</v>
       </c>
     </row>
     <row r="567" spans="1:1">
       <c r="A567" t="s">
-        <v>603</v>
+        <v>608</v>
       </c>
     </row>
     <row r="568" spans="1:1">
       <c r="A568" t="s">
-        <v>604</v>
+        <v>609</v>
       </c>
     </row>
     <row r="569" spans="1:1">
       <c r="A569" t="s">
-        <v>605</v>
+        <v>610</v>
       </c>
     </row>
     <row r="570" spans="1:1">
       <c r="A570" t="s">
-        <v>606</v>
+        <v>611</v>
       </c>
     </row>
     <row r="572" spans="1:1">
       <c r="A572" t="s">
-        <v>607</v>
+        <v>612</v>
       </c>
     </row>
     <row r="573" spans="1:1">
       <c r="A573" t="s">
-        <v>608</v>
+        <v>613</v>
       </c>
     </row>
     <row r="574" spans="1:1">
       <c r="A574" t="s">
-        <v>609</v>
+        <v>614</v>
       </c>
     </row>
     <row r="575" spans="1:1">
       <c r="A575" t="s">
-        <v>610</v>
+        <v>615</v>
       </c>
     </row>
     <row r="576" spans="1:1">
       <c r="A576" t="s">
-        <v>611</v>
+        <v>616</v>
       </c>
     </row>
     <row r="577" spans="1:1">
       <c r="A577" t="s">
-        <v>612</v>
+        <v>617</v>
       </c>
     </row>
     <row r="578" spans="1:1">
       <c r="A578" t="s">
-        <v>613</v>
+        <v>618</v>
       </c>
     </row>
     <row r="579" spans="1:1">
       <c r="A579" t="s">
-        <v>614</v>
+        <v>619</v>
       </c>
     </row>
     <row r="580" spans="1:1">
       <c r="A580" t="s">
-        <v>615</v>
+        <v>620</v>
       </c>
     </row>
     <row r="581" spans="1:1">
       <c r="A581" t="s">
-        <v>616</v>
+        <v>621</v>
       </c>
     </row>
     <row r="582" spans="1:1">
       <c r="A582" t="s">
-        <v>617</v>
+        <v>622</v>
       </c>
     </row>
     <row r="583" spans="1:1">
       <c r="A583" t="s">
-        <v>618</v>
+        <v>623</v>
       </c>
     </row>
     <row r="584" spans="1:1">
       <c r="A584" t="s">
-        <v>619</v>
+        <v>624</v>
       </c>
     </row>
     <row r="585" spans="1:1">
       <c r="A585" t="s">
-        <v>620</v>
+        <v>625</v>
       </c>
     </row>
     <row r="586" spans="1:1">
       <c r="A586" t="s">
-        <v>621</v>
+        <v>626</v>
       </c>
     </row>
     <row r="588" spans="1:1">
       <c r="A588" t="s">
-        <v>622</v>
+        <v>627</v>
       </c>
     </row>
     <row r="589" spans="1:1">
       <c r="A589" t="s">
-        <v>623</v>
+        <v>628</v>
       </c>
     </row>
     <row r="590" spans="1:1">
       <c r="A590" t="s">
-        <v>624</v>
+        <v>629</v>
       </c>
     </row>
     <row r="591" spans="1:1">
       <c r="A591" t="s">
-        <v>625</v>
+        <v>630</v>
       </c>
     </row>
     <row r="592" spans="1:1">
       <c r="A592" t="s">
-        <v>626</v>
+        <v>631</v>
       </c>
     </row>
     <row r="593" spans="1:1">
       <c r="A593" t="s">
-        <v>627</v>
+        <v>632</v>
       </c>
     </row>
     <row r="594" spans="1:1">
       <c r="A594" t="s">
-        <v>628</v>
+        <v>633</v>
       </c>
     </row>
     <row r="595" spans="1:1">
       <c r="A595" t="s">
-        <v>629</v>
+        <v>634</v>
       </c>
     </row>
     <row r="596" spans="1:1">
       <c r="A596" t="s">
-        <v>630</v>
+        <v>635</v>
       </c>
     </row>
     <row r="597" spans="1:1">
       <c r="A597" t="s">
-        <v>631</v>
+        <v>636</v>
       </c>
     </row>
     <row r="598" spans="1:1">
       <c r="A598" t="s">
-        <v>632</v>
+        <v>637</v>
       </c>
     </row>
     <row r="599" spans="1:1">
       <c r="A599" t="s">
-        <v>633</v>
+        <v>638</v>
       </c>
     </row>
     <row r="600" spans="1:1">
       <c r="A600" t="s">
-        <v>634</v>
+        <v>639</v>
       </c>
     </row>
     <row r="601" spans="1:1">
       <c r="A601" t="s">
-        <v>635</v>
+        <v>640</v>
       </c>
     </row>
     <row r="602" spans="1:1">
       <c r="A602" t="s">
-        <v>636</v>
+        <v>641</v>
       </c>
     </row>
     <row r="603" spans="1:1">
       <c r="A603" t="s">
-        <v>637</v>
+        <v>642</v>
       </c>
     </row>
     <row r="604" spans="1:1">
       <c r="A604" t="s">
-        <v>638</v>
+        <v>643</v>
       </c>
     </row>
     <row r="605" spans="1:1">
       <c r="A605" t="s">
-        <v>639</v>
+        <v>644</v>
       </c>
     </row>
     <row r="606" spans="1:1">
       <c r="A606" t="s">
-        <v>640</v>
+        <v>645</v>
       </c>
     </row>
     <row r="607" spans="1:1">
       <c r="A607" t="s">
-        <v>641</v>
+        <v>646</v>
       </c>
     </row>
     <row r="608" spans="1:1">
       <c r="A608" t="s">
-        <v>642</v>
+        <v>647</v>
       </c>
     </row>
     <row r="609" spans="1:1">
       <c r="A609" t="s">
-        <v>643</v>
+        <v>648</v>
       </c>
     </row>
     <row r="610" spans="1:1">
       <c r="A610" t="s">
-        <v>644</v>
+        <v>649</v>
       </c>
     </row>
     <row r="611" spans="1:1">
       <c r="A611" t="s">
-        <v>645</v>
+        <v>650</v>
       </c>
     </row>
     <row r="612" spans="1:1">
       <c r="A612" t="s">
-        <v>646</v>
+        <v>651</v>
       </c>
     </row>
     <row r="613" spans="1:1">
       <c r="A613" t="s">
-        <v>647</v>
+        <v>652</v>
       </c>
     </row>
     <row r="614" spans="1:1">
       <c r="A614" t="s">
-        <v>648</v>
+        <v>653</v>
       </c>
     </row>
     <row r="615" spans="1:1">
       <c r="A615" t="s">
-        <v>649</v>
+        <v>654</v>
       </c>
     </row>
     <row r="616" spans="1:1">
       <c r="A616" t="s">
-        <v>650</v>
+        <v>655</v>
       </c>
     </row>
     <row r="617" spans="1:1">
       <c r="A617" t="s">
-        <v>651</v>
+        <v>656</v>
       </c>
     </row>
     <row r="618" spans="1:1">
       <c r="A618" t="s">
-        <v>652</v>
+        <v>657</v>
       </c>
     </row>
     <row r="619" spans="1:1">
       <c r="A619" t="s">
-        <v>653</v>
+        <v>658</v>
       </c>
     </row>
     <row r="620" spans="1:1">
       <c r="A620" t="s">
-        <v>654</v>
+        <v>659</v>
       </c>
     </row>
     <row r="621" spans="1:1">
       <c r="A621" t="s">
-        <v>655</v>
+        <v>660</v>
       </c>
     </row>
     <row r="622" spans="1:1">
       <c r="A622" t="s">
-        <v>656</v>
+        <v>661</v>
       </c>
     </row>
     <row r="623" spans="1:1">
       <c r="A623" t="s">
-        <v>657</v>
+        <v>662</v>
       </c>
     </row>
     <row r="624" spans="1:1">
       <c r="A624" t="s">
-        <v>658</v>
+        <v>663</v>
       </c>
     </row>
     <row r="625" spans="1:1">
       <c r="A625" t="s">
-        <v>659</v>
+        <v>664</v>
       </c>
     </row>
     <row r="626" spans="1:1">
       <c r="A626" t="s">
-        <v>660</v>
+        <v>665</v>
       </c>
     </row>
     <row r="627" spans="1:1">
       <c r="A627" t="s">
-        <v>661</v>
+        <v>666</v>
       </c>
     </row>
     <row r="628" spans="1:1">
       <c r="A628" t="s">
-        <v>662</v>
+        <v>667</v>
       </c>
     </row>
     <row r="629" spans="1:1">
       <c r="A629" t="s">
-        <v>663</v>
+        <v>668</v>
       </c>
     </row>
     <row r="630" spans="1:1">
       <c r="A630" t="s">
-        <v>664</v>
+        <v>669</v>
       </c>
     </row>
     <row r="631" spans="1:1">
       <c r="A631" t="s">
-        <v>665</v>
+        <v>670</v>
       </c>
     </row>
     <row r="632" spans="1:1">
       <c r="A632" t="s">
-        <v>666</v>
+        <v>671</v>
       </c>
     </row>
     <row r="633" spans="1:1">
       <c r="A633" t="s">
-        <v>667</v>
+        <v>672</v>
       </c>
     </row>
     <row r="634" spans="1:1">
       <c r="A634" t="s">
-        <v>668</v>
+        <v>673</v>
       </c>
     </row>
     <row r="635" spans="1:1">
       <c r="A635" t="s">
-        <v>669</v>
+        <v>674</v>
       </c>
     </row>
     <row r="636" spans="1:1">
       <c r="A636" t="s">
-        <v>670</v>
+        <v>675</v>
       </c>
     </row>
     <row r="637" spans="1:1">
       <c r="A637" t="s">
-        <v>671</v>
+        <v>676</v>
       </c>
     </row>
     <row r="638" spans="1:1">
       <c r="A638" t="s">
-        <v>672</v>
+        <v>677</v>
       </c>
     </row>
     <row r="639" spans="1:1">
       <c r="A639" t="s">
-        <v>673</v>
+        <v>678</v>
       </c>
     </row>
     <row r="640" spans="1:1">
       <c r="A640" t="s">
-        <v>674</v>
+        <v>679</v>
       </c>
     </row>
     <row r="641" spans="1:1">
       <c r="A641" t="s">
-        <v>675</v>
+        <v>680</v>
       </c>
     </row>
     <row r="642" spans="1:1">
       <c r="A642" t="s">
-        <v>676</v>
+        <v>681</v>
       </c>
     </row>
     <row r="643" spans="1:1">
       <c r="A643" t="s">
-        <v>677</v>
+        <v>682</v>
       </c>
     </row>
     <row r="644" spans="1:1">
       <c r="A644" t="s">
-        <v>678</v>
+        <v>683</v>
       </c>
     </row>
     <row r="645" spans="1:1">
       <c r="A645" t="s">
-        <v>679</v>
+        <v>684</v>
       </c>
     </row>
     <row r="646" spans="1:1">
       <c r="A646" t="s">
-        <v>680</v>
+        <v>685</v>
       </c>
     </row>
     <row r="647" spans="1:1">
       <c r="A647" t="s">
-        <v>681</v>
+        <v>686</v>
       </c>
     </row>
     <row r="648" spans="1:1">
       <c r="A648" t="s">
-        <v>682</v>
+        <v>687</v>
       </c>
     </row>
     <row r="649" spans="1:1">
       <c r="A649" t="s">
-        <v>683</v>
+        <v>688</v>
       </c>
     </row>
     <row r="650" spans="1:1">
       <c r="A650" t="s">
-        <v>684</v>
+        <v>689</v>
       </c>
     </row>
     <row r="651" spans="1:1">
       <c r="A651" t="s">
-        <v>685</v>
+        <v>690</v>
       </c>
     </row>
     <row r="652" spans="1:1">
       <c r="A652" t="s">
-        <v>686</v>
+        <v>691</v>
       </c>
     </row>
     <row r="653" spans="1:1">
       <c r="A653" t="s">
-        <v>687</v>
+        <v>692</v>
       </c>
     </row>
     <row r="654" spans="1:1">
       <c r="A654" t="s">
-        <v>688</v>
+        <v>693</v>
       </c>
     </row>
     <row r="655" spans="1:1">
       <c r="A655" t="s">
-        <v>689</v>
+        <v>694</v>
       </c>
     </row>
     <row r="656" spans="1:1">
       <c r="A656" t="s">
-        <v>690</v>
+        <v>695</v>
       </c>
     </row>
     <row r="657" spans="1:1">
       <c r="A657" t="s">
-        <v>691</v>
+        <v>696</v>
       </c>
     </row>
     <row r="658" spans="1:1">
       <c r="A658" t="s">
-        <v>692</v>
+        <v>697</v>
       </c>
     </row>
     <row r="660" spans="1:1">
       <c r="A660" t="s">
-        <v>693</v>
+        <v>698</v>
       </c>
     </row>
     <row r="661" spans="1:1">
       <c r="A661" t="s">
-        <v>694</v>
+        <v>699</v>
       </c>
     </row>
     <row r="662" spans="1:1">
       <c r="A662" t="s">
-        <v>695</v>
+        <v>700</v>
       </c>
     </row>
     <row r="663" spans="1:1">
       <c r="A663" t="s">
-        <v>696</v>
+        <v>701</v>
       </c>
     </row>
     <row r="664" spans="1:1">
       <c r="A664" t="s">
-        <v>697</v>
+        <v>702</v>
       </c>
     </row>
     <row r="665" spans="1:1">
       <c r="A665" t="s">
-        <v>698</v>
+        <v>703</v>
       </c>
     </row>
     <row r="666" spans="1:1">
       <c r="A666" t="s">
-        <v>699</v>
+        <v>704</v>
       </c>
     </row>
     <row r="667" spans="1:1">
       <c r="A667" t="s">
-        <v>700</v>
+        <v>705</v>
       </c>
     </row>
     <row r="668" spans="1:1">
       <c r="A668" t="s">
-        <v>701</v>
+        <v>706</v>
       </c>
     </row>
     <row r="669" spans="1:1">
       <c r="A669" t="s">
-        <v>702</v>
+        <v>707</v>
       </c>
     </row>
     <row r="671" spans="1:1">
       <c r="A671" t="s">
-        <v>703</v>
+        <v>708</v>
       </c>
     </row>
     <row r="672" spans="1:1">
       <c r="A672" t="s">
-        <v>704</v>
+        <v>709</v>
       </c>
     </row>
     <row r="673" spans="1:1">
       <c r="A673" t="s">
-        <v>705</v>
+        <v>710</v>
       </c>
     </row>
     <row r="674" spans="1:1">
       <c r="A674" t="s">
-        <v>706</v>
+        <v>711</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
set export bundle variables to defaults
</commit_message>
<xml_diff>
--- a/templates/panos/set_commands/iron_skillet_panos_full.xlsx
+++ b/templates/panos/set_commands/iron_skillet_panos_full.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="712">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="707">
   <si>
     <t>Variable Name</t>
   </si>
@@ -78,21 +78,6 @@
   </si>
   <si>
     <t>IP address for scheduled config exports</t>
-  </si>
-  <si>
-    <t>CONFIG_EXPORT_USER</t>
-  </si>
-  <si>
-    <t>testuser</t>
-  </si>
-  <si>
-    <t>username for config export</t>
-  </si>
-  <si>
-    <t>CONFIG_EXPORT_PASSWORD</t>
-  </si>
-  <si>
-    <t>password for config export</t>
   </si>
   <si>
     <t>TEMPLATE</t>
@@ -2491,7 +2476,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2594,40 +2579,40 @@
         <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="C12" t="s">
         <v>34</v>
@@ -2649,62 +2634,62 @@
         <v>38</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B17" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C17" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C18" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B19" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C19" t="s">
         <v>54</v>
@@ -2726,95 +2711,95 @@
         <v>58</v>
       </c>
       <c r="B21" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C21" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B22" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C22" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B23" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C23" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B24" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C24" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B25" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C25" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B26" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C26" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B27" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C27" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B28" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C28" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>81</v>
-      </c>
-      <c r="B29" t="s">
         <v>82</v>
+      </c>
+      <c r="B29">
+        <v>525600</v>
       </c>
       <c r="C29" t="s">
         <v>83</v>
@@ -2829,28 +2814,6 @@
       </c>
       <c r="C30" t="s">
         <v>86</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" t="s">
-        <v>87</v>
-      </c>
-      <c r="B31">
-        <v>525600</v>
-      </c>
-      <c r="C31" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" t="s">
-        <v>89</v>
-      </c>
-      <c r="B32" t="s">
-        <v>90</v>
-      </c>
-      <c r="C32" t="s">
-        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -2868,3269 +2831,3269 @@
   <sheetData>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8">
-        <f>SUBSTITUTE("set deviceconfig system hostname {{ FW_NAME }}", "{{ FW_NAME }}", 'values'!B13)</f>
+        <f>SUBSTITUTE("set deviceconfig system hostname {{ FW_NAME }}", "{{ FW_NAME }}", 'values'!B11)</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9">
-        <f>SUBSTITUTE("set deviceconfig system ip-address {{ MGMT_IP }}", "{{ MGMT_IP }}", 'values'!B15)</f>
+        <f>SUBSTITUTE("set deviceconfig system ip-address {{ MGMT_IP }}", "{{ MGMT_IP }}", 'values'!B13)</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10">
-        <f>SUBSTITUTE("set deviceconfig system netmask {{ MGMT_MASK }}", "{{ MGMT_MASK }}", 'values'!B16)</f>
+        <f>SUBSTITUTE("set deviceconfig system netmask {{ MGMT_MASK }}", "{{ MGMT_MASK }}", 'values'!B14)</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11">
-        <f>SUBSTITUTE("set deviceconfig system default-gateway {{ MGMT_DG }}", "{{ MGMT_DG }}", 'values'!B17)</f>
+        <f>SUBSTITUTE("set deviceconfig system default-gateway {{ MGMT_DG }}", "{{ MGMT_DG }}", 'values'!B15)</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12">
-        <f>SUBSTITUTE("set deviceconfig system dns-setting servers primary {{ DNS_1 }}", "{{ DNS_1 }}", 'values'!B22)</f>
+        <f>SUBSTITUTE("set deviceconfig system dns-setting servers primary {{ DNS_1 }}", "{{ DNS_1 }}", 'values'!B20)</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13">
-        <f>SUBSTITUTE("set deviceconfig system dns-setting servers secondary {{ DNS_2 }}", "{{ DNS_2 }}", 'values'!B23)</f>
+        <f>SUBSTITUTE("set deviceconfig system dns-setting servers secondary {{ DNS_2 }}", "{{ DNS_2 }}", 'values'!B21)</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14">
-        <f>SUBSTITUTE("set deviceconfig system ntp-servers primary-ntp-server ntp-server-address {{ NTP_1 }}", "{{ NTP_1 }}", 'values'!B18)</f>
+        <f>SUBSTITUTE("set deviceconfig system ntp-servers primary-ntp-server ntp-server-address {{ NTP_1 }}", "{{ NTP_1 }}", 'values'!B16)</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15">
-        <f>SUBSTITUTE("set deviceconfig system ntp-servers secondary-ntp-server ntp-server-address {{ NTP_2 }}", "{{ NTP_2 }}", 'values'!B19)</f>
+        <f>SUBSTITUTE("set deviceconfig system ntp-servers secondary-ntp-server ntp-server-address {{ NTP_2 }}", "{{ NTP_2 }}", 'values'!B17)</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18">
-        <f>SUBSTITUTE("set mgt-config users {{ ADMINISTRATOR_USERNAME }} password", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B20)</f>
+        <f>SUBSTITUTE("set mgt-config users {{ ADMINISTRATOR_USERNAME }} password", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B18)</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19">
-        <f>SUBSTITUTE("set mgt-config users {{ ADMINISTRATOR_USERNAME }} permissions role-based superuser yes", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B20)</f>
+        <f>SUBSTITUTE("set mgt-config users {{ ADMINISTRATOR_USERNAME }} permissions role-based superuser yes", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B18)</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68">
-        <f>SUBSTITUTE("set deviceconfig setting management api key lifetime {{ API_KEY_LIFETIME }}", "{{ API_KEY_LIFETIME }}", 'values'!B31)</f>
+        <f>SUBSTITUTE("set deviceconfig setting management api key lifetime {{ API_KEY_LIFETIME }}", "{{ API_KEY_LIFETIME }}", 'values'!B29)</f>
         <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="85" spans="1:1">
       <c r="A85" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="87" spans="1:1">
       <c r="A87" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="89" spans="1:1">
       <c r="A89" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="90" spans="1:1">
       <c r="A90" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="91" spans="1:1">
       <c r="A91" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="92" spans="1:1">
       <c r="A92" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="94" spans="1:1">
       <c r="A94" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="97" spans="1:1">
       <c r="A97" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="98" spans="1:1">
       <c r="A98" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99">
-        <f>SUBSTITUTE("set shared log-settings email Sample_Email_Profile server Sample_Email_Profile gateway {{ EMAIL_PROFILE_GATEWAY }}", "{{ EMAIL_PROFILE_GATEWAY }}", 'values'!B27)</f>
+        <f>SUBSTITUTE("set shared log-settings email Sample_Email_Profile server Sample_Email_Profile gateway {{ EMAIL_PROFILE_GATEWAY }}", "{{ EMAIL_PROFILE_GATEWAY }}", 'values'!B25)</f>
         <v>0</v>
       </c>
     </row>
     <row r="100" spans="1:1">
       <c r="A100">
-        <f>SUBSTITUTE("set shared log-settings email Sample_Email_Profile server Sample_Email_Profile from {{ EMAIL_PROFILE_FROM }}", "{{ EMAIL_PROFILE_FROM }}", 'values'!B28)</f>
+        <f>SUBSTITUTE("set shared log-settings email Sample_Email_Profile server Sample_Email_Profile from {{ EMAIL_PROFILE_FROM }}", "{{ EMAIL_PROFILE_FROM }}", 'values'!B26)</f>
         <v>0</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101">
-        <f>SUBSTITUTE("set shared log-settings email Sample_Email_Profile server Sample_Email_Profile to {{ EMAIL_PROFILE_TO }}", "{{ EMAIL_PROFILE_TO }}", 'values'!B29)</f>
+        <f>SUBSTITUTE("set shared log-settings email Sample_Email_Profile server Sample_Email_Profile to {{ EMAIL_PROFILE_TO }}", "{{ EMAIL_PROFILE_TO }}", 'values'!B27)</f>
         <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:1">
       <c r="A102" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="104" spans="1:1">
       <c r="A104" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="105" spans="1:1">
       <c r="A105">
-        <f>SUBSTITUTE("set shared log-settings syslog Sample_Syslog_Profile server Sample_Syslog server {{ SYSLOG_SERVER }}", "{{ SYSLOG_SERVER }}", 'values'!B30)</f>
+        <f>SUBSTITUTE("set shared log-settings syslog Sample_Syslog_Profile server Sample_Syslog server {{ SYSLOG_SERVER }}", "{{ SYSLOG_SERVER }}", 'values'!B28)</f>
         <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:1">
       <c r="A106" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="108" spans="1:1">
       <c r="A108" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="109" spans="1:1">
       <c r="A109" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
     </row>
     <row r="110" spans="1:1">
       <c r="A110" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="111" spans="1:1">
       <c r="A111" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
     </row>
     <row r="112" spans="1:1">
       <c r="A112" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="113" spans="1:1">
       <c r="A113" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
     </row>
     <row r="114" spans="1:1">
       <c r="A114" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="115" spans="1:1">
       <c r="A115" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
     </row>
     <row r="116" spans="1:1">
       <c r="A116" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="117" spans="1:1">
       <c r="A117" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="118" spans="1:1">
       <c r="A118" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="119" spans="1:1">
       <c r="A119" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="120" spans="1:1">
       <c r="A120" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="121" spans="1:1">
       <c r="A121" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
     </row>
     <row r="122" spans="1:1">
       <c r="A122" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="123" spans="1:1">
       <c r="A123" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="125" spans="1:1">
       <c r="A125" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="126" spans="1:1">
       <c r="A126" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="127" spans="1:1">
       <c r="A127" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="128" spans="1:1">
       <c r="A128" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="129" spans="1:1">
       <c r="A129" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="130" spans="1:1">
       <c r="A130" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="131" spans="1:1">
       <c r="A131" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="132" spans="1:1">
       <c r="A132" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
     <row r="133" spans="1:1">
       <c r="A133" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
     <row r="134" spans="1:1">
       <c r="A134" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="135" spans="1:1">
       <c r="A135" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="136" spans="1:1">
       <c r="A136" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="137" spans="1:1">
       <c r="A137" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="138" spans="1:1">
       <c r="A138" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="139" spans="1:1">
       <c r="A139" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="140" spans="1:1">
       <c r="A140" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
     </row>
     <row r="141" spans="1:1">
       <c r="A141" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
     </row>
     <row r="142" spans="1:1">
       <c r="A142" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
     </row>
     <row r="143" spans="1:1">
       <c r="A143" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
     </row>
     <row r="144" spans="1:1">
       <c r="A144" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="145" spans="1:1">
       <c r="A145" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
     </row>
     <row r="146" spans="1:1">
       <c r="A146" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="147" spans="1:1">
       <c r="A147" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
     </row>
     <row r="148" spans="1:1">
       <c r="A148" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
     </row>
     <row r="149" spans="1:1">
       <c r="A149" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
     </row>
     <row r="150" spans="1:1">
       <c r="A150" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
     </row>
     <row r="151" spans="1:1">
       <c r="A151" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
     </row>
     <row r="152" spans="1:1">
       <c r="A152" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
     </row>
     <row r="153" spans="1:1">
       <c r="A153" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
     </row>
     <row r="154" spans="1:1">
       <c r="A154" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
     </row>
     <row r="155" spans="1:1">
       <c r="A155" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
     </row>
     <row r="156" spans="1:1">
       <c r="A156" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
     </row>
     <row r="157" spans="1:1">
       <c r="A157" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
     </row>
     <row r="158" spans="1:1">
       <c r="A158" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
     </row>
     <row r="159" spans="1:1">
       <c r="A159" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
     </row>
     <row r="160" spans="1:1">
       <c r="A160" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
     </row>
     <row r="161" spans="1:1">
       <c r="A161" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
     </row>
     <row r="162" spans="1:1">
       <c r="A162" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
     </row>
     <row r="163" spans="1:1">
       <c r="A163" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
     </row>
     <row r="165" spans="1:1">
       <c r="A165" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
     </row>
     <row r="166" spans="1:1">
       <c r="A166" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
     </row>
     <row r="167" spans="1:1">
       <c r="A167" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
     </row>
     <row r="168" spans="1:1">
       <c r="A168" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
     </row>
     <row r="169" spans="1:1">
       <c r="A169" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
     </row>
     <row r="171" spans="1:1">
       <c r="A171" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
     </row>
     <row r="172" spans="1:1">
       <c r="A172">
-        <f>SUBSTITUTE("set address Sinkhole-IPv4 ip-netmask {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B24)</f>
+        <f>SUBSTITUTE("set address Sinkhole-IPv4 ip-netmask {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
         <v>0</v>
       </c>
     </row>
     <row r="173" spans="1:1">
       <c r="A173">
-        <f>SUBSTITUTE("set address Sinkhole-IPv6 ip-netmask {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B25)</f>
+        <f>SUBSTITUTE("set address Sinkhole-IPv6 ip-netmask {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
         <v>0</v>
       </c>
     </row>
     <row r="175" spans="1:1">
       <c r="A175" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
     </row>
     <row r="176" spans="1:1">
       <c r="A176" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
     </row>
     <row r="177" spans="1:1">
       <c r="A177" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
     </row>
     <row r="178" spans="1:1">
       <c r="A178" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
     </row>
     <row r="179" spans="1:1">
       <c r="A179" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
     </row>
     <row r="180" spans="1:1">
       <c r="A180" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
     </row>
     <row r="181" spans="1:1">
       <c r="A181" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
     </row>
     <row r="182" spans="1:1">
       <c r="A182" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
     </row>
     <row r="183" spans="1:1">
       <c r="A183" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
     </row>
     <row r="184" spans="1:1">
       <c r="A184" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
     </row>
     <row r="185" spans="1:1">
       <c r="A185" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="186" spans="1:1">
       <c r="A186" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
     </row>
     <row r="187" spans="1:1">
       <c r="A187" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="188" spans="1:1">
       <c r="A188" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="189" spans="1:1">
       <c r="A189" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
     </row>
     <row r="190" spans="1:1">
       <c r="A190" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
     </row>
     <row r="191" spans="1:1">
       <c r="A191" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
     </row>
     <row r="192" spans="1:1">
       <c r="A192" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
     </row>
     <row r="193" spans="1:1">
       <c r="A193" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
     </row>
     <row r="194" spans="1:1">
       <c r="A194" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
     <row r="195" spans="1:1">
       <c r="A195" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
     </row>
     <row r="196" spans="1:1">
       <c r="A196" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
     </row>
     <row r="197" spans="1:1">
       <c r="A197" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
     <row r="198" spans="1:1">
       <c r="A198" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
     </row>
     <row r="199" spans="1:1">
       <c r="A199" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="200" spans="1:1">
       <c r="A200" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="201" spans="1:1">
       <c r="A201" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
     </row>
     <row r="202" spans="1:1">
       <c r="A202" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="203" spans="1:1">
       <c r="A203" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
     </row>
     <row r="205" spans="1:1">
       <c r="A205" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="206" spans="1:1">
       <c r="A206">
-        <f>SUBSTITUTE("set profiles spyware Outbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B24)</f>
+        <f>SUBSTITUTE("set profiles spyware Outbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
         <v>0</v>
       </c>
     </row>
     <row r="207" spans="1:1">
       <c r="A207">
-        <f>SUBSTITUTE("set profiles spyware Outbound-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B25)</f>
+        <f>SUBSTITUTE("set profiles spyware Outbound-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
         <v>0</v>
       </c>
     </row>
     <row r="208" spans="1:1">
       <c r="A208" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
     </row>
     <row r="209" spans="1:1">
       <c r="A209" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
     </row>
     <row r="210" spans="1:1">
       <c r="A210" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="211" spans="1:1">
       <c r="A211" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
     </row>
     <row r="212" spans="1:1">
       <c r="A212" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
     </row>
     <row r="213" spans="1:1">
       <c r="A213" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
     </row>
     <row r="214" spans="1:1">
       <c r="A214" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
     </row>
     <row r="215" spans="1:1">
       <c r="A215" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="216" spans="1:1">
       <c r="A216" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
     </row>
     <row r="217" spans="1:1">
       <c r="A217" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
     </row>
     <row r="218" spans="1:1">
       <c r="A218" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
     </row>
     <row r="219" spans="1:1">
       <c r="A219" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
     </row>
     <row r="220" spans="1:1">
       <c r="A220" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
     </row>
     <row r="221" spans="1:1">
       <c r="A221" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
     </row>
     <row r="222" spans="1:1">
       <c r="A222">
-        <f>SUBSTITUTE("set profiles spyware Inbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B24)</f>
+        <f>SUBSTITUTE("set profiles spyware Inbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
         <v>0</v>
       </c>
     </row>
     <row r="223" spans="1:1">
       <c r="A223">
-        <f>SUBSTITUTE("set profiles spyware Inbound-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B25)</f>
+        <f>SUBSTITUTE("set profiles spyware Inbound-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
         <v>0</v>
       </c>
     </row>
     <row r="224" spans="1:1">
       <c r="A224" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
     </row>
     <row r="225" spans="1:1">
       <c r="A225" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
     </row>
     <row r="226" spans="1:1">
       <c r="A226" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
     </row>
     <row r="227" spans="1:1">
       <c r="A227" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
     </row>
     <row r="228" spans="1:1">
       <c r="A228" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
     </row>
     <row r="229" spans="1:1">
       <c r="A229" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
     </row>
     <row r="230" spans="1:1">
       <c r="A230" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
     </row>
     <row r="231" spans="1:1">
       <c r="A231" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
     </row>
     <row r="232" spans="1:1">
       <c r="A232" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
     </row>
     <row r="233" spans="1:1">
       <c r="A233" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
     </row>
     <row r="234" spans="1:1">
       <c r="A234" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
     </row>
     <row r="235" spans="1:1">
       <c r="A235" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
     </row>
     <row r="236" spans="1:1">
       <c r="A236" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
     </row>
     <row r="237" spans="1:1">
       <c r="A237" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
     </row>
     <row r="238" spans="1:1">
       <c r="A238">
-        <f>SUBSTITUTE("set profiles spyware Internal-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B24)</f>
+        <f>SUBSTITUTE("set profiles spyware Internal-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
         <v>0</v>
       </c>
     </row>
     <row r="239" spans="1:1">
       <c r="A239">
-        <f>SUBSTITUTE("set profiles spyware Internal-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B25)</f>
+        <f>SUBSTITUTE("set profiles spyware Internal-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
         <v>0</v>
       </c>
     </row>
     <row r="240" spans="1:1">
       <c r="A240" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
     </row>
     <row r="241" spans="1:1">
       <c r="A241" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
     </row>
     <row r="242" spans="1:1">
       <c r="A242" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
     </row>
     <row r="243" spans="1:1">
       <c r="A243" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
     </row>
     <row r="244" spans="1:1">
       <c r="A244" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
     </row>
     <row r="245" spans="1:1">
       <c r="A245" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
     </row>
     <row r="246" spans="1:1">
       <c r="A246" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
     </row>
     <row r="247" spans="1:1">
       <c r="A247" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
     </row>
     <row r="248" spans="1:1">
       <c r="A248" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
     </row>
     <row r="249" spans="1:1">
       <c r="A249" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
     </row>
     <row r="250" spans="1:1">
       <c r="A250" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
     </row>
     <row r="251" spans="1:1">
       <c r="A251" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
     </row>
     <row r="252" spans="1:1">
       <c r="A252" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
     </row>
     <row r="253" spans="1:1">
       <c r="A253" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
     </row>
     <row r="254" spans="1:1">
       <c r="A254" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
     </row>
     <row r="255" spans="1:1">
       <c r="A255">
-        <f>SUBSTITUTE("set profiles spyware Alert-Only-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B24)</f>
+        <f>SUBSTITUTE("set profiles spyware Alert-Only-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
         <v>0</v>
       </c>
     </row>
     <row r="256" spans="1:1">
       <c r="A256">
-        <f>SUBSTITUTE("set profiles spyware Alert-Only-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B25)</f>
+        <f>SUBSTITUTE("set profiles spyware Alert-Only-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
         <v>0</v>
       </c>
     </row>
     <row r="257" spans="1:1">
       <c r="A257" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
     </row>
     <row r="258" spans="1:1">
       <c r="A258" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
     </row>
     <row r="259" spans="1:1">
       <c r="A259" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
     </row>
     <row r="260" spans="1:1">
       <c r="A260" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
     </row>
     <row r="261" spans="1:1">
       <c r="A261" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
     </row>
     <row r="262" spans="1:1">
       <c r="A262" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
     </row>
     <row r="263" spans="1:1">
       <c r="A263" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
     </row>
     <row r="264" spans="1:1">
       <c r="A264" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
     </row>
     <row r="265" spans="1:1">
       <c r="A265" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
     </row>
     <row r="266" spans="1:1">
       <c r="A266">
-        <f>SUBSTITUTE("set profiles spyware Exception-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B24)</f>
+        <f>SUBSTITUTE("set profiles spyware Exception-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
         <v>0</v>
       </c>
     </row>
     <row r="267" spans="1:1">
       <c r="A267">
-        <f>SUBSTITUTE("set profiles spyware Exception-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B25)</f>
+        <f>SUBSTITUTE("set profiles spyware Exception-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
         <v>0</v>
       </c>
     </row>
     <row r="268" spans="1:1">
       <c r="A268" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
     </row>
     <row r="269" spans="1:1">
       <c r="A269" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
     </row>
     <row r="270" spans="1:1">
       <c r="A270" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
     </row>
     <row r="271" spans="1:1">
       <c r="A271" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
     </row>
     <row r="273" spans="1:1">
       <c r="A273" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
     </row>
     <row r="274" spans="1:1">
       <c r="A274" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
     </row>
     <row r="275" spans="1:1">
       <c r="A275" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
     </row>
     <row r="276" spans="1:1">
       <c r="A276" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
     </row>
     <row r="277" spans="1:1">
       <c r="A277" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
     </row>
     <row r="278" spans="1:1">
       <c r="A278" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
     </row>
     <row r="279" spans="1:1">
       <c r="A279" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
     </row>
     <row r="280" spans="1:1">
       <c r="A280" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
     </row>
     <row r="281" spans="1:1">
       <c r="A281" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
     </row>
     <row r="282" spans="1:1">
       <c r="A282" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
     </row>
     <row r="283" spans="1:1">
       <c r="A283" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
     </row>
     <row r="284" spans="1:1">
       <c r="A284" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
     </row>
     <row r="285" spans="1:1">
       <c r="A285" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
     </row>
     <row r="286" spans="1:1">
       <c r="A286" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
     </row>
     <row r="287" spans="1:1">
       <c r="A287" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="288" spans="1:1">
       <c r="A288" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
     </row>
     <row r="289" spans="1:1">
       <c r="A289" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
     </row>
     <row r="290" spans="1:1">
       <c r="A290" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
     </row>
     <row r="291" spans="1:1">
       <c r="A291" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
     </row>
     <row r="292" spans="1:1">
       <c r="A292" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
     </row>
     <row r="293" spans="1:1">
       <c r="A293" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
     </row>
     <row r="294" spans="1:1">
       <c r="A294" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
     </row>
     <row r="295" spans="1:1">
       <c r="A295" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
     </row>
     <row r="296" spans="1:1">
       <c r="A296" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
     </row>
     <row r="298" spans="1:1">
       <c r="A298" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
     </row>
     <row r="299" spans="1:1">
       <c r="A299" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
     </row>
     <row r="300" spans="1:1">
       <c r="A300" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
     </row>
     <row r="301" spans="1:1">
       <c r="A301" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
     </row>
     <row r="302" spans="1:1">
       <c r="A302" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
     </row>
     <row r="303" spans="1:1">
       <c r="A303" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
     </row>
     <row r="304" spans="1:1">
       <c r="A304" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
     </row>
     <row r="305" spans="1:1">
       <c r="A305" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
     </row>
     <row r="306" spans="1:1">
       <c r="A306" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
     </row>
     <row r="307" spans="1:1">
       <c r="A307" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
     </row>
     <row r="308" spans="1:1">
       <c r="A308" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
     </row>
     <row r="309" spans="1:1">
       <c r="A309" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
     </row>
     <row r="310" spans="1:1">
       <c r="A310" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
     </row>
     <row r="311" spans="1:1">
       <c r="A311" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
     </row>
     <row r="312" spans="1:1">
       <c r="A312" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
     </row>
     <row r="313" spans="1:1">
       <c r="A313" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
     </row>
     <row r="314" spans="1:1">
       <c r="A314" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
     </row>
     <row r="315" spans="1:1">
       <c r="A315" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
     </row>
     <row r="316" spans="1:1">
       <c r="A316" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
     </row>
     <row r="317" spans="1:1">
       <c r="A317" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
     </row>
     <row r="318" spans="1:1">
       <c r="A318" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
     </row>
     <row r="319" spans="1:1">
       <c r="A319" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
     </row>
     <row r="320" spans="1:1">
       <c r="A320" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
     </row>
     <row r="321" spans="1:1">
       <c r="A321" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
     </row>
     <row r="322" spans="1:1">
       <c r="A322" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
     </row>
     <row r="323" spans="1:1">
       <c r="A323" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
     </row>
     <row r="324" spans="1:1">
       <c r="A324" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
     </row>
     <row r="325" spans="1:1">
       <c r="A325" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
     </row>
     <row r="326" spans="1:1">
       <c r="A326" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
     </row>
     <row r="327" spans="1:1">
       <c r="A327" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
     </row>
     <row r="328" spans="1:1">
       <c r="A328" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
     </row>
     <row r="329" spans="1:1">
       <c r="A329" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
     </row>
     <row r="330" spans="1:1">
       <c r="A330" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
     </row>
     <row r="331" spans="1:1">
       <c r="A331" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
     </row>
     <row r="332" spans="1:1">
       <c r="A332" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
     </row>
     <row r="333" spans="1:1">
       <c r="A333" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
     </row>
     <row r="334" spans="1:1">
       <c r="A334" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
     </row>
     <row r="335" spans="1:1">
       <c r="A335" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
     </row>
     <row r="336" spans="1:1">
       <c r="A336" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
     </row>
     <row r="337" spans="1:1">
       <c r="A337" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
     </row>
     <row r="338" spans="1:1">
       <c r="A338" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
     </row>
     <row r="339" spans="1:1">
       <c r="A339" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
     </row>
     <row r="340" spans="1:1">
       <c r="A340" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
     </row>
     <row r="341" spans="1:1">
       <c r="A341" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
     </row>
     <row r="342" spans="1:1">
       <c r="A342" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
     </row>
     <row r="343" spans="1:1">
       <c r="A343" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
     </row>
     <row r="344" spans="1:1">
       <c r="A344" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
     </row>
     <row r="345" spans="1:1">
       <c r="A345" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
     </row>
     <row r="346" spans="1:1">
       <c r="A346" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
     </row>
     <row r="347" spans="1:1">
       <c r="A347" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
     </row>
     <row r="348" spans="1:1">
       <c r="A348" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
     </row>
     <row r="349" spans="1:1">
       <c r="A349" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
     </row>
     <row r="350" spans="1:1">
       <c r="A350" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
     </row>
     <row r="351" spans="1:1">
       <c r="A351" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
     </row>
     <row r="352" spans="1:1">
       <c r="A352" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
     </row>
     <row r="353" spans="1:1">
       <c r="A353" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
     </row>
     <row r="354" spans="1:1">
       <c r="A354" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
     </row>
     <row r="355" spans="1:1">
       <c r="A355" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
     </row>
     <row r="356" spans="1:1">
       <c r="A356" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
     </row>
     <row r="357" spans="1:1">
       <c r="A357" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
     </row>
     <row r="358" spans="1:1">
       <c r="A358" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
     </row>
     <row r="359" spans="1:1">
       <c r="A359" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
     </row>
     <row r="360" spans="1:1">
       <c r="A360" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
     </row>
     <row r="361" spans="1:1">
       <c r="A361" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
     </row>
     <row r="362" spans="1:1">
       <c r="A362" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
     </row>
     <row r="363" spans="1:1">
       <c r="A363" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
     </row>
     <row r="364" spans="1:1">
       <c r="A364" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
     </row>
     <row r="365" spans="1:1">
       <c r="A365" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
     </row>
     <row r="366" spans="1:1">
       <c r="A366" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
     </row>
     <row r="367" spans="1:1">
       <c r="A367" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
     </row>
     <row r="368" spans="1:1">
       <c r="A368" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
     </row>
     <row r="369" spans="1:1">
       <c r="A369" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
     </row>
     <row r="371" spans="1:1">
       <c r="A371" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
     </row>
     <row r="372" spans="1:1">
       <c r="A372" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
     </row>
     <row r="373" spans="1:1">
       <c r="A373" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
     </row>
     <row r="374" spans="1:1">
       <c r="A374" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
     </row>
     <row r="375" spans="1:1">
       <c r="A375" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
     </row>
     <row r="376" spans="1:1">
       <c r="A376" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
     </row>
     <row r="377" spans="1:1">
       <c r="A377" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
     </row>
     <row r="378" spans="1:1">
       <c r="A378" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
     </row>
     <row r="379" spans="1:1">
       <c r="A379" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
     </row>
     <row r="380" spans="1:1">
       <c r="A380" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
     </row>
     <row r="381" spans="1:1">
       <c r="A381" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
     </row>
     <row r="382" spans="1:1">
       <c r="A382" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
     </row>
     <row r="383" spans="1:1">
       <c r="A383" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
     </row>
     <row r="384" spans="1:1">
       <c r="A384" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
     </row>
     <row r="385" spans="1:1">
       <c r="A385" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
     </row>
     <row r="386" spans="1:1">
       <c r="A386" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
     </row>
     <row r="387" spans="1:1">
       <c r="A387" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
     </row>
     <row r="388" spans="1:1">
       <c r="A388" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
     </row>
     <row r="389" spans="1:1">
       <c r="A389" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
     </row>
     <row r="390" spans="1:1">
       <c r="A390" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
     </row>
     <row r="391" spans="1:1">
       <c r="A391" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
     </row>
     <row r="392" spans="1:1">
       <c r="A392" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
     </row>
     <row r="393" spans="1:1">
       <c r="A393" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
     </row>
     <row r="394" spans="1:1">
       <c r="A394" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
     </row>
     <row r="395" spans="1:1">
       <c r="A395" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
     </row>
     <row r="396" spans="1:1">
       <c r="A396" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
     </row>
     <row r="397" spans="1:1">
       <c r="A397" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
     </row>
     <row r="398" spans="1:1">
       <c r="A398" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
     </row>
     <row r="399" spans="1:1">
       <c r="A399" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
     </row>
     <row r="400" spans="1:1">
       <c r="A400" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
     </row>
     <row r="401" spans="1:1">
       <c r="A401" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
     </row>
     <row r="402" spans="1:1">
       <c r="A402" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
     </row>
     <row r="403" spans="1:1">
       <c r="A403" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
     </row>
     <row r="404" spans="1:1">
       <c r="A404" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
     </row>
     <row r="405" spans="1:1">
       <c r="A405" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
     </row>
     <row r="406" spans="1:1">
       <c r="A406" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
     </row>
     <row r="407" spans="1:1">
       <c r="A407" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
     </row>
     <row r="408" spans="1:1">
       <c r="A408" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
     </row>
     <row r="409" spans="1:1">
       <c r="A409" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
     </row>
     <row r="410" spans="1:1">
       <c r="A410" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
     </row>
     <row r="411" spans="1:1">
       <c r="A411" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
     </row>
     <row r="412" spans="1:1">
       <c r="A412" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
     </row>
     <row r="413" spans="1:1">
       <c r="A413" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
     </row>
     <row r="414" spans="1:1">
       <c r="A414" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
     </row>
     <row r="415" spans="1:1">
       <c r="A415" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
     </row>
     <row r="416" spans="1:1">
       <c r="A416" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
     </row>
     <row r="417" spans="1:1">
       <c r="A417" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
     </row>
     <row r="418" spans="1:1">
       <c r="A418" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
     </row>
     <row r="419" spans="1:1">
       <c r="A419" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
     </row>
     <row r="420" spans="1:1">
       <c r="A420" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
     </row>
     <row r="421" spans="1:1">
       <c r="A421" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
     </row>
     <row r="422" spans="1:1">
       <c r="A422" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
     </row>
     <row r="423" spans="1:1">
       <c r="A423" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
     </row>
     <row r="424" spans="1:1">
       <c r="A424" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
     </row>
     <row r="425" spans="1:1">
       <c r="A425" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
     </row>
     <row r="426" spans="1:1">
       <c r="A426" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
     </row>
     <row r="427" spans="1:1">
       <c r="A427" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
     </row>
     <row r="428" spans="1:1">
       <c r="A428" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
     </row>
     <row r="430" spans="1:1">
       <c r="A430" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
     </row>
     <row r="431" spans="1:1">
       <c r="A431" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
     </row>
     <row r="432" spans="1:1">
       <c r="A432" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
     </row>
     <row r="433" spans="1:1">
       <c r="A433" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
     </row>
     <row r="434" spans="1:1">
       <c r="A434" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
     </row>
     <row r="435" spans="1:1">
       <c r="A435" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
     </row>
     <row r="436" spans="1:1">
       <c r="A436" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
     </row>
     <row r="437" spans="1:1">
       <c r="A437" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
     </row>
     <row r="438" spans="1:1">
       <c r="A438" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
     </row>
     <row r="439" spans="1:1">
       <c r="A439" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
     </row>
     <row r="440" spans="1:1">
       <c r="A440" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
     </row>
     <row r="441" spans="1:1">
       <c r="A441" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
     </row>
     <row r="442" spans="1:1">
       <c r="A442" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
     </row>
     <row r="443" spans="1:1">
       <c r="A443" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
     </row>
     <row r="444" spans="1:1">
       <c r="A444" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
     </row>
     <row r="445" spans="1:1">
       <c r="A445" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
     </row>
     <row r="446" spans="1:1">
       <c r="A446" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
     </row>
     <row r="448" spans="1:1">
       <c r="A448" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
     </row>
     <row r="449" spans="1:1">
       <c r="A449" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
     </row>
     <row r="450" spans="1:1">
       <c r="A450" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
     </row>
     <row r="451" spans="1:1">
       <c r="A451" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
     </row>
     <row r="452" spans="1:1">
       <c r="A452" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
     </row>
     <row r="453" spans="1:1">
       <c r="A453" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
     </row>
     <row r="454" spans="1:1">
       <c r="A454" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
     </row>
     <row r="455" spans="1:1">
       <c r="A455" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
     </row>
     <row r="456" spans="1:1">
       <c r="A456" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
     </row>
     <row r="457" spans="1:1">
       <c r="A457" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
     </row>
     <row r="458" spans="1:1">
       <c r="A458" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
     </row>
     <row r="459" spans="1:1">
       <c r="A459" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
     </row>
     <row r="460" spans="1:1">
       <c r="A460" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
     </row>
     <row r="461" spans="1:1">
       <c r="A461" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
     </row>
     <row r="462" spans="1:1">
       <c r="A462" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
     </row>
     <row r="463" spans="1:1">
       <c r="A463" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
     </row>
     <row r="464" spans="1:1">
       <c r="A464" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
     </row>
     <row r="465" spans="1:1">
       <c r="A465" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
     </row>
     <row r="466" spans="1:1">
       <c r="A466" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
     </row>
     <row r="467" spans="1:1">
       <c r="A467" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
     </row>
     <row r="468" spans="1:1">
       <c r="A468" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
     </row>
     <row r="469" spans="1:1">
       <c r="A469" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
     </row>
     <row r="470" spans="1:1">
       <c r="A470" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
     </row>
     <row r="471" spans="1:1">
       <c r="A471" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
     </row>
     <row r="472" spans="1:1">
       <c r="A472" t="s">
-        <v>516</v>
+        <v>511</v>
       </c>
     </row>
     <row r="473" spans="1:1">
       <c r="A473" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
     </row>
     <row r="474" spans="1:1">
       <c r="A474" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
     </row>
     <row r="475" spans="1:1">
       <c r="A475" t="s">
-        <v>519</v>
+        <v>514</v>
       </c>
     </row>
     <row r="476" spans="1:1">
       <c r="A476" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="478" spans="1:1">
       <c r="A478" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
     </row>
     <row r="479" spans="1:1">
       <c r="A479" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
     </row>
     <row r="480" spans="1:1">
       <c r="A480" t="s">
-        <v>523</v>
+        <v>518</v>
       </c>
     </row>
     <row r="481" spans="1:1">
       <c r="A481" t="s">
-        <v>524</v>
+        <v>519</v>
       </c>
     </row>
     <row r="482" spans="1:1">
       <c r="A482" t="s">
-        <v>525</v>
+        <v>520</v>
       </c>
     </row>
     <row r="483" spans="1:1">
       <c r="A483" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="484" spans="1:1">
       <c r="A484" t="s">
-        <v>527</v>
+        <v>522</v>
       </c>
     </row>
     <row r="485" spans="1:1">
       <c r="A485" t="s">
-        <v>528</v>
+        <v>523</v>
       </c>
     </row>
     <row r="486" spans="1:1">
       <c r="A486" t="s">
-        <v>529</v>
+        <v>524</v>
       </c>
     </row>
     <row r="487" spans="1:1">
       <c r="A487" t="s">
-        <v>530</v>
+        <v>525</v>
       </c>
     </row>
     <row r="488" spans="1:1">
       <c r="A488" t="s">
-        <v>531</v>
+        <v>526</v>
       </c>
     </row>
     <row r="489" spans="1:1">
       <c r="A489" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
     </row>
     <row r="490" spans="1:1">
       <c r="A490" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
     </row>
     <row r="491" spans="1:1">
       <c r="A491" t="s">
-        <v>534</v>
+        <v>529</v>
       </c>
     </row>
     <row r="492" spans="1:1">
       <c r="A492" t="s">
-        <v>535</v>
+        <v>530</v>
       </c>
     </row>
     <row r="493" spans="1:1">
       <c r="A493" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
     </row>
     <row r="494" spans="1:1">
       <c r="A494" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
     </row>
     <row r="495" spans="1:1">
       <c r="A495" t="s">
-        <v>538</v>
+        <v>533</v>
       </c>
     </row>
     <row r="496" spans="1:1">
       <c r="A496" t="s">
-        <v>539</v>
+        <v>534</v>
       </c>
     </row>
     <row r="497" spans="1:1">
       <c r="A497" t="s">
-        <v>540</v>
+        <v>535</v>
       </c>
     </row>
     <row r="498" spans="1:1">
       <c r="A498" t="s">
-        <v>541</v>
+        <v>536</v>
       </c>
     </row>
     <row r="499" spans="1:1">
       <c r="A499" t="s">
-        <v>542</v>
+        <v>537</v>
       </c>
     </row>
     <row r="500" spans="1:1">
       <c r="A500" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
     </row>
     <row r="501" spans="1:1">
       <c r="A501" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
     </row>
     <row r="502" spans="1:1">
       <c r="A502" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
     </row>
     <row r="503" spans="1:1">
       <c r="A503" t="s">
-        <v>546</v>
+        <v>541</v>
       </c>
     </row>
     <row r="504" spans="1:1">
       <c r="A504" t="s">
-        <v>547</v>
+        <v>542</v>
       </c>
     </row>
     <row r="505" spans="1:1">
       <c r="A505" t="s">
-        <v>548</v>
+        <v>543</v>
       </c>
     </row>
     <row r="506" spans="1:1">
       <c r="A506" t="s">
-        <v>549</v>
+        <v>544</v>
       </c>
     </row>
     <row r="507" spans="1:1">
       <c r="A507" t="s">
-        <v>550</v>
+        <v>545</v>
       </c>
     </row>
     <row r="508" spans="1:1">
       <c r="A508" t="s">
-        <v>551</v>
+        <v>546</v>
       </c>
     </row>
     <row r="509" spans="1:1">
       <c r="A509" t="s">
-        <v>552</v>
+        <v>547</v>
       </c>
     </row>
     <row r="510" spans="1:1">
       <c r="A510" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
     </row>
     <row r="511" spans="1:1">
       <c r="A511" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
     </row>
     <row r="512" spans="1:1">
       <c r="A512" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
     </row>
     <row r="513" spans="1:1">
       <c r="A513" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
     </row>
     <row r="514" spans="1:1">
       <c r="A514" t="s">
-        <v>557</v>
+        <v>552</v>
       </c>
     </row>
     <row r="515" spans="1:1">
       <c r="A515" t="s">
-        <v>558</v>
+        <v>553</v>
       </c>
     </row>
     <row r="516" spans="1:1">
       <c r="A516" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
     </row>
     <row r="517" spans="1:1">
       <c r="A517" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
     </row>
     <row r="518" spans="1:1">
       <c r="A518" t="s">
-        <v>561</v>
+        <v>556</v>
       </c>
     </row>
     <row r="519" spans="1:1">
       <c r="A519" t="s">
-        <v>562</v>
+        <v>557</v>
       </c>
     </row>
     <row r="520" spans="1:1">
       <c r="A520" t="s">
-        <v>563</v>
+        <v>558</v>
       </c>
     </row>
     <row r="521" spans="1:1">
       <c r="A521" t="s">
-        <v>564</v>
+        <v>559</v>
       </c>
     </row>
     <row r="522" spans="1:1">
       <c r="A522" t="s">
-        <v>565</v>
+        <v>560</v>
       </c>
     </row>
     <row r="523" spans="1:1">
       <c r="A523" t="s">
-        <v>566</v>
+        <v>561</v>
       </c>
     </row>
     <row r="524" spans="1:1">
       <c r="A524" t="s">
-        <v>567</v>
+        <v>562</v>
       </c>
     </row>
     <row r="525" spans="1:1">
       <c r="A525" t="s">
-        <v>568</v>
+        <v>563</v>
       </c>
     </row>
     <row r="526" spans="1:1">
       <c r="A526" t="s">
-        <v>569</v>
+        <v>564</v>
       </c>
     </row>
     <row r="528" spans="1:1">
       <c r="A528" t="s">
-        <v>570</v>
+        <v>565</v>
       </c>
     </row>
     <row r="529" spans="1:1">
       <c r="A529" t="s">
-        <v>571</v>
+        <v>566</v>
       </c>
     </row>
     <row r="530" spans="1:1">
       <c r="A530" t="s">
-        <v>572</v>
+        <v>567</v>
       </c>
     </row>
     <row r="531" spans="1:1">
       <c r="A531" t="s">
-        <v>573</v>
+        <v>568</v>
       </c>
     </row>
     <row r="532" spans="1:1">
       <c r="A532" t="s">
-        <v>574</v>
+        <v>569</v>
       </c>
     </row>
     <row r="533" spans="1:1">
       <c r="A533" t="s">
-        <v>575</v>
+        <v>570</v>
       </c>
     </row>
     <row r="534" spans="1:1">
       <c r="A534" t="s">
-        <v>576</v>
+        <v>571</v>
       </c>
     </row>
     <row r="535" spans="1:1">
       <c r="A535" t="s">
-        <v>577</v>
+        <v>572</v>
       </c>
     </row>
     <row r="536" spans="1:1">
       <c r="A536" t="s">
-        <v>578</v>
+        <v>573</v>
       </c>
     </row>
     <row r="537" spans="1:1">
       <c r="A537" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
     </row>
     <row r="538" spans="1:1">
       <c r="A538" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
     </row>
     <row r="539" spans="1:1">
       <c r="A539" t="s">
-        <v>581</v>
+        <v>576</v>
       </c>
     </row>
     <row r="540" spans="1:1">
       <c r="A540" t="s">
-        <v>582</v>
+        <v>577</v>
       </c>
     </row>
     <row r="541" spans="1:1">
       <c r="A541" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
     </row>
     <row r="542" spans="1:1">
       <c r="A542" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
     </row>
     <row r="543" spans="1:1">
       <c r="A543" t="s">
-        <v>585</v>
+        <v>580</v>
       </c>
     </row>
     <row r="544" spans="1:1">
       <c r="A544" t="s">
-        <v>586</v>
+        <v>581</v>
       </c>
     </row>
     <row r="545" spans="1:1">
       <c r="A545" t="s">
-        <v>587</v>
+        <v>582</v>
       </c>
     </row>
     <row r="547" spans="1:1">
       <c r="A547" t="s">
-        <v>588</v>
+        <v>583</v>
       </c>
     </row>
     <row r="548" spans="1:1">
       <c r="A548" t="s">
-        <v>589</v>
+        <v>584</v>
       </c>
     </row>
     <row r="549" spans="1:1">
       <c r="A549" t="s">
-        <v>590</v>
+        <v>585</v>
       </c>
     </row>
     <row r="550" spans="1:1">
       <c r="A550" t="s">
-        <v>591</v>
+        <v>586</v>
       </c>
     </row>
     <row r="551" spans="1:1">
       <c r="A551" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
     </row>
     <row r="552" spans="1:1">
       <c r="A552" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
     </row>
     <row r="553" spans="1:1">
       <c r="A553" t="s">
-        <v>594</v>
+        <v>589</v>
       </c>
     </row>
     <row r="554" spans="1:1">
       <c r="A554" t="s">
-        <v>595</v>
+        <v>590</v>
       </c>
     </row>
     <row r="555" spans="1:1">
       <c r="A555" t="s">
-        <v>596</v>
+        <v>591</v>
       </c>
     </row>
     <row r="556" spans="1:1">
       <c r="A556" t="s">
-        <v>597</v>
+        <v>592</v>
       </c>
     </row>
     <row r="557" spans="1:1">
       <c r="A557" t="s">
-        <v>598</v>
+        <v>593</v>
       </c>
     </row>
     <row r="558" spans="1:1">
       <c r="A558" t="s">
-        <v>599</v>
+        <v>594</v>
       </c>
     </row>
     <row r="559" spans="1:1">
       <c r="A559" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
     </row>
     <row r="560" spans="1:1">
       <c r="A560" t="s">
-        <v>601</v>
+        <v>596</v>
       </c>
     </row>
     <row r="561" spans="1:1">
       <c r="A561" t="s">
-        <v>602</v>
+        <v>597</v>
       </c>
     </row>
     <row r="562" spans="1:1">
       <c r="A562" t="s">
-        <v>603</v>
+        <v>598</v>
       </c>
     </row>
     <row r="563" spans="1:1">
       <c r="A563" t="s">
-        <v>604</v>
+        <v>599</v>
       </c>
     </row>
     <row r="564" spans="1:1">
       <c r="A564" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
     </row>
     <row r="565" spans="1:1">
       <c r="A565" t="s">
-        <v>606</v>
+        <v>601</v>
       </c>
     </row>
     <row r="566" spans="1:1">
       <c r="A566" t="s">
-        <v>607</v>
+        <v>602</v>
       </c>
     </row>
     <row r="567" spans="1:1">
       <c r="A567" t="s">
-        <v>608</v>
+        <v>603</v>
       </c>
     </row>
     <row r="568" spans="1:1">
       <c r="A568" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
     </row>
     <row r="569" spans="1:1">
       <c r="A569" t="s">
-        <v>610</v>
+        <v>605</v>
       </c>
     </row>
     <row r="570" spans="1:1">
       <c r="A570" t="s">
-        <v>611</v>
+        <v>606</v>
       </c>
     </row>
     <row r="572" spans="1:1">
       <c r="A572" t="s">
-        <v>612</v>
+        <v>607</v>
       </c>
     </row>
     <row r="573" spans="1:1">
       <c r="A573" t="s">
-        <v>613</v>
+        <v>608</v>
       </c>
     </row>
     <row r="574" spans="1:1">
       <c r="A574" t="s">
-        <v>614</v>
+        <v>609</v>
       </c>
     </row>
     <row r="575" spans="1:1">
       <c r="A575" t="s">
-        <v>615</v>
+        <v>610</v>
       </c>
     </row>
     <row r="576" spans="1:1">
       <c r="A576" t="s">
-        <v>616</v>
+        <v>611</v>
       </c>
     </row>
     <row r="577" spans="1:1">
       <c r="A577" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
     </row>
     <row r="578" spans="1:1">
       <c r="A578" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
     </row>
     <row r="579" spans="1:1">
       <c r="A579" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
     </row>
     <row r="580" spans="1:1">
       <c r="A580" t="s">
-        <v>620</v>
+        <v>615</v>
       </c>
     </row>
     <row r="581" spans="1:1">
       <c r="A581" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
     </row>
     <row r="582" spans="1:1">
       <c r="A582" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
     </row>
     <row r="583" spans="1:1">
       <c r="A583" t="s">
-        <v>623</v>
+        <v>618</v>
       </c>
     </row>
     <row r="584" spans="1:1">
       <c r="A584" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
     </row>
     <row r="585" spans="1:1">
       <c r="A585" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
     </row>
     <row r="586" spans="1:1">
       <c r="A586" t="s">
-        <v>626</v>
+        <v>621</v>
       </c>
     </row>
     <row r="588" spans="1:1">
       <c r="A588" t="s">
-        <v>627</v>
+        <v>622</v>
       </c>
     </row>
     <row r="589" spans="1:1">
       <c r="A589" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
     </row>
     <row r="590" spans="1:1">
       <c r="A590" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
     </row>
     <row r="591" spans="1:1">
       <c r="A591" t="s">
-        <v>630</v>
+        <v>625</v>
       </c>
     </row>
     <row r="592" spans="1:1">
       <c r="A592" t="s">
-        <v>631</v>
+        <v>626</v>
       </c>
     </row>
     <row r="593" spans="1:1">
       <c r="A593" t="s">
-        <v>632</v>
+        <v>627</v>
       </c>
     </row>
     <row r="594" spans="1:1">
       <c r="A594" t="s">
-        <v>633</v>
+        <v>628</v>
       </c>
     </row>
     <row r="595" spans="1:1">
       <c r="A595" t="s">
-        <v>634</v>
+        <v>629</v>
       </c>
     </row>
     <row r="596" spans="1:1">
       <c r="A596" t="s">
-        <v>635</v>
+        <v>630</v>
       </c>
     </row>
     <row r="597" spans="1:1">
       <c r="A597" t="s">
-        <v>636</v>
+        <v>631</v>
       </c>
     </row>
     <row r="598" spans="1:1">
       <c r="A598" t="s">
-        <v>637</v>
+        <v>632</v>
       </c>
     </row>
     <row r="599" spans="1:1">
       <c r="A599" t="s">
-        <v>638</v>
+        <v>633</v>
       </c>
     </row>
     <row r="600" spans="1:1">
       <c r="A600" t="s">
-        <v>639</v>
+        <v>634</v>
       </c>
     </row>
     <row r="601" spans="1:1">
       <c r="A601" t="s">
-        <v>640</v>
+        <v>635</v>
       </c>
     </row>
     <row r="602" spans="1:1">
       <c r="A602" t="s">
-        <v>641</v>
+        <v>636</v>
       </c>
     </row>
     <row r="603" spans="1:1">
       <c r="A603" t="s">
-        <v>642</v>
+        <v>637</v>
       </c>
     </row>
     <row r="604" spans="1:1">
       <c r="A604" t="s">
-        <v>643</v>
+        <v>638</v>
       </c>
     </row>
     <row r="605" spans="1:1">
       <c r="A605" t="s">
-        <v>644</v>
+        <v>639</v>
       </c>
     </row>
     <row r="606" spans="1:1">
       <c r="A606" t="s">
-        <v>645</v>
+        <v>640</v>
       </c>
     </row>
     <row r="607" spans="1:1">
       <c r="A607" t="s">
-        <v>646</v>
+        <v>641</v>
       </c>
     </row>
     <row r="608" spans="1:1">
       <c r="A608" t="s">
-        <v>647</v>
+        <v>642</v>
       </c>
     </row>
     <row r="609" spans="1:1">
       <c r="A609" t="s">
-        <v>648</v>
+        <v>643</v>
       </c>
     </row>
     <row r="610" spans="1:1">
       <c r="A610" t="s">
-        <v>649</v>
+        <v>644</v>
       </c>
     </row>
     <row r="611" spans="1:1">
       <c r="A611" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
     </row>
     <row r="612" spans="1:1">
       <c r="A612" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
     </row>
     <row r="613" spans="1:1">
       <c r="A613" t="s">
-        <v>652</v>
+        <v>647</v>
       </c>
     </row>
     <row r="614" spans="1:1">
       <c r="A614" t="s">
-        <v>653</v>
+        <v>648</v>
       </c>
     </row>
     <row r="615" spans="1:1">
       <c r="A615" t="s">
-        <v>654</v>
+        <v>649</v>
       </c>
     </row>
     <row r="616" spans="1:1">
       <c r="A616" t="s">
-        <v>655</v>
+        <v>650</v>
       </c>
     </row>
     <row r="617" spans="1:1">
       <c r="A617" t="s">
-        <v>656</v>
+        <v>651</v>
       </c>
     </row>
     <row r="618" spans="1:1">
       <c r="A618" t="s">
-        <v>657</v>
+        <v>652</v>
       </c>
     </row>
     <row r="619" spans="1:1">
       <c r="A619" t="s">
-        <v>658</v>
+        <v>653</v>
       </c>
     </row>
     <row r="620" spans="1:1">
       <c r="A620" t="s">
-        <v>659</v>
+        <v>654</v>
       </c>
     </row>
     <row r="621" spans="1:1">
       <c r="A621" t="s">
-        <v>660</v>
+        <v>655</v>
       </c>
     </row>
     <row r="622" spans="1:1">
       <c r="A622" t="s">
-        <v>661</v>
+        <v>656</v>
       </c>
     </row>
     <row r="623" spans="1:1">
       <c r="A623" t="s">
-        <v>662</v>
+        <v>657</v>
       </c>
     </row>
     <row r="624" spans="1:1">
       <c r="A624" t="s">
-        <v>663</v>
+        <v>658</v>
       </c>
     </row>
     <row r="625" spans="1:1">
       <c r="A625" t="s">
-        <v>664</v>
+        <v>659</v>
       </c>
     </row>
     <row r="626" spans="1:1">
       <c r="A626" t="s">
-        <v>665</v>
+        <v>660</v>
       </c>
     </row>
     <row r="627" spans="1:1">
       <c r="A627" t="s">
-        <v>666</v>
+        <v>661</v>
       </c>
     </row>
     <row r="628" spans="1:1">
       <c r="A628" t="s">
-        <v>667</v>
+        <v>662</v>
       </c>
     </row>
     <row r="629" spans="1:1">
       <c r="A629" t="s">
-        <v>668</v>
+        <v>663</v>
       </c>
     </row>
     <row r="630" spans="1:1">
       <c r="A630" t="s">
-        <v>669</v>
+        <v>664</v>
       </c>
     </row>
     <row r="631" spans="1:1">
       <c r="A631" t="s">
-        <v>670</v>
+        <v>665</v>
       </c>
     </row>
     <row r="632" spans="1:1">
       <c r="A632" t="s">
-        <v>671</v>
+        <v>666</v>
       </c>
     </row>
     <row r="633" spans="1:1">
       <c r="A633" t="s">
-        <v>672</v>
+        <v>667</v>
       </c>
     </row>
     <row r="634" spans="1:1">
       <c r="A634" t="s">
-        <v>673</v>
+        <v>668</v>
       </c>
     </row>
     <row r="635" spans="1:1">
       <c r="A635" t="s">
-        <v>674</v>
+        <v>669</v>
       </c>
     </row>
     <row r="636" spans="1:1">
       <c r="A636" t="s">
-        <v>675</v>
+        <v>670</v>
       </c>
     </row>
     <row r="637" spans="1:1">
       <c r="A637" t="s">
-        <v>676</v>
+        <v>671</v>
       </c>
     </row>
     <row r="638" spans="1:1">
       <c r="A638" t="s">
-        <v>677</v>
+        <v>672</v>
       </c>
     </row>
     <row r="639" spans="1:1">
       <c r="A639" t="s">
-        <v>678</v>
+        <v>673</v>
       </c>
     </row>
     <row r="640" spans="1:1">
       <c r="A640" t="s">
-        <v>679</v>
+        <v>674</v>
       </c>
     </row>
     <row r="641" spans="1:1">
       <c r="A641" t="s">
-        <v>680</v>
+        <v>675</v>
       </c>
     </row>
     <row r="642" spans="1:1">
       <c r="A642" t="s">
-        <v>681</v>
+        <v>676</v>
       </c>
     </row>
     <row r="643" spans="1:1">
       <c r="A643" t="s">
-        <v>682</v>
+        <v>677</v>
       </c>
     </row>
     <row r="644" spans="1:1">
       <c r="A644" t="s">
-        <v>683</v>
+        <v>678</v>
       </c>
     </row>
     <row r="645" spans="1:1">
       <c r="A645" t="s">
-        <v>684</v>
+        <v>679</v>
       </c>
     </row>
     <row r="646" spans="1:1">
       <c r="A646" t="s">
-        <v>685</v>
+        <v>680</v>
       </c>
     </row>
     <row r="647" spans="1:1">
       <c r="A647" t="s">
-        <v>686</v>
+        <v>681</v>
       </c>
     </row>
     <row r="648" spans="1:1">
       <c r="A648" t="s">
-        <v>687</v>
+        <v>682</v>
       </c>
     </row>
     <row r="649" spans="1:1">
       <c r="A649" t="s">
-        <v>688</v>
+        <v>683</v>
       </c>
     </row>
     <row r="650" spans="1:1">
       <c r="A650" t="s">
-        <v>689</v>
+        <v>684</v>
       </c>
     </row>
     <row r="651" spans="1:1">
       <c r="A651" t="s">
-        <v>690</v>
+        <v>685</v>
       </c>
     </row>
     <row r="652" spans="1:1">
       <c r="A652" t="s">
-        <v>691</v>
+        <v>686</v>
       </c>
     </row>
     <row r="653" spans="1:1">
       <c r="A653" t="s">
-        <v>692</v>
+        <v>687</v>
       </c>
     </row>
     <row r="654" spans="1:1">
       <c r="A654" t="s">
-        <v>693</v>
+        <v>688</v>
       </c>
     </row>
     <row r="655" spans="1:1">
       <c r="A655" t="s">
-        <v>694</v>
+        <v>689</v>
       </c>
     </row>
     <row r="656" spans="1:1">
       <c r="A656" t="s">
-        <v>695</v>
+        <v>690</v>
       </c>
     </row>
     <row r="657" spans="1:1">
       <c r="A657" t="s">
-        <v>696</v>
+        <v>691</v>
       </c>
     </row>
     <row r="658" spans="1:1">
       <c r="A658" t="s">
-        <v>697</v>
+        <v>692</v>
       </c>
     </row>
     <row r="660" spans="1:1">
       <c r="A660" t="s">
-        <v>698</v>
+        <v>693</v>
       </c>
     </row>
     <row r="661" spans="1:1">
       <c r="A661" t="s">
-        <v>699</v>
+        <v>694</v>
       </c>
     </row>
     <row r="662" spans="1:1">
       <c r="A662" t="s">
-        <v>700</v>
+        <v>695</v>
       </c>
     </row>
     <row r="663" spans="1:1">
       <c r="A663" t="s">
-        <v>701</v>
+        <v>696</v>
       </c>
     </row>
     <row r="664" spans="1:1">
       <c r="A664" t="s">
-        <v>702</v>
+        <v>697</v>
       </c>
     </row>
     <row r="665" spans="1:1">
       <c r="A665" t="s">
-        <v>703</v>
+        <v>698</v>
       </c>
     </row>
     <row r="666" spans="1:1">
       <c r="A666" t="s">
-        <v>704</v>
+        <v>699</v>
       </c>
     </row>
     <row r="667" spans="1:1">
       <c r="A667" t="s">
-        <v>705</v>
+        <v>700</v>
       </c>
     </row>
     <row r="668" spans="1:1">
       <c r="A668" t="s">
-        <v>706</v>
+        <v>701</v>
       </c>
     </row>
     <row r="669" spans="1:1">
       <c r="A669" t="s">
-        <v>707</v>
+        <v>702</v>
       </c>
     </row>
     <row r="671" spans="1:1">
       <c r="A671" t="s">
-        <v>708</v>
+        <v>703</v>
       </c>
     </row>
     <row r="672" spans="1:1">
       <c r="A672" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
     </row>
     <row r="673" spans="1:1">
       <c r="A673" t="s">
-        <v>710</v>
+        <v>705</v>
       </c>
     </row>
     <row r="674" spans="1:1">
       <c r="A674" t="s">
-        <v>711</v>
+        <v>706</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix missing url category info
</commit_message>
<xml_diff>
--- a/templates/panos/set_commands/iron_skillet_panos_full.xlsx
+++ b/templates/panos/set_commands/iron_skillet_panos_full.xlsx
@@ -980,13 +980,13 @@
     <t>set profiles url-filtering Alert-Only-URL credential-enforcement log-severity medium</t>
   </si>
   <si>
-    <t>set profiles url-filtering Alert-Only-URL credential-enforcement alert [ abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government hacking health-and-medicine home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal malware military motor-vehicles music news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting ]</t>
+    <t>set profiles url-filtering Alert-Only-URL credential-enforcement alert [ abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government hacking health-and-medicine home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal malware military motor-vehicles music news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting Black-List White-List ]</t>
   </si>
   <si>
     <t>set profiles url-filtering Alert-Only-URL action block</t>
   </si>
   <si>
-    <t>set profiles url-filtering Alert-Only-URL alert [ abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government hacking health-and-medicine home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal malware military motor-vehicles music news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting ]</t>
+    <t>set profiles url-filtering Alert-Only-URL alert [ abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government hacking health-and-medicine home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal malware military motor-vehicles music news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting Black-List White-List ]</t>
   </si>
   <si>
     <t>set profiles url-filtering Exception-URL credential-enforcement mode ip-user</t>
@@ -995,7 +995,7 @@
     <t>set profiles url-filtering Exception-URL credential-enforcement log-severity high</t>
   </si>
   <si>
-    <t>set profiles url-filtering Exception-URL credential-enforcement block [ abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government hacking health-and-medicine home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal malware military motor-vehicles music news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting Black-List ]</t>
+    <t>set profiles url-filtering Exception-URL credential-enforcement block [ abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government hacking health-and-medicine home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal malware military motor-vehicles music news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting Black-List White-List ]</t>
   </si>
   <si>
     <t>set profiles url-filtering Exception-URL log-http-hdr-user-agent yes</t>

</xml_diff>

<commit_message>
push new 91dev based on 90dev
</commit_message>
<xml_diff>
--- a/templates/panos/set_commands/iron_skillet_panos_full.xlsx
+++ b/templates/panos/set_commands/iron_skillet_panos_full.xlsx
@@ -278,7 +278,7 @@
     <t>include the predefined Palo Alto Networks external lists security rules</t>
   </si>
   <si>
-    <t># set command configuration for panos version 9.0</t>
+    <t># set command configuration for panos v9.1</t>
   </si>
   <si>
     <t># commands are expected to be loaded in order</t>
@@ -707,7 +707,7 @@
     <t>set tag Internal comments ""Internal to Internal""</t>
   </si>
   <si>
-    <t>set tag iron-skillet-version comments ""version 0.0.4 for 9.0: version of this IronSkillet template file""</t>
+    <t>set tag iron-skillet-version comments ""version 0.0.1 for 9.1: version of this IronSkillet template file""</t>
   </si>
   <si>
     <t>#Address objects used for sinkholing and security rules match</t>

</xml_diff>

<commit_message>
set commands for panorama
</commit_message>
<xml_diff>
--- a/templates/panos/set_commands/iron_skillet_panos_full.xlsx
+++ b/templates/panos/set_commands/iron_skillet_panos_full.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="793">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="759">
   <si>
     <t>Variable Name</t>
   </si>
@@ -26,117 +26,39 @@
     <t>Description</t>
   </si>
   <si>
-    <t>PANORAMA_NAME</t>
-  </si>
-  <si>
-    <t>panorama01</t>
-  </si>
-  <si>
-    <t>Panorama hostname</t>
-  </si>
-  <si>
-    <t>PANORAMA_TYPE</t>
-  </si>
-  <si>
-    <t>static</t>
-  </si>
-  <si>
-    <t>Panorama management IP type - static or cloud (for dhcp)</t>
-  </si>
-  <si>
-    <t>PANORAMA_IP</t>
-  </si>
-  <si>
-    <t>192.168.55.161</t>
-  </si>
-  <si>
-    <t>Panorama IP</t>
-  </si>
-  <si>
-    <t>PANORAMA_MASK</t>
+    <t>FW_NAME</t>
+  </si>
+  <si>
+    <t>panos-01</t>
+  </si>
+  <si>
+    <t>Firewall hostname</t>
+  </si>
+  <si>
+    <t>MGMT_TYPE</t>
+  </si>
+  <si>
+    <t>dhcp-client</t>
+  </si>
+  <si>
+    <t>firewall management IP type</t>
+  </si>
+  <si>
+    <t>MGMT_IP</t>
+  </si>
+  <si>
+    <t>192.0.2.6</t>
+  </si>
+  <si>
+    <t>NGFW management IP</t>
+  </si>
+  <si>
+    <t>MGMT_MASK</t>
   </si>
   <si>
     <t>255.255.255.0</t>
   </si>
   <si>
-    <t>Panorama netmask</t>
-  </si>
-  <si>
-    <t>PANORAMA_DG</t>
-  </si>
-  <si>
-    <t>192.168.55.2</t>
-  </si>
-  <si>
-    <t>Panorama default gateway</t>
-  </si>
-  <si>
-    <t>CONFIG_EXPORT_IP</t>
-  </si>
-  <si>
-    <t>192.0.2.3</t>
-  </si>
-  <si>
-    <t>IP address for scheduled config exports</t>
-  </si>
-  <si>
-    <t>TEMPLATE</t>
-  </si>
-  <si>
-    <t>sample_template</t>
-  </si>
-  <si>
-    <t>Template name for Panorama</t>
-  </si>
-  <si>
-    <t>STACK</t>
-  </si>
-  <si>
-    <t>sample_stack</t>
-  </si>
-  <si>
-    <t>Template stack name for Panorama</t>
-  </si>
-  <si>
-    <t>DEVICE_GROUP</t>
-  </si>
-  <si>
-    <t>sample_devicegroup</t>
-  </si>
-  <si>
-    <t>Device-group name for Panorama</t>
-  </si>
-  <si>
-    <t>FW_NAME</t>
-  </si>
-  <si>
-    <t>sample</t>
-  </si>
-  <si>
-    <t>Device Name for NGFW</t>
-  </si>
-  <si>
-    <t>MGMT_TYPE</t>
-  </si>
-  <si>
-    <t>firewall management IP type (static or dhcp-client)</t>
-  </si>
-  <si>
-    <t>MGMT_IP</t>
-  </si>
-  <si>
-    <t>192.0.2.6</t>
-  </si>
-  <si>
-    <t>NGFW management IP</t>
-  </si>
-  <si>
-    <t>MGMT_MASK</t>
-  </si>
-  <si>
-    <t>255.255.128.0</t>
-  </si>
-  <si>
     <t>NGFW management netmask</t>
   </si>
   <si>
@@ -155,7 +77,7 @@
     <t>0.pool.ntp.org</t>
   </si>
   <si>
-    <t>Network Time Protocol Server</t>
+    <t>primary NTP server</t>
   </si>
   <si>
     <t>NTP_2</t>
@@ -164,24 +86,18 @@
     <t>1.pool.ntp.org</t>
   </si>
   <si>
-    <t>Network Time Protocol Server 2</t>
+    <t>secondary NTP server</t>
   </si>
   <si>
     <t>ADMINISTRATOR_USERNAME</t>
   </si>
   <si>
-    <t>admin</t>
+    <t>adminuser</t>
   </si>
   <si>
     <t>admin username</t>
   </si>
   <si>
-    <t>ADMINISTRATOR_PASSWORD</t>
-  </si>
-  <si>
-    <t>admin password</t>
-  </si>
-  <si>
     <t>DNS_1</t>
   </si>
   <si>
@@ -206,7 +122,7 @@
     <t>sinkhole.paloaltonetworks.com</t>
   </si>
   <si>
-    <t>sinkhole address IPv4</t>
+    <t>sinkhole FQDN IPv4</t>
   </si>
   <si>
     <t>SINKHOLE_IPV6</t>
@@ -218,15 +134,6 @@
     <t>sinkhole address IPv6</t>
   </si>
   <si>
-    <t>INTERNET_ZONE</t>
-  </si>
-  <si>
-    <t>internet</t>
-  </si>
-  <si>
-    <t>untrust zone to filter out in reports</t>
-  </si>
-  <si>
     <t>EMAIL_PROFILE_GATEWAY</t>
   </si>
   <si>
@@ -267,15 +174,6 @@
   </si>
   <si>
     <t>lifetime for the api key in minutes</t>
-  </si>
-  <si>
-    <t>INCLUDE_PAN_EDL</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>include the predefined Palo Alto Networks external lists security rules</t>
   </si>
   <si>
     <t># set command configuration for panos v10.0</t>
@@ -2734,7 +2632,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2870,208 +2768,76 @@
         <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C15" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>50</v>
-      </c>
-      <c r="B18" t="s">
         <v>51</v>
+      </c>
+      <c r="B18">
+        <v>525600</v>
       </c>
       <c r="C18" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
-        <v>53</v>
-      </c>
-      <c r="B19" t="s">
-        <v>51</v>
-      </c>
-      <c r="C19" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="s">
-        <v>55</v>
-      </c>
-      <c r="B20" t="s">
-        <v>56</v>
-      </c>
-      <c r="C20" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" t="s">
-        <v>58</v>
-      </c>
-      <c r="B21" t="s">
-        <v>59</v>
-      </c>
-      <c r="C21" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" t="s">
-        <v>61</v>
-      </c>
-      <c r="B22" t="s">
-        <v>62</v>
-      </c>
-      <c r="C22" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" t="s">
-        <v>64</v>
-      </c>
-      <c r="B23" t="s">
-        <v>65</v>
-      </c>
-      <c r="C23" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" t="s">
-        <v>67</v>
-      </c>
-      <c r="B24" t="s">
-        <v>68</v>
-      </c>
-      <c r="C24" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" t="s">
-        <v>70</v>
-      </c>
-      <c r="B25" t="s">
-        <v>71</v>
-      </c>
-      <c r="C25" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" t="s">
-        <v>73</v>
-      </c>
-      <c r="B26" t="s">
-        <v>74</v>
-      </c>
-      <c r="C26" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" t="s">
-        <v>76</v>
-      </c>
-      <c r="B27" t="s">
-        <v>77</v>
-      </c>
-      <c r="C27" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" t="s">
-        <v>79</v>
-      </c>
-      <c r="B28" t="s">
-        <v>80</v>
-      </c>
-      <c r="C28" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" t="s">
-        <v>82</v>
-      </c>
-      <c r="B29">
-        <v>525600</v>
-      </c>
-      <c r="C29" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" t="s">
-        <v>84</v>
-      </c>
-      <c r="B30" t="s">
-        <v>85</v>
-      </c>
-      <c r="C30" t="s">
-        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -3089,3682 +2855,3682 @@
   <sheetData>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>88</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>89</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>90</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>91</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8">
-        <f>SUBSTITUTE("set deviceconfig system hostname {{ FW_NAME }}", "{{ FW_NAME }}", 'values'!B11)</f>
+        <f>SUBSTITUTE("set deviceconfig system hostname {{ FW_NAME }}", "{{ FW_NAME }}", 'values'!B2)</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9">
-        <f>SUBSTITUTE("set deviceconfig system ip-address {{ MGMT_IP }}", "{{ MGMT_IP }}", 'values'!B13)</f>
+        <f>SUBSTITUTE("set deviceconfig system ip-address {{ MGMT_IP }}", "{{ MGMT_IP }}", 'values'!B4)</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10">
-        <f>SUBSTITUTE("set deviceconfig system netmask {{ MGMT_MASK }}", "{{ MGMT_MASK }}", 'values'!B14)</f>
+        <f>SUBSTITUTE("set deviceconfig system netmask {{ MGMT_MASK }}", "{{ MGMT_MASK }}", 'values'!B5)</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11">
-        <f>SUBSTITUTE("set deviceconfig system default-gateway {{ MGMT_DG }}", "{{ MGMT_DG }}", 'values'!B15)</f>
+        <f>SUBSTITUTE("set deviceconfig system default-gateway {{ MGMT_DG }}", "{{ MGMT_DG }}", 'values'!B6)</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12">
-        <f>SUBSTITUTE("set deviceconfig system dns-setting servers primary {{ DNS_1 }}", "{{ DNS_1 }}", 'values'!B20)</f>
+        <f>SUBSTITUTE("set deviceconfig system dns-setting servers primary {{ DNS_1 }}", "{{ DNS_1 }}", 'values'!B10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13">
-        <f>SUBSTITUTE("set deviceconfig system dns-setting servers secondary {{ DNS_2 }}", "{{ DNS_2 }}", 'values'!B21)</f>
+        <f>SUBSTITUTE("set deviceconfig system dns-setting servers secondary {{ DNS_2 }}", "{{ DNS_2 }}", 'values'!B11)</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>92</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>93</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>94</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>95</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>96</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>97</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22">
-        <f>SUBSTITUTE("set deviceconfig system ntp-servers primary-ntp-server ntp-server-address {{ NTP_1 }}", "{{ NTP_1 }}", 'values'!B16)</f>
+        <f>SUBSTITUTE("set deviceconfig system ntp-servers primary-ntp-server ntp-server-address {{ NTP_1 }}", "{{ NTP_1 }}", 'values'!B7)</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23">
-        <f>SUBSTITUTE("set deviceconfig system ntp-servers secondary-ntp-server ntp-server-address {{ NTP_2 }}", "{{ NTP_2 }}", 'values'!B17)</f>
+        <f>SUBSTITUTE("set deviceconfig system ntp-servers secondary-ntp-server ntp-server-address {{ NTP_2 }}", "{{ NTP_2 }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>98</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26">
-        <f>SUBSTITUTE("set mgt-config users {{ ADMINISTRATOR_USERNAME }} password", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B18)</f>
+        <f>SUBSTITUTE("set mgt-config users {{ ADMINISTRATOR_USERNAME }} password", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27">
-        <f>SUBSTITUTE("set mgt-config users {{ ADMINISTRATOR_USERNAME }} permissions role-based superuser yes", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B18)</f>
+        <f>SUBSTITUTE("set mgt-config users {{ ADMINISTRATOR_USERNAME }} permissions role-based superuser yes", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>99</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>100</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>101</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>102</v>
+        <v>68</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>103</v>
+        <v>69</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>104</v>
+        <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>105</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>106</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>107</v>
+        <v>73</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>108</v>
+        <v>74</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" t="s">
-        <v>109</v>
+        <v>75</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" t="s">
-        <v>110</v>
+        <v>76</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>111</v>
+        <v>77</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>112</v>
+        <v>78</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" t="s">
-        <v>113</v>
+        <v>79</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" t="s">
-        <v>117</v>
+        <v>83</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" t="s">
-        <v>118</v>
+        <v>84</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" t="s">
-        <v>119</v>
+        <v>85</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" t="s">
-        <v>120</v>
+        <v>86</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" t="s">
-        <v>121</v>
+        <v>87</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" t="s">
-        <v>122</v>
+        <v>88</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" t="s">
-        <v>123</v>
+        <v>89</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" t="s">
-        <v>124</v>
+        <v>90</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" t="s">
-        <v>125</v>
+        <v>91</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" t="s">
-        <v>126</v>
+        <v>92</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" t="s">
-        <v>127</v>
+        <v>93</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60">
-        <f>SUBSTITUTE("set deviceconfig setting management api key lifetime {{ API_KEY_LIFETIME }}", "{{ API_KEY_LIFETIME }}", 'values'!B29)</f>
+        <f>SUBSTITUTE("set deviceconfig setting management api key lifetime {{ API_KEY_LIFETIME }}", "{{ API_KEY_LIFETIME }}", 'values'!B18)</f>
         <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" t="s">
-        <v>128</v>
+        <v>94</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" t="s">
-        <v>129</v>
+        <v>95</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" t="s">
-        <v>130</v>
+        <v>96</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64" t="s">
-        <v>131</v>
+        <v>97</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" t="s">
-        <v>132</v>
+        <v>98</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" t="s">
-        <v>133</v>
+        <v>99</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" t="s">
-        <v>134</v>
+        <v>100</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" t="s">
-        <v>135</v>
+        <v>101</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" t="s">
-        <v>136</v>
+        <v>102</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" t="s">
-        <v>137</v>
+        <v>103</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" t="s">
-        <v>138</v>
+        <v>104</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" t="s">
-        <v>139</v>
+        <v>105</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73" t="s">
-        <v>140</v>
+        <v>106</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74" t="s">
-        <v>141</v>
+        <v>107</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75" t="s">
-        <v>142</v>
+        <v>108</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" t="s">
-        <v>143</v>
+        <v>109</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77" t="s">
-        <v>144</v>
+        <v>110</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" t="s">
-        <v>145</v>
+        <v>111</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79" t="s">
-        <v>146</v>
+        <v>112</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80" t="s">
-        <v>147</v>
+        <v>113</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81" t="s">
-        <v>148</v>
+        <v>114</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" t="s">
-        <v>149</v>
+        <v>115</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83" t="s">
-        <v>150</v>
+        <v>116</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84" t="s">
-        <v>151</v>
+        <v>117</v>
       </c>
     </row>
     <row r="85" spans="1:1">
       <c r="A85" t="s">
-        <v>152</v>
+        <v>118</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86" t="s">
-        <v>153</v>
+        <v>119</v>
       </c>
     </row>
     <row r="89" spans="1:1">
       <c r="A89" t="s">
-        <v>154</v>
+        <v>120</v>
       </c>
     </row>
     <row r="90" spans="1:1">
       <c r="A90" t="s">
-        <v>155</v>
+        <v>121</v>
       </c>
     </row>
     <row r="91" spans="1:1">
       <c r="A91">
-        <f>SUBSTITUTE("set shared log-settings email Sample_Email_Profile server Sample_Email_Profile gateway {{ EMAIL_PROFILE_GATEWAY }}", "{{ EMAIL_PROFILE_GATEWAY }}", 'values'!B25)</f>
+        <f>SUBSTITUTE("set shared log-settings email Sample_Email_Profile server Sample_Email_Profile gateway {{ EMAIL_PROFILE_GATEWAY }}", "{{ EMAIL_PROFILE_GATEWAY }}", 'values'!B14)</f>
         <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:1">
       <c r="A92">
-        <f>SUBSTITUTE("set shared log-settings email Sample_Email_Profile server Sample_Email_Profile from {{ EMAIL_PROFILE_FROM }}", "{{ EMAIL_PROFILE_FROM }}", 'values'!B26)</f>
+        <f>SUBSTITUTE("set shared log-settings email Sample_Email_Profile server Sample_Email_Profile from {{ EMAIL_PROFILE_FROM }}", "{{ EMAIL_PROFILE_FROM }}", 'values'!B15)</f>
         <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93">
-        <f>SUBSTITUTE("set shared log-settings email Sample_Email_Profile server Sample_Email_Profile to {{ EMAIL_PROFILE_TO }}", "{{ EMAIL_PROFILE_TO }}", 'values'!B27)</f>
+        <f>SUBSTITUTE("set shared log-settings email Sample_Email_Profile server Sample_Email_Profile to {{ EMAIL_PROFILE_TO }}", "{{ EMAIL_PROFILE_TO }}", 'values'!B16)</f>
         <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:1">
       <c r="A94" t="s">
-        <v>156</v>
+        <v>122</v>
       </c>
     </row>
     <row r="95" spans="1:1">
       <c r="A95" t="s">
-        <v>157</v>
+        <v>123</v>
       </c>
     </row>
     <row r="96" spans="1:1">
       <c r="A96" t="s">
-        <v>158</v>
+        <v>124</v>
       </c>
     </row>
     <row r="97" spans="1:1">
       <c r="A97" t="s">
-        <v>159</v>
+        <v>125</v>
       </c>
     </row>
     <row r="98" spans="1:1">
       <c r="A98">
-        <f>SUBSTITUTE("set shared log-settings syslog Sample_Syslog_Profile server Sample_Syslog server {{ SYSLOG_SERVER }}", "{{ SYSLOG_SERVER }}", 'values'!B28)</f>
+        <f>SUBSTITUTE("set shared log-settings syslog Sample_Syslog_Profile server Sample_Syslog server {{ SYSLOG_SERVER }}", "{{ SYSLOG_SERVER }}", 'values'!B17)</f>
         <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99" t="s">
-        <v>160</v>
+        <v>126</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101" t="s">
-        <v>161</v>
+        <v>127</v>
       </c>
     </row>
     <row r="102" spans="1:1">
       <c r="A102" t="s">
-        <v>162</v>
+        <v>128</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103" t="s">
-        <v>163</v>
+        <v>129</v>
       </c>
     </row>
     <row r="104" spans="1:1">
       <c r="A104" t="s">
-        <v>164</v>
+        <v>130</v>
       </c>
     </row>
     <row r="105" spans="1:1">
       <c r="A105" t="s">
-        <v>165</v>
+        <v>131</v>
       </c>
     </row>
     <row r="106" spans="1:1">
       <c r="A106" t="s">
-        <v>166</v>
+        <v>132</v>
       </c>
     </row>
     <row r="107" spans="1:1">
       <c r="A107" t="s">
-        <v>167</v>
+        <v>133</v>
       </c>
     </row>
     <row r="108" spans="1:1">
       <c r="A108" t="s">
-        <v>168</v>
+        <v>134</v>
       </c>
     </row>
     <row r="109" spans="1:1">
       <c r="A109" t="s">
-        <v>169</v>
+        <v>135</v>
       </c>
     </row>
     <row r="110" spans="1:1">
       <c r="A110" t="s">
-        <v>170</v>
+        <v>136</v>
       </c>
     </row>
     <row r="111" spans="1:1">
       <c r="A111" t="s">
-        <v>171</v>
+        <v>137</v>
       </c>
     </row>
     <row r="112" spans="1:1">
       <c r="A112" t="s">
-        <v>172</v>
+        <v>138</v>
       </c>
     </row>
     <row r="113" spans="1:1">
       <c r="A113" t="s">
-        <v>173</v>
+        <v>139</v>
       </c>
     </row>
     <row r="114" spans="1:1">
       <c r="A114" t="s">
-        <v>174</v>
+        <v>140</v>
       </c>
     </row>
     <row r="115" spans="1:1">
       <c r="A115" t="s">
-        <v>175</v>
+        <v>141</v>
       </c>
     </row>
     <row r="116" spans="1:1">
       <c r="A116" t="s">
-        <v>176</v>
+        <v>142</v>
       </c>
     </row>
     <row r="117" spans="1:1">
       <c r="A117" t="s">
-        <v>177</v>
+        <v>143</v>
       </c>
     </row>
     <row r="118" spans="1:1">
       <c r="A118" t="s">
-        <v>178</v>
+        <v>144</v>
       </c>
     </row>
     <row r="121" spans="1:1">
       <c r="A121" t="s">
-        <v>179</v>
+        <v>145</v>
       </c>
     </row>
     <row r="122" spans="1:1">
       <c r="A122" t="s">
-        <v>180</v>
+        <v>146</v>
       </c>
     </row>
     <row r="123" spans="1:1">
       <c r="A123" t="s">
-        <v>181</v>
+        <v>147</v>
       </c>
     </row>
     <row r="124" spans="1:1">
       <c r="A124" t="s">
-        <v>182</v>
+        <v>148</v>
       </c>
     </row>
     <row r="125" spans="1:1">
       <c r="A125" t="s">
-        <v>183</v>
+        <v>149</v>
       </c>
     </row>
     <row r="126" spans="1:1">
       <c r="A126" t="s">
-        <v>184</v>
+        <v>150</v>
       </c>
     </row>
     <row r="127" spans="1:1">
       <c r="A127" t="s">
-        <v>185</v>
+        <v>151</v>
       </c>
     </row>
     <row r="128" spans="1:1">
       <c r="A128" t="s">
-        <v>186</v>
+        <v>152</v>
       </c>
     </row>
     <row r="129" spans="1:1">
       <c r="A129" t="s">
-        <v>187</v>
+        <v>153</v>
       </c>
     </row>
     <row r="130" spans="1:1">
       <c r="A130" t="s">
-        <v>188</v>
+        <v>154</v>
       </c>
     </row>
     <row r="131" spans="1:1">
       <c r="A131" t="s">
-        <v>189</v>
+        <v>155</v>
       </c>
     </row>
     <row r="132" spans="1:1">
       <c r="A132" t="s">
-        <v>190</v>
+        <v>156</v>
       </c>
     </row>
     <row r="133" spans="1:1">
       <c r="A133" t="s">
-        <v>191</v>
+        <v>157</v>
       </c>
     </row>
     <row r="134" spans="1:1">
       <c r="A134" t="s">
-        <v>192</v>
+        <v>158</v>
       </c>
     </row>
     <row r="135" spans="1:1">
       <c r="A135" t="s">
-        <v>193</v>
+        <v>159</v>
       </c>
     </row>
     <row r="136" spans="1:1">
       <c r="A136" t="s">
-        <v>194</v>
+        <v>160</v>
       </c>
     </row>
     <row r="137" spans="1:1">
       <c r="A137" t="s">
-        <v>195</v>
+        <v>161</v>
       </c>
     </row>
     <row r="138" spans="1:1">
       <c r="A138" t="s">
-        <v>196</v>
+        <v>162</v>
       </c>
     </row>
     <row r="139" spans="1:1">
       <c r="A139" t="s">
-        <v>197</v>
+        <v>163</v>
       </c>
     </row>
     <row r="140" spans="1:1">
       <c r="A140" t="s">
-        <v>198</v>
+        <v>164</v>
       </c>
     </row>
     <row r="141" spans="1:1">
       <c r="A141" t="s">
-        <v>199</v>
+        <v>165</v>
       </c>
     </row>
     <row r="142" spans="1:1">
       <c r="A142" t="s">
-        <v>200</v>
+        <v>166</v>
       </c>
     </row>
     <row r="143" spans="1:1">
       <c r="A143" t="s">
-        <v>201</v>
+        <v>167</v>
       </c>
     </row>
     <row r="144" spans="1:1">
       <c r="A144" t="s">
-        <v>202</v>
+        <v>168</v>
       </c>
     </row>
     <row r="145" spans="1:1">
       <c r="A145" t="s">
-        <v>203</v>
+        <v>169</v>
       </c>
     </row>
     <row r="146" spans="1:1">
       <c r="A146" t="s">
-        <v>204</v>
+        <v>170</v>
       </c>
     </row>
     <row r="147" spans="1:1">
       <c r="A147" t="s">
-        <v>205</v>
+        <v>171</v>
       </c>
     </row>
     <row r="148" spans="1:1">
       <c r="A148" t="s">
-        <v>206</v>
+        <v>172</v>
       </c>
     </row>
     <row r="149" spans="1:1">
       <c r="A149" t="s">
-        <v>207</v>
+        <v>173</v>
       </c>
     </row>
     <row r="150" spans="1:1">
       <c r="A150" t="s">
-        <v>208</v>
+        <v>174</v>
       </c>
     </row>
     <row r="151" spans="1:1">
       <c r="A151" t="s">
-        <v>209</v>
+        <v>175</v>
       </c>
     </row>
     <row r="152" spans="1:1">
       <c r="A152" t="s">
-        <v>210</v>
+        <v>176</v>
       </c>
     </row>
     <row r="153" spans="1:1">
       <c r="A153" t="s">
-        <v>211</v>
+        <v>177</v>
       </c>
     </row>
     <row r="154" spans="1:1">
       <c r="A154" t="s">
-        <v>212</v>
+        <v>178</v>
       </c>
     </row>
     <row r="156" spans="1:1">
       <c r="A156" t="s">
-        <v>213</v>
+        <v>179</v>
       </c>
     </row>
     <row r="157" spans="1:1">
       <c r="A157" t="s">
-        <v>214</v>
+        <v>180</v>
       </c>
     </row>
     <row r="158" spans="1:1">
       <c r="A158" t="s">
-        <v>215</v>
+        <v>181</v>
       </c>
     </row>
     <row r="159" spans="1:1">
       <c r="A159" t="s">
-        <v>216</v>
+        <v>182</v>
       </c>
     </row>
     <row r="160" spans="1:1">
       <c r="A160" t="s">
-        <v>217</v>
+        <v>183</v>
       </c>
     </row>
     <row r="162" spans="1:1">
       <c r="A162" t="s">
-        <v>218</v>
+        <v>184</v>
       </c>
     </row>
     <row r="163" spans="1:1">
       <c r="A163" t="s">
-        <v>219</v>
+        <v>185</v>
       </c>
     </row>
     <row r="164" spans="1:1">
       <c r="A164" t="s">
-        <v>220</v>
+        <v>186</v>
       </c>
     </row>
     <row r="165" spans="1:1">
       <c r="A165" t="s">
-        <v>221</v>
+        <v>187</v>
       </c>
     </row>
     <row r="166" spans="1:1">
       <c r="A166" t="s">
-        <v>222</v>
+        <v>188</v>
       </c>
     </row>
     <row r="167" spans="1:1">
       <c r="A167" t="s">
-        <v>223</v>
+        <v>189</v>
       </c>
     </row>
     <row r="168" spans="1:1">
       <c r="A168" t="s">
-        <v>224</v>
+        <v>190</v>
       </c>
     </row>
     <row r="169" spans="1:1">
       <c r="A169" t="s">
-        <v>225</v>
+        <v>191</v>
       </c>
     </row>
     <row r="170" spans="1:1">
       <c r="A170" t="s">
-        <v>226</v>
+        <v>192</v>
       </c>
     </row>
     <row r="171" spans="1:1">
       <c r="A171" t="s">
-        <v>227</v>
+        <v>193</v>
       </c>
     </row>
     <row r="172" spans="1:1">
       <c r="A172" t="s">
-        <v>228</v>
+        <v>194</v>
       </c>
     </row>
     <row r="173" spans="1:1">
       <c r="A173" t="s">
-        <v>229</v>
+        <v>195</v>
       </c>
     </row>
     <row r="174" spans="1:1">
       <c r="A174" t="s">
-        <v>230</v>
+        <v>196</v>
       </c>
     </row>
     <row r="175" spans="1:1">
       <c r="A175" t="s">
-        <v>231</v>
+        <v>197</v>
       </c>
     </row>
     <row r="176" spans="1:1">
       <c r="A176" t="s">
-        <v>232</v>
+        <v>198</v>
       </c>
     </row>
     <row r="177" spans="1:1">
       <c r="A177" t="s">
-        <v>233</v>
+        <v>199</v>
       </c>
     </row>
     <row r="178" spans="1:1">
       <c r="A178" t="s">
-        <v>234</v>
+        <v>200</v>
       </c>
     </row>
     <row r="179" spans="1:1">
       <c r="A179" t="s">
-        <v>235</v>
+        <v>201</v>
       </c>
     </row>
     <row r="180" spans="1:1">
       <c r="A180" t="s">
-        <v>236</v>
+        <v>202</v>
       </c>
     </row>
     <row r="181" spans="1:1">
       <c r="A181" t="s">
-        <v>237</v>
+        <v>203</v>
       </c>
     </row>
     <row r="182" spans="1:1">
       <c r="A182" t="s">
-        <v>238</v>
+        <v>204</v>
       </c>
     </row>
     <row r="183" spans="1:1">
       <c r="A183" t="s">
-        <v>239</v>
+        <v>205</v>
       </c>
     </row>
     <row r="184" spans="1:1">
       <c r="A184" t="s">
-        <v>240</v>
+        <v>206</v>
       </c>
     </row>
     <row r="185" spans="1:1">
       <c r="A185" t="s">
-        <v>241</v>
+        <v>207</v>
       </c>
     </row>
     <row r="186" spans="1:1">
       <c r="A186" t="s">
-        <v>242</v>
+        <v>208</v>
       </c>
     </row>
     <row r="187" spans="1:1">
       <c r="A187" t="s">
-        <v>243</v>
+        <v>209</v>
       </c>
     </row>
     <row r="188" spans="1:1">
       <c r="A188" t="s">
-        <v>244</v>
+        <v>210</v>
       </c>
     </row>
     <row r="189" spans="1:1">
       <c r="A189" t="s">
-        <v>245</v>
+        <v>211</v>
       </c>
     </row>
     <row r="190" spans="1:1">
       <c r="A190" t="s">
-        <v>246</v>
+        <v>212</v>
       </c>
     </row>
     <row r="192" spans="1:1">
       <c r="A192" t="s">
-        <v>247</v>
+        <v>213</v>
       </c>
     </row>
     <row r="193" spans="1:1">
       <c r="A193">
-        <f>SUBSTITUTE("set profiles spyware Outbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
+        <f>SUBSTITUTE("set profiles spyware Outbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B12)</f>
         <v>0</v>
       </c>
     </row>
     <row r="194" spans="1:1">
       <c r="A194">
-        <f>SUBSTITUTE("set profiles spyware Outbound-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
+        <f>SUBSTITUTE("set profiles spyware Outbound-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B13)</f>
         <v>0</v>
       </c>
     </row>
     <row r="195" spans="1:1">
       <c r="A195" t="s">
-        <v>248</v>
+        <v>214</v>
       </c>
     </row>
     <row r="196" spans="1:1">
       <c r="A196" t="s">
-        <v>249</v>
+        <v>215</v>
       </c>
     </row>
     <row r="197" spans="1:1">
       <c r="A197" t="s">
-        <v>250</v>
+        <v>216</v>
       </c>
     </row>
     <row r="198" spans="1:1">
       <c r="A198" t="s">
-        <v>251</v>
+        <v>217</v>
       </c>
     </row>
     <row r="199" spans="1:1">
       <c r="A199" t="s">
-        <v>252</v>
+        <v>218</v>
       </c>
     </row>
     <row r="200" spans="1:1">
       <c r="A200" t="s">
-        <v>253</v>
+        <v>219</v>
       </c>
     </row>
     <row r="201" spans="1:1">
       <c r="A201" t="s">
-        <v>254</v>
+        <v>220</v>
       </c>
     </row>
     <row r="202" spans="1:1">
       <c r="A202" t="s">
-        <v>255</v>
+        <v>221</v>
       </c>
     </row>
     <row r="203" spans="1:1">
       <c r="A203" t="s">
-        <v>256</v>
+        <v>222</v>
       </c>
     </row>
     <row r="204" spans="1:1">
       <c r="A204" t="s">
-        <v>257</v>
+        <v>223</v>
       </c>
     </row>
     <row r="205" spans="1:1">
       <c r="A205" t="s">
-        <v>258</v>
+        <v>224</v>
       </c>
     </row>
     <row r="206" spans="1:1">
       <c r="A206" t="s">
-        <v>259</v>
+        <v>225</v>
       </c>
     </row>
     <row r="207" spans="1:1">
       <c r="A207" t="s">
-        <v>260</v>
+        <v>226</v>
       </c>
     </row>
     <row r="208" spans="1:1">
       <c r="A208" t="s">
-        <v>261</v>
+        <v>227</v>
       </c>
     </row>
     <row r="209" spans="1:1">
       <c r="A209" t="s">
-        <v>262</v>
+        <v>228</v>
       </c>
     </row>
     <row r="210" spans="1:1">
       <c r="A210" t="s">
-        <v>263</v>
+        <v>229</v>
       </c>
     </row>
     <row r="211" spans="1:1">
       <c r="A211" t="s">
-        <v>264</v>
+        <v>230</v>
       </c>
     </row>
     <row r="212" spans="1:1">
       <c r="A212" t="s">
-        <v>265</v>
+        <v>231</v>
       </c>
     </row>
     <row r="213" spans="1:1">
       <c r="A213" t="s">
-        <v>266</v>
+        <v>232</v>
       </c>
     </row>
     <row r="214" spans="1:1">
       <c r="A214" t="s">
-        <v>267</v>
+        <v>233</v>
       </c>
     </row>
     <row r="215" spans="1:1">
       <c r="A215" t="s">
-        <v>268</v>
+        <v>234</v>
       </c>
     </row>
     <row r="216" spans="1:1">
       <c r="A216" t="s">
-        <v>269</v>
+        <v>235</v>
       </c>
     </row>
     <row r="217" spans="1:1">
       <c r="A217" t="s">
-        <v>270</v>
+        <v>236</v>
       </c>
     </row>
     <row r="218" spans="1:1">
       <c r="A218" t="s">
-        <v>271</v>
+        <v>237</v>
       </c>
     </row>
     <row r="219" spans="1:1">
       <c r="A219" t="s">
-        <v>272</v>
+        <v>238</v>
       </c>
     </row>
     <row r="220" spans="1:1">
       <c r="A220" t="s">
-        <v>273</v>
+        <v>239</v>
       </c>
     </row>
     <row r="221" spans="1:1">
       <c r="A221" t="s">
-        <v>274</v>
+        <v>240</v>
       </c>
     </row>
     <row r="222" spans="1:1">
       <c r="A222">
-        <f>SUBSTITUTE("set profiles spyware Inbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
+        <f>SUBSTITUTE("set profiles spyware Inbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B12)</f>
         <v>0</v>
       </c>
     </row>
     <row r="223" spans="1:1">
       <c r="A223">
-        <f>SUBSTITUTE("set profiles spyware Inbound-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
+        <f>SUBSTITUTE("set profiles spyware Inbound-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B13)</f>
         <v>0</v>
       </c>
     </row>
     <row r="224" spans="1:1">
       <c r="A224" t="s">
-        <v>275</v>
+        <v>241</v>
       </c>
     </row>
     <row r="225" spans="1:1">
       <c r="A225" t="s">
-        <v>276</v>
+        <v>242</v>
       </c>
     </row>
     <row r="226" spans="1:1">
       <c r="A226" t="s">
-        <v>277</v>
+        <v>243</v>
       </c>
     </row>
     <row r="227" spans="1:1">
       <c r="A227" t="s">
-        <v>278</v>
+        <v>244</v>
       </c>
     </row>
     <row r="228" spans="1:1">
       <c r="A228" t="s">
-        <v>279</v>
+        <v>245</v>
       </c>
     </row>
     <row r="229" spans="1:1">
       <c r="A229" t="s">
-        <v>280</v>
+        <v>246</v>
       </c>
     </row>
     <row r="230" spans="1:1">
       <c r="A230" t="s">
-        <v>281</v>
+        <v>247</v>
       </c>
     </row>
     <row r="231" spans="1:1">
       <c r="A231" t="s">
-        <v>282</v>
+        <v>248</v>
       </c>
     </row>
     <row r="232" spans="1:1">
       <c r="A232" t="s">
-        <v>283</v>
+        <v>249</v>
       </c>
     </row>
     <row r="233" spans="1:1">
       <c r="A233" t="s">
-        <v>284</v>
+        <v>250</v>
       </c>
     </row>
     <row r="234" spans="1:1">
       <c r="A234" t="s">
-        <v>285</v>
+        <v>251</v>
       </c>
     </row>
     <row r="235" spans="1:1">
       <c r="A235" t="s">
-        <v>286</v>
+        <v>252</v>
       </c>
     </row>
     <row r="236" spans="1:1">
       <c r="A236" t="s">
-        <v>287</v>
+        <v>253</v>
       </c>
     </row>
     <row r="237" spans="1:1">
       <c r="A237" t="s">
-        <v>288</v>
+        <v>254</v>
       </c>
     </row>
     <row r="238" spans="1:1">
       <c r="A238" t="s">
-        <v>289</v>
+        <v>255</v>
       </c>
     </row>
     <row r="239" spans="1:1">
       <c r="A239" t="s">
-        <v>290</v>
+        <v>256</v>
       </c>
     </row>
     <row r="240" spans="1:1">
       <c r="A240" t="s">
-        <v>291</v>
+        <v>257</v>
       </c>
     </row>
     <row r="241" spans="1:1">
       <c r="A241" t="s">
-        <v>292</v>
+        <v>258</v>
       </c>
     </row>
     <row r="242" spans="1:1">
       <c r="A242" t="s">
-        <v>293</v>
+        <v>259</v>
       </c>
     </row>
     <row r="243" spans="1:1">
       <c r="A243" t="s">
-        <v>294</v>
+        <v>260</v>
       </c>
     </row>
     <row r="244" spans="1:1">
       <c r="A244" t="s">
-        <v>295</v>
+        <v>261</v>
       </c>
     </row>
     <row r="245" spans="1:1">
       <c r="A245" t="s">
-        <v>296</v>
+        <v>262</v>
       </c>
     </row>
     <row r="246" spans="1:1">
       <c r="A246" t="s">
-        <v>297</v>
+        <v>263</v>
       </c>
     </row>
     <row r="247" spans="1:1">
       <c r="A247" t="s">
-        <v>298</v>
+        <v>264</v>
       </c>
     </row>
     <row r="248" spans="1:1">
       <c r="A248" t="s">
-        <v>299</v>
+        <v>265</v>
       </c>
     </row>
     <row r="249" spans="1:1">
       <c r="A249" t="s">
-        <v>300</v>
+        <v>266</v>
       </c>
     </row>
     <row r="250" spans="1:1">
       <c r="A250" t="s">
-        <v>301</v>
+        <v>267</v>
       </c>
     </row>
     <row r="251" spans="1:1">
       <c r="A251">
-        <f>SUBSTITUTE("set profiles spyware Internal-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
+        <f>SUBSTITUTE("set profiles spyware Internal-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B12)</f>
         <v>0</v>
       </c>
     </row>
     <row r="252" spans="1:1">
       <c r="A252">
-        <f>SUBSTITUTE("set profiles spyware Internal-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
+        <f>SUBSTITUTE("set profiles spyware Internal-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B13)</f>
         <v>0</v>
       </c>
     </row>
     <row r="253" spans="1:1">
       <c r="A253" t="s">
-        <v>302</v>
+        <v>268</v>
       </c>
     </row>
     <row r="254" spans="1:1">
       <c r="A254" t="s">
-        <v>303</v>
+        <v>269</v>
       </c>
     </row>
     <row r="255" spans="1:1">
       <c r="A255" t="s">
-        <v>304</v>
+        <v>270</v>
       </c>
     </row>
     <row r="256" spans="1:1">
       <c r="A256" t="s">
-        <v>305</v>
+        <v>271</v>
       </c>
     </row>
     <row r="257" spans="1:1">
       <c r="A257" t="s">
-        <v>306</v>
+        <v>272</v>
       </c>
     </row>
     <row r="258" spans="1:1">
       <c r="A258" t="s">
-        <v>307</v>
+        <v>273</v>
       </c>
     </row>
     <row r="259" spans="1:1">
       <c r="A259" t="s">
-        <v>308</v>
+        <v>274</v>
       </c>
     </row>
     <row r="260" spans="1:1">
       <c r="A260" t="s">
-        <v>309</v>
+        <v>275</v>
       </c>
     </row>
     <row r="261" spans="1:1">
       <c r="A261" t="s">
-        <v>310</v>
+        <v>276</v>
       </c>
     </row>
     <row r="262" spans="1:1">
       <c r="A262" t="s">
-        <v>311</v>
+        <v>277</v>
       </c>
     </row>
     <row r="263" spans="1:1">
       <c r="A263" t="s">
-        <v>312</v>
+        <v>278</v>
       </c>
     </row>
     <row r="264" spans="1:1">
       <c r="A264" t="s">
-        <v>313</v>
+        <v>279</v>
       </c>
     </row>
     <row r="265" spans="1:1">
       <c r="A265" t="s">
-        <v>314</v>
+        <v>280</v>
       </c>
     </row>
     <row r="266" spans="1:1">
       <c r="A266" t="s">
-        <v>315</v>
+        <v>281</v>
       </c>
     </row>
     <row r="267" spans="1:1">
       <c r="A267" t="s">
-        <v>316</v>
+        <v>282</v>
       </c>
     </row>
     <row r="268" spans="1:1">
       <c r="A268" t="s">
-        <v>317</v>
+        <v>283</v>
       </c>
     </row>
     <row r="269" spans="1:1">
       <c r="A269" t="s">
-        <v>318</v>
+        <v>284</v>
       </c>
     </row>
     <row r="270" spans="1:1">
       <c r="A270" t="s">
-        <v>319</v>
+        <v>285</v>
       </c>
     </row>
     <row r="271" spans="1:1">
       <c r="A271" t="s">
-        <v>320</v>
+        <v>286</v>
       </c>
     </row>
     <row r="272" spans="1:1">
       <c r="A272" t="s">
-        <v>321</v>
+        <v>287</v>
       </c>
     </row>
     <row r="273" spans="1:1">
       <c r="A273" t="s">
-        <v>322</v>
+        <v>288</v>
       </c>
     </row>
     <row r="274" spans="1:1">
       <c r="A274" t="s">
-        <v>323</v>
+        <v>289</v>
       </c>
     </row>
     <row r="275" spans="1:1">
       <c r="A275" t="s">
-        <v>324</v>
+        <v>290</v>
       </c>
     </row>
     <row r="276" spans="1:1">
       <c r="A276" t="s">
-        <v>325</v>
+        <v>291</v>
       </c>
     </row>
     <row r="277" spans="1:1">
       <c r="A277" t="s">
-        <v>326</v>
+        <v>292</v>
       </c>
     </row>
     <row r="278" spans="1:1">
       <c r="A278" t="s">
-        <v>327</v>
+        <v>293</v>
       </c>
     </row>
     <row r="279" spans="1:1">
       <c r="A279" t="s">
-        <v>328</v>
+        <v>294</v>
       </c>
     </row>
     <row r="280" spans="1:1">
       <c r="A280">
-        <f>SUBSTITUTE("set profiles spyware Alert-Only-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
+        <f>SUBSTITUTE("set profiles spyware Alert-Only-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B12)</f>
         <v>0</v>
       </c>
     </row>
     <row r="281" spans="1:1">
       <c r="A281">
-        <f>SUBSTITUTE("set profiles spyware Alert-Only-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
+        <f>SUBSTITUTE("set profiles spyware Alert-Only-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B13)</f>
         <v>0</v>
       </c>
     </row>
     <row r="282" spans="1:1">
       <c r="A282" t="s">
-        <v>329</v>
+        <v>295</v>
       </c>
     </row>
     <row r="283" spans="1:1">
       <c r="A283" t="s">
-        <v>330</v>
+        <v>296</v>
       </c>
     </row>
     <row r="284" spans="1:1">
       <c r="A284" t="s">
-        <v>331</v>
+        <v>297</v>
       </c>
     </row>
     <row r="285" spans="1:1">
       <c r="A285" t="s">
-        <v>332</v>
+        <v>298</v>
       </c>
     </row>
     <row r="286" spans="1:1">
       <c r="A286" t="s">
-        <v>333</v>
+        <v>299</v>
       </c>
     </row>
     <row r="287" spans="1:1">
       <c r="A287" t="s">
-        <v>334</v>
+        <v>300</v>
       </c>
     </row>
     <row r="288" spans="1:1">
       <c r="A288" t="s">
-        <v>335</v>
+        <v>301</v>
       </c>
     </row>
     <row r="289" spans="1:1">
       <c r="A289" t="s">
-        <v>336</v>
+        <v>302</v>
       </c>
     </row>
     <row r="290" spans="1:1">
       <c r="A290" t="s">
-        <v>337</v>
+        <v>303</v>
       </c>
     </row>
     <row r="291" spans="1:1">
       <c r="A291" t="s">
-        <v>338</v>
+        <v>304</v>
       </c>
     </row>
     <row r="292" spans="1:1">
       <c r="A292" t="s">
-        <v>339</v>
+        <v>305</v>
       </c>
     </row>
     <row r="293" spans="1:1">
       <c r="A293" t="s">
-        <v>340</v>
+        <v>306</v>
       </c>
     </row>
     <row r="294" spans="1:1">
       <c r="A294" t="s">
-        <v>341</v>
+        <v>307</v>
       </c>
     </row>
     <row r="295" spans="1:1">
       <c r="A295" t="s">
-        <v>342</v>
+        <v>308</v>
       </c>
     </row>
     <row r="296" spans="1:1">
       <c r="A296" t="s">
-        <v>343</v>
+        <v>309</v>
       </c>
     </row>
     <row r="297" spans="1:1">
       <c r="A297" t="s">
-        <v>344</v>
+        <v>310</v>
       </c>
     </row>
     <row r="298" spans="1:1">
       <c r="A298" t="s">
-        <v>345</v>
+        <v>311</v>
       </c>
     </row>
     <row r="299" spans="1:1">
       <c r="A299" t="s">
-        <v>346</v>
+        <v>312</v>
       </c>
     </row>
     <row r="300" spans="1:1">
       <c r="A300" t="s">
-        <v>347</v>
+        <v>313</v>
       </c>
     </row>
     <row r="301" spans="1:1">
       <c r="A301" t="s">
-        <v>348</v>
+        <v>314</v>
       </c>
     </row>
     <row r="302" spans="1:1">
       <c r="A302" t="s">
-        <v>349</v>
+        <v>315</v>
       </c>
     </row>
     <row r="303" spans="1:1">
       <c r="A303" t="s">
-        <v>350</v>
+        <v>316</v>
       </c>
     </row>
     <row r="304" spans="1:1">
       <c r="A304" t="s">
-        <v>351</v>
+        <v>317</v>
       </c>
     </row>
     <row r="305" spans="1:1">
       <c r="A305">
-        <f>SUBSTITUTE("set profiles spyware Exception-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
+        <f>SUBSTITUTE("set profiles spyware Exception-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B12)</f>
         <v>0</v>
       </c>
     </row>
     <row r="306" spans="1:1">
       <c r="A306">
-        <f>SUBSTITUTE("set profiles spyware Exception-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
+        <f>SUBSTITUTE("set profiles spyware Exception-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B13)</f>
         <v>0</v>
       </c>
     </row>
     <row r="307" spans="1:1">
       <c r="A307" t="s">
-        <v>352</v>
+        <v>318</v>
       </c>
     </row>
     <row r="308" spans="1:1">
       <c r="A308" t="s">
-        <v>353</v>
+        <v>319</v>
       </c>
     </row>
     <row r="309" spans="1:1">
       <c r="A309" t="s">
-        <v>354</v>
+        <v>320</v>
       </c>
     </row>
     <row r="310" spans="1:1">
       <c r="A310" t="s">
-        <v>355</v>
+        <v>321</v>
       </c>
     </row>
     <row r="311" spans="1:1">
       <c r="A311" t="s">
-        <v>356</v>
+        <v>322</v>
       </c>
     </row>
     <row r="312" spans="1:1">
       <c r="A312" t="s">
-        <v>357</v>
+        <v>323</v>
       </c>
     </row>
     <row r="313" spans="1:1">
       <c r="A313" t="s">
-        <v>358</v>
+        <v>324</v>
       </c>
     </row>
     <row r="314" spans="1:1">
       <c r="A314" t="s">
-        <v>359</v>
+        <v>325</v>
       </c>
     </row>
     <row r="315" spans="1:1">
       <c r="A315" t="s">
-        <v>360</v>
+        <v>326</v>
       </c>
     </row>
     <row r="316" spans="1:1">
       <c r="A316" t="s">
-        <v>361</v>
+        <v>327</v>
       </c>
     </row>
     <row r="317" spans="1:1">
       <c r="A317" t="s">
-        <v>362</v>
+        <v>328</v>
       </c>
     </row>
     <row r="318" spans="1:1">
       <c r="A318" t="s">
-        <v>363</v>
+        <v>329</v>
       </c>
     </row>
     <row r="319" spans="1:1">
       <c r="A319" t="s">
-        <v>364</v>
+        <v>330</v>
       </c>
     </row>
     <row r="320" spans="1:1">
       <c r="A320" t="s">
-        <v>365</v>
+        <v>331</v>
       </c>
     </row>
     <row r="321" spans="1:1">
       <c r="A321" t="s">
-        <v>366</v>
+        <v>332</v>
       </c>
     </row>
     <row r="322" spans="1:1">
       <c r="A322" t="s">
-        <v>367</v>
+        <v>333</v>
       </c>
     </row>
     <row r="323" spans="1:1">
       <c r="A323" t="s">
-        <v>368</v>
+        <v>334</v>
       </c>
     </row>
     <row r="325" spans="1:1">
       <c r="A325" t="s">
-        <v>369</v>
+        <v>335</v>
       </c>
     </row>
     <row r="326" spans="1:1">
       <c r="A326" t="s">
-        <v>370</v>
+        <v>336</v>
       </c>
     </row>
     <row r="327" spans="1:1">
       <c r="A327" t="s">
-        <v>371</v>
+        <v>337</v>
       </c>
     </row>
     <row r="328" spans="1:1">
       <c r="A328" t="s">
-        <v>372</v>
+        <v>338</v>
       </c>
     </row>
     <row r="329" spans="1:1">
       <c r="A329" t="s">
-        <v>373</v>
+        <v>339</v>
       </c>
     </row>
     <row r="330" spans="1:1">
       <c r="A330" t="s">
-        <v>374</v>
+        <v>340</v>
       </c>
     </row>
     <row r="331" spans="1:1">
       <c r="A331" t="s">
-        <v>375</v>
+        <v>341</v>
       </c>
     </row>
     <row r="332" spans="1:1">
       <c r="A332" t="s">
-        <v>376</v>
+        <v>342</v>
       </c>
     </row>
     <row r="333" spans="1:1">
       <c r="A333" t="s">
-        <v>377</v>
+        <v>343</v>
       </c>
     </row>
     <row r="334" spans="1:1">
       <c r="A334" t="s">
-        <v>378</v>
+        <v>344</v>
       </c>
     </row>
     <row r="335" spans="1:1">
       <c r="A335" t="s">
-        <v>379</v>
+        <v>345</v>
       </c>
     </row>
     <row r="336" spans="1:1">
       <c r="A336" t="s">
-        <v>380</v>
+        <v>346</v>
       </c>
     </row>
     <row r="337" spans="1:1">
       <c r="A337" t="s">
-        <v>381</v>
+        <v>347</v>
       </c>
     </row>
     <row r="338" spans="1:1">
       <c r="A338" t="s">
-        <v>382</v>
+        <v>348</v>
       </c>
     </row>
     <row r="339" spans="1:1">
       <c r="A339" t="s">
-        <v>383</v>
+        <v>349</v>
       </c>
     </row>
     <row r="340" spans="1:1">
       <c r="A340" t="s">
-        <v>384</v>
+        <v>350</v>
       </c>
     </row>
     <row r="341" spans="1:1">
       <c r="A341" t="s">
-        <v>385</v>
+        <v>351</v>
       </c>
     </row>
     <row r="342" spans="1:1">
       <c r="A342" t="s">
-        <v>386</v>
+        <v>352</v>
       </c>
     </row>
     <row r="343" spans="1:1">
       <c r="A343" t="s">
-        <v>387</v>
+        <v>353</v>
       </c>
     </row>
     <row r="344" spans="1:1">
       <c r="A344" t="s">
-        <v>388</v>
+        <v>354</v>
       </c>
     </row>
     <row r="345" spans="1:1">
       <c r="A345" t="s">
-        <v>389</v>
+        <v>355</v>
       </c>
     </row>
     <row r="346" spans="1:1">
       <c r="A346" t="s">
-        <v>390</v>
+        <v>356</v>
       </c>
     </row>
     <row r="347" spans="1:1">
       <c r="A347" t="s">
-        <v>391</v>
+        <v>357</v>
       </c>
     </row>
     <row r="348" spans="1:1">
       <c r="A348" t="s">
-        <v>392</v>
+        <v>358</v>
       </c>
     </row>
     <row r="349" spans="1:1">
       <c r="A349" t="s">
-        <v>393</v>
+        <v>359</v>
       </c>
     </row>
     <row r="350" spans="1:1">
       <c r="A350" t="s">
-        <v>394</v>
+        <v>360</v>
       </c>
     </row>
     <row r="351" spans="1:1">
       <c r="A351" t="s">
-        <v>395</v>
+        <v>361</v>
       </c>
     </row>
     <row r="352" spans="1:1">
       <c r="A352" t="s">
-        <v>396</v>
+        <v>362</v>
       </c>
     </row>
     <row r="353" spans="1:1">
       <c r="A353" t="s">
-        <v>397</v>
+        <v>363</v>
       </c>
     </row>
     <row r="354" spans="1:1">
       <c r="A354" t="s">
-        <v>398</v>
+        <v>364</v>
       </c>
     </row>
     <row r="356" spans="1:1">
       <c r="A356" t="s">
-        <v>399</v>
+        <v>365</v>
       </c>
     </row>
     <row r="357" spans="1:1">
       <c r="A357" t="s">
-        <v>400</v>
+        <v>366</v>
       </c>
     </row>
     <row r="358" spans="1:1">
       <c r="A358" t="s">
-        <v>401</v>
+        <v>367</v>
       </c>
     </row>
     <row r="359" spans="1:1">
       <c r="A359" t="s">
-        <v>402</v>
+        <v>368</v>
       </c>
     </row>
     <row r="360" spans="1:1">
       <c r="A360" t="s">
-        <v>403</v>
+        <v>369</v>
       </c>
     </row>
     <row r="361" spans="1:1">
       <c r="A361" t="s">
-        <v>404</v>
+        <v>370</v>
       </c>
     </row>
     <row r="362" spans="1:1">
       <c r="A362" t="s">
-        <v>405</v>
+        <v>371</v>
       </c>
     </row>
     <row r="363" spans="1:1">
       <c r="A363" t="s">
-        <v>406</v>
+        <v>372</v>
       </c>
     </row>
     <row r="364" spans="1:1">
       <c r="A364" t="s">
-        <v>407</v>
+        <v>373</v>
       </c>
     </row>
     <row r="365" spans="1:1">
       <c r="A365" t="s">
-        <v>408</v>
+        <v>374</v>
       </c>
     </row>
     <row r="366" spans="1:1">
       <c r="A366" t="s">
-        <v>409</v>
+        <v>375</v>
       </c>
     </row>
     <row r="367" spans="1:1">
       <c r="A367" t="s">
-        <v>410</v>
+        <v>376</v>
       </c>
     </row>
     <row r="368" spans="1:1">
       <c r="A368" t="s">
-        <v>411</v>
+        <v>377</v>
       </c>
     </row>
     <row r="369" spans="1:1">
       <c r="A369" t="s">
-        <v>412</v>
+        <v>378</v>
       </c>
     </row>
     <row r="370" spans="1:1">
       <c r="A370" t="s">
-        <v>413</v>
+        <v>379</v>
       </c>
     </row>
     <row r="371" spans="1:1">
       <c r="A371" t="s">
-        <v>414</v>
+        <v>380</v>
       </c>
     </row>
     <row r="372" spans="1:1">
       <c r="A372" t="s">
-        <v>415</v>
+        <v>381</v>
       </c>
     </row>
     <row r="373" spans="1:1">
       <c r="A373" t="s">
-        <v>416</v>
+        <v>382</v>
       </c>
     </row>
     <row r="374" spans="1:1">
       <c r="A374" t="s">
-        <v>417</v>
+        <v>383</v>
       </c>
     </row>
     <row r="375" spans="1:1">
       <c r="A375" t="s">
-        <v>418</v>
+        <v>384</v>
       </c>
     </row>
     <row r="376" spans="1:1">
       <c r="A376" t="s">
-        <v>419</v>
+        <v>385</v>
       </c>
     </row>
     <row r="377" spans="1:1">
       <c r="A377" t="s">
-        <v>420</v>
+        <v>386</v>
       </c>
     </row>
     <row r="378" spans="1:1">
       <c r="A378" t="s">
-        <v>421</v>
+        <v>387</v>
       </c>
     </row>
     <row r="379" spans="1:1">
       <c r="A379" t="s">
-        <v>422</v>
+        <v>388</v>
       </c>
     </row>
     <row r="380" spans="1:1">
       <c r="A380" t="s">
-        <v>423</v>
+        <v>389</v>
       </c>
     </row>
     <row r="381" spans="1:1">
       <c r="A381" t="s">
-        <v>424</v>
+        <v>390</v>
       </c>
     </row>
     <row r="382" spans="1:1">
       <c r="A382" t="s">
-        <v>425</v>
+        <v>391</v>
       </c>
     </row>
     <row r="383" spans="1:1">
       <c r="A383" t="s">
-        <v>426</v>
+        <v>392</v>
       </c>
     </row>
     <row r="384" spans="1:1">
       <c r="A384" t="s">
-        <v>427</v>
+        <v>393</v>
       </c>
     </row>
     <row r="385" spans="1:1">
       <c r="A385" t="s">
-        <v>428</v>
+        <v>394</v>
       </c>
     </row>
     <row r="386" spans="1:1">
       <c r="A386" t="s">
-        <v>429</v>
+        <v>395</v>
       </c>
     </row>
     <row r="387" spans="1:1">
       <c r="A387" t="s">
-        <v>430</v>
+        <v>396</v>
       </c>
     </row>
     <row r="388" spans="1:1">
       <c r="A388" t="s">
-        <v>431</v>
+        <v>397</v>
       </c>
     </row>
     <row r="389" spans="1:1">
       <c r="A389" t="s">
-        <v>432</v>
+        <v>398</v>
       </c>
     </row>
     <row r="390" spans="1:1">
       <c r="A390" t="s">
-        <v>433</v>
+        <v>399</v>
       </c>
     </row>
     <row r="391" spans="1:1">
       <c r="A391" t="s">
-        <v>434</v>
+        <v>400</v>
       </c>
     </row>
     <row r="392" spans="1:1">
       <c r="A392" t="s">
-        <v>435</v>
+        <v>401</v>
       </c>
     </row>
     <row r="393" spans="1:1">
       <c r="A393" t="s">
-        <v>436</v>
+        <v>402</v>
       </c>
     </row>
     <row r="394" spans="1:1">
       <c r="A394" t="s">
-        <v>437</v>
+        <v>403</v>
       </c>
     </row>
     <row r="395" spans="1:1">
       <c r="A395" t="s">
-        <v>438</v>
+        <v>404</v>
       </c>
     </row>
     <row r="396" spans="1:1">
       <c r="A396" t="s">
-        <v>439</v>
+        <v>405</v>
       </c>
     </row>
     <row r="397" spans="1:1">
       <c r="A397" t="s">
-        <v>440</v>
+        <v>406</v>
       </c>
     </row>
     <row r="398" spans="1:1">
       <c r="A398" t="s">
-        <v>441</v>
+        <v>407</v>
       </c>
     </row>
     <row r="399" spans="1:1">
       <c r="A399" t="s">
-        <v>442</v>
+        <v>408</v>
       </c>
     </row>
     <row r="400" spans="1:1">
       <c r="A400" t="s">
-        <v>443</v>
+        <v>409</v>
       </c>
     </row>
     <row r="401" spans="1:1">
       <c r="A401" t="s">
-        <v>444</v>
+        <v>410</v>
       </c>
     </row>
     <row r="402" spans="1:1">
       <c r="A402" t="s">
-        <v>445</v>
+        <v>411</v>
       </c>
     </row>
     <row r="403" spans="1:1">
       <c r="A403" t="s">
-        <v>446</v>
+        <v>412</v>
       </c>
     </row>
     <row r="404" spans="1:1">
       <c r="A404" t="s">
-        <v>447</v>
+        <v>413</v>
       </c>
     </row>
     <row r="405" spans="1:1">
       <c r="A405" t="s">
-        <v>448</v>
+        <v>414</v>
       </c>
     </row>
     <row r="406" spans="1:1">
       <c r="A406" t="s">
-        <v>449</v>
+        <v>415</v>
       </c>
     </row>
     <row r="407" spans="1:1">
       <c r="A407" t="s">
-        <v>450</v>
+        <v>416</v>
       </c>
     </row>
     <row r="408" spans="1:1">
       <c r="A408" t="s">
-        <v>451</v>
+        <v>417</v>
       </c>
     </row>
     <row r="409" spans="1:1">
       <c r="A409" t="s">
-        <v>452</v>
+        <v>418</v>
       </c>
     </row>
     <row r="410" spans="1:1">
       <c r="A410" t="s">
-        <v>453</v>
+        <v>419</v>
       </c>
     </row>
     <row r="411" spans="1:1">
       <c r="A411" t="s">
-        <v>454</v>
+        <v>420</v>
       </c>
     </row>
     <row r="412" spans="1:1">
       <c r="A412" t="s">
-        <v>455</v>
+        <v>421</v>
       </c>
     </row>
     <row r="413" spans="1:1">
       <c r="A413" t="s">
-        <v>456</v>
+        <v>422</v>
       </c>
     </row>
     <row r="414" spans="1:1">
       <c r="A414" t="s">
-        <v>457</v>
+        <v>423</v>
       </c>
     </row>
     <row r="415" spans="1:1">
       <c r="A415" t="s">
-        <v>458</v>
+        <v>424</v>
       </c>
     </row>
     <row r="416" spans="1:1">
       <c r="A416" t="s">
-        <v>459</v>
+        <v>425</v>
       </c>
     </row>
     <row r="417" spans="1:1">
       <c r="A417" t="s">
-        <v>460</v>
+        <v>426</v>
       </c>
     </row>
     <row r="418" spans="1:1">
       <c r="A418" t="s">
-        <v>461</v>
+        <v>427</v>
       </c>
     </row>
     <row r="419" spans="1:1">
       <c r="A419" t="s">
-        <v>462</v>
+        <v>428</v>
       </c>
     </row>
     <row r="420" spans="1:1">
       <c r="A420" t="s">
-        <v>463</v>
+        <v>429</v>
       </c>
     </row>
     <row r="421" spans="1:1">
       <c r="A421" t="s">
-        <v>464</v>
+        <v>430</v>
       </c>
     </row>
     <row r="422" spans="1:1">
       <c r="A422" t="s">
-        <v>465</v>
+        <v>431</v>
       </c>
     </row>
     <row r="423" spans="1:1">
       <c r="A423" t="s">
-        <v>466</v>
+        <v>432</v>
       </c>
     </row>
     <row r="424" spans="1:1">
       <c r="A424" t="s">
-        <v>467</v>
+        <v>433</v>
       </c>
     </row>
     <row r="425" spans="1:1">
       <c r="A425" t="s">
-        <v>468</v>
+        <v>434</v>
       </c>
     </row>
     <row r="426" spans="1:1">
       <c r="A426" t="s">
-        <v>469</v>
+        <v>435</v>
       </c>
     </row>
     <row r="427" spans="1:1">
       <c r="A427" t="s">
-        <v>470</v>
+        <v>436</v>
       </c>
     </row>
     <row r="428" spans="1:1">
       <c r="A428" t="s">
-        <v>471</v>
+        <v>437</v>
       </c>
     </row>
     <row r="429" spans="1:1">
       <c r="A429" t="s">
-        <v>472</v>
+        <v>438</v>
       </c>
     </row>
     <row r="430" spans="1:1">
       <c r="A430" t="s">
-        <v>473</v>
+        <v>439</v>
       </c>
     </row>
     <row r="431" spans="1:1">
       <c r="A431" t="s">
-        <v>474</v>
+        <v>440</v>
       </c>
     </row>
     <row r="432" spans="1:1">
       <c r="A432" t="s">
-        <v>475</v>
+        <v>441</v>
       </c>
     </row>
     <row r="433" spans="1:1">
       <c r="A433" t="s">
-        <v>476</v>
+        <v>442</v>
       </c>
     </row>
     <row r="434" spans="1:1">
       <c r="A434" t="s">
-        <v>477</v>
+        <v>443</v>
       </c>
     </row>
     <row r="435" spans="1:1">
       <c r="A435" t="s">
-        <v>478</v>
+        <v>444</v>
       </c>
     </row>
     <row r="436" spans="1:1">
       <c r="A436" t="s">
-        <v>479</v>
+        <v>445</v>
       </c>
     </row>
     <row r="437" spans="1:1">
       <c r="A437" t="s">
-        <v>480</v>
+        <v>446</v>
       </c>
     </row>
     <row r="438" spans="1:1">
       <c r="A438" t="s">
-        <v>481</v>
+        <v>447</v>
       </c>
     </row>
     <row r="439" spans="1:1">
       <c r="A439" t="s">
-        <v>482</v>
+        <v>448</v>
       </c>
     </row>
     <row r="440" spans="1:1">
       <c r="A440" t="s">
-        <v>483</v>
+        <v>449</v>
       </c>
     </row>
     <row r="441" spans="1:1">
       <c r="A441" t="s">
-        <v>484</v>
+        <v>450</v>
       </c>
     </row>
     <row r="442" spans="1:1">
       <c r="A442" t="s">
-        <v>485</v>
+        <v>451</v>
       </c>
     </row>
     <row r="443" spans="1:1">
       <c r="A443" t="s">
-        <v>486</v>
+        <v>452</v>
       </c>
     </row>
     <row r="444" spans="1:1">
       <c r="A444" t="s">
-        <v>487</v>
+        <v>453</v>
       </c>
     </row>
     <row r="445" spans="1:1">
       <c r="A445" t="s">
-        <v>488</v>
+        <v>454</v>
       </c>
     </row>
     <row r="446" spans="1:1">
       <c r="A446" t="s">
-        <v>489</v>
+        <v>455</v>
       </c>
     </row>
     <row r="447" spans="1:1">
       <c r="A447" t="s">
-        <v>490</v>
+        <v>456</v>
       </c>
     </row>
     <row r="448" spans="1:1">
       <c r="A448" t="s">
-        <v>491</v>
+        <v>457</v>
       </c>
     </row>
     <row r="449" spans="1:1">
       <c r="A449" t="s">
-        <v>492</v>
+        <v>458</v>
       </c>
     </row>
     <row r="450" spans="1:1">
       <c r="A450" t="s">
-        <v>493</v>
+        <v>459</v>
       </c>
     </row>
     <row r="451" spans="1:1">
       <c r="A451" t="s">
-        <v>494</v>
+        <v>460</v>
       </c>
     </row>
     <row r="452" spans="1:1">
       <c r="A452" t="s">
-        <v>495</v>
+        <v>461</v>
       </c>
     </row>
     <row r="453" spans="1:1">
       <c r="A453" t="s">
-        <v>496</v>
+        <v>462</v>
       </c>
     </row>
     <row r="454" spans="1:1">
       <c r="A454" t="s">
-        <v>497</v>
+        <v>463</v>
       </c>
     </row>
     <row r="455" spans="1:1">
       <c r="A455" t="s">
-        <v>498</v>
+        <v>464</v>
       </c>
     </row>
     <row r="456" spans="1:1">
       <c r="A456" t="s">
-        <v>499</v>
+        <v>465</v>
       </c>
     </row>
     <row r="457" spans="1:1">
       <c r="A457" t="s">
-        <v>500</v>
+        <v>466</v>
       </c>
     </row>
     <row r="458" spans="1:1">
       <c r="A458" t="s">
-        <v>501</v>
+        <v>467</v>
       </c>
     </row>
     <row r="459" spans="1:1">
       <c r="A459" t="s">
-        <v>502</v>
+        <v>468</v>
       </c>
     </row>
     <row r="460" spans="1:1">
       <c r="A460" t="s">
-        <v>503</v>
+        <v>469</v>
       </c>
     </row>
     <row r="461" spans="1:1">
       <c r="A461" t="s">
-        <v>504</v>
+        <v>470</v>
       </c>
     </row>
     <row r="462" spans="1:1">
       <c r="A462" t="s">
-        <v>505</v>
+        <v>471</v>
       </c>
     </row>
     <row r="463" spans="1:1">
       <c r="A463" t="s">
-        <v>506</v>
+        <v>472</v>
       </c>
     </row>
     <row r="464" spans="1:1">
       <c r="A464" t="s">
-        <v>507</v>
+        <v>473</v>
       </c>
     </row>
     <row r="465" spans="1:1">
       <c r="A465" t="s">
-        <v>508</v>
+        <v>474</v>
       </c>
     </row>
     <row r="466" spans="1:1">
       <c r="A466" t="s">
-        <v>509</v>
+        <v>475</v>
       </c>
     </row>
     <row r="467" spans="1:1">
       <c r="A467" t="s">
-        <v>510</v>
+        <v>476</v>
       </c>
     </row>
     <row r="468" spans="1:1">
       <c r="A468" t="s">
-        <v>511</v>
+        <v>477</v>
       </c>
     </row>
     <row r="469" spans="1:1">
       <c r="A469" t="s">
-        <v>512</v>
+        <v>478</v>
       </c>
     </row>
     <row r="470" spans="1:1">
       <c r="A470" t="s">
-        <v>513</v>
+        <v>479</v>
       </c>
     </row>
     <row r="471" spans="1:1">
       <c r="A471" t="s">
-        <v>514</v>
+        <v>480</v>
       </c>
     </row>
     <row r="472" spans="1:1">
       <c r="A472" t="s">
-        <v>515</v>
+        <v>481</v>
       </c>
     </row>
     <row r="473" spans="1:1">
       <c r="A473" t="s">
-        <v>516</v>
+        <v>482</v>
       </c>
     </row>
     <row r="474" spans="1:1">
       <c r="A474" t="s">
-        <v>517</v>
+        <v>483</v>
       </c>
     </row>
     <row r="475" spans="1:1">
       <c r="A475" t="s">
-        <v>518</v>
+        <v>484</v>
       </c>
     </row>
     <row r="476" spans="1:1">
       <c r="A476" t="s">
-        <v>519</v>
+        <v>485</v>
       </c>
     </row>
     <row r="477" spans="1:1">
       <c r="A477" t="s">
-        <v>520</v>
+        <v>486</v>
       </c>
     </row>
     <row r="479" spans="1:1">
       <c r="A479" t="s">
-        <v>521</v>
+        <v>487</v>
       </c>
     </row>
     <row r="480" spans="1:1">
       <c r="A480" t="s">
-        <v>522</v>
+        <v>488</v>
       </c>
     </row>
     <row r="481" spans="1:1">
       <c r="A481" t="s">
-        <v>523</v>
+        <v>489</v>
       </c>
     </row>
     <row r="482" spans="1:1">
       <c r="A482" t="s">
-        <v>524</v>
+        <v>490</v>
       </c>
     </row>
     <row r="483" spans="1:1">
       <c r="A483" t="s">
-        <v>525</v>
+        <v>491</v>
       </c>
     </row>
     <row r="484" spans="1:1">
       <c r="A484" t="s">
-        <v>526</v>
+        <v>492</v>
       </c>
     </row>
     <row r="485" spans="1:1">
       <c r="A485" t="s">
-        <v>527</v>
+        <v>493</v>
       </c>
     </row>
     <row r="486" spans="1:1">
       <c r="A486" t="s">
-        <v>528</v>
+        <v>494</v>
       </c>
     </row>
     <row r="487" spans="1:1">
       <c r="A487" t="s">
-        <v>529</v>
+        <v>495</v>
       </c>
     </row>
     <row r="488" spans="1:1">
       <c r="A488" t="s">
-        <v>530</v>
+        <v>496</v>
       </c>
     </row>
     <row r="489" spans="1:1">
       <c r="A489" t="s">
-        <v>531</v>
+        <v>497</v>
       </c>
     </row>
     <row r="490" spans="1:1">
       <c r="A490" t="s">
-        <v>532</v>
+        <v>498</v>
       </c>
     </row>
     <row r="491" spans="1:1">
       <c r="A491" t="s">
-        <v>533</v>
+        <v>499</v>
       </c>
     </row>
     <row r="492" spans="1:1">
       <c r="A492" t="s">
-        <v>534</v>
+        <v>500</v>
       </c>
     </row>
     <row r="493" spans="1:1">
       <c r="A493" t="s">
-        <v>535</v>
+        <v>501</v>
       </c>
     </row>
     <row r="494" spans="1:1">
       <c r="A494" t="s">
-        <v>536</v>
+        <v>502</v>
       </c>
     </row>
     <row r="495" spans="1:1">
       <c r="A495" t="s">
-        <v>537</v>
+        <v>503</v>
       </c>
     </row>
     <row r="496" spans="1:1">
       <c r="A496" t="s">
-        <v>538</v>
+        <v>504</v>
       </c>
     </row>
     <row r="497" spans="1:1">
       <c r="A497" t="s">
-        <v>539</v>
+        <v>505</v>
       </c>
     </row>
     <row r="498" spans="1:1">
       <c r="A498" t="s">
-        <v>540</v>
+        <v>506</v>
       </c>
     </row>
     <row r="499" spans="1:1">
       <c r="A499" t="s">
-        <v>541</v>
+        <v>507</v>
       </c>
     </row>
     <row r="500" spans="1:1">
       <c r="A500" t="s">
-        <v>542</v>
+        <v>508</v>
       </c>
     </row>
     <row r="501" spans="1:1">
       <c r="A501" t="s">
-        <v>543</v>
+        <v>509</v>
       </c>
     </row>
     <row r="502" spans="1:1">
       <c r="A502" t="s">
-        <v>544</v>
+        <v>510</v>
       </c>
     </row>
     <row r="503" spans="1:1">
       <c r="A503" t="s">
-        <v>545</v>
+        <v>511</v>
       </c>
     </row>
     <row r="504" spans="1:1">
       <c r="A504" t="s">
-        <v>546</v>
+        <v>512</v>
       </c>
     </row>
     <row r="505" spans="1:1">
       <c r="A505" t="s">
-        <v>547</v>
+        <v>513</v>
       </c>
     </row>
     <row r="506" spans="1:1">
       <c r="A506" t="s">
-        <v>548</v>
+        <v>514</v>
       </c>
     </row>
     <row r="507" spans="1:1">
       <c r="A507" t="s">
-        <v>549</v>
+        <v>515</v>
       </c>
     </row>
     <row r="508" spans="1:1">
       <c r="A508" t="s">
-        <v>550</v>
+        <v>516</v>
       </c>
     </row>
     <row r="509" spans="1:1">
       <c r="A509" t="s">
-        <v>551</v>
+        <v>517</v>
       </c>
     </row>
     <row r="510" spans="1:1">
       <c r="A510" t="s">
-        <v>552</v>
+        <v>518</v>
       </c>
     </row>
     <row r="511" spans="1:1">
       <c r="A511" t="s">
-        <v>553</v>
+        <v>519</v>
       </c>
     </row>
     <row r="512" spans="1:1">
       <c r="A512" t="s">
-        <v>554</v>
+        <v>520</v>
       </c>
     </row>
     <row r="513" spans="1:1">
       <c r="A513" t="s">
-        <v>555</v>
+        <v>521</v>
       </c>
     </row>
     <row r="514" spans="1:1">
       <c r="A514" t="s">
-        <v>556</v>
+        <v>522</v>
       </c>
     </row>
     <row r="515" spans="1:1">
       <c r="A515" t="s">
-        <v>557</v>
+        <v>523</v>
       </c>
     </row>
     <row r="516" spans="1:1">
       <c r="A516" t="s">
-        <v>558</v>
+        <v>524</v>
       </c>
     </row>
     <row r="517" spans="1:1">
       <c r="A517" t="s">
-        <v>559</v>
+        <v>525</v>
       </c>
     </row>
     <row r="518" spans="1:1">
       <c r="A518" t="s">
-        <v>560</v>
+        <v>526</v>
       </c>
     </row>
     <row r="519" spans="1:1">
       <c r="A519" t="s">
-        <v>561</v>
+        <v>527</v>
       </c>
     </row>
     <row r="520" spans="1:1">
       <c r="A520" t="s">
-        <v>562</v>
+        <v>528</v>
       </c>
     </row>
     <row r="521" spans="1:1">
       <c r="A521" t="s">
-        <v>563</v>
+        <v>529</v>
       </c>
     </row>
     <row r="522" spans="1:1">
       <c r="A522" t="s">
-        <v>564</v>
+        <v>530</v>
       </c>
     </row>
     <row r="523" spans="1:1">
       <c r="A523" t="s">
-        <v>565</v>
+        <v>531</v>
       </c>
     </row>
     <row r="524" spans="1:1">
       <c r="A524" t="s">
-        <v>566</v>
+        <v>532</v>
       </c>
     </row>
     <row r="525" spans="1:1">
       <c r="A525" t="s">
-        <v>567</v>
+        <v>533</v>
       </c>
     </row>
     <row r="526" spans="1:1">
       <c r="A526" t="s">
-        <v>568</v>
+        <v>534</v>
       </c>
     </row>
     <row r="527" spans="1:1">
       <c r="A527" t="s">
-        <v>569</v>
+        <v>535</v>
       </c>
     </row>
     <row r="528" spans="1:1">
       <c r="A528" t="s">
-        <v>570</v>
+        <v>536</v>
       </c>
     </row>
     <row r="529" spans="1:1">
       <c r="A529" t="s">
-        <v>571</v>
+        <v>537</v>
       </c>
     </row>
     <row r="530" spans="1:1">
       <c r="A530" t="s">
-        <v>572</v>
+        <v>538</v>
       </c>
     </row>
     <row r="531" spans="1:1">
       <c r="A531" t="s">
-        <v>573</v>
+        <v>539</v>
       </c>
     </row>
     <row r="532" spans="1:1">
       <c r="A532" t="s">
-        <v>574</v>
+        <v>540</v>
       </c>
     </row>
     <row r="533" spans="1:1">
       <c r="A533" t="s">
-        <v>575</v>
+        <v>541</v>
       </c>
     </row>
     <row r="534" spans="1:1">
       <c r="A534" t="s">
-        <v>576</v>
+        <v>542</v>
       </c>
     </row>
     <row r="535" spans="1:1">
       <c r="A535" t="s">
-        <v>577</v>
+        <v>543</v>
       </c>
     </row>
     <row r="536" spans="1:1">
       <c r="A536" t="s">
-        <v>578</v>
+        <v>544</v>
       </c>
     </row>
     <row r="538" spans="1:1">
       <c r="A538" t="s">
-        <v>579</v>
+        <v>545</v>
       </c>
     </row>
     <row r="539" spans="1:1">
       <c r="A539" t="s">
-        <v>580</v>
+        <v>546</v>
       </c>
     </row>
     <row r="540" spans="1:1">
       <c r="A540" t="s">
-        <v>581</v>
+        <v>547</v>
       </c>
     </row>
     <row r="541" spans="1:1">
       <c r="A541" t="s">
-        <v>582</v>
+        <v>548</v>
       </c>
     </row>
     <row r="542" spans="1:1">
       <c r="A542" t="s">
-        <v>583</v>
+        <v>549</v>
       </c>
     </row>
     <row r="543" spans="1:1">
       <c r="A543" t="s">
-        <v>584</v>
+        <v>550</v>
       </c>
     </row>
     <row r="544" spans="1:1">
       <c r="A544" t="s">
-        <v>585</v>
+        <v>551</v>
       </c>
     </row>
     <row r="545" spans="1:1">
       <c r="A545" t="s">
-        <v>586</v>
+        <v>552</v>
       </c>
     </row>
     <row r="546" spans="1:1">
       <c r="A546" t="s">
-        <v>587</v>
+        <v>553</v>
       </c>
     </row>
     <row r="547" spans="1:1">
       <c r="A547" t="s">
-        <v>588</v>
+        <v>554</v>
       </c>
     </row>
     <row r="548" spans="1:1">
       <c r="A548" t="s">
-        <v>589</v>
+        <v>555</v>
       </c>
     </row>
     <row r="549" spans="1:1">
       <c r="A549" t="s">
-        <v>590</v>
+        <v>556</v>
       </c>
     </row>
     <row r="550" spans="1:1">
       <c r="A550" t="s">
-        <v>591</v>
+        <v>557</v>
       </c>
     </row>
     <row r="551" spans="1:1">
       <c r="A551" t="s">
-        <v>592</v>
+        <v>558</v>
       </c>
     </row>
     <row r="552" spans="1:1">
       <c r="A552" t="s">
-        <v>593</v>
+        <v>559</v>
       </c>
     </row>
     <row r="553" spans="1:1">
       <c r="A553" t="s">
-        <v>594</v>
+        <v>560</v>
       </c>
     </row>
     <row r="554" spans="1:1">
       <c r="A554" t="s">
-        <v>595</v>
+        <v>561</v>
       </c>
     </row>
     <row r="556" spans="1:1">
       <c r="A556" t="s">
-        <v>596</v>
+        <v>562</v>
       </c>
     </row>
     <row r="557" spans="1:1">
       <c r="A557" t="s">
-        <v>597</v>
+        <v>563</v>
       </c>
     </row>
     <row r="558" spans="1:1">
       <c r="A558" t="s">
-        <v>598</v>
+        <v>564</v>
       </c>
     </row>
     <row r="559" spans="1:1">
       <c r="A559" t="s">
-        <v>599</v>
+        <v>565</v>
       </c>
     </row>
     <row r="560" spans="1:1">
       <c r="A560" t="s">
-        <v>600</v>
+        <v>566</v>
       </c>
     </row>
     <row r="561" spans="1:1">
       <c r="A561" t="s">
-        <v>601</v>
+        <v>567</v>
       </c>
     </row>
     <row r="562" spans="1:1">
       <c r="A562" t="s">
-        <v>602</v>
+        <v>568</v>
       </c>
     </row>
     <row r="563" spans="1:1">
       <c r="A563" t="s">
-        <v>603</v>
+        <v>569</v>
       </c>
     </row>
     <row r="564" spans="1:1">
       <c r="A564" t="s">
-        <v>604</v>
+        <v>570</v>
       </c>
     </row>
     <row r="565" spans="1:1">
       <c r="A565" t="s">
-        <v>605</v>
+        <v>571</v>
       </c>
     </row>
     <row r="566" spans="1:1">
       <c r="A566" t="s">
-        <v>606</v>
+        <v>572</v>
       </c>
     </row>
     <row r="567" spans="1:1">
       <c r="A567" t="s">
-        <v>607</v>
+        <v>573</v>
       </c>
     </row>
     <row r="568" spans="1:1">
       <c r="A568" t="s">
-        <v>608</v>
+        <v>574</v>
       </c>
     </row>
     <row r="569" spans="1:1">
       <c r="A569" t="s">
-        <v>609</v>
+        <v>575</v>
       </c>
     </row>
     <row r="570" spans="1:1">
       <c r="A570" t="s">
-        <v>610</v>
+        <v>576</v>
       </c>
     </row>
     <row r="571" spans="1:1">
       <c r="A571" t="s">
-        <v>611</v>
+        <v>577</v>
       </c>
     </row>
     <row r="572" spans="1:1">
       <c r="A572" t="s">
-        <v>612</v>
+        <v>578</v>
       </c>
     </row>
     <row r="573" spans="1:1">
       <c r="A573" t="s">
-        <v>613</v>
+        <v>579</v>
       </c>
     </row>
     <row r="574" spans="1:1">
       <c r="A574" t="s">
-        <v>614</v>
+        <v>580</v>
       </c>
     </row>
     <row r="575" spans="1:1">
       <c r="A575" t="s">
-        <v>615</v>
+        <v>581</v>
       </c>
     </row>
     <row r="576" spans="1:1">
       <c r="A576" t="s">
-        <v>616</v>
+        <v>582</v>
       </c>
     </row>
     <row r="577" spans="1:1">
       <c r="A577" t="s">
-        <v>617</v>
+        <v>583</v>
       </c>
     </row>
     <row r="578" spans="1:1">
       <c r="A578" t="s">
-        <v>618</v>
+        <v>584</v>
       </c>
     </row>
     <row r="579" spans="1:1">
       <c r="A579" t="s">
-        <v>619</v>
+        <v>585</v>
       </c>
     </row>
     <row r="580" spans="1:1">
       <c r="A580" t="s">
-        <v>620</v>
+        <v>586</v>
       </c>
     </row>
     <row r="581" spans="1:1">
       <c r="A581" t="s">
-        <v>621</v>
+        <v>587</v>
       </c>
     </row>
     <row r="582" spans="1:1">
       <c r="A582" t="s">
-        <v>622</v>
+        <v>588</v>
       </c>
     </row>
     <row r="583" spans="1:1">
       <c r="A583" t="s">
-        <v>623</v>
+        <v>589</v>
       </c>
     </row>
     <row r="584" spans="1:1">
       <c r="A584" t="s">
-        <v>624</v>
+        <v>590</v>
       </c>
     </row>
     <row r="586" spans="1:1">
       <c r="A586" t="s">
-        <v>625</v>
+        <v>591</v>
       </c>
     </row>
     <row r="587" spans="1:1">
       <c r="A587" t="s">
-        <v>626</v>
+        <v>592</v>
       </c>
     </row>
     <row r="588" spans="1:1">
       <c r="A588" t="s">
-        <v>627</v>
+        <v>593</v>
       </c>
     </row>
     <row r="589" spans="1:1">
       <c r="A589" t="s">
-        <v>628</v>
+        <v>594</v>
       </c>
     </row>
     <row r="590" spans="1:1">
       <c r="A590" t="s">
-        <v>629</v>
+        <v>595</v>
       </c>
     </row>
     <row r="591" spans="1:1">
       <c r="A591" t="s">
-        <v>630</v>
+        <v>596</v>
       </c>
     </row>
     <row r="592" spans="1:1">
       <c r="A592" t="s">
-        <v>631</v>
+        <v>597</v>
       </c>
     </row>
     <row r="593" spans="1:1">
       <c r="A593" t="s">
-        <v>632</v>
+        <v>598</v>
       </c>
     </row>
     <row r="594" spans="1:1">
       <c r="A594" t="s">
-        <v>633</v>
+        <v>599</v>
       </c>
     </row>
     <row r="595" spans="1:1">
       <c r="A595" t="s">
-        <v>634</v>
+        <v>600</v>
       </c>
     </row>
     <row r="596" spans="1:1">
       <c r="A596" t="s">
-        <v>635</v>
+        <v>601</v>
       </c>
     </row>
     <row r="597" spans="1:1">
       <c r="A597" t="s">
-        <v>636</v>
+        <v>602</v>
       </c>
     </row>
     <row r="598" spans="1:1">
       <c r="A598" t="s">
-        <v>637</v>
+        <v>603</v>
       </c>
     </row>
     <row r="599" spans="1:1">
       <c r="A599" t="s">
-        <v>638</v>
+        <v>604</v>
       </c>
     </row>
     <row r="600" spans="1:1">
       <c r="A600" t="s">
-        <v>639</v>
+        <v>605</v>
       </c>
     </row>
     <row r="601" spans="1:1">
       <c r="A601" t="s">
-        <v>640</v>
+        <v>606</v>
       </c>
     </row>
     <row r="602" spans="1:1">
       <c r="A602" t="s">
-        <v>641</v>
+        <v>607</v>
       </c>
     </row>
     <row r="603" spans="1:1">
       <c r="A603" t="s">
-        <v>642</v>
+        <v>608</v>
       </c>
     </row>
     <row r="604" spans="1:1">
       <c r="A604" t="s">
-        <v>643</v>
+        <v>609</v>
       </c>
     </row>
     <row r="605" spans="1:1">
       <c r="A605" t="s">
-        <v>644</v>
+        <v>610</v>
       </c>
     </row>
     <row r="606" spans="1:1">
       <c r="A606" t="s">
-        <v>645</v>
+        <v>611</v>
       </c>
     </row>
     <row r="607" spans="1:1">
       <c r="A607" t="s">
-        <v>646</v>
+        <v>612</v>
       </c>
     </row>
     <row r="608" spans="1:1">
       <c r="A608" t="s">
-        <v>647</v>
+        <v>613</v>
       </c>
     </row>
     <row r="609" spans="1:1">
       <c r="A609" t="s">
-        <v>648</v>
+        <v>614</v>
       </c>
     </row>
     <row r="610" spans="1:1">
       <c r="A610" t="s">
-        <v>649</v>
+        <v>615</v>
       </c>
     </row>
     <row r="611" spans="1:1">
       <c r="A611" t="s">
-        <v>650</v>
+        <v>616</v>
       </c>
     </row>
     <row r="612" spans="1:1">
       <c r="A612" t="s">
-        <v>651</v>
+        <v>617</v>
       </c>
     </row>
     <row r="613" spans="1:1">
       <c r="A613" t="s">
-        <v>652</v>
+        <v>618</v>
       </c>
     </row>
     <row r="614" spans="1:1">
       <c r="A614" t="s">
-        <v>653</v>
+        <v>619</v>
       </c>
     </row>
     <row r="615" spans="1:1">
       <c r="A615" t="s">
-        <v>654</v>
+        <v>620</v>
       </c>
     </row>
     <row r="616" spans="1:1">
       <c r="A616" t="s">
-        <v>655</v>
+        <v>621</v>
       </c>
     </row>
     <row r="617" spans="1:1">
       <c r="A617" t="s">
-        <v>656</v>
+        <v>622</v>
       </c>
     </row>
     <row r="618" spans="1:1">
       <c r="A618" t="s">
-        <v>657</v>
+        <v>623</v>
       </c>
     </row>
     <row r="619" spans="1:1">
       <c r="A619" t="s">
-        <v>658</v>
+        <v>624</v>
       </c>
     </row>
     <row r="620" spans="1:1">
       <c r="A620" t="s">
-        <v>659</v>
+        <v>625</v>
       </c>
     </row>
     <row r="621" spans="1:1">
       <c r="A621" t="s">
-        <v>660</v>
+        <v>626</v>
       </c>
     </row>
     <row r="623" spans="1:1">
       <c r="A623" t="s">
-        <v>661</v>
+        <v>627</v>
       </c>
     </row>
     <row r="624" spans="1:1">
       <c r="A624" t="s">
-        <v>662</v>
+        <v>628</v>
       </c>
     </row>
     <row r="625" spans="1:1">
       <c r="A625" t="s">
-        <v>663</v>
+        <v>629</v>
       </c>
     </row>
     <row r="626" spans="1:1">
       <c r="A626" t="s">
-        <v>664</v>
+        <v>630</v>
       </c>
     </row>
     <row r="627" spans="1:1">
       <c r="A627" t="s">
-        <v>665</v>
+        <v>631</v>
       </c>
     </row>
     <row r="628" spans="1:1">
       <c r="A628" t="s">
-        <v>666</v>
+        <v>632</v>
       </c>
     </row>
     <row r="629" spans="1:1">
       <c r="A629" t="s">
-        <v>667</v>
+        <v>633</v>
       </c>
     </row>
     <row r="630" spans="1:1">
       <c r="A630" t="s">
-        <v>668</v>
+        <v>634</v>
       </c>
     </row>
     <row r="631" spans="1:1">
       <c r="A631" t="s">
-        <v>669</v>
+        <v>635</v>
       </c>
     </row>
     <row r="632" spans="1:1">
       <c r="A632" t="s">
-        <v>670</v>
+        <v>636</v>
       </c>
     </row>
     <row r="633" spans="1:1">
       <c r="A633" t="s">
-        <v>671</v>
+        <v>637</v>
       </c>
     </row>
     <row r="634" spans="1:1">
       <c r="A634" t="s">
-        <v>672</v>
+        <v>638</v>
       </c>
     </row>
     <row r="635" spans="1:1">
       <c r="A635" t="s">
-        <v>673</v>
+        <v>639</v>
       </c>
     </row>
     <row r="636" spans="1:1">
       <c r="A636" t="s">
-        <v>674</v>
+        <v>640</v>
       </c>
     </row>
     <row r="637" spans="1:1">
       <c r="A637" t="s">
-        <v>675</v>
+        <v>641</v>
       </c>
     </row>
     <row r="638" spans="1:1">
       <c r="A638" t="s">
-        <v>676</v>
+        <v>642</v>
       </c>
     </row>
     <row r="639" spans="1:1">
       <c r="A639" t="s">
-        <v>677</v>
+        <v>643</v>
       </c>
     </row>
     <row r="640" spans="1:1">
       <c r="A640" t="s">
-        <v>678</v>
+        <v>644</v>
       </c>
     </row>
     <row r="641" spans="1:1">
       <c r="A641" t="s">
-        <v>679</v>
+        <v>645</v>
       </c>
     </row>
     <row r="643" spans="1:1">
       <c r="A643" t="s">
-        <v>680</v>
+        <v>646</v>
       </c>
     </row>
     <row r="644" spans="1:1">
       <c r="A644" t="s">
-        <v>681</v>
+        <v>647</v>
       </c>
     </row>
     <row r="645" spans="1:1">
       <c r="A645" t="s">
-        <v>682</v>
+        <v>648</v>
       </c>
     </row>
     <row r="646" spans="1:1">
       <c r="A646" t="s">
-        <v>683</v>
+        <v>649</v>
       </c>
     </row>
     <row r="647" spans="1:1">
       <c r="A647" t="s">
-        <v>684</v>
+        <v>650</v>
       </c>
     </row>
     <row r="648" spans="1:1">
       <c r="A648" t="s">
-        <v>685</v>
+        <v>651</v>
       </c>
     </row>
     <row r="649" spans="1:1">
       <c r="A649" t="s">
-        <v>686</v>
+        <v>652</v>
       </c>
     </row>
     <row r="650" spans="1:1">
       <c r="A650" t="s">
-        <v>687</v>
+        <v>653</v>
       </c>
     </row>
     <row r="651" spans="1:1">
       <c r="A651" t="s">
-        <v>688</v>
+        <v>654</v>
       </c>
     </row>
     <row r="652" spans="1:1">
       <c r="A652" t="s">
-        <v>689</v>
+        <v>655</v>
       </c>
     </row>
     <row r="653" spans="1:1">
       <c r="A653" t="s">
-        <v>690</v>
+        <v>656</v>
       </c>
     </row>
     <row r="654" spans="1:1">
       <c r="A654" t="s">
-        <v>691</v>
+        <v>657</v>
       </c>
     </row>
     <row r="655" spans="1:1">
       <c r="A655" t="s">
-        <v>692</v>
+        <v>658</v>
       </c>
     </row>
     <row r="657" spans="1:1">
       <c r="A657" t="s">
-        <v>693</v>
+        <v>659</v>
       </c>
     </row>
     <row r="658" spans="1:1">
       <c r="A658" t="s">
-        <v>694</v>
+        <v>660</v>
       </c>
     </row>
     <row r="659" spans="1:1">
       <c r="A659" t="s">
-        <v>695</v>
+        <v>661</v>
       </c>
     </row>
     <row r="660" spans="1:1">
       <c r="A660" t="s">
-        <v>696</v>
+        <v>662</v>
       </c>
     </row>
     <row r="661" spans="1:1">
       <c r="A661" t="s">
-        <v>697</v>
+        <v>663</v>
       </c>
     </row>
     <row r="662" spans="1:1">
       <c r="A662" t="s">
-        <v>698</v>
+        <v>664</v>
       </c>
     </row>
     <row r="663" spans="1:1">
       <c r="A663" t="s">
-        <v>699</v>
+        <v>665</v>
       </c>
     </row>
     <row r="664" spans="1:1">
       <c r="A664" t="s">
-        <v>700</v>
+        <v>666</v>
       </c>
     </row>
     <row r="665" spans="1:1">
       <c r="A665" t="s">
-        <v>701</v>
+        <v>667</v>
       </c>
     </row>
     <row r="666" spans="1:1">
       <c r="A666" t="s">
-        <v>702</v>
+        <v>668</v>
       </c>
     </row>
     <row r="667" spans="1:1">
       <c r="A667" t="s">
-        <v>703</v>
+        <v>669</v>
       </c>
     </row>
     <row r="668" spans="1:1">
       <c r="A668" t="s">
-        <v>704</v>
+        <v>670</v>
       </c>
     </row>
     <row r="669" spans="1:1">
       <c r="A669" t="s">
-        <v>705</v>
+        <v>671</v>
       </c>
     </row>
     <row r="670" spans="1:1">
       <c r="A670" t="s">
-        <v>706</v>
+        <v>672</v>
       </c>
     </row>
     <row r="671" spans="1:1">
       <c r="A671" t="s">
-        <v>707</v>
+        <v>673</v>
       </c>
     </row>
     <row r="673" spans="1:1">
       <c r="A673" t="s">
-        <v>708</v>
+        <v>674</v>
       </c>
     </row>
     <row r="674" spans="1:1">
       <c r="A674" t="s">
-        <v>709</v>
+        <v>675</v>
       </c>
     </row>
     <row r="675" spans="1:1">
       <c r="A675" t="s">
-        <v>710</v>
+        <v>676</v>
       </c>
     </row>
     <row r="676" spans="1:1">
       <c r="A676" t="s">
-        <v>711</v>
+        <v>677</v>
       </c>
     </row>
     <row r="677" spans="1:1">
       <c r="A677" t="s">
-        <v>712</v>
+        <v>678</v>
       </c>
     </row>
     <row r="678" spans="1:1">
       <c r="A678" t="s">
-        <v>713</v>
+        <v>679</v>
       </c>
     </row>
     <row r="679" spans="1:1">
       <c r="A679" t="s">
-        <v>714</v>
+        <v>680</v>
       </c>
     </row>
     <row r="680" spans="1:1">
       <c r="A680" t="s">
-        <v>715</v>
+        <v>681</v>
       </c>
     </row>
     <row r="681" spans="1:1">
       <c r="A681" t="s">
-        <v>716</v>
+        <v>682</v>
       </c>
     </row>
     <row r="682" spans="1:1">
       <c r="A682" t="s">
-        <v>717</v>
+        <v>683</v>
       </c>
     </row>
     <row r="683" spans="1:1">
       <c r="A683" t="s">
-        <v>718</v>
+        <v>684</v>
       </c>
     </row>
     <row r="684" spans="1:1">
       <c r="A684" t="s">
-        <v>719</v>
+        <v>685</v>
       </c>
     </row>
     <row r="685" spans="1:1">
       <c r="A685" t="s">
-        <v>720</v>
+        <v>686</v>
       </c>
     </row>
     <row r="686" spans="1:1">
       <c r="A686" t="s">
-        <v>721</v>
+        <v>687</v>
       </c>
     </row>
     <row r="687" spans="1:1">
       <c r="A687" t="s">
-        <v>722</v>
+        <v>688</v>
       </c>
     </row>
     <row r="688" spans="1:1">
       <c r="A688" t="s">
-        <v>723</v>
+        <v>689</v>
       </c>
     </row>
     <row r="689" spans="1:1">
       <c r="A689" t="s">
-        <v>724</v>
+        <v>690</v>
       </c>
     </row>
     <row r="690" spans="1:1">
       <c r="A690" t="s">
-        <v>725</v>
+        <v>691</v>
       </c>
     </row>
     <row r="691" spans="1:1">
       <c r="A691" t="s">
-        <v>726</v>
+        <v>692</v>
       </c>
     </row>
     <row r="692" spans="1:1">
       <c r="A692" t="s">
-        <v>727</v>
+        <v>693</v>
       </c>
     </row>
     <row r="693" spans="1:1">
       <c r="A693" t="s">
-        <v>728</v>
+        <v>694</v>
       </c>
     </row>
     <row r="694" spans="1:1">
       <c r="A694" t="s">
-        <v>729</v>
+        <v>695</v>
       </c>
     </row>
     <row r="695" spans="1:1">
       <c r="A695" t="s">
-        <v>730</v>
+        <v>696</v>
       </c>
     </row>
     <row r="696" spans="1:1">
       <c r="A696" t="s">
-        <v>731</v>
+        <v>697</v>
       </c>
     </row>
     <row r="697" spans="1:1">
       <c r="A697" t="s">
-        <v>732</v>
+        <v>698</v>
       </c>
     </row>
     <row r="698" spans="1:1">
       <c r="A698" t="s">
-        <v>733</v>
+        <v>699</v>
       </c>
     </row>
     <row r="699" spans="1:1">
       <c r="A699" t="s">
-        <v>734</v>
+        <v>700</v>
       </c>
     </row>
     <row r="700" spans="1:1">
       <c r="A700" t="s">
-        <v>735</v>
+        <v>701</v>
       </c>
     </row>
     <row r="701" spans="1:1">
       <c r="A701" t="s">
-        <v>736</v>
+        <v>702</v>
       </c>
     </row>
     <row r="702" spans="1:1">
       <c r="A702" t="s">
-        <v>737</v>
+        <v>703</v>
       </c>
     </row>
     <row r="703" spans="1:1">
       <c r="A703" t="s">
-        <v>738</v>
+        <v>704</v>
       </c>
     </row>
     <row r="704" spans="1:1">
       <c r="A704" t="s">
-        <v>739</v>
+        <v>705</v>
       </c>
     </row>
     <row r="705" spans="1:1">
       <c r="A705" t="s">
-        <v>740</v>
+        <v>706</v>
       </c>
     </row>
     <row r="706" spans="1:1">
       <c r="A706" t="s">
-        <v>741</v>
+        <v>707</v>
       </c>
     </row>
     <row r="707" spans="1:1">
       <c r="A707" t="s">
-        <v>742</v>
+        <v>708</v>
       </c>
     </row>
     <row r="708" spans="1:1">
       <c r="A708" t="s">
-        <v>743</v>
+        <v>709</v>
       </c>
     </row>
     <row r="709" spans="1:1">
       <c r="A709" t="s">
-        <v>744</v>
+        <v>710</v>
       </c>
     </row>
     <row r="710" spans="1:1">
       <c r="A710" t="s">
-        <v>745</v>
+        <v>711</v>
       </c>
     </row>
     <row r="711" spans="1:1">
       <c r="A711" t="s">
-        <v>746</v>
+        <v>712</v>
       </c>
     </row>
     <row r="712" spans="1:1">
       <c r="A712" t="s">
-        <v>747</v>
+        <v>713</v>
       </c>
     </row>
     <row r="713" spans="1:1">
       <c r="A713" t="s">
-        <v>748</v>
+        <v>714</v>
       </c>
     </row>
     <row r="714" spans="1:1">
       <c r="A714" t="s">
-        <v>749</v>
+        <v>715</v>
       </c>
     </row>
     <row r="715" spans="1:1">
       <c r="A715" t="s">
-        <v>750</v>
+        <v>716</v>
       </c>
     </row>
     <row r="716" spans="1:1">
       <c r="A716" t="s">
-        <v>751</v>
+        <v>717</v>
       </c>
     </row>
     <row r="717" spans="1:1">
       <c r="A717" t="s">
-        <v>752</v>
+        <v>718</v>
       </c>
     </row>
     <row r="718" spans="1:1">
       <c r="A718" t="s">
-        <v>753</v>
+        <v>719</v>
       </c>
     </row>
     <row r="719" spans="1:1">
       <c r="A719" t="s">
-        <v>754</v>
+        <v>720</v>
       </c>
     </row>
     <row r="720" spans="1:1">
       <c r="A720" t="s">
-        <v>755</v>
+        <v>721</v>
       </c>
     </row>
     <row r="721" spans="1:1">
       <c r="A721" t="s">
-        <v>756</v>
+        <v>722</v>
       </c>
     </row>
     <row r="722" spans="1:1">
       <c r="A722" t="s">
-        <v>757</v>
+        <v>723</v>
       </c>
     </row>
     <row r="723" spans="1:1">
       <c r="A723" t="s">
-        <v>758</v>
+        <v>724</v>
       </c>
     </row>
     <row r="724" spans="1:1">
       <c r="A724" t="s">
-        <v>759</v>
+        <v>725</v>
       </c>
     </row>
     <row r="725" spans="1:1">
       <c r="A725" t="s">
-        <v>760</v>
+        <v>726</v>
       </c>
     </row>
     <row r="726" spans="1:1">
       <c r="A726" t="s">
-        <v>761</v>
+        <v>727</v>
       </c>
     </row>
     <row r="727" spans="1:1">
       <c r="A727" t="s">
-        <v>762</v>
+        <v>728</v>
       </c>
     </row>
     <row r="728" spans="1:1">
       <c r="A728" t="s">
-        <v>763</v>
+        <v>729</v>
       </c>
     </row>
     <row r="729" spans="1:1">
       <c r="A729" t="s">
-        <v>764</v>
+        <v>730</v>
       </c>
     </row>
     <row r="730" spans="1:1">
       <c r="A730" t="s">
-        <v>765</v>
+        <v>731</v>
       </c>
     </row>
     <row r="731" spans="1:1">
       <c r="A731" t="s">
-        <v>766</v>
+        <v>732</v>
       </c>
     </row>
     <row r="732" spans="1:1">
       <c r="A732" t="s">
-        <v>767</v>
+        <v>733</v>
       </c>
     </row>
     <row r="733" spans="1:1">
       <c r="A733" t="s">
-        <v>768</v>
+        <v>734</v>
       </c>
     </row>
     <row r="734" spans="1:1">
       <c r="A734" t="s">
-        <v>769</v>
+        <v>735</v>
       </c>
     </row>
     <row r="735" spans="1:1">
       <c r="A735" t="s">
-        <v>770</v>
+        <v>736</v>
       </c>
     </row>
     <row r="736" spans="1:1">
       <c r="A736" t="s">
-        <v>771</v>
+        <v>737</v>
       </c>
     </row>
     <row r="737" spans="1:1">
       <c r="A737" t="s">
-        <v>772</v>
+        <v>738</v>
       </c>
     </row>
     <row r="738" spans="1:1">
       <c r="A738" t="s">
-        <v>773</v>
+        <v>739</v>
       </c>
     </row>
     <row r="739" spans="1:1">
       <c r="A739" t="s">
-        <v>774</v>
+        <v>740</v>
       </c>
     </row>
     <row r="740" spans="1:1">
       <c r="A740" t="s">
-        <v>775</v>
+        <v>741</v>
       </c>
     </row>
     <row r="741" spans="1:1">
       <c r="A741" t="s">
-        <v>776</v>
+        <v>742</v>
       </c>
     </row>
     <row r="742" spans="1:1">
       <c r="A742" t="s">
-        <v>777</v>
+        <v>743</v>
       </c>
     </row>
     <row r="743" spans="1:1">
       <c r="A743" t="s">
-        <v>778</v>
+        <v>744</v>
       </c>
     </row>
     <row r="745" spans="1:1">
       <c r="A745" t="s">
-        <v>779</v>
+        <v>745</v>
       </c>
     </row>
     <row r="746" spans="1:1">
       <c r="A746" t="s">
-        <v>780</v>
+        <v>746</v>
       </c>
     </row>
     <row r="747" spans="1:1">
       <c r="A747" t="s">
-        <v>781</v>
+        <v>747</v>
       </c>
     </row>
     <row r="748" spans="1:1">
       <c r="A748" t="s">
-        <v>782</v>
+        <v>748</v>
       </c>
     </row>
     <row r="749" spans="1:1">
       <c r="A749" t="s">
-        <v>783</v>
+        <v>749</v>
       </c>
     </row>
     <row r="750" spans="1:1">
       <c r="A750" t="s">
-        <v>784</v>
+        <v>750</v>
       </c>
     </row>
     <row r="751" spans="1:1">
       <c r="A751" t="s">
-        <v>785</v>
+        <v>751</v>
       </c>
     </row>
     <row r="752" spans="1:1">
       <c r="A752" t="s">
-        <v>786</v>
+        <v>752</v>
       </c>
     </row>
     <row r="753" spans="1:1">
       <c r="A753" t="s">
-        <v>787</v>
+        <v>753</v>
       </c>
     </row>
     <row r="754" spans="1:1">
       <c r="A754" t="s">
-        <v>788</v>
+        <v>754</v>
       </c>
     </row>
     <row r="756" spans="1:1">
       <c r="A756" t="s">
-        <v>789</v>
+        <v>755</v>
       </c>
     </row>
     <row r="757" spans="1:1">
       <c r="A757" t="s">
-        <v>790</v>
+        <v>756</v>
       </c>
     </row>
     <row r="758" spans="1:1">
       <c r="A758" t="s">
-        <v>791</v>
+        <v>757</v>
       </c>
     </row>
     <row r="759" spans="1:1">
       <c r="A759" t="s">
-        <v>792</v>
+        <v>758</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
edits to align with 10.0 changes
</commit_message>
<xml_diff>
--- a/templates/panos/set_commands/iron_skillet_panos_full.xlsx
+++ b/templates/panos/set_commands/iron_skillet_panos_full.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="710">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="647">
   <si>
     <t>Variable Name</t>
   </si>
@@ -26,117 +26,39 @@
     <t>Description</t>
   </si>
   <si>
-    <t>PANORAMA_NAME</t>
-  </si>
-  <si>
-    <t>panorama01</t>
-  </si>
-  <si>
-    <t>Panorama hostname</t>
-  </si>
-  <si>
-    <t>PANORAMA_TYPE</t>
-  </si>
-  <si>
-    <t>static</t>
-  </si>
-  <si>
-    <t>Panorama management IP type - static or cloud (for dhcp)</t>
-  </si>
-  <si>
-    <t>PANORAMA_IP</t>
-  </si>
-  <si>
-    <t>192.168.55.161</t>
-  </si>
-  <si>
-    <t>Panorama IP</t>
-  </si>
-  <si>
-    <t>PANORAMA_MASK</t>
+    <t>FW_NAME</t>
+  </si>
+  <si>
+    <t>panos-01</t>
+  </si>
+  <si>
+    <t>Firewall hostname</t>
+  </si>
+  <si>
+    <t>MGMT_TYPE</t>
+  </si>
+  <si>
+    <t>dhcp-client</t>
+  </si>
+  <si>
+    <t>firewall management IP type</t>
+  </si>
+  <si>
+    <t>MGMT_IP</t>
+  </si>
+  <si>
+    <t>192.0.2.6</t>
+  </si>
+  <si>
+    <t>NGFW management IP</t>
+  </si>
+  <si>
+    <t>MGMT_MASK</t>
   </si>
   <si>
     <t>255.255.255.0</t>
   </si>
   <si>
-    <t>Panorama netmask</t>
-  </si>
-  <si>
-    <t>PANORAMA_DG</t>
-  </si>
-  <si>
-    <t>192.168.55.2</t>
-  </si>
-  <si>
-    <t>Panorama default gateway</t>
-  </si>
-  <si>
-    <t>CONFIG_EXPORT_IP</t>
-  </si>
-  <si>
-    <t>192.0.2.3</t>
-  </si>
-  <si>
-    <t>IP address for scheduled config exports</t>
-  </si>
-  <si>
-    <t>TEMPLATE</t>
-  </si>
-  <si>
-    <t>sample_template</t>
-  </si>
-  <si>
-    <t>Template name for Panorama</t>
-  </si>
-  <si>
-    <t>STACK</t>
-  </si>
-  <si>
-    <t>sample_stack</t>
-  </si>
-  <si>
-    <t>Template stack name for Panorama</t>
-  </si>
-  <si>
-    <t>DEVICE_GROUP</t>
-  </si>
-  <si>
-    <t>sample_devicegroup</t>
-  </si>
-  <si>
-    <t>Device-group name for Panorama</t>
-  </si>
-  <si>
-    <t>FW_NAME</t>
-  </si>
-  <si>
-    <t>sample</t>
-  </si>
-  <si>
-    <t>Device Name for NGFW</t>
-  </si>
-  <si>
-    <t>MGMT_TYPE</t>
-  </si>
-  <si>
-    <t>firewall management IP type (static or dhcp-client)</t>
-  </si>
-  <si>
-    <t>MGMT_IP</t>
-  </si>
-  <si>
-    <t>192.0.2.6</t>
-  </si>
-  <si>
-    <t>NGFW management IP</t>
-  </si>
-  <si>
-    <t>MGMT_MASK</t>
-  </si>
-  <si>
-    <t>255.255.128.0</t>
-  </si>
-  <si>
     <t>NGFW management netmask</t>
   </si>
   <si>
@@ -155,7 +77,7 @@
     <t>0.pool.ntp.org</t>
   </si>
   <si>
-    <t>Network Time Protocol Server</t>
+    <t>primary NTP server</t>
   </si>
   <si>
     <t>NTP_2</t>
@@ -164,7 +86,7 @@
     <t>1.pool.ntp.org</t>
   </si>
   <si>
-    <t>Network Time Protocol Server 2</t>
+    <t>secondary NTP server</t>
   </si>
   <si>
     <t>ADMINISTRATOR_USERNAME</t>
@@ -206,7 +128,7 @@
     <t>sinkhole.paloaltonetworks.com</t>
   </si>
   <si>
-    <t>sinkhole address IPv4</t>
+    <t>sinkhole FQDN IPv4</t>
   </si>
   <si>
     <t>SINKHOLE_IPV6</t>
@@ -218,15 +140,6 @@
     <t>sinkhole address IPv6</t>
   </si>
   <si>
-    <t>INTERNET_ZONE</t>
-  </si>
-  <si>
-    <t>internet</t>
-  </si>
-  <si>
-    <t>untrust zone to filter out in reports</t>
-  </si>
-  <si>
     <t>EMAIL_PROFILE_GATEWAY</t>
   </si>
   <si>
@@ -269,15 +182,6 @@
     <t>lifetime for the api key in minutes</t>
   </si>
   <si>
-    <t>INCLUDE_PAN_EDL</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>include the predefined Palo Alto Networks external lists security rules</t>
-  </si>
-  <si>
     <t># set command configuration for panos v9.1</t>
   </si>
   <si>
@@ -422,9 +326,6 @@
     <t>set deviceconfig setting ctd x-forwarded-for yes</t>
   </si>
   <si>
-    <t>set deviceconfig setting ctd allow-http-range no</t>
-  </si>
-  <si>
     <t>set deviceconfig setting ctd tcp-bypass-exceed-queue no</t>
   </si>
   <si>
@@ -620,27 +521,12 @@
     <t>set shared log-settings profiles default match-list Email_Malicious_Verdicts log-type wildfire</t>
   </si>
   <si>
-    <t>set shared log-settings profiles default match-list Email_Malicious_Verdicts filter ""(verdict eq malicious)""</t>
+    <t>set shared log-settings profiles default match-list Email_Malicious_Verdicts filter ""(verdict neq benign)""</t>
   </si>
   <si>
     <t>set shared log-settings profiles default match-list Email_Malicious_Verdicts send-to-panorama no</t>
   </si>
   <si>
-    <t>set shared log-settings profiles default match-list Email_Phishing_Verdicts send-email Sample_Email_Profile</t>
-  </si>
-  <si>
-    <t>set shared log-settings profiles default match-list Email_Phishing_Verdicts action-desc ""Email Phishing Wildfire Verdicts""</t>
-  </si>
-  <si>
-    <t>set shared log-settings profiles default match-list Email_Phishing_Verdicts log-type wildfire</t>
-  </si>
-  <si>
-    <t>set shared log-settings profiles default match-list Email_Phishing_Verdicts filter ""(verdict eq phishing)""</t>
-  </si>
-  <si>
-    <t>set shared log-settings profiles default match-list Email_Phishing_Verdicts send-to-panorama no</t>
-  </si>
-  <si>
     <t>set shared log-settings profiles default match-list Wildfire_Log_Forwarding log-type wildfire</t>
   </si>
   <si>
@@ -713,10 +599,7 @@
     <t>set tag Internal comments ""Internal to Internal""</t>
   </si>
   <si>
-    <t>set tag iron-skillet-version comments ""version 0.0.1 for 9.1: version of this IronSkillet template file""</t>
-  </si>
-  <si>
-    <t>#Address objects used for sinkholing and security rules match</t>
+    <t>set tag iron-skillet-version comments ""version 0.0.2 for 9.1: version of this IronSkillet template file""</t>
   </si>
   <si>
     <t>#File Blocking Profile</t>
@@ -977,10 +860,10 @@
     <t>#URL Filtering Profile</t>
   </si>
   <si>
-    <t>set profiles custom-url-category Black-List type ""URL List""</t>
-  </si>
-  <si>
-    <t>set profiles custom-url-category White-List type ""URL List""</t>
+    <t>set profiles custom-url-category Block type ""URL List""</t>
+  </si>
+  <si>
+    <t>set profiles custom-url-category Allow type ""URL List""</t>
   </si>
   <si>
     <t>set profiles custom-url-category Custom-No-Decrypt type ""URL List""</t>
@@ -992,7 +875,7 @@
     <t>set profiles url-filtering Outbound-URL credential-enforcement log-severity high</t>
   </si>
   <si>
-    <t>set profiles url-filtering Outbound-URL credential-enforcement block [ Black-List White-List abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement cryptocurrency dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government grayware hacking health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk malware medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting ]</t>
+    <t>set profiles url-filtering Outbound-URL credential-enforcement block [ Block Allow abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement cryptocurrency dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government grayware hacking health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk malware medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting ]</t>
   </si>
   <si>
     <t>set profiles url-filtering Outbound-URL log-http-hdr-user-agent yes</t>
@@ -1004,10 +887,10 @@
     <t>set profiles url-filtering Outbound-URL log-http-hdr-xff yes</t>
   </si>
   <si>
-    <t>set profiles url-filtering Outbound-URL alert [ White-List abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy computer-and-internet-info content-delivery-networks copyright-infringement cryptocurrency dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting ]</t>
-  </si>
-  <si>
-    <t>set profiles url-filtering Outbound-URL block [ Black-List command-and-control grayware hacking malware phishing ]</t>
+    <t>set profiles url-filtering Outbound-URL alert [ Allow abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy computer-and-internet-info content-delivery-networks copyright-infringement cryptocurrency dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government hacking health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting ]</t>
+  </si>
+  <si>
+    <t>set profiles url-filtering Outbound-URL block [ Block command-and-control grayware malware phishing ]</t>
   </si>
   <si>
     <t>set profiles url-filtering Alert-Only-URL credential-enforcement mode ip-user</t>
@@ -1016,10 +899,10 @@
     <t>set profiles url-filtering Alert-Only-URL credential-enforcement log-severity medium</t>
   </si>
   <si>
-    <t>set profiles url-filtering Alert-Only-URL credential-enforcement alert [ Black-List White-List abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement cryptocurrency dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government grayware hacking health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk malware medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting ]</t>
-  </si>
-  <si>
-    <t>set profiles url-filtering Alert-Only-URL alert [ Black-List White-List abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement cryptocurrency dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government grayware hacking health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk malware medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting ]</t>
+    <t>set profiles url-filtering Alert-Only-URL credential-enforcement alert [ Block Allow abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement cryptocurrency dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government grayware hacking health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk malware medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting ]</t>
+  </si>
+  <si>
+    <t>set profiles url-filtering Alert-Only-URL alert [ Block Allow abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement cryptocurrency dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government grayware hacking health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk malware medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting ]</t>
   </si>
   <si>
     <t>set profiles url-filtering Exception-URL credential-enforcement mode ip-user</t>
@@ -1028,7 +911,7 @@
     <t>set profiles url-filtering Exception-URL credential-enforcement log-severity high</t>
   </si>
   <si>
-    <t>set profiles url-filtering Exception-URL credential-enforcement block [ Black-List White-List abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement cryptocurrency dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government grayware hacking health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk malware medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting ]</t>
+    <t>set profiles url-filtering Exception-URL credential-enforcement block [ Block Allow abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy command-and-control computer-and-internet-info content-delivery-networks copyright-infringement cryptocurrency dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government grayware hacking health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk malware medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy phishing private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting ]</t>
   </si>
   <si>
     <t>set profiles url-filtering Exception-URL log-http-hdr-user-agent yes</t>
@@ -1040,10 +923,10 @@
     <t>set profiles url-filtering Exception-URL log-http-hdr-xff yes</t>
   </si>
   <si>
-    <t>set profiles url-filtering Exception-URL alert [ White-List abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy computer-and-internet-info content-delivery-networks copyright-infringement cryptocurrency dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting ]</t>
-  </si>
-  <si>
-    <t>set profiles url-filtering Exception-URL block [ Black-List command-and-control grayware hacking malware phishing ]</t>
+    <t>set profiles url-filtering Exception-URL alert [ Allow abortion abused-drugs adult alcohol-and-tobacco auctions business-and-economy computer-and-internet-info content-delivery-networks copyright-infringement cryptocurrency dating dynamic-dns educational-institutions entertainment-and-arts extremism financial-services gambling games government hacking health-and-medicine high-risk home-and-garden hunting-and-fishing insufficient-content internet-communications-and-telephony internet-portals job-search legal low-risk medium-risk military motor-vehicles music newly-registered-domain news not-resolved nudity online-storage-and-backup parked peer-to-peer personal-sites-and-blogs philosophy-and-political-advocacy private-ip-addresses proxy-avoidance-and-anonymizers questionable real-estate recreation-and-hobbies reference-and-research religion search-engines sex-education shareware-and-freeware shopping social-networking society sports stock-advice-and-tools streaming-media swimsuits-and-intimate-apparel training-and-tools translation travel unknown weapons web-advertisements web-based-email web-hosting ]</t>
+  </si>
+  <si>
+    <t>set profiles url-filtering Exception-URL block [ Block command-and-control grayware malware phishing ]</t>
   </si>
   <si>
     <t>#AntiVirus Profiles</t>
@@ -1682,45 +1565,6 @@
     <t>set rulebase security rules ""Inbound Block Rule"" tag Inbound</t>
   </si>
   <si>
-    <t>set rulebase security rules ""DNS Sinkhole Block"" description ""Block outbound sessions that match a malicious domain and have been redirected to a configured sinkhole IP address.""</t>
-  </si>
-  <si>
-    <t>set rulebase security rules ""DNS Sinkhole Block"" to any</t>
-  </si>
-  <si>
-    <t>set rulebase security rules ""DNS Sinkhole Block"" from any</t>
-  </si>
-  <si>
-    <t>set rulebase security rules ""DNS Sinkhole Block"" source any</t>
-  </si>
-  <si>
-    <t>set rulebase security rules ""DNS Sinkhole Block"" destination [ Sinkhole-IPv4 Sinkhole-IPv6 ]</t>
-  </si>
-  <si>
-    <t>set rulebase security rules ""DNS Sinkhole Block"" source-user any</t>
-  </si>
-  <si>
-    <t>set rulebase security rules ""DNS Sinkhole Block"" category any</t>
-  </si>
-  <si>
-    <t>set rulebase security rules ""DNS Sinkhole Block"" application any</t>
-  </si>
-  <si>
-    <t>set rulebase security rules ""DNS Sinkhole Block"" service any</t>
-  </si>
-  <si>
-    <t>set rulebase security rules ""DNS Sinkhole Block"" hip-profiles any</t>
-  </si>
-  <si>
-    <t>set rulebase security rules ""DNS Sinkhole Block"" action deny</t>
-  </si>
-  <si>
-    <t>set rulebase security rules ""DNS Sinkhole Block"" log-setting default</t>
-  </si>
-  <si>
-    <t>set rulebase security rules ""DNS Sinkhole Block"" tag Outbound</t>
-  </si>
-  <si>
     <t>#Recommended Decryption Profiles</t>
   </si>
   <si>
@@ -1812,39 +1656,6 @@
   </si>
   <si>
     <t>set rulebase decryption rules ""NO-Decrypt URL Categories"" description ""This rule does not do Decryption.  This rule is validating SSL Protocol Communications.""</t>
-  </si>
-  <si>
-    <t>set rulebase decryption rules ""NO-Decrypt Rule"" category any</t>
-  </si>
-  <si>
-    <t>set rulebase decryption rules ""NO-Decrypt Rule"" service any</t>
-  </si>
-  <si>
-    <t>set rulebase decryption rules ""NO-Decrypt Rule"" type ssl-forward-proxy</t>
-  </si>
-  <si>
-    <t>set rulebase decryption rules ""NO-Decrypt Rule"" from any</t>
-  </si>
-  <si>
-    <t>set rulebase decryption rules ""NO-Decrypt Rule"" to any</t>
-  </si>
-  <si>
-    <t>set rulebase decryption rules ""NO-Decrypt Rule"" source any</t>
-  </si>
-  <si>
-    <t>set rulebase decryption rules ""NO-Decrypt Rule"" destination any</t>
-  </si>
-  <si>
-    <t>set rulebase decryption rules ""NO-Decrypt Rule"" source-user any</t>
-  </si>
-  <si>
-    <t>set rulebase decryption rules ""NO-Decrypt Rule"" profile Recommended_Decryption_Profile</t>
-  </si>
-  <si>
-    <t>set rulebase decryption rules ""NO-Decrypt Rule"" action no-decrypt</t>
-  </si>
-  <si>
-    <t>set rulebase decryption rules ""NO-Decrypt Rule"" description ""This rule does not do Decryption.  This rule is validating SSL Protocol Communications.""</t>
   </si>
   <si>
     <t>#Zone Protection Profiles - To Be Added to each Configured Zone</t>
@@ -2485,7 +2296,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2599,29 +2410,29 @@
         <v>27</v>
       </c>
       <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
         <v>28</v>
-      </c>
-      <c r="C10" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
         <v>30</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>31</v>
-      </c>
-      <c r="C11" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
         <v>33</v>
-      </c>
-      <c r="B12" t="s">
-        <v>7</v>
       </c>
       <c r="C12" t="s">
         <v>34</v>
@@ -2697,132 +2508,11 @@
       <c r="A19" t="s">
         <v>53</v>
       </c>
-      <c r="B19" t="s">
-        <v>51</v>
+      <c r="B19">
+        <v>525600</v>
       </c>
       <c r="C19" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="s">
-        <v>55</v>
-      </c>
-      <c r="B20" t="s">
-        <v>56</v>
-      </c>
-      <c r="C20" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" t="s">
-        <v>58</v>
-      </c>
-      <c r="B21" t="s">
-        <v>59</v>
-      </c>
-      <c r="C21" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" t="s">
-        <v>61</v>
-      </c>
-      <c r="B22" t="s">
-        <v>62</v>
-      </c>
-      <c r="C22" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" t="s">
-        <v>64</v>
-      </c>
-      <c r="B23" t="s">
-        <v>65</v>
-      </c>
-      <c r="C23" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" t="s">
-        <v>67</v>
-      </c>
-      <c r="B24" t="s">
-        <v>68</v>
-      </c>
-      <c r="C24" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" t="s">
-        <v>70</v>
-      </c>
-      <c r="B25" t="s">
-        <v>71</v>
-      </c>
-      <c r="C25" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" t="s">
-        <v>73</v>
-      </c>
-      <c r="B26" t="s">
-        <v>74</v>
-      </c>
-      <c r="C26" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" t="s">
-        <v>76</v>
-      </c>
-      <c r="B27" t="s">
-        <v>77</v>
-      </c>
-      <c r="C27" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" t="s">
-        <v>79</v>
-      </c>
-      <c r="B28" t="s">
-        <v>80</v>
-      </c>
-      <c r="C28" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" t="s">
-        <v>82</v>
-      </c>
-      <c r="B29">
-        <v>525600</v>
-      </c>
-      <c r="C29" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" t="s">
-        <v>84</v>
-      </c>
-      <c r="B30" t="s">
-        <v>85</v>
-      </c>
-      <c r="C30" t="s">
-        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -2832,7 +2522,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:A680"/>
+  <dimension ref="A2:A646"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2840,3284 +2530,3117 @@
   <sheetData>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>88</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>89</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>90</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>91</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8">
-        <f>SUBSTITUTE("set deviceconfig system hostname {{ FW_NAME }}", "{{ FW_NAME }}", 'values'!B11)</f>
+        <f>SUBSTITUTE("set deviceconfig system hostname {{ FW_NAME }}", "{{ FW_NAME }}", 'values'!B2)</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9">
-        <f>SUBSTITUTE("set deviceconfig system ip-address {{ MGMT_IP }}", "{{ MGMT_IP }}", 'values'!B13)</f>
+        <f>SUBSTITUTE("set deviceconfig system ip-address {{ MGMT_IP }}", "{{ MGMT_IP }}", 'values'!B4)</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10">
-        <f>SUBSTITUTE("set deviceconfig system netmask {{ MGMT_MASK }}", "{{ MGMT_MASK }}", 'values'!B14)</f>
+        <f>SUBSTITUTE("set deviceconfig system netmask {{ MGMT_MASK }}", "{{ MGMT_MASK }}", 'values'!B5)</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11">
-        <f>SUBSTITUTE("set deviceconfig system default-gateway {{ MGMT_DG }}", "{{ MGMT_DG }}", 'values'!B15)</f>
+        <f>SUBSTITUTE("set deviceconfig system default-gateway {{ MGMT_DG }}", "{{ MGMT_DG }}", 'values'!B6)</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12">
-        <f>SUBSTITUTE("set deviceconfig system dns-setting servers primary {{ DNS_1 }}", "{{ DNS_1 }}", 'values'!B20)</f>
+        <f>SUBSTITUTE("set deviceconfig system dns-setting servers primary {{ DNS_1 }}", "{{ DNS_1 }}", 'values'!B11)</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13">
-        <f>SUBSTITUTE("set deviceconfig system dns-setting servers secondary {{ DNS_2 }}", "{{ DNS_2 }}", 'values'!B21)</f>
+        <f>SUBSTITUTE("set deviceconfig system dns-setting servers secondary {{ DNS_2 }}", "{{ DNS_2 }}", 'values'!B12)</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>92</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>93</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>94</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>95</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22">
-        <f>SUBSTITUTE("set deviceconfig system ntp-servers primary-ntp-server ntp-server-address {{ NTP_1 }}", "{{ NTP_1 }}", 'values'!B16)</f>
+        <f>SUBSTITUTE("set deviceconfig system ntp-servers primary-ntp-server ntp-server-address {{ NTP_1 }}", "{{ NTP_1 }}", 'values'!B7)</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23">
-        <f>SUBSTITUTE("set deviceconfig system ntp-servers secondary-ntp-server ntp-server-address {{ NTP_2 }}", "{{ NTP_2 }}", 'values'!B17)</f>
+        <f>SUBSTITUTE("set deviceconfig system ntp-servers secondary-ntp-server ntp-server-address {{ NTP_2 }}", "{{ NTP_2 }}", 'values'!B8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>98</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26">
-        <f>SUBSTITUTE("set mgt-config users {{ ADMINISTRATOR_USERNAME }} password", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B18)</f>
+        <f>SUBSTITUTE("set mgt-config users {{ ADMINISTRATOR_USERNAME }} password", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27">
-        <f>SUBSTITUTE("set mgt-config users {{ ADMINISTRATOR_USERNAME }} permissions role-based superuser yes", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B18)</f>
+        <f>SUBSTITUTE("set mgt-config users {{ ADMINISTRATOR_USERNAME }} permissions role-based superuser yes", "{{ ADMINISTRATOR_USERNAME }}", 'values'!B9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>99</v>
+        <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>100</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>101</v>
+        <v>69</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>102</v>
+        <v>70</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>103</v>
+        <v>71</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>104</v>
+        <v>72</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>105</v>
+        <v>73</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>106</v>
+        <v>74</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>107</v>
+        <v>75</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>108</v>
+        <v>76</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" t="s">
-        <v>110</v>
+        <v>78</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>111</v>
+        <v>79</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>112</v>
+        <v>80</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" t="s">
-        <v>113</v>
+        <v>81</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" t="s">
-        <v>114</v>
+        <v>82</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" t="s">
-        <v>115</v>
+        <v>83</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" t="s">
-        <v>116</v>
+        <v>84</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" t="s">
-        <v>117</v>
+        <v>85</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" t="s">
-        <v>118</v>
+        <v>86</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" t="s">
-        <v>119</v>
+        <v>87</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" t="s">
-        <v>120</v>
+        <v>88</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" t="s">
-        <v>121</v>
+        <v>89</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" t="s">
-        <v>122</v>
+        <v>90</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" t="s">
-        <v>123</v>
+        <v>91</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" t="s">
-        <v>124</v>
+        <v>92</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" t="s">
-        <v>125</v>
+        <v>93</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" t="s">
-        <v>126</v>
+        <v>94</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" t="s">
-        <v>127</v>
+        <v>95</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60" t="s">
-        <v>128</v>
+        <v>96</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" t="s">
-        <v>129</v>
+        <v>97</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" t="s">
-        <v>130</v>
+        <v>98</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" t="s">
-        <v>131</v>
+        <v>99</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64" t="s">
-        <v>132</v>
+        <v>100</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" t="s">
-        <v>133</v>
+        <v>101</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" t="s">
-        <v>134</v>
+        <v>102</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" t="s">
-        <v>135</v>
+        <v>103</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" t="s">
-        <v>136</v>
+        <v>104</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" t="s">
-        <v>137</v>
+        <v>105</v>
       </c>
     </row>
     <row r="70" spans="1:1">
-      <c r="A70" t="s">
-        <v>138</v>
+      <c r="A70">
+        <f>SUBSTITUTE("set deviceconfig setting management api key lifetime {{ API_KEY_LIFETIME }}", "{{ API_KEY_LIFETIME }}", 'values'!B19)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:1">
-      <c r="A71">
-        <f>SUBSTITUTE("set deviceconfig setting management api key lifetime {{ API_KEY_LIFETIME }}", "{{ API_KEY_LIFETIME }}", 'values'!B29)</f>
-        <v>0</v>
+      <c r="A71" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" t="s">
-        <v>139</v>
+        <v>107</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73" t="s">
-        <v>140</v>
+        <v>108</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74" t="s">
-        <v>141</v>
+        <v>109</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75" t="s">
-        <v>142</v>
+        <v>110</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" t="s">
-        <v>143</v>
+        <v>111</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77" t="s">
-        <v>144</v>
+        <v>112</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" t="s">
-        <v>145</v>
+        <v>113</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79" t="s">
-        <v>146</v>
+        <v>114</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80" t="s">
-        <v>147</v>
+        <v>115</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81" t="s">
-        <v>148</v>
+        <v>116</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" t="s">
-        <v>149</v>
+        <v>117</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83" t="s">
-        <v>150</v>
+        <v>118</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84" t="s">
-        <v>151</v>
+        <v>119</v>
       </c>
     </row>
     <row r="85" spans="1:1">
       <c r="A85" t="s">
-        <v>152</v>
+        <v>120</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86" t="s">
-        <v>153</v>
+        <v>121</v>
       </c>
     </row>
     <row r="87" spans="1:1">
       <c r="A87" t="s">
-        <v>154</v>
+        <v>122</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88" t="s">
-        <v>155</v>
+        <v>123</v>
       </c>
     </row>
     <row r="89" spans="1:1">
       <c r="A89" t="s">
-        <v>156</v>
+        <v>124</v>
       </c>
     </row>
     <row r="90" spans="1:1">
       <c r="A90" t="s">
-        <v>157</v>
+        <v>125</v>
       </c>
     </row>
     <row r="91" spans="1:1">
       <c r="A91" t="s">
-        <v>158</v>
+        <v>126</v>
       </c>
     </row>
     <row r="92" spans="1:1">
       <c r="A92" t="s">
-        <v>159</v>
+        <v>127</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93" t="s">
-        <v>160</v>
+        <v>128</v>
       </c>
     </row>
     <row r="94" spans="1:1">
       <c r="A94" t="s">
-        <v>161</v>
+        <v>129</v>
       </c>
     </row>
     <row r="95" spans="1:1">
       <c r="A95" t="s">
-        <v>162</v>
+        <v>130</v>
       </c>
     </row>
     <row r="96" spans="1:1">
       <c r="A96" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="97" spans="1:1">
-      <c r="A97" t="s">
-        <v>164</v>
+        <v>131</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="100" spans="1:1">
       <c r="A100" t="s">
-        <v>165</v>
+        <v>133</v>
       </c>
     </row>
     <row r="101" spans="1:1">
-      <c r="A101" t="s">
-        <v>166</v>
+      <c r="A101">
+        <f>SUBSTITUTE("set shared log-settings email Sample_Email_Profile server Sample_Email_Profile gateway {{ EMAIL_PROFILE_GATEWAY }}", "{{ EMAIL_PROFILE_GATEWAY }}", 'values'!B15)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:1">
       <c r="A102">
-        <f>SUBSTITUTE("set shared log-settings email Sample_Email_Profile server Sample_Email_Profile gateway {{ EMAIL_PROFILE_GATEWAY }}", "{{ EMAIL_PROFILE_GATEWAY }}", 'values'!B25)</f>
+        <f>SUBSTITUTE("set shared log-settings email Sample_Email_Profile server Sample_Email_Profile from {{ EMAIL_PROFILE_FROM }}", "{{ EMAIL_PROFILE_FROM }}", 'values'!B16)</f>
         <v>0</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103">
-        <f>SUBSTITUTE("set shared log-settings email Sample_Email_Profile server Sample_Email_Profile from {{ EMAIL_PROFILE_FROM }}", "{{ EMAIL_PROFILE_FROM }}", 'values'!B26)</f>
+        <f>SUBSTITUTE("set shared log-settings email Sample_Email_Profile server Sample_Email_Profile to {{ EMAIL_PROFILE_TO }}", "{{ EMAIL_PROFILE_TO }}", 'values'!B17)</f>
         <v>0</v>
       </c>
     </row>
     <row r="104" spans="1:1">
-      <c r="A104">
-        <f>SUBSTITUTE("set shared log-settings email Sample_Email_Profile server Sample_Email_Profile to {{ EMAIL_PROFILE_TO }}", "{{ EMAIL_PROFILE_TO }}", 'values'!B27)</f>
-        <v>0</v>
+      <c r="A104" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="105" spans="1:1">
       <c r="A105" t="s">
-        <v>167</v>
+        <v>135</v>
       </c>
     </row>
     <row r="106" spans="1:1">
       <c r="A106" t="s">
-        <v>168</v>
+        <v>136</v>
       </c>
     </row>
     <row r="107" spans="1:1">
-      <c r="A107" t="s">
-        <v>169</v>
+      <c r="A107">
+        <f>SUBSTITUTE("set shared log-settings syslog Sample_Syslog_Profile server Sample_Syslog server {{ SYSLOG_SERVER }}", "{{ SYSLOG_SERVER }}", 'values'!B18)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="108" spans="1:1">
-      <c r="A108">
-        <f>SUBSTITUTE("set shared log-settings syslog Sample_Syslog_Profile server Sample_Syslog server {{ SYSLOG_SERVER }}", "{{ SYSLOG_SERVER }}", 'values'!B28)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="109" spans="1:1">
-      <c r="A109" t="s">
-        <v>170</v>
+      <c r="A108" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1">
+      <c r="A110" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="111" spans="1:1">
       <c r="A111" t="s">
-        <v>171</v>
+        <v>139</v>
       </c>
     </row>
     <row r="112" spans="1:1">
       <c r="A112" t="s">
-        <v>172</v>
+        <v>140</v>
       </c>
     </row>
     <row r="113" spans="1:1">
       <c r="A113" t="s">
-        <v>173</v>
+        <v>141</v>
       </c>
     </row>
     <row r="114" spans="1:1">
       <c r="A114" t="s">
-        <v>174</v>
+        <v>142</v>
       </c>
     </row>
     <row r="115" spans="1:1">
       <c r="A115" t="s">
-        <v>175</v>
+        <v>143</v>
       </c>
     </row>
     <row r="116" spans="1:1">
       <c r="A116" t="s">
-        <v>176</v>
+        <v>144</v>
       </c>
     </row>
     <row r="117" spans="1:1">
       <c r="A117" t="s">
-        <v>177</v>
+        <v>145</v>
       </c>
     </row>
     <row r="118" spans="1:1">
       <c r="A118" t="s">
-        <v>178</v>
+        <v>146</v>
       </c>
     </row>
     <row r="119" spans="1:1">
       <c r="A119" t="s">
-        <v>179</v>
+        <v>147</v>
       </c>
     </row>
     <row r="120" spans="1:1">
       <c r="A120" t="s">
-        <v>180</v>
+        <v>148</v>
       </c>
     </row>
     <row r="121" spans="1:1">
       <c r="A121" t="s">
-        <v>181</v>
+        <v>149</v>
       </c>
     </row>
     <row r="122" spans="1:1">
       <c r="A122" t="s">
-        <v>182</v>
+        <v>150</v>
       </c>
     </row>
     <row r="123" spans="1:1">
       <c r="A123" t="s">
-        <v>183</v>
+        <v>151</v>
       </c>
     </row>
     <row r="124" spans="1:1">
       <c r="A124" t="s">
-        <v>184</v>
+        <v>152</v>
       </c>
     </row>
     <row r="125" spans="1:1">
       <c r="A125" t="s">
-        <v>185</v>
+        <v>153</v>
       </c>
     </row>
     <row r="126" spans="1:1">
       <c r="A126" t="s">
-        <v>186</v>
+        <v>154</v>
       </c>
     </row>
     <row r="127" spans="1:1">
       <c r="A127" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="128" spans="1:1">
-      <c r="A128" t="s">
-        <v>188</v>
+        <v>155</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1">
+      <c r="A130" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="131" spans="1:1">
       <c r="A131" t="s">
-        <v>189</v>
+        <v>157</v>
       </c>
     </row>
     <row r="132" spans="1:1">
       <c r="A132" t="s">
-        <v>190</v>
+        <v>158</v>
       </c>
     </row>
     <row r="133" spans="1:1">
       <c r="A133" t="s">
-        <v>191</v>
+        <v>159</v>
       </c>
     </row>
     <row r="134" spans="1:1">
       <c r="A134" t="s">
-        <v>192</v>
+        <v>160</v>
       </c>
     </row>
     <row r="135" spans="1:1">
       <c r="A135" t="s">
-        <v>193</v>
+        <v>161</v>
       </c>
     </row>
     <row r="136" spans="1:1">
       <c r="A136" t="s">
-        <v>194</v>
+        <v>162</v>
       </c>
     </row>
     <row r="137" spans="1:1">
       <c r="A137" t="s">
-        <v>195</v>
+        <v>163</v>
       </c>
     </row>
     <row r="138" spans="1:1">
       <c r="A138" t="s">
-        <v>196</v>
+        <v>164</v>
       </c>
     </row>
     <row r="139" spans="1:1">
       <c r="A139" t="s">
-        <v>197</v>
+        <v>165</v>
       </c>
     </row>
     <row r="140" spans="1:1">
       <c r="A140" t="s">
-        <v>198</v>
+        <v>166</v>
       </c>
     </row>
     <row r="141" spans="1:1">
       <c r="A141" t="s">
-        <v>199</v>
+        <v>167</v>
       </c>
     </row>
     <row r="142" spans="1:1">
       <c r="A142" t="s">
-        <v>200</v>
+        <v>168</v>
       </c>
     </row>
     <row r="143" spans="1:1">
       <c r="A143" t="s">
-        <v>201</v>
+        <v>169</v>
       </c>
     </row>
     <row r="144" spans="1:1">
       <c r="A144" t="s">
-        <v>202</v>
+        <v>170</v>
       </c>
     </row>
     <row r="145" spans="1:1">
       <c r="A145" t="s">
-        <v>203</v>
+        <v>171</v>
       </c>
     </row>
     <row r="146" spans="1:1">
       <c r="A146" t="s">
-        <v>204</v>
+        <v>172</v>
       </c>
     </row>
     <row r="147" spans="1:1">
       <c r="A147" t="s">
-        <v>205</v>
+        <v>173</v>
       </c>
     </row>
     <row r="148" spans="1:1">
       <c r="A148" t="s">
-        <v>206</v>
+        <v>174</v>
       </c>
     </row>
     <row r="149" spans="1:1">
       <c r="A149" t="s">
-        <v>207</v>
+        <v>175</v>
       </c>
     </row>
     <row r="150" spans="1:1">
       <c r="A150" t="s">
-        <v>208</v>
+        <v>176</v>
       </c>
     </row>
     <row r="151" spans="1:1">
       <c r="A151" t="s">
-        <v>209</v>
+        <v>177</v>
       </c>
     </row>
     <row r="152" spans="1:1">
       <c r="A152" t="s">
-        <v>210</v>
+        <v>178</v>
       </c>
     </row>
     <row r="153" spans="1:1">
       <c r="A153" t="s">
-        <v>211</v>
+        <v>179</v>
       </c>
     </row>
     <row r="154" spans="1:1">
       <c r="A154" t="s">
-        <v>212</v>
+        <v>180</v>
       </c>
     </row>
     <row r="155" spans="1:1">
       <c r="A155" t="s">
-        <v>213</v>
+        <v>181</v>
       </c>
     </row>
     <row r="156" spans="1:1">
       <c r="A156" t="s">
-        <v>214</v>
+        <v>182</v>
       </c>
     </row>
     <row r="157" spans="1:1">
       <c r="A157" t="s">
-        <v>215</v>
+        <v>183</v>
       </c>
     </row>
     <row r="158" spans="1:1">
       <c r="A158" t="s">
-        <v>216</v>
+        <v>184</v>
       </c>
     </row>
     <row r="159" spans="1:1">
       <c r="A159" t="s">
-        <v>217</v>
+        <v>185</v>
       </c>
     </row>
     <row r="160" spans="1:1">
       <c r="A160" t="s">
-        <v>218</v>
+        <v>186</v>
       </c>
     </row>
     <row r="161" spans="1:1">
       <c r="A161" t="s">
-        <v>219</v>
+        <v>187</v>
       </c>
     </row>
     <row r="162" spans="1:1">
       <c r="A162" t="s">
-        <v>220</v>
+        <v>188</v>
       </c>
     </row>
     <row r="163" spans="1:1">
       <c r="A163" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="164" spans="1:1">
-      <c r="A164" t="s">
-        <v>222</v>
+        <v>189</v>
       </c>
     </row>
     <row r="165" spans="1:1">
       <c r="A165" t="s">
-        <v>223</v>
+        <v>190</v>
       </c>
     </row>
     <row r="166" spans="1:1">
       <c r="A166" t="s">
-        <v>224</v>
+        <v>191</v>
       </c>
     </row>
     <row r="167" spans="1:1">
       <c r="A167" t="s">
-        <v>225</v>
+        <v>192</v>
       </c>
     </row>
     <row r="168" spans="1:1">
       <c r="A168" t="s">
-        <v>226</v>
+        <v>193</v>
       </c>
     </row>
     <row r="169" spans="1:1">
       <c r="A169" t="s">
-        <v>227</v>
+        <v>194</v>
       </c>
     </row>
     <row r="171" spans="1:1">
       <c r="A171" t="s">
-        <v>228</v>
+        <v>195</v>
       </c>
     </row>
     <row r="172" spans="1:1">
       <c r="A172" t="s">
-        <v>229</v>
+        <v>196</v>
       </c>
     </row>
     <row r="173" spans="1:1">
       <c r="A173" t="s">
-        <v>230</v>
+        <v>197</v>
       </c>
     </row>
     <row r="174" spans="1:1">
       <c r="A174" t="s">
-        <v>231</v>
+        <v>198</v>
       </c>
     </row>
     <row r="175" spans="1:1">
       <c r="A175" t="s">
-        <v>232</v>
+        <v>199</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1">
+      <c r="A176" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="177" spans="1:1">
       <c r="A177" t="s">
-        <v>233</v>
+        <v>201</v>
       </c>
     </row>
     <row r="178" spans="1:1">
-      <c r="A178">
-        <f>SUBSTITUTE("set address Sinkhole-IPv4 fqdn {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
-        <v>0</v>
+      <c r="A178" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="179" spans="1:1">
-      <c r="A179">
-        <f>SUBSTITUTE("set address Sinkhole-IPv6 ip-netmask {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
-        <v>0</v>
+      <c r="A179" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1">
+      <c r="A180" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="181" spans="1:1">
       <c r="A181" t="s">
-        <v>234</v>
+        <v>205</v>
       </c>
     </row>
     <row r="182" spans="1:1">
       <c r="A182" t="s">
-        <v>235</v>
+        <v>206</v>
       </c>
     </row>
     <row r="183" spans="1:1">
       <c r="A183" t="s">
-        <v>236</v>
+        <v>207</v>
       </c>
     </row>
     <row r="184" spans="1:1">
       <c r="A184" t="s">
-        <v>237</v>
+        <v>208</v>
       </c>
     </row>
     <row r="185" spans="1:1">
       <c r="A185" t="s">
-        <v>238</v>
+        <v>209</v>
       </c>
     </row>
     <row r="186" spans="1:1">
       <c r="A186" t="s">
-        <v>239</v>
+        <v>210</v>
       </c>
     </row>
     <row r="187" spans="1:1">
       <c r="A187" t="s">
-        <v>240</v>
+        <v>211</v>
       </c>
     </row>
     <row r="188" spans="1:1">
       <c r="A188" t="s">
-        <v>241</v>
+        <v>212</v>
       </c>
     </row>
     <row r="189" spans="1:1">
       <c r="A189" t="s">
-        <v>242</v>
+        <v>213</v>
       </c>
     </row>
     <row r="190" spans="1:1">
       <c r="A190" t="s">
-        <v>243</v>
+        <v>214</v>
       </c>
     </row>
     <row r="191" spans="1:1">
       <c r="A191" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="192" spans="1:1">
       <c r="A192" t="s">
-        <v>245</v>
+        <v>216</v>
       </c>
     </row>
     <row r="193" spans="1:1">
       <c r="A193" t="s">
-        <v>246</v>
+        <v>217</v>
       </c>
     </row>
     <row r="194" spans="1:1">
       <c r="A194" t="s">
-        <v>247</v>
+        <v>218</v>
       </c>
     </row>
     <row r="195" spans="1:1">
       <c r="A195" t="s">
-        <v>248</v>
+        <v>219</v>
       </c>
     </row>
     <row r="196" spans="1:1">
       <c r="A196" t="s">
-        <v>249</v>
+        <v>220</v>
       </c>
     </row>
     <row r="197" spans="1:1">
       <c r="A197" t="s">
-        <v>250</v>
+        <v>221</v>
       </c>
     </row>
     <row r="198" spans="1:1">
       <c r="A198" t="s">
-        <v>251</v>
+        <v>222</v>
       </c>
     </row>
     <row r="199" spans="1:1">
       <c r="A199" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="200" spans="1:1">
-      <c r="A200" t="s">
-        <v>253</v>
+        <v>223</v>
       </c>
     </row>
     <row r="201" spans="1:1">
       <c r="A201" t="s">
-        <v>254</v>
+        <v>224</v>
       </c>
     </row>
     <row r="202" spans="1:1">
-      <c r="A202" t="s">
-        <v>255</v>
+      <c r="A202">
+        <f>SUBSTITUTE("set profiles spyware Outbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B13)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="203" spans="1:1">
-      <c r="A203" t="s">
-        <v>256</v>
+      <c r="A203">
+        <f>SUBSTITUTE("set profiles spyware Outbound-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B14)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="204" spans="1:1">
       <c r="A204" t="s">
-        <v>257</v>
+        <v>225</v>
       </c>
     </row>
     <row r="205" spans="1:1">
       <c r="A205" t="s">
-        <v>258</v>
+        <v>226</v>
       </c>
     </row>
     <row r="206" spans="1:1">
       <c r="A206" t="s">
-        <v>259</v>
+        <v>227</v>
       </c>
     </row>
     <row r="207" spans="1:1">
       <c r="A207" t="s">
-        <v>260</v>
+        <v>228</v>
       </c>
     </row>
     <row r="208" spans="1:1">
       <c r="A208" t="s">
-        <v>261</v>
+        <v>229</v>
       </c>
     </row>
     <row r="209" spans="1:1">
       <c r="A209" t="s">
-        <v>262</v>
+        <v>230</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1">
+      <c r="A210" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="211" spans="1:1">
       <c r="A211" t="s">
-        <v>263</v>
+        <v>232</v>
       </c>
     </row>
     <row r="212" spans="1:1">
-      <c r="A212">
-        <f>SUBSTITUTE("set profiles spyware Outbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
-        <v>0</v>
+      <c r="A212" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="213" spans="1:1">
-      <c r="A213">
-        <f>SUBSTITUTE("set profiles spyware Outbound-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
-        <v>0</v>
+      <c r="A213" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="214" spans="1:1">
       <c r="A214" t="s">
-        <v>264</v>
+        <v>235</v>
       </c>
     </row>
     <row r="215" spans="1:1">
       <c r="A215" t="s">
-        <v>265</v>
+        <v>236</v>
       </c>
     </row>
     <row r="216" spans="1:1">
       <c r="A216" t="s">
-        <v>266</v>
+        <v>237</v>
       </c>
     </row>
     <row r="217" spans="1:1">
       <c r="A217" t="s">
-        <v>267</v>
+        <v>238</v>
       </c>
     </row>
     <row r="218" spans="1:1">
-      <c r="A218" t="s">
-        <v>268</v>
+      <c r="A218">
+        <f>SUBSTITUTE("set profiles spyware Inbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B13)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="219" spans="1:1">
-      <c r="A219" t="s">
-        <v>269</v>
+      <c r="A219">
+        <f>SUBSTITUTE("set profiles spyware Inbound-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B14)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="220" spans="1:1">
       <c r="A220" t="s">
-        <v>270</v>
+        <v>239</v>
       </c>
     </row>
     <row r="221" spans="1:1">
       <c r="A221" t="s">
-        <v>271</v>
+        <v>240</v>
       </c>
     </row>
     <row r="222" spans="1:1">
       <c r="A222" t="s">
-        <v>272</v>
+        <v>241</v>
       </c>
     </row>
     <row r="223" spans="1:1">
       <c r="A223" t="s">
-        <v>273</v>
+        <v>242</v>
       </c>
     </row>
     <row r="224" spans="1:1">
       <c r="A224" t="s">
-        <v>274</v>
+        <v>243</v>
       </c>
     </row>
     <row r="225" spans="1:1">
       <c r="A225" t="s">
-        <v>275</v>
+        <v>244</v>
       </c>
     </row>
     <row r="226" spans="1:1">
       <c r="A226" t="s">
-        <v>276</v>
+        <v>245</v>
       </c>
     </row>
     <row r="227" spans="1:1">
       <c r="A227" t="s">
-        <v>277</v>
+        <v>246</v>
       </c>
     </row>
     <row r="228" spans="1:1">
-      <c r="A228">
-        <f>SUBSTITUTE("set profiles spyware Inbound-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
-        <v>0</v>
+      <c r="A228" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="229" spans="1:1">
-      <c r="A229">
-        <f>SUBSTITUTE("set profiles spyware Inbound-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
-        <v>0</v>
+      <c r="A229" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="230" spans="1:1">
       <c r="A230" t="s">
-        <v>278</v>
+        <v>249</v>
       </c>
     </row>
     <row r="231" spans="1:1">
       <c r="A231" t="s">
-        <v>279</v>
+        <v>250</v>
       </c>
     </row>
     <row r="232" spans="1:1">
       <c r="A232" t="s">
-        <v>280</v>
+        <v>251</v>
       </c>
     </row>
     <row r="233" spans="1:1">
       <c r="A233" t="s">
-        <v>281</v>
+        <v>252</v>
       </c>
     </row>
     <row r="234" spans="1:1">
-      <c r="A234" t="s">
-        <v>282</v>
+      <c r="A234">
+        <f>SUBSTITUTE("set profiles spyware Internal-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B13)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="235" spans="1:1">
-      <c r="A235" t="s">
-        <v>283</v>
+      <c r="A235">
+        <f>SUBSTITUTE("set profiles spyware Internal-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B14)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="236" spans="1:1">
       <c r="A236" t="s">
-        <v>284</v>
+        <v>253</v>
       </c>
     </row>
     <row r="237" spans="1:1">
       <c r="A237" t="s">
-        <v>285</v>
+        <v>254</v>
       </c>
     </row>
     <row r="238" spans="1:1">
       <c r="A238" t="s">
-        <v>286</v>
+        <v>255</v>
       </c>
     </row>
     <row r="239" spans="1:1">
       <c r="A239" t="s">
-        <v>287</v>
+        <v>256</v>
       </c>
     </row>
     <row r="240" spans="1:1">
       <c r="A240" t="s">
-        <v>288</v>
+        <v>257</v>
       </c>
     </row>
     <row r="241" spans="1:1">
       <c r="A241" t="s">
-        <v>289</v>
+        <v>258</v>
       </c>
     </row>
     <row r="242" spans="1:1">
       <c r="A242" t="s">
-        <v>290</v>
+        <v>259</v>
       </c>
     </row>
     <row r="243" spans="1:1">
       <c r="A243" t="s">
-        <v>291</v>
+        <v>260</v>
       </c>
     </row>
     <row r="244" spans="1:1">
-      <c r="A244">
-        <f>SUBSTITUTE("set profiles spyware Internal-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
-        <v>0</v>
+      <c r="A244" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="245" spans="1:1">
-      <c r="A245">
-        <f>SUBSTITUTE("set profiles spyware Internal-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
-        <v>0</v>
+      <c r="A245" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="246" spans="1:1">
       <c r="A246" t="s">
-        <v>292</v>
+        <v>263</v>
       </c>
     </row>
     <row r="247" spans="1:1">
       <c r="A247" t="s">
-        <v>293</v>
+        <v>264</v>
       </c>
     </row>
     <row r="248" spans="1:1">
       <c r="A248" t="s">
-        <v>294</v>
+        <v>265</v>
       </c>
     </row>
     <row r="249" spans="1:1">
       <c r="A249" t="s">
-        <v>295</v>
+        <v>266</v>
       </c>
     </row>
     <row r="250" spans="1:1">
       <c r="A250" t="s">
-        <v>296</v>
+        <v>267</v>
       </c>
     </row>
     <row r="251" spans="1:1">
-      <c r="A251" t="s">
-        <v>297</v>
+      <c r="A251">
+        <f>SUBSTITUTE("set profiles spyware Alert-Only-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B13)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="252" spans="1:1">
-      <c r="A252" t="s">
-        <v>298</v>
+      <c r="A252">
+        <f>SUBSTITUTE("set profiles spyware Alert-Only-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B14)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="253" spans="1:1">
       <c r="A253" t="s">
-        <v>299</v>
+        <v>268</v>
       </c>
     </row>
     <row r="254" spans="1:1">
       <c r="A254" t="s">
-        <v>300</v>
+        <v>267</v>
       </c>
     </row>
     <row r="255" spans="1:1">
       <c r="A255" t="s">
-        <v>301</v>
+        <v>269</v>
       </c>
     </row>
     <row r="256" spans="1:1">
       <c r="A256" t="s">
-        <v>302</v>
+        <v>270</v>
       </c>
     </row>
     <row r="257" spans="1:1">
       <c r="A257" t="s">
-        <v>303</v>
+        <v>271</v>
       </c>
     </row>
     <row r="258" spans="1:1">
       <c r="A258" t="s">
-        <v>304</v>
+        <v>272</v>
       </c>
     </row>
     <row r="259" spans="1:1">
       <c r="A259" t="s">
-        <v>305</v>
+        <v>273</v>
       </c>
     </row>
     <row r="260" spans="1:1">
       <c r="A260" t="s">
-        <v>306</v>
+        <v>274</v>
       </c>
     </row>
     <row r="261" spans="1:1">
-      <c r="A261">
-        <f>SUBSTITUTE("set profiles spyware Alert-Only-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
-        <v>0</v>
+      <c r="A261" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="262" spans="1:1">
       <c r="A262">
-        <f>SUBSTITUTE("set profiles spyware Alert-Only-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
+        <f>SUBSTITUTE("set profiles spyware Exception-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B13)</f>
         <v>0</v>
       </c>
     </row>
     <row r="263" spans="1:1">
-      <c r="A263" t="s">
-        <v>307</v>
+      <c r="A263">
+        <f>SUBSTITUTE("set profiles spyware Exception-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B14)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="264" spans="1:1">
       <c r="A264" t="s">
-        <v>306</v>
+        <v>276</v>
       </c>
     </row>
     <row r="265" spans="1:1">
       <c r="A265" t="s">
-        <v>308</v>
+        <v>277</v>
       </c>
     </row>
     <row r="266" spans="1:1">
       <c r="A266" t="s">
-        <v>309</v>
+        <v>278</v>
       </c>
     </row>
     <row r="267" spans="1:1">
       <c r="A267" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="268" spans="1:1">
-      <c r="A268" t="s">
-        <v>311</v>
+        <v>279</v>
       </c>
     </row>
     <row r="269" spans="1:1">
       <c r="A269" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
     </row>
     <row r="270" spans="1:1">
       <c r="A270" t="s">
-        <v>313</v>
+        <v>281</v>
       </c>
     </row>
     <row r="271" spans="1:1">
       <c r="A271" t="s">
-        <v>314</v>
+        <v>282</v>
       </c>
     </row>
     <row r="272" spans="1:1">
-      <c r="A272">
-        <f>SUBSTITUTE("set profiles spyware Exception-AS botnet-domains sinkhole ipv4-address {{ SINKHOLE_IPV4 }}", "{{ SINKHOLE_IPV4 }}", 'values'!B22)</f>
-        <v>0</v>
+      <c r="A272" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="273" spans="1:1">
-      <c r="A273">
-        <f>SUBSTITUTE("set profiles spyware Exception-AS botnet-domains sinkhole ipv6-address {{ SINKHOLE_IPV6 }}", "{{ SINKHOLE_IPV6 }}", 'values'!B23)</f>
-        <v>0</v>
+      <c r="A273" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="274" spans="1:1">
       <c r="A274" t="s">
-        <v>315</v>
+        <v>285</v>
       </c>
     </row>
     <row r="275" spans="1:1">
       <c r="A275" t="s">
-        <v>316</v>
+        <v>286</v>
       </c>
     </row>
     <row r="276" spans="1:1">
       <c r="A276" t="s">
-        <v>317</v>
+        <v>287</v>
       </c>
     </row>
     <row r="277" spans="1:1">
       <c r="A277" t="s">
-        <v>318</v>
+        <v>288</v>
+      </c>
+    </row>
+    <row r="278" spans="1:1">
+      <c r="A278" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="279" spans="1:1">
       <c r="A279" t="s">
-        <v>319</v>
+        <v>290</v>
       </c>
     </row>
     <row r="280" spans="1:1">
       <c r="A280" t="s">
-        <v>320</v>
+        <v>291</v>
       </c>
     </row>
     <row r="281" spans="1:1">
       <c r="A281" t="s">
-        <v>321</v>
+        <v>292</v>
       </c>
     </row>
     <row r="282" spans="1:1">
       <c r="A282" t="s">
-        <v>322</v>
+        <v>293</v>
       </c>
     </row>
     <row r="283" spans="1:1">
       <c r="A283" t="s">
-        <v>323</v>
+        <v>294</v>
       </c>
     </row>
     <row r="284" spans="1:1">
       <c r="A284" t="s">
-        <v>324</v>
+        <v>295</v>
       </c>
     </row>
     <row r="285" spans="1:1">
       <c r="A285" t="s">
-        <v>325</v>
+        <v>296</v>
       </c>
     </row>
     <row r="286" spans="1:1">
       <c r="A286" t="s">
-        <v>326</v>
+        <v>297</v>
       </c>
     </row>
     <row r="287" spans="1:1">
       <c r="A287" t="s">
-        <v>327</v>
+        <v>298</v>
       </c>
     </row>
     <row r="288" spans="1:1">
       <c r="A288" t="s">
-        <v>328</v>
+        <v>299</v>
       </c>
     </row>
     <row r="289" spans="1:1">
       <c r="A289" t="s">
-        <v>329</v>
+        <v>300</v>
       </c>
     </row>
     <row r="290" spans="1:1">
       <c r="A290" t="s">
-        <v>330</v>
+        <v>301</v>
       </c>
     </row>
     <row r="291" spans="1:1">
       <c r="A291" t="s">
-        <v>331</v>
+        <v>302</v>
       </c>
     </row>
     <row r="292" spans="1:1">
       <c r="A292" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="293" spans="1:1">
-      <c r="A293" t="s">
-        <v>333</v>
+        <v>303</v>
       </c>
     </row>
     <row r="294" spans="1:1">
       <c r="A294" t="s">
-        <v>334</v>
+        <v>304</v>
       </c>
     </row>
     <row r="295" spans="1:1">
       <c r="A295" t="s">
-        <v>335</v>
+        <v>305</v>
       </c>
     </row>
     <row r="296" spans="1:1">
       <c r="A296" t="s">
-        <v>336</v>
+        <v>306</v>
       </c>
     </row>
     <row r="297" spans="1:1">
       <c r="A297" t="s">
-        <v>337</v>
+        <v>307</v>
       </c>
     </row>
     <row r="298" spans="1:1">
       <c r="A298" t="s">
-        <v>338</v>
+        <v>308</v>
       </c>
     </row>
     <row r="299" spans="1:1">
       <c r="A299" t="s">
-        <v>339</v>
+        <v>309</v>
       </c>
     </row>
     <row r="300" spans="1:1">
       <c r="A300" t="s">
-        <v>340</v>
+        <v>310</v>
       </c>
     </row>
     <row r="301" spans="1:1">
       <c r="A301" t="s">
-        <v>341</v>
+        <v>311</v>
       </c>
     </row>
     <row r="302" spans="1:1">
       <c r="A302" t="s">
-        <v>342</v>
+        <v>312</v>
+      </c>
+    </row>
+    <row r="303" spans="1:1">
+      <c r="A303" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="304" spans="1:1">
       <c r="A304" t="s">
-        <v>343</v>
+        <v>314</v>
       </c>
     </row>
     <row r="305" spans="1:1">
       <c r="A305" t="s">
-        <v>344</v>
+        <v>315</v>
       </c>
     </row>
     <row r="306" spans="1:1">
       <c r="A306" t="s">
-        <v>345</v>
+        <v>316</v>
       </c>
     </row>
     <row r="307" spans="1:1">
       <c r="A307" t="s">
-        <v>346</v>
+        <v>317</v>
       </c>
     </row>
     <row r="308" spans="1:1">
       <c r="A308" t="s">
-        <v>347</v>
+        <v>318</v>
       </c>
     </row>
     <row r="309" spans="1:1">
       <c r="A309" t="s">
-        <v>348</v>
+        <v>319</v>
       </c>
     </row>
     <row r="310" spans="1:1">
       <c r="A310" t="s">
-        <v>349</v>
+        <v>320</v>
       </c>
     </row>
     <row r="311" spans="1:1">
       <c r="A311" t="s">
-        <v>350</v>
+        <v>321</v>
       </c>
     </row>
     <row r="312" spans="1:1">
       <c r="A312" t="s">
-        <v>351</v>
+        <v>322</v>
       </c>
     </row>
     <row r="313" spans="1:1">
       <c r="A313" t="s">
-        <v>352</v>
+        <v>323</v>
       </c>
     </row>
     <row r="314" spans="1:1">
       <c r="A314" t="s">
-        <v>353</v>
+        <v>324</v>
       </c>
     </row>
     <row r="315" spans="1:1">
       <c r="A315" t="s">
-        <v>354</v>
+        <v>325</v>
       </c>
     </row>
     <row r="316" spans="1:1">
       <c r="A316" t="s">
-        <v>355</v>
+        <v>326</v>
       </c>
     </row>
     <row r="317" spans="1:1">
       <c r="A317" t="s">
-        <v>356</v>
+        <v>327</v>
       </c>
     </row>
     <row r="318" spans="1:1">
       <c r="A318" t="s">
-        <v>357</v>
+        <v>328</v>
       </c>
     </row>
     <row r="319" spans="1:1">
       <c r="A319" t="s">
-        <v>358</v>
+        <v>329</v>
       </c>
     </row>
     <row r="320" spans="1:1">
       <c r="A320" t="s">
-        <v>359</v>
+        <v>330</v>
       </c>
     </row>
     <row r="321" spans="1:1">
       <c r="A321" t="s">
-        <v>360</v>
+        <v>331</v>
       </c>
     </row>
     <row r="322" spans="1:1">
       <c r="A322" t="s">
-        <v>361</v>
+        <v>332</v>
       </c>
     </row>
     <row r="323" spans="1:1">
       <c r="A323" t="s">
-        <v>362</v>
+        <v>333</v>
       </c>
     </row>
     <row r="324" spans="1:1">
       <c r="A324" t="s">
-        <v>363</v>
+        <v>334</v>
       </c>
     </row>
     <row r="325" spans="1:1">
       <c r="A325" t="s">
-        <v>364</v>
+        <v>335</v>
       </c>
     </row>
     <row r="326" spans="1:1">
       <c r="A326" t="s">
-        <v>365</v>
+        <v>336</v>
       </c>
     </row>
     <row r="327" spans="1:1">
       <c r="A327" t="s">
-        <v>366</v>
+        <v>337</v>
       </c>
     </row>
     <row r="328" spans="1:1">
       <c r="A328" t="s">
-        <v>367</v>
+        <v>338</v>
       </c>
     </row>
     <row r="329" spans="1:1">
       <c r="A329" t="s">
-        <v>368</v>
+        <v>339</v>
       </c>
     </row>
     <row r="330" spans="1:1">
       <c r="A330" t="s">
-        <v>369</v>
+        <v>340</v>
       </c>
     </row>
     <row r="331" spans="1:1">
       <c r="A331" t="s">
-        <v>370</v>
+        <v>341</v>
       </c>
     </row>
     <row r="332" spans="1:1">
       <c r="A332" t="s">
-        <v>371</v>
+        <v>342</v>
       </c>
     </row>
     <row r="333" spans="1:1">
       <c r="A333" t="s">
-        <v>372</v>
+        <v>343</v>
       </c>
     </row>
     <row r="334" spans="1:1">
       <c r="A334" t="s">
-        <v>373</v>
+        <v>344</v>
       </c>
     </row>
     <row r="335" spans="1:1">
       <c r="A335" t="s">
-        <v>374</v>
+        <v>345</v>
       </c>
     </row>
     <row r="336" spans="1:1">
       <c r="A336" t="s">
-        <v>375</v>
+        <v>346</v>
       </c>
     </row>
     <row r="337" spans="1:1">
       <c r="A337" t="s">
-        <v>376</v>
+        <v>347</v>
       </c>
     </row>
     <row r="338" spans="1:1">
       <c r="A338" t="s">
-        <v>377</v>
+        <v>348</v>
       </c>
     </row>
     <row r="339" spans="1:1">
       <c r="A339" t="s">
-        <v>378</v>
+        <v>349</v>
       </c>
     </row>
     <row r="340" spans="1:1">
       <c r="A340" t="s">
-        <v>379</v>
+        <v>350</v>
       </c>
     </row>
     <row r="341" spans="1:1">
       <c r="A341" t="s">
-        <v>380</v>
+        <v>351</v>
       </c>
     </row>
     <row r="342" spans="1:1">
       <c r="A342" t="s">
-        <v>381</v>
+        <v>352</v>
       </c>
     </row>
     <row r="343" spans="1:1">
       <c r="A343" t="s">
-        <v>382</v>
+        <v>353</v>
       </c>
     </row>
     <row r="344" spans="1:1">
       <c r="A344" t="s">
-        <v>383</v>
+        <v>354</v>
       </c>
     </row>
     <row r="345" spans="1:1">
       <c r="A345" t="s">
-        <v>384</v>
+        <v>355</v>
       </c>
     </row>
     <row r="346" spans="1:1">
       <c r="A346" t="s">
-        <v>385</v>
+        <v>356</v>
       </c>
     </row>
     <row r="347" spans="1:1">
       <c r="A347" t="s">
-        <v>386</v>
+        <v>357</v>
       </c>
     </row>
     <row r="348" spans="1:1">
       <c r="A348" t="s">
-        <v>387</v>
+        <v>358</v>
       </c>
     </row>
     <row r="349" spans="1:1">
       <c r="A349" t="s">
-        <v>388</v>
+        <v>359</v>
       </c>
     </row>
     <row r="350" spans="1:1">
       <c r="A350" t="s">
-        <v>389</v>
+        <v>360</v>
       </c>
     </row>
     <row r="351" spans="1:1">
       <c r="A351" t="s">
-        <v>390</v>
+        <v>361</v>
       </c>
     </row>
     <row r="352" spans="1:1">
       <c r="A352" t="s">
-        <v>391</v>
+        <v>362</v>
       </c>
     </row>
     <row r="353" spans="1:1">
       <c r="A353" t="s">
-        <v>392</v>
+        <v>363</v>
       </c>
     </row>
     <row r="354" spans="1:1">
       <c r="A354" t="s">
-        <v>393</v>
+        <v>364</v>
       </c>
     </row>
     <row r="355" spans="1:1">
       <c r="A355" t="s">
-        <v>394</v>
+        <v>365</v>
       </c>
     </row>
     <row r="356" spans="1:1">
       <c r="A356" t="s">
-        <v>395</v>
+        <v>366</v>
       </c>
     </row>
     <row r="357" spans="1:1">
       <c r="A357" t="s">
-        <v>396</v>
+        <v>367</v>
       </c>
     </row>
     <row r="358" spans="1:1">
       <c r="A358" t="s">
-        <v>397</v>
+        <v>368</v>
       </c>
     </row>
     <row r="359" spans="1:1">
       <c r="A359" t="s">
-        <v>398</v>
+        <v>369</v>
       </c>
     </row>
     <row r="360" spans="1:1">
       <c r="A360" t="s">
-        <v>399</v>
+        <v>370</v>
       </c>
     </row>
     <row r="361" spans="1:1">
       <c r="A361" t="s">
-        <v>400</v>
+        <v>371</v>
       </c>
     </row>
     <row r="362" spans="1:1">
       <c r="A362" t="s">
-        <v>401</v>
+        <v>372</v>
       </c>
     </row>
     <row r="363" spans="1:1">
       <c r="A363" t="s">
-        <v>402</v>
+        <v>373</v>
       </c>
     </row>
     <row r="364" spans="1:1">
       <c r="A364" t="s">
-        <v>403</v>
+        <v>374</v>
       </c>
     </row>
     <row r="365" spans="1:1">
       <c r="A365" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="366" spans="1:1">
-      <c r="A366" t="s">
-        <v>405</v>
+        <v>375</v>
       </c>
     </row>
     <row r="367" spans="1:1">
       <c r="A367" t="s">
-        <v>406</v>
+        <v>376</v>
       </c>
     </row>
     <row r="368" spans="1:1">
       <c r="A368" t="s">
-        <v>407</v>
+        <v>377</v>
       </c>
     </row>
     <row r="369" spans="1:1">
       <c r="A369" t="s">
-        <v>408</v>
+        <v>378</v>
       </c>
     </row>
     <row r="370" spans="1:1">
       <c r="A370" t="s">
-        <v>409</v>
+        <v>379</v>
       </c>
     </row>
     <row r="371" spans="1:1">
       <c r="A371" t="s">
-        <v>410</v>
+        <v>380</v>
       </c>
     </row>
     <row r="372" spans="1:1">
       <c r="A372" t="s">
-        <v>411</v>
+        <v>381</v>
       </c>
     </row>
     <row r="373" spans="1:1">
       <c r="A373" t="s">
-        <v>412</v>
+        <v>382</v>
       </c>
     </row>
     <row r="374" spans="1:1">
       <c r="A374" t="s">
-        <v>413</v>
+        <v>383</v>
       </c>
     </row>
     <row r="375" spans="1:1">
       <c r="A375" t="s">
-        <v>414</v>
+        <v>384</v>
+      </c>
+    </row>
+    <row r="376" spans="1:1">
+      <c r="A376" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="377" spans="1:1">
       <c r="A377" t="s">
-        <v>415</v>
+        <v>386</v>
       </c>
     </row>
     <row r="378" spans="1:1">
       <c r="A378" t="s">
-        <v>416</v>
+        <v>387</v>
       </c>
     </row>
     <row r="379" spans="1:1">
       <c r="A379" t="s">
-        <v>417</v>
+        <v>388</v>
       </c>
     </row>
     <row r="380" spans="1:1">
       <c r="A380" t="s">
-        <v>418</v>
+        <v>389</v>
       </c>
     </row>
     <row r="381" spans="1:1">
       <c r="A381" t="s">
-        <v>419</v>
+        <v>390</v>
       </c>
     </row>
     <row r="382" spans="1:1">
       <c r="A382" t="s">
-        <v>420</v>
+        <v>391</v>
       </c>
     </row>
     <row r="383" spans="1:1">
       <c r="A383" t="s">
-        <v>421</v>
+        <v>392</v>
       </c>
     </row>
     <row r="384" spans="1:1">
       <c r="A384" t="s">
-        <v>422</v>
+        <v>393</v>
       </c>
     </row>
     <row r="385" spans="1:1">
       <c r="A385" t="s">
-        <v>423</v>
+        <v>394</v>
       </c>
     </row>
     <row r="386" spans="1:1">
       <c r="A386" t="s">
-        <v>424</v>
+        <v>395</v>
       </c>
     </row>
     <row r="387" spans="1:1">
       <c r="A387" t="s">
-        <v>425</v>
+        <v>396</v>
       </c>
     </row>
     <row r="388" spans="1:1">
       <c r="A388" t="s">
-        <v>426</v>
+        <v>397</v>
       </c>
     </row>
     <row r="389" spans="1:1">
       <c r="A389" t="s">
-        <v>427</v>
+        <v>398</v>
       </c>
     </row>
     <row r="390" spans="1:1">
       <c r="A390" t="s">
-        <v>428</v>
+        <v>399</v>
       </c>
     </row>
     <row r="391" spans="1:1">
       <c r="A391" t="s">
-        <v>429</v>
+        <v>400</v>
       </c>
     </row>
     <row r="392" spans="1:1">
       <c r="A392" t="s">
-        <v>430</v>
+        <v>401</v>
       </c>
     </row>
     <row r="393" spans="1:1">
       <c r="A393" t="s">
-        <v>431</v>
+        <v>402</v>
       </c>
     </row>
     <row r="394" spans="1:1">
       <c r="A394" t="s">
-        <v>432</v>
+        <v>403</v>
       </c>
     </row>
     <row r="395" spans="1:1">
       <c r="A395" t="s">
-        <v>433</v>
+        <v>404</v>
       </c>
     </row>
     <row r="396" spans="1:1">
       <c r="A396" t="s">
-        <v>434</v>
+        <v>405</v>
       </c>
     </row>
     <row r="397" spans="1:1">
       <c r="A397" t="s">
-        <v>435</v>
+        <v>406</v>
       </c>
     </row>
     <row r="398" spans="1:1">
       <c r="A398" t="s">
-        <v>436</v>
+        <v>407</v>
       </c>
     </row>
     <row r="399" spans="1:1">
       <c r="A399" t="s">
-        <v>437</v>
+        <v>408</v>
       </c>
     </row>
     <row r="400" spans="1:1">
       <c r="A400" t="s">
-        <v>438</v>
+        <v>409</v>
       </c>
     </row>
     <row r="401" spans="1:1">
       <c r="A401" t="s">
-        <v>439</v>
+        <v>410</v>
       </c>
     </row>
     <row r="402" spans="1:1">
       <c r="A402" t="s">
-        <v>440</v>
+        <v>411</v>
       </c>
     </row>
     <row r="403" spans="1:1">
       <c r="A403" t="s">
-        <v>441</v>
+        <v>412</v>
       </c>
     </row>
     <row r="404" spans="1:1">
       <c r="A404" t="s">
-        <v>442</v>
+        <v>413</v>
       </c>
     </row>
     <row r="405" spans="1:1">
       <c r="A405" t="s">
-        <v>443</v>
+        <v>414</v>
       </c>
     </row>
     <row r="406" spans="1:1">
       <c r="A406" t="s">
-        <v>444</v>
+        <v>415</v>
       </c>
     </row>
     <row r="407" spans="1:1">
       <c r="A407" t="s">
-        <v>445</v>
+        <v>416</v>
       </c>
     </row>
     <row r="408" spans="1:1">
       <c r="A408" t="s">
-        <v>446</v>
+        <v>417</v>
       </c>
     </row>
     <row r="409" spans="1:1">
       <c r="A409" t="s">
-        <v>447</v>
+        <v>418</v>
       </c>
     </row>
     <row r="410" spans="1:1">
       <c r="A410" t="s">
-        <v>448</v>
+        <v>419</v>
       </c>
     </row>
     <row r="411" spans="1:1">
       <c r="A411" t="s">
-        <v>449</v>
+        <v>420</v>
       </c>
     </row>
     <row r="412" spans="1:1">
       <c r="A412" t="s">
-        <v>450</v>
+        <v>421</v>
       </c>
     </row>
     <row r="413" spans="1:1">
       <c r="A413" t="s">
-        <v>451</v>
+        <v>422</v>
       </c>
     </row>
     <row r="414" spans="1:1">
       <c r="A414" t="s">
-        <v>452</v>
+        <v>423</v>
       </c>
     </row>
     <row r="415" spans="1:1">
       <c r="A415" t="s">
-        <v>453</v>
+        <v>424</v>
       </c>
     </row>
     <row r="416" spans="1:1">
       <c r="A416" t="s">
-        <v>454</v>
+        <v>425</v>
       </c>
     </row>
     <row r="417" spans="1:1">
       <c r="A417" t="s">
-        <v>455</v>
+        <v>426</v>
       </c>
     </row>
     <row r="418" spans="1:1">
       <c r="A418" t="s">
-        <v>456</v>
+        <v>427</v>
       </c>
     </row>
     <row r="419" spans="1:1">
       <c r="A419" t="s">
-        <v>457</v>
+        <v>428</v>
       </c>
     </row>
     <row r="420" spans="1:1">
       <c r="A420" t="s">
-        <v>458</v>
+        <v>429</v>
       </c>
     </row>
     <row r="421" spans="1:1">
       <c r="A421" t="s">
-        <v>459</v>
+        <v>430</v>
       </c>
     </row>
     <row r="422" spans="1:1">
       <c r="A422" t="s">
-        <v>460</v>
+        <v>431</v>
       </c>
     </row>
     <row r="423" spans="1:1">
       <c r="A423" t="s">
-        <v>461</v>
+        <v>432</v>
       </c>
     </row>
     <row r="424" spans="1:1">
       <c r="A424" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="425" spans="1:1">
-      <c r="A425" t="s">
-        <v>463</v>
+        <v>433</v>
       </c>
     </row>
     <row r="426" spans="1:1">
       <c r="A426" t="s">
-        <v>464</v>
+        <v>434</v>
       </c>
     </row>
     <row r="427" spans="1:1">
       <c r="A427" t="s">
-        <v>465</v>
+        <v>435</v>
       </c>
     </row>
     <row r="428" spans="1:1">
       <c r="A428" t="s">
-        <v>466</v>
+        <v>436</v>
       </c>
     </row>
     <row r="429" spans="1:1">
       <c r="A429" t="s">
-        <v>467</v>
+        <v>437</v>
       </c>
     </row>
     <row r="430" spans="1:1">
       <c r="A430" t="s">
-        <v>468</v>
+        <v>438</v>
       </c>
     </row>
     <row r="431" spans="1:1">
       <c r="A431" t="s">
-        <v>469</v>
+        <v>439</v>
       </c>
     </row>
     <row r="432" spans="1:1">
       <c r="A432" t="s">
-        <v>470</v>
+        <v>440</v>
       </c>
     </row>
     <row r="433" spans="1:1">
       <c r="A433" t="s">
-        <v>471</v>
+        <v>441</v>
       </c>
     </row>
     <row r="434" spans="1:1">
       <c r="A434" t="s">
-        <v>472</v>
+        <v>442</v>
+      </c>
+    </row>
+    <row r="435" spans="1:1">
+      <c r="A435" t="s">
+        <v>443</v>
       </c>
     </row>
     <row r="436" spans="1:1">
       <c r="A436" t="s">
-        <v>473</v>
+        <v>444</v>
       </c>
     </row>
     <row r="437" spans="1:1">
       <c r="A437" t="s">
-        <v>474</v>
+        <v>445</v>
       </c>
     </row>
     <row r="438" spans="1:1">
       <c r="A438" t="s">
-        <v>475</v>
+        <v>446</v>
       </c>
     </row>
     <row r="439" spans="1:1">
       <c r="A439" t="s">
-        <v>476</v>
+        <v>447</v>
       </c>
     </row>
     <row r="440" spans="1:1">
       <c r="A440" t="s">
-        <v>477</v>
+        <v>448</v>
       </c>
     </row>
     <row r="441" spans="1:1">
       <c r="A441" t="s">
-        <v>478</v>
+        <v>449</v>
       </c>
     </row>
     <row r="442" spans="1:1">
       <c r="A442" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="443" spans="1:1">
-      <c r="A443" t="s">
-        <v>480</v>
+        <v>450</v>
       </c>
     </row>
     <row r="444" spans="1:1">
       <c r="A444" t="s">
-        <v>481</v>
+        <v>451</v>
       </c>
     </row>
     <row r="445" spans="1:1">
       <c r="A445" t="s">
-        <v>482</v>
+        <v>452</v>
       </c>
     </row>
     <row r="446" spans="1:1">
       <c r="A446" t="s">
-        <v>483</v>
+        <v>453</v>
       </c>
     </row>
     <row r="447" spans="1:1">
       <c r="A447" t="s">
-        <v>484</v>
+        <v>454</v>
       </c>
     </row>
     <row r="448" spans="1:1">
       <c r="A448" t="s">
-        <v>485</v>
+        <v>455</v>
       </c>
     </row>
     <row r="449" spans="1:1">
       <c r="A449" t="s">
-        <v>486</v>
+        <v>456</v>
       </c>
     </row>
     <row r="450" spans="1:1">
       <c r="A450" t="s">
-        <v>487</v>
+        <v>457</v>
       </c>
     </row>
     <row r="451" spans="1:1">
       <c r="A451" t="s">
-        <v>488</v>
+        <v>458</v>
       </c>
     </row>
     <row r="452" spans="1:1">
       <c r="A452" t="s">
-        <v>489</v>
+        <v>459</v>
+      </c>
+    </row>
+    <row r="453" spans="1:1">
+      <c r="A453" t="s">
+        <v>460</v>
       </c>
     </row>
     <row r="454" spans="1:1">
       <c r="A454" t="s">
-        <v>490</v>
+        <v>461</v>
       </c>
     </row>
     <row r="455" spans="1:1">
       <c r="A455" t="s">
-        <v>491</v>
+        <v>462</v>
       </c>
     </row>
     <row r="456" spans="1:1">
       <c r="A456" t="s">
-        <v>492</v>
+        <v>463</v>
       </c>
     </row>
     <row r="457" spans="1:1">
       <c r="A457" t="s">
-        <v>493</v>
+        <v>464</v>
       </c>
     </row>
     <row r="458" spans="1:1">
       <c r="A458" t="s">
-        <v>494</v>
+        <v>465</v>
       </c>
     </row>
     <row r="459" spans="1:1">
       <c r="A459" t="s">
-        <v>495</v>
+        <v>466</v>
       </c>
     </row>
     <row r="460" spans="1:1">
       <c r="A460" t="s">
-        <v>496</v>
+        <v>467</v>
       </c>
     </row>
     <row r="461" spans="1:1">
       <c r="A461" t="s">
-        <v>497</v>
+        <v>468</v>
       </c>
     </row>
     <row r="462" spans="1:1">
       <c r="A462" t="s">
-        <v>498</v>
+        <v>469</v>
       </c>
     </row>
     <row r="463" spans="1:1">
       <c r="A463" t="s">
-        <v>499</v>
+        <v>470</v>
       </c>
     </row>
     <row r="464" spans="1:1">
       <c r="A464" t="s">
-        <v>500</v>
+        <v>471</v>
       </c>
     </row>
     <row r="465" spans="1:1">
       <c r="A465" t="s">
-        <v>501</v>
+        <v>472</v>
       </c>
     </row>
     <row r="466" spans="1:1">
       <c r="A466" t="s">
-        <v>502</v>
+        <v>473</v>
       </c>
     </row>
     <row r="467" spans="1:1">
       <c r="A467" t="s">
-        <v>503</v>
+        <v>474</v>
       </c>
     </row>
     <row r="468" spans="1:1">
       <c r="A468" t="s">
-        <v>504</v>
+        <v>475</v>
       </c>
     </row>
     <row r="469" spans="1:1">
       <c r="A469" t="s">
-        <v>505</v>
+        <v>476</v>
       </c>
     </row>
     <row r="470" spans="1:1">
       <c r="A470" t="s">
-        <v>506</v>
+        <v>477</v>
       </c>
     </row>
     <row r="471" spans="1:1">
       <c r="A471" t="s">
-        <v>507</v>
+        <v>478</v>
       </c>
     </row>
     <row r="472" spans="1:1">
       <c r="A472" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="473" spans="1:1">
-      <c r="A473" t="s">
-        <v>509</v>
+        <v>479</v>
       </c>
     </row>
     <row r="474" spans="1:1">
       <c r="A474" t="s">
-        <v>510</v>
+        <v>480</v>
       </c>
     </row>
     <row r="475" spans="1:1">
       <c r="A475" t="s">
-        <v>511</v>
+        <v>481</v>
       </c>
     </row>
     <row r="476" spans="1:1">
       <c r="A476" t="s">
-        <v>512</v>
+        <v>482</v>
       </c>
     </row>
     <row r="477" spans="1:1">
       <c r="A477" t="s">
-        <v>513</v>
+        <v>483</v>
       </c>
     </row>
     <row r="478" spans="1:1">
       <c r="A478" t="s">
-        <v>514</v>
+        <v>484</v>
       </c>
     </row>
     <row r="479" spans="1:1">
       <c r="A479" t="s">
-        <v>515</v>
+        <v>485</v>
       </c>
     </row>
     <row r="480" spans="1:1">
       <c r="A480" t="s">
-        <v>516</v>
+        <v>486</v>
       </c>
     </row>
     <row r="481" spans="1:1">
       <c r="A481" t="s">
-        <v>517</v>
+        <v>487</v>
       </c>
     </row>
     <row r="482" spans="1:1">
       <c r="A482" t="s">
-        <v>518</v>
+        <v>488</v>
+      </c>
+    </row>
+    <row r="483" spans="1:1">
+      <c r="A483" t="s">
+        <v>489</v>
       </c>
     </row>
     <row r="484" spans="1:1">
       <c r="A484" t="s">
-        <v>519</v>
+        <v>490</v>
       </c>
     </row>
     <row r="485" spans="1:1">
       <c r="A485" t="s">
-        <v>520</v>
+        <v>491</v>
       </c>
     </row>
     <row r="486" spans="1:1">
       <c r="A486" t="s">
-        <v>521</v>
+        <v>492</v>
       </c>
     </row>
     <row r="487" spans="1:1">
       <c r="A487" t="s">
-        <v>522</v>
+        <v>493</v>
       </c>
     </row>
     <row r="488" spans="1:1">
       <c r="A488" t="s">
-        <v>523</v>
+        <v>494</v>
       </c>
     </row>
     <row r="489" spans="1:1">
       <c r="A489" t="s">
-        <v>524</v>
+        <v>495</v>
       </c>
     </row>
     <row r="490" spans="1:1">
       <c r="A490" t="s">
-        <v>525</v>
+        <v>496</v>
       </c>
     </row>
     <row r="491" spans="1:1">
       <c r="A491" t="s">
-        <v>526</v>
+        <v>497</v>
       </c>
     </row>
     <row r="492" spans="1:1">
       <c r="A492" t="s">
-        <v>527</v>
+        <v>498</v>
       </c>
     </row>
     <row r="493" spans="1:1">
       <c r="A493" t="s">
-        <v>528</v>
+        <v>499</v>
       </c>
     </row>
     <row r="494" spans="1:1">
       <c r="A494" t="s">
-        <v>529</v>
+        <v>500</v>
       </c>
     </row>
     <row r="495" spans="1:1">
       <c r="A495" t="s">
-        <v>530</v>
+        <v>501</v>
       </c>
     </row>
     <row r="496" spans="1:1">
       <c r="A496" t="s">
-        <v>531</v>
+        <v>502</v>
       </c>
     </row>
     <row r="497" spans="1:1">
       <c r="A497" t="s">
-        <v>532</v>
+        <v>503</v>
       </c>
     </row>
     <row r="498" spans="1:1">
       <c r="A498" t="s">
-        <v>533</v>
+        <v>504</v>
       </c>
     </row>
     <row r="499" spans="1:1">
       <c r="A499" t="s">
-        <v>534</v>
+        <v>505</v>
       </c>
     </row>
     <row r="500" spans="1:1">
       <c r="A500" t="s">
-        <v>535</v>
+        <v>506</v>
       </c>
     </row>
     <row r="501" spans="1:1">
       <c r="A501" t="s">
-        <v>536</v>
+        <v>507</v>
       </c>
     </row>
     <row r="502" spans="1:1">
       <c r="A502" t="s">
-        <v>537</v>
+        <v>508</v>
       </c>
     </row>
     <row r="503" spans="1:1">
       <c r="A503" t="s">
-        <v>538</v>
+        <v>509</v>
       </c>
     </row>
     <row r="504" spans="1:1">
       <c r="A504" t="s">
-        <v>539</v>
+        <v>510</v>
       </c>
     </row>
     <row r="505" spans="1:1">
       <c r="A505" t="s">
-        <v>540</v>
+        <v>511</v>
       </c>
     </row>
     <row r="506" spans="1:1">
       <c r="A506" t="s">
-        <v>541</v>
+        <v>512</v>
       </c>
     </row>
     <row r="507" spans="1:1">
       <c r="A507" t="s">
-        <v>542</v>
+        <v>513</v>
       </c>
     </row>
     <row r="508" spans="1:1">
       <c r="A508" t="s">
-        <v>543</v>
+        <v>514</v>
       </c>
     </row>
     <row r="509" spans="1:1">
       <c r="A509" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="510" spans="1:1">
-      <c r="A510" t="s">
-        <v>545</v>
+        <v>515</v>
       </c>
     </row>
     <row r="511" spans="1:1">
       <c r="A511" t="s">
-        <v>546</v>
+        <v>516</v>
       </c>
     </row>
     <row r="512" spans="1:1">
       <c r="A512" t="s">
-        <v>547</v>
+        <v>517</v>
       </c>
     </row>
     <row r="513" spans="1:1">
       <c r="A513" t="s">
-        <v>548</v>
+        <v>518</v>
       </c>
     </row>
     <row r="514" spans="1:1">
       <c r="A514" t="s">
-        <v>549</v>
+        <v>519</v>
       </c>
     </row>
     <row r="515" spans="1:1">
       <c r="A515" t="s">
-        <v>550</v>
+        <v>520</v>
       </c>
     </row>
     <row r="516" spans="1:1">
       <c r="A516" t="s">
-        <v>551</v>
+        <v>521</v>
       </c>
     </row>
     <row r="517" spans="1:1">
       <c r="A517" t="s">
-        <v>552</v>
+        <v>522</v>
       </c>
     </row>
     <row r="518" spans="1:1">
       <c r="A518" t="s">
-        <v>553</v>
+        <v>523</v>
       </c>
     </row>
     <row r="519" spans="1:1">
       <c r="A519" t="s">
-        <v>554</v>
+        <v>524</v>
       </c>
     </row>
     <row r="520" spans="1:1">
       <c r="A520" t="s">
-        <v>555</v>
+        <v>525</v>
       </c>
     </row>
     <row r="521" spans="1:1">
       <c r="A521" t="s">
-        <v>556</v>
+        <v>526</v>
       </c>
     </row>
     <row r="522" spans="1:1">
       <c r="A522" t="s">
-        <v>557</v>
+        <v>527</v>
       </c>
     </row>
     <row r="523" spans="1:1">
       <c r="A523" t="s">
-        <v>558</v>
+        <v>528</v>
       </c>
     </row>
     <row r="524" spans="1:1">
       <c r="A524" t="s">
-        <v>559</v>
+        <v>529</v>
       </c>
     </row>
     <row r="525" spans="1:1">
       <c r="A525" t="s">
-        <v>560</v>
+        <v>530</v>
       </c>
     </row>
     <row r="526" spans="1:1">
       <c r="A526" t="s">
-        <v>561</v>
+        <v>531</v>
       </c>
     </row>
     <row r="527" spans="1:1">
       <c r="A527" t="s">
-        <v>562</v>
+        <v>532</v>
       </c>
     </row>
     <row r="528" spans="1:1">
       <c r="A528" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="529" spans="1:1">
-      <c r="A529" t="s">
-        <v>564</v>
+        <v>533</v>
       </c>
     </row>
     <row r="530" spans="1:1">
       <c r="A530" t="s">
-        <v>565</v>
+        <v>534</v>
       </c>
     </row>
     <row r="531" spans="1:1">
       <c r="A531" t="s">
-        <v>566</v>
+        <v>535</v>
       </c>
     </row>
     <row r="532" spans="1:1">
       <c r="A532" t="s">
-        <v>567</v>
+        <v>536</v>
+      </c>
+    </row>
+    <row r="533" spans="1:1">
+      <c r="A533" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="534" spans="1:1">
       <c r="A534" t="s">
-        <v>568</v>
+        <v>538</v>
       </c>
     </row>
     <row r="535" spans="1:1">
       <c r="A535" t="s">
-        <v>569</v>
+        <v>539</v>
       </c>
     </row>
     <row r="536" spans="1:1">
       <c r="A536" t="s">
-        <v>570</v>
+        <v>540</v>
       </c>
     </row>
     <row r="537" spans="1:1">
       <c r="A537" t="s">
-        <v>571</v>
+        <v>541</v>
       </c>
     </row>
     <row r="538" spans="1:1">
       <c r="A538" t="s">
-        <v>572</v>
+        <v>542</v>
       </c>
     </row>
     <row r="539" spans="1:1">
       <c r="A539" t="s">
-        <v>573</v>
+        <v>543</v>
       </c>
     </row>
     <row r="540" spans="1:1">
       <c r="A540" t="s">
-        <v>574</v>
+        <v>544</v>
       </c>
     </row>
     <row r="541" spans="1:1">
       <c r="A541" t="s">
-        <v>575</v>
+        <v>545</v>
       </c>
     </row>
     <row r="542" spans="1:1">
       <c r="A542" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="543" spans="1:1">
-      <c r="A543" t="s">
-        <v>577</v>
+        <v>546</v>
       </c>
     </row>
     <row r="544" spans="1:1">
       <c r="A544" t="s">
-        <v>578</v>
+        <v>547</v>
       </c>
     </row>
     <row r="545" spans="1:1">
       <c r="A545" t="s">
-        <v>579</v>
+        <v>548</v>
       </c>
     </row>
     <row r="546" spans="1:1">
       <c r="A546" t="s">
-        <v>580</v>
+        <v>549</v>
       </c>
     </row>
     <row r="547" spans="1:1">
       <c r="A547" t="s">
-        <v>581</v>
+        <v>550</v>
       </c>
     </row>
     <row r="548" spans="1:1">
       <c r="A548" t="s">
-        <v>582</v>
+        <v>551</v>
       </c>
     </row>
     <row r="549" spans="1:1">
       <c r="A549" t="s">
-        <v>583</v>
+        <v>552</v>
       </c>
     </row>
     <row r="550" spans="1:1">
       <c r="A550" t="s">
-        <v>584</v>
+        <v>553</v>
       </c>
     </row>
     <row r="551" spans="1:1">
       <c r="A551" t="s">
-        <v>585</v>
+        <v>554</v>
+      </c>
+    </row>
+    <row r="552" spans="1:1">
+      <c r="A552" t="s">
+        <v>555</v>
       </c>
     </row>
     <row r="553" spans="1:1">
       <c r="A553" t="s">
-        <v>586</v>
+        <v>556</v>
       </c>
     </row>
     <row r="554" spans="1:1">
       <c r="A554" t="s">
-        <v>587</v>
+        <v>557</v>
       </c>
     </row>
     <row r="555" spans="1:1">
       <c r="A555" t="s">
-        <v>588</v>
+        <v>558</v>
       </c>
     </row>
     <row r="556" spans="1:1">
       <c r="A556" t="s">
-        <v>589</v>
+        <v>559</v>
       </c>
     </row>
     <row r="557" spans="1:1">
       <c r="A557" t="s">
-        <v>590</v>
+        <v>560</v>
       </c>
     </row>
     <row r="558" spans="1:1">
       <c r="A558" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="559" spans="1:1">
-      <c r="A559" t="s">
-        <v>592</v>
+        <v>561</v>
       </c>
     </row>
     <row r="560" spans="1:1">
       <c r="A560" t="s">
-        <v>593</v>
+        <v>562</v>
       </c>
     </row>
     <row r="561" spans="1:1">
       <c r="A561" t="s">
-        <v>594</v>
+        <v>563</v>
       </c>
     </row>
     <row r="562" spans="1:1">
       <c r="A562" t="s">
-        <v>595</v>
+        <v>564</v>
       </c>
     </row>
     <row r="563" spans="1:1">
       <c r="A563" t="s">
-        <v>596</v>
+        <v>565</v>
       </c>
     </row>
     <row r="564" spans="1:1">
       <c r="A564" t="s">
-        <v>597</v>
+        <v>566</v>
       </c>
     </row>
     <row r="565" spans="1:1">
       <c r="A565" t="s">
-        <v>598</v>
+        <v>567</v>
       </c>
     </row>
     <row r="566" spans="1:1">
       <c r="A566" t="s">
-        <v>599</v>
+        <v>568</v>
       </c>
     </row>
     <row r="567" spans="1:1">
       <c r="A567" t="s">
-        <v>600</v>
+        <v>569</v>
       </c>
     </row>
     <row r="568" spans="1:1">
       <c r="A568" t="s">
-        <v>601</v>
+        <v>570</v>
       </c>
     </row>
     <row r="569" spans="1:1">
       <c r="A569" t="s">
-        <v>602</v>
+        <v>571</v>
       </c>
     </row>
     <row r="570" spans="1:1">
       <c r="A570" t="s">
-        <v>603</v>
+        <v>572</v>
       </c>
     </row>
     <row r="571" spans="1:1">
       <c r="A571" t="s">
-        <v>604</v>
+        <v>573</v>
       </c>
     </row>
     <row r="572" spans="1:1">
       <c r="A572" t="s">
-        <v>605</v>
+        <v>574</v>
       </c>
     </row>
     <row r="573" spans="1:1">
       <c r="A573" t="s">
-        <v>606</v>
+        <v>575</v>
       </c>
     </row>
     <row r="574" spans="1:1">
       <c r="A574" t="s">
-        <v>607</v>
+        <v>576</v>
       </c>
     </row>
     <row r="575" spans="1:1">
       <c r="A575" t="s">
-        <v>608</v>
+        <v>577</v>
       </c>
     </row>
     <row r="576" spans="1:1">
       <c r="A576" t="s">
-        <v>609</v>
+        <v>578</v>
+      </c>
+    </row>
+    <row r="577" spans="1:1">
+      <c r="A577" t="s">
+        <v>579</v>
       </c>
     </row>
     <row r="578" spans="1:1">
       <c r="A578" t="s">
-        <v>610</v>
+        <v>580</v>
       </c>
     </row>
     <row r="579" spans="1:1">
       <c r="A579" t="s">
-        <v>611</v>
+        <v>581</v>
       </c>
     </row>
     <row r="580" spans="1:1">
       <c r="A580" t="s">
-        <v>612</v>
+        <v>582</v>
       </c>
     </row>
     <row r="581" spans="1:1">
       <c r="A581" t="s">
-        <v>613</v>
+        <v>583</v>
       </c>
     </row>
     <row r="582" spans="1:1">
       <c r="A582" t="s">
-        <v>614</v>
+        <v>584</v>
       </c>
     </row>
     <row r="583" spans="1:1">
       <c r="A583" t="s">
-        <v>615</v>
+        <v>585</v>
       </c>
     </row>
     <row r="584" spans="1:1">
       <c r="A584" t="s">
-        <v>616</v>
+        <v>586</v>
       </c>
     </row>
     <row r="585" spans="1:1">
       <c r="A585" t="s">
-        <v>617</v>
+        <v>587</v>
       </c>
     </row>
     <row r="586" spans="1:1">
       <c r="A586" t="s">
-        <v>618</v>
+        <v>588</v>
       </c>
     </row>
     <row r="587" spans="1:1">
       <c r="A587" t="s">
-        <v>619</v>
+        <v>589</v>
       </c>
     </row>
     <row r="588" spans="1:1">
       <c r="A588" t="s">
-        <v>620</v>
+        <v>590</v>
       </c>
     </row>
     <row r="589" spans="1:1">
       <c r="A589" t="s">
-        <v>621</v>
+        <v>591</v>
       </c>
     </row>
     <row r="590" spans="1:1">
       <c r="A590" t="s">
-        <v>622</v>
+        <v>592</v>
       </c>
     </row>
     <row r="591" spans="1:1">
       <c r="A591" t="s">
-        <v>623</v>
+        <v>593</v>
       </c>
     </row>
     <row r="592" spans="1:1">
       <c r="A592" t="s">
-        <v>624</v>
+        <v>594</v>
+      </c>
+    </row>
+    <row r="593" spans="1:1">
+      <c r="A593" t="s">
+        <v>595</v>
       </c>
     </row>
     <row r="594" spans="1:1">
       <c r="A594" t="s">
-        <v>625</v>
+        <v>596</v>
       </c>
     </row>
     <row r="595" spans="1:1">
       <c r="A595" t="s">
-        <v>626</v>
+        <v>597</v>
       </c>
     </row>
     <row r="596" spans="1:1">
       <c r="A596" t="s">
-        <v>627</v>
+        <v>598</v>
       </c>
     </row>
     <row r="597" spans="1:1">
       <c r="A597" t="s">
-        <v>628</v>
+        <v>599</v>
       </c>
     </row>
     <row r="598" spans="1:1">
       <c r="A598" t="s">
-        <v>629</v>
+        <v>600</v>
       </c>
     </row>
     <row r="599" spans="1:1">
       <c r="A599" t="s">
-        <v>630</v>
+        <v>601</v>
       </c>
     </row>
     <row r="600" spans="1:1">
       <c r="A600" t="s">
-        <v>631</v>
+        <v>602</v>
       </c>
     </row>
     <row r="601" spans="1:1">
       <c r="A601" t="s">
-        <v>632</v>
+        <v>603</v>
       </c>
     </row>
     <row r="602" spans="1:1">
       <c r="A602" t="s">
-        <v>633</v>
+        <v>604</v>
       </c>
     </row>
     <row r="603" spans="1:1">
       <c r="A603" t="s">
-        <v>634</v>
+        <v>605</v>
       </c>
     </row>
     <row r="604" spans="1:1">
       <c r="A604" t="s">
-        <v>635</v>
+        <v>606</v>
       </c>
     </row>
     <row r="605" spans="1:1">
       <c r="A605" t="s">
-        <v>636</v>
+        <v>607</v>
       </c>
     </row>
     <row r="606" spans="1:1">
       <c r="A606" t="s">
-        <v>637</v>
+        <v>608</v>
       </c>
     </row>
     <row r="607" spans="1:1">
       <c r="A607" t="s">
-        <v>638</v>
+        <v>609</v>
       </c>
     </row>
     <row r="608" spans="1:1">
       <c r="A608" t="s">
-        <v>639</v>
+        <v>610</v>
       </c>
     </row>
     <row r="609" spans="1:1">
       <c r="A609" t="s">
-        <v>640</v>
+        <v>611</v>
       </c>
     </row>
     <row r="610" spans="1:1">
       <c r="A610" t="s">
-        <v>641</v>
+        <v>612</v>
       </c>
     </row>
     <row r="611" spans="1:1">
       <c r="A611" t="s">
-        <v>642</v>
+        <v>613</v>
       </c>
     </row>
     <row r="612" spans="1:1">
       <c r="A612" t="s">
-        <v>643</v>
+        <v>614</v>
       </c>
     </row>
     <row r="613" spans="1:1">
       <c r="A613" t="s">
-        <v>644</v>
+        <v>615</v>
       </c>
     </row>
     <row r="614" spans="1:1">
       <c r="A614" t="s">
-        <v>645</v>
+        <v>616</v>
       </c>
     </row>
     <row r="615" spans="1:1">
       <c r="A615" t="s">
-        <v>646</v>
+        <v>617</v>
       </c>
     </row>
     <row r="616" spans="1:1">
       <c r="A616" t="s">
-        <v>647</v>
+        <v>618</v>
       </c>
     </row>
     <row r="617" spans="1:1">
       <c r="A617" t="s">
-        <v>648</v>
+        <v>619</v>
       </c>
     </row>
     <row r="618" spans="1:1">
       <c r="A618" t="s">
-        <v>649</v>
+        <v>620</v>
       </c>
     </row>
     <row r="619" spans="1:1">
       <c r="A619" t="s">
-        <v>650</v>
+        <v>621</v>
       </c>
     </row>
     <row r="620" spans="1:1">
       <c r="A620" t="s">
-        <v>651</v>
+        <v>622</v>
       </c>
     </row>
     <row r="621" spans="1:1">
       <c r="A621" t="s">
-        <v>652</v>
+        <v>623</v>
       </c>
     </row>
     <row r="622" spans="1:1">
       <c r="A622" t="s">
-        <v>653</v>
+        <v>624</v>
       </c>
     </row>
     <row r="623" spans="1:1">
       <c r="A623" t="s">
-        <v>654</v>
+        <v>625</v>
       </c>
     </row>
     <row r="624" spans="1:1">
       <c r="A624" t="s">
-        <v>655</v>
+        <v>626</v>
       </c>
     </row>
     <row r="625" spans="1:1">
       <c r="A625" t="s">
-        <v>656</v>
+        <v>627</v>
       </c>
     </row>
     <row r="626" spans="1:1">
       <c r="A626" t="s">
-        <v>657</v>
+        <v>628</v>
       </c>
     </row>
     <row r="627" spans="1:1">
       <c r="A627" t="s">
-        <v>658</v>
+        <v>629</v>
       </c>
     </row>
     <row r="628" spans="1:1">
       <c r="A628" t="s">
-        <v>659</v>
+        <v>630</v>
       </c>
     </row>
     <row r="629" spans="1:1">
       <c r="A629" t="s">
-        <v>660</v>
+        <v>631</v>
       </c>
     </row>
     <row r="630" spans="1:1">
       <c r="A630" t="s">
-        <v>661</v>
-      </c>
-    </row>
-    <row r="631" spans="1:1">
-      <c r="A631" t="s">
-        <v>662</v>
+        <v>632</v>
       </c>
     </row>
     <row r="632" spans="1:1">
       <c r="A632" t="s">
-        <v>663</v>
+        <v>633</v>
       </c>
     </row>
     <row r="633" spans="1:1">
       <c r="A633" t="s">
-        <v>664</v>
+        <v>634</v>
       </c>
     </row>
     <row r="634" spans="1:1">
       <c r="A634" t="s">
-        <v>665</v>
+        <v>635</v>
       </c>
     </row>
     <row r="635" spans="1:1">
       <c r="A635" t="s">
-        <v>666</v>
+        <v>636</v>
       </c>
     </row>
     <row r="636" spans="1:1">
       <c r="A636" t="s">
-        <v>667</v>
+        <v>637</v>
       </c>
     </row>
     <row r="637" spans="1:1">
       <c r="A637" t="s">
-        <v>668</v>
+        <v>638</v>
       </c>
     </row>
     <row r="638" spans="1:1">
       <c r="A638" t="s">
-        <v>669</v>
+        <v>639</v>
       </c>
     </row>
     <row r="639" spans="1:1">
       <c r="A639" t="s">
-        <v>670</v>
+        <v>640</v>
       </c>
     </row>
     <row r="640" spans="1:1">
       <c r="A640" t="s">
-        <v>671</v>
+        <v>641</v>
       </c>
     </row>
     <row r="641" spans="1:1">
       <c r="A641" t="s">
-        <v>672</v>
-      </c>
-    </row>
-    <row r="642" spans="1:1">
-      <c r="A642" t="s">
-        <v>673</v>
+        <v>642</v>
       </c>
     </row>
     <row r="643" spans="1:1">
       <c r="A643" t="s">
-        <v>674</v>
+        <v>643</v>
       </c>
     </row>
     <row r="644" spans="1:1">
       <c r="A644" t="s">
-        <v>675</v>
+        <v>644</v>
       </c>
     </row>
     <row r="645" spans="1:1">
       <c r="A645" t="s">
-        <v>676</v>
+        <v>645</v>
       </c>
     </row>
     <row r="646" spans="1:1">
       <c r="A646" t="s">
-        <v>677</v>
-      </c>
-    </row>
-    <row r="647" spans="1:1">
-      <c r="A647" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="648" spans="1:1">
-      <c r="A648" t="s">
-        <v>679</v>
-      </c>
-    </row>
-    <row r="649" spans="1:1">
-      <c r="A649" t="s">
-        <v>680</v>
-      </c>
-    </row>
-    <row r="650" spans="1:1">
-      <c r="A650" t="s">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="651" spans="1:1">
-      <c r="A651" t="s">
-        <v>682</v>
-      </c>
-    </row>
-    <row r="652" spans="1:1">
-      <c r="A652" t="s">
-        <v>683</v>
-      </c>
-    </row>
-    <row r="653" spans="1:1">
-      <c r="A653" t="s">
-        <v>684</v>
-      </c>
-    </row>
-    <row r="654" spans="1:1">
-      <c r="A654" t="s">
-        <v>685</v>
-      </c>
-    </row>
-    <row r="655" spans="1:1">
-      <c r="A655" t="s">
-        <v>686</v>
-      </c>
-    </row>
-    <row r="656" spans="1:1">
-      <c r="A656" t="s">
-        <v>687</v>
-      </c>
-    </row>
-    <row r="657" spans="1:1">
-      <c r="A657" t="s">
-        <v>688</v>
-      </c>
-    </row>
-    <row r="658" spans="1:1">
-      <c r="A658" t="s">
-        <v>689</v>
-      </c>
-    </row>
-    <row r="659" spans="1:1">
-      <c r="A659" t="s">
-        <v>690</v>
-      </c>
-    </row>
-    <row r="660" spans="1:1">
-      <c r="A660" t="s">
-        <v>691</v>
-      </c>
-    </row>
-    <row r="661" spans="1:1">
-      <c r="A661" t="s">
-        <v>692</v>
-      </c>
-    </row>
-    <row r="662" spans="1:1">
-      <c r="A662" t="s">
-        <v>693</v>
-      </c>
-    </row>
-    <row r="663" spans="1:1">
-      <c r="A663" t="s">
-        <v>694</v>
-      </c>
-    </row>
-    <row r="664" spans="1:1">
-      <c r="A664" t="s">
-        <v>695</v>
-      </c>
-    </row>
-    <row r="666" spans="1:1">
-      <c r="A666" t="s">
-        <v>696</v>
-      </c>
-    </row>
-    <row r="667" spans="1:1">
-      <c r="A667" t="s">
-        <v>697</v>
-      </c>
-    </row>
-    <row r="668" spans="1:1">
-      <c r="A668" t="s">
-        <v>698</v>
-      </c>
-    </row>
-    <row r="669" spans="1:1">
-      <c r="A669" t="s">
-        <v>699</v>
-      </c>
-    </row>
-    <row r="670" spans="1:1">
-      <c r="A670" t="s">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="671" spans="1:1">
-      <c r="A671" t="s">
-        <v>701</v>
-      </c>
-    </row>
-    <row r="672" spans="1:1">
-      <c r="A672" t="s">
-        <v>702</v>
-      </c>
-    </row>
-    <row r="673" spans="1:1">
-      <c r="A673" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="674" spans="1:1">
-      <c r="A674" t="s">
-        <v>704</v>
-      </c>
-    </row>
-    <row r="675" spans="1:1">
-      <c r="A675" t="s">
-        <v>705</v>
-      </c>
-    </row>
-    <row r="677" spans="1:1">
-      <c r="A677" t="s">
-        <v>706</v>
-      </c>
-    </row>
-    <row r="678" spans="1:1">
-      <c r="A678" t="s">
-        <v>707</v>
-      </c>
-    </row>
-    <row r="679" spans="1:1">
-      <c r="A679" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="680" spans="1:1">
-      <c r="A680" t="s">
-        <v>709</v>
+        <v>646</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed hip profile issue
</commit_message>
<xml_diff>
--- a/templates/panos/set_commands/iron_skillet_panos_full.xlsx
+++ b/templates/panos/set_commands/iron_skillet_panos_full.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="812">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="813">
   <si>
     <t>Variable Name</t>
   </si>
@@ -1923,6 +1923,9 @@
   </si>
   <si>
     <t>set rulebase security rules ""Outbound Block Rule"" service any</t>
+  </si>
+  <si>
+    <t>set rulebase security rules ""Outbound Block Rule"" source-hip any</t>
   </si>
   <si>
     <t>set rulebase security rules ""Outbound Block Rule"" action deny</t>
@@ -3003,7 +3006,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:A810"/>
+  <dimension ref="A2:A812"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -6134,11 +6137,16 @@
     </row>
     <row r="642" spans="1:1">
       <c r="A642" t="s">
-        <v>649</v>
+        <v>636</v>
       </c>
     </row>
     <row r="643" spans="1:1">
       <c r="A643" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="644" spans="1:1">
+      <c r="A644" t="s">
         <v>650</v>
       </c>
     </row>
@@ -6147,93 +6155,93 @@
         <v>651</v>
       </c>
     </row>
-    <row r="646" spans="1:1">
-      <c r="A646" t="s">
-        <v>652</v>
-      </c>
-    </row>
     <row r="647" spans="1:1">
       <c r="A647" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="648" spans="1:1">
       <c r="A648" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="649" spans="1:1">
       <c r="A649" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="650" spans="1:1">
       <c r="A650" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="651" spans="1:1">
       <c r="A651" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="652" spans="1:1">
       <c r="A652" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="653" spans="1:1">
       <c r="A653" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="654" spans="1:1">
       <c r="A654" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="655" spans="1:1">
       <c r="A655" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="656" spans="1:1">
       <c r="A656" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="657" spans="1:1">
       <c r="A657" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="658" spans="1:1">
       <c r="A658" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="659" spans="1:1">
       <c r="A659" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="660" spans="1:1">
       <c r="A660" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="661" spans="1:1">
       <c r="A661" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="662" spans="1:1">
       <c r="A662" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="663" spans="1:1">
       <c r="A663" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="664" spans="1:1">
+      <c r="A664" t="s">
         <v>669</v>
       </c>
     </row>
@@ -6242,63 +6250,63 @@
         <v>670</v>
       </c>
     </row>
-    <row r="666" spans="1:1">
-      <c r="A666" t="s">
-        <v>671</v>
-      </c>
-    </row>
     <row r="667" spans="1:1">
       <c r="A667" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="668" spans="1:1">
       <c r="A668" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="669" spans="1:1">
       <c r="A669" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="670" spans="1:1">
       <c r="A670" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="671" spans="1:1">
       <c r="A671" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="672" spans="1:1">
       <c r="A672" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="673" spans="1:1">
       <c r="A673" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="674" spans="1:1">
       <c r="A674" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="675" spans="1:1">
       <c r="A675" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="676" spans="1:1">
       <c r="A676" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="677" spans="1:1">
       <c r="A677" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="678" spans="1:1">
+      <c r="A678" t="s">
         <v>682</v>
       </c>
     </row>
@@ -6307,218 +6315,218 @@
         <v>683</v>
       </c>
     </row>
-    <row r="680" spans="1:1">
-      <c r="A680" t="s">
-        <v>684</v>
-      </c>
-    </row>
     <row r="681" spans="1:1">
       <c r="A681" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="682" spans="1:1">
       <c r="A682" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="683" spans="1:1">
       <c r="A683" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="684" spans="1:1">
       <c r="A684" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="685" spans="1:1">
       <c r="A685" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="686" spans="1:1">
       <c r="A686" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="687" spans="1:1">
       <c r="A687" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="688" spans="1:1">
       <c r="A688" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="689" spans="1:1">
       <c r="A689" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="690" spans="1:1">
       <c r="A690" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="691" spans="1:1">
       <c r="A691" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="692" spans="1:1">
       <c r="A692" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="693" spans="1:1">
       <c r="A693" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="694" spans="1:1">
       <c r="A694" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="695" spans="1:1">
       <c r="A695" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="696" spans="1:1">
       <c r="A696" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="697" spans="1:1">
       <c r="A697" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="698" spans="1:1">
       <c r="A698" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="699" spans="1:1">
       <c r="A699" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="700" spans="1:1">
       <c r="A700" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="701" spans="1:1">
       <c r="A701" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="702" spans="1:1">
       <c r="A702" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="703" spans="1:1">
       <c r="A703" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="704" spans="1:1">
       <c r="A704" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="705" spans="1:1">
       <c r="A705" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="706" spans="1:1">
       <c r="A706" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="707" spans="1:1">
       <c r="A707" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="708" spans="1:1">
       <c r="A708" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="709" spans="1:1">
       <c r="A709" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="710" spans="1:1">
       <c r="A710" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="711" spans="1:1">
       <c r="A711" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="712" spans="1:1">
       <c r="A712" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="713" spans="1:1">
       <c r="A713" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="714" spans="1:1">
       <c r="A714" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="715" spans="1:1">
       <c r="A715" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="716" spans="1:1">
       <c r="A716" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="717" spans="1:1">
       <c r="A717" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="718" spans="1:1">
       <c r="A718" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="719" spans="1:1">
       <c r="A719" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="720" spans="1:1">
       <c r="A720" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="721" spans="1:1">
       <c r="A721" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="722" spans="1:1">
       <c r="A722" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="723" spans="1:1">
+      <c r="A723" t="s">
         <v>726</v>
       </c>
     </row>
@@ -6527,353 +6535,353 @@
         <v>727</v>
       </c>
     </row>
-    <row r="725" spans="1:1">
-      <c r="A725" t="s">
-        <v>728</v>
-      </c>
-    </row>
     <row r="726" spans="1:1">
       <c r="A726" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="727" spans="1:1">
       <c r="A727" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="728" spans="1:1">
       <c r="A728" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="729" spans="1:1">
       <c r="A729" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="730" spans="1:1">
       <c r="A730" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="731" spans="1:1">
       <c r="A731" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="732" spans="1:1">
       <c r="A732" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="733" spans="1:1">
       <c r="A733" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="734" spans="1:1">
       <c r="A734" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="735" spans="1:1">
       <c r="A735" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="736" spans="1:1">
       <c r="A736" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="737" spans="1:1">
       <c r="A737" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="738" spans="1:1">
       <c r="A738" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="739" spans="1:1">
       <c r="A739" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="740" spans="1:1">
       <c r="A740" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="741" spans="1:1">
       <c r="A741" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="742" spans="1:1">
       <c r="A742" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="743" spans="1:1">
       <c r="A743" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="744" spans="1:1">
       <c r="A744" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="745" spans="1:1">
       <c r="A745" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="746" spans="1:1">
       <c r="A746" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="747" spans="1:1">
       <c r="A747" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="748" spans="1:1">
       <c r="A748" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="749" spans="1:1">
       <c r="A749" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="750" spans="1:1">
       <c r="A750" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="751" spans="1:1">
       <c r="A751" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="752" spans="1:1">
       <c r="A752" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="753" spans="1:1">
       <c r="A753" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
     </row>
     <row r="754" spans="1:1">
       <c r="A754" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="755" spans="1:1">
       <c r="A755" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="756" spans="1:1">
       <c r="A756" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="757" spans="1:1">
       <c r="A757" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="758" spans="1:1">
       <c r="A758" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="759" spans="1:1">
       <c r="A759" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
     </row>
     <row r="760" spans="1:1">
       <c r="A760" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
     </row>
     <row r="761" spans="1:1">
       <c r="A761" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="762" spans="1:1">
       <c r="A762" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="763" spans="1:1">
       <c r="A763" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="764" spans="1:1">
       <c r="A764" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="765" spans="1:1">
       <c r="A765" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="766" spans="1:1">
       <c r="A766" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="767" spans="1:1">
       <c r="A767" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="768" spans="1:1">
       <c r="A768" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="769" spans="1:1">
       <c r="A769" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="770" spans="1:1">
       <c r="A770" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="771" spans="1:1">
       <c r="A771" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="772" spans="1:1">
       <c r="A772" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="773" spans="1:1">
       <c r="A773" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="774" spans="1:1">
       <c r="A774" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="775" spans="1:1">
       <c r="A775" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="776" spans="1:1">
       <c r="A776" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="777" spans="1:1">
       <c r="A777" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="778" spans="1:1">
       <c r="A778" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="779" spans="1:1">
       <c r="A779" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="780" spans="1:1">
       <c r="A780" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="781" spans="1:1">
       <c r="A781" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="782" spans="1:1">
       <c r="A782" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="783" spans="1:1">
       <c r="A783" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="784" spans="1:1">
       <c r="A784" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="785" spans="1:1">
       <c r="A785" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="786" spans="1:1">
       <c r="A786" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="787" spans="1:1">
       <c r="A787" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="788" spans="1:1">
       <c r="A788" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="789" spans="1:1">
       <c r="A789" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="790" spans="1:1">
       <c r="A790" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="791" spans="1:1">
       <c r="A791" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="792" spans="1:1">
       <c r="A792" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row r="793" spans="1:1">
       <c r="A793" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
     <row r="794" spans="1:1">
       <c r="A794" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="795" spans="1:1">
+      <c r="A795" t="s">
         <v>797</v>
       </c>
     </row>
@@ -6882,48 +6890,48 @@
         <v>798</v>
       </c>
     </row>
-    <row r="797" spans="1:1">
-      <c r="A797" t="s">
-        <v>799</v>
-      </c>
-    </row>
     <row r="798" spans="1:1">
       <c r="A798" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="799" spans="1:1">
       <c r="A799" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
     </row>
     <row r="800" spans="1:1">
       <c r="A800" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="801" spans="1:1">
       <c r="A801" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="802" spans="1:1">
       <c r="A802" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="803" spans="1:1">
       <c r="A803" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="804" spans="1:1">
       <c r="A804" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="805" spans="1:1">
       <c r="A805" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="806" spans="1:1">
+      <c r="A806" t="s">
         <v>807</v>
       </c>
     </row>
@@ -6932,19 +6940,24 @@
         <v>808</v>
       </c>
     </row>
-    <row r="808" spans="1:1">
-      <c r="A808" t="s">
-        <v>809</v>
-      </c>
-    </row>
     <row r="809" spans="1:1">
       <c r="A809" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="810" spans="1:1">
       <c r="A810" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="811" spans="1:1">
+      <c r="A811" t="s">
         <v>811</v>
+      </c>
+    </row>
+    <row r="812" spans="1:1">
+      <c r="A812" t="s">
+        <v>812</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixes for hip profile bug
</commit_message>
<xml_diff>
--- a/templates/panos/set_commands/iron_skillet_panos_full.xlsx
+++ b/templates/panos/set_commands/iron_skillet_panos_full.xlsx
@@ -1889,7 +1889,7 @@
     <t>set rulebase security rules ""Outbound Block Rule"" service any</t>
   </si>
   <si>
-    <t>set rulebase security rules ""Outbound Block Rule"" hip-profiles any</t>
+    <t>set rulebase security rules ""Outbound Block Rule"" source-hip any</t>
   </si>
   <si>
     <t>set rulebase security rules ""Outbound Block Rule"" action deny</t>
@@ -1928,7 +1928,7 @@
     <t>set rulebase security rules ""Inbound Block Rule"" service any</t>
   </si>
   <si>
-    <t>set rulebase security rules ""Inbound Block Rule"" hip-profiles any</t>
+    <t>set rulebase security rules ""Inbound Block Rule"" source-hip any</t>
   </si>
   <si>
     <t>set rulebase security rules ""Inbound Block Rule"" action deny</t>

</xml_diff>